<commit_message>
Timeline updated following team meeting 3 on 22 may 22
</commit_message>
<xml_diff>
--- a/Timeline/Project_Timeline.xlsx
+++ b/Timeline/Project_Timeline.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Library/Mobile Documents/com~apple~CloudDocs/Uni/Level_5_Modules/CM2020_AgileSoftwareProjects/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Desktop/agile/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEFA630F-918D-B448-9394-B6F2689A1C8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86357510-2C0A-6940-8B68-A5FC3546FF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="28040" windowHeight="16660" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
+    <workbookView xWindow="360" yWindow="500" windowWidth="48860" windowHeight="16660" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>ASP - Group Project</t>
   </si>
@@ -70,10 +70,6 @@
   <si>
     <t xml:space="preserve">Midterm 
 Group submission </t>
-  </si>
-  <si>
-    <t>Team Meeting 2 - Requirements
-Determine collective project requirements</t>
   </si>
   <si>
     <t xml:space="preserve">Group introductions and initial contact on Slack </t>
@@ -171,6 +167,210 @@
   <si>
     <t xml:space="preserve">Connor unable to attend due to medical appointments, information will be submitted to the Slack channel prior to the meeting.
 </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Team Meeting 3 - Finalising Requirements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Determine collective project requirements and ensure everyone is happy with the plan moving forward 
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Team Meeting 2 - Requirements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Determine collective project requirements</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Team Meeting 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- scheduled for 1400 GMT - link to be provided on Slack
+Initial design updates </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">All team members to review the following for presentation at the next team meeting.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>User requirements</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- functional requirements 
+- technical requirements
+The overall aim of the project
+The key project stakeholders
+Explore other programs that provide a similar service to the one proposed</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Positive meeting with the following being discussed
+- Connor will take the team leader position after unianomous approval from the group. 
+- Github has been updated with a file directory for each phase of the project
+- Requirements have been finalised pending review when the midterm marking rubric is released. 
+- p5.js and charts.js will form the backbone of the project
+- the team will look into the viability of the svelte framework for ease of producing the frontend. This will be reviewed at the next team meeting
+- the project now enters the design phase. Ben and Thavelarn will scope wireframes, Connor, David and Kashka will scope pseudocode for some of the functions contained in the project.
+- The team meetings will now be held on Sundays at 1400GMT as it is more convenient to the team.
+- files uploaded to GitHub will be markdown file format from now on to allow ease of use within GitHub. There was an issue with .doc files in GitHub and would force each team member to download the file to see the contents
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All team members to review the following for presentation at the next team meeting.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- viability of using the svelte framework for web design 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Connor, Kashka, David</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Start to scope pseudocode for certain functions that may be required in the project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ben, Thavelarn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Start to design the wireframes for the individual functionality and design of the project.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -178,9 +378,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
+    <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -224,6 +424,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="9">
@@ -276,7 +481,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -398,11 +603,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -410,30 +652,42 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -464,43 +718,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="18">
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -508,16 +742,6 @@
       <fill>
         <patternFill>
           <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -538,126 +762,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C5700"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0" tint="-0.14996795556505021"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="2" tint="-0.24994659260841701"/>
         </patternFill>
       </fill>
     </dxf>
@@ -978,8 +1082,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3400B0-A312-474B-BDD8-7EBBB1942BA5}">
   <dimension ref="A1:FA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" topLeftCell="R2" workbookViewId="0">
+      <selection activeCell="AC5" sqref="AC5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -988,266 +1092,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="13"/>
-      <c r="K1" s="13"/>
-      <c r="L1" s="13"/>
-      <c r="M1" s="13"/>
-      <c r="N1" s="13"/>
-      <c r="O1" s="13"/>
-      <c r="P1" s="13"/>
-      <c r="Q1" s="13"/>
-      <c r="R1" s="13"/>
-      <c r="S1" s="13"/>
-      <c r="T1" s="13"/>
-      <c r="U1" s="13"/>
-      <c r="V1" s="13"/>
-      <c r="W1" s="13"/>
-      <c r="X1" s="13"/>
-      <c r="Y1" s="13"/>
-      <c r="Z1" s="13"/>
-      <c r="AA1" s="13"/>
-      <c r="AB1" s="13"/>
-      <c r="AC1" s="13"/>
-      <c r="AD1" s="13"/>
-      <c r="AE1" s="13"/>
-      <c r="AF1" s="13"/>
-      <c r="AG1" s="13"/>
-      <c r="AH1" s="13"/>
-      <c r="AI1" s="13"/>
-      <c r="AJ1" s="13"/>
-      <c r="AK1" s="13"/>
-      <c r="AL1" s="13"/>
-      <c r="AM1" s="13"/>
-      <c r="AN1" s="13"/>
-      <c r="AO1" s="13"/>
-      <c r="AP1" s="13"/>
-      <c r="AQ1" s="13"/>
-      <c r="AR1" s="13"/>
-      <c r="AS1" s="13"/>
-      <c r="AT1" s="13"/>
-      <c r="AU1" s="13"/>
-      <c r="AV1" s="13"/>
-      <c r="AW1" s="13"/>
-      <c r="AX1" s="13"/>
-      <c r="AY1" s="13"/>
-      <c r="AZ1" s="13"/>
-      <c r="BA1" s="13"/>
-      <c r="BB1" s="13"/>
-      <c r="BC1" s="13"/>
-      <c r="BD1" s="13"/>
-      <c r="BE1" s="13"/>
-      <c r="BF1" s="13"/>
-      <c r="BG1" s="13"/>
-      <c r="BH1" s="13"/>
-      <c r="BI1" s="13"/>
-      <c r="BJ1" s="13"/>
-      <c r="BK1" s="13"/>
-      <c r="BL1" s="13"/>
-      <c r="BM1" s="13"/>
-      <c r="BN1" s="13"/>
-      <c r="BO1" s="13"/>
-      <c r="BP1" s="13"/>
-      <c r="BQ1" s="13"/>
-      <c r="BR1" s="13"/>
-      <c r="BS1" s="13"/>
-      <c r="BT1" s="13"/>
-      <c r="BU1" s="13"/>
-      <c r="BV1" s="13"/>
-      <c r="BW1" s="13"/>
-      <c r="BX1" s="13"/>
-      <c r="BY1" s="13"/>
-      <c r="BZ1" s="13"/>
-      <c r="CA1" s="13"/>
-      <c r="CB1" s="13"/>
-      <c r="CC1" s="13"/>
-      <c r="CD1" s="13"/>
-      <c r="CE1" s="13"/>
-      <c r="CF1" s="13"/>
-      <c r="CG1" s="13"/>
-      <c r="CH1" s="13"/>
-      <c r="CI1" s="13"/>
-      <c r="CJ1" s="13"/>
-      <c r="CK1" s="13"/>
-      <c r="CL1" s="13"/>
-      <c r="CM1" s="13"/>
-      <c r="CN1" s="13"/>
-      <c r="CO1" s="13"/>
-      <c r="CP1" s="13"/>
-      <c r="CQ1" s="13"/>
-      <c r="CR1" s="13"/>
-      <c r="CS1" s="13"/>
-      <c r="CT1" s="13"/>
-      <c r="CU1" s="13"/>
-      <c r="CV1" s="13"/>
-      <c r="CW1" s="13"/>
-      <c r="CX1" s="13"/>
-      <c r="CY1" s="13"/>
-      <c r="CZ1" s="13"/>
-      <c r="DA1" s="13"/>
-      <c r="DB1" s="13"/>
-      <c r="DC1" s="13"/>
-      <c r="DD1" s="13"/>
-      <c r="DE1" s="13"/>
-      <c r="DF1" s="13"/>
-      <c r="DG1" s="13"/>
-      <c r="DH1" s="13"/>
-      <c r="DI1" s="13"/>
-      <c r="DJ1" s="13"/>
-      <c r="DK1" s="13"/>
-      <c r="DL1" s="13"/>
-      <c r="DM1" s="13"/>
-      <c r="DN1" s="13"/>
-      <c r="DO1" s="13"/>
-      <c r="DP1" s="13"/>
-      <c r="DQ1" s="13"/>
-      <c r="DR1" s="13"/>
-      <c r="DS1" s="13"/>
-      <c r="DT1" s="13"/>
-      <c r="DU1" s="13"/>
-      <c r="DV1" s="13"/>
-      <c r="DW1" s="13"/>
-      <c r="DX1" s="14"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="17"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="17"/>
+      <c r="AZ1" s="17"/>
+      <c r="BA1" s="17"/>
+      <c r="BB1" s="17"/>
+      <c r="BC1" s="17"/>
+      <c r="BD1" s="17"/>
+      <c r="BE1" s="17"/>
+      <c r="BF1" s="17"/>
+      <c r="BG1" s="17"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
+      <c r="BM1" s="17"/>
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="17"/>
+      <c r="BP1" s="17"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
+      <c r="BS1" s="17"/>
+      <c r="BT1" s="17"/>
+      <c r="BU1" s="17"/>
+      <c r="BV1" s="17"/>
+      <c r="BW1" s="17"/>
+      <c r="BX1" s="17"/>
+      <c r="BY1" s="17"/>
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="17"/>
+      <c r="CB1" s="17"/>
+      <c r="CC1" s="17"/>
+      <c r="CD1" s="17"/>
+      <c r="CE1" s="17"/>
+      <c r="CF1" s="17"/>
+      <c r="CG1" s="17"/>
+      <c r="CH1" s="17"/>
+      <c r="CI1" s="17"/>
+      <c r="CJ1" s="17"/>
+      <c r="CK1" s="17"/>
+      <c r="CL1" s="17"/>
+      <c r="CM1" s="17"/>
+      <c r="CN1" s="17"/>
+      <c r="CO1" s="17"/>
+      <c r="CP1" s="17"/>
+      <c r="CQ1" s="17"/>
+      <c r="CR1" s="17"/>
+      <c r="CS1" s="17"/>
+      <c r="CT1" s="17"/>
+      <c r="CU1" s="17"/>
+      <c r="CV1" s="17"/>
+      <c r="CW1" s="17"/>
+      <c r="CX1" s="17"/>
+      <c r="CY1" s="17"/>
+      <c r="CZ1" s="17"/>
+      <c r="DA1" s="17"/>
+      <c r="DB1" s="17"/>
+      <c r="DC1" s="17"/>
+      <c r="DD1" s="17"/>
+      <c r="DE1" s="17"/>
+      <c r="DF1" s="17"/>
+      <c r="DG1" s="17"/>
+      <c r="DH1" s="17"/>
+      <c r="DI1" s="17"/>
+      <c r="DJ1" s="17"/>
+      <c r="DK1" s="17"/>
+      <c r="DL1" s="17"/>
+      <c r="DM1" s="17"/>
+      <c r="DN1" s="17"/>
+      <c r="DO1" s="17"/>
+      <c r="DP1" s="17"/>
+      <c r="DQ1" s="17"/>
+      <c r="DR1" s="17"/>
+      <c r="DS1" s="17"/>
+      <c r="DT1" s="17"/>
+      <c r="DU1" s="17"/>
+      <c r="DV1" s="17"/>
+      <c r="DW1" s="17"/>
+      <c r="DX1" s="18"/>
     </row>
     <row r="2" spans="1:157" s="4" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="15"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="16"/>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="16"/>
-      <c r="I2" s="16"/>
-      <c r="J2" s="16"/>
-      <c r="K2" s="16"/>
-      <c r="L2" s="16"/>
-      <c r="M2" s="16"/>
-      <c r="N2" s="16"/>
-      <c r="O2" s="16"/>
-      <c r="P2" s="16"/>
-      <c r="Q2" s="16"/>
-      <c r="R2" s="16"/>
-      <c r="S2" s="16"/>
-      <c r="T2" s="16"/>
-      <c r="U2" s="16"/>
-      <c r="V2" s="16"/>
-      <c r="W2" s="16"/>
-      <c r="X2" s="16"/>
-      <c r="Y2" s="16"/>
-      <c r="Z2" s="16"/>
-      <c r="AA2" s="16"/>
-      <c r="AB2" s="16"/>
-      <c r="AC2" s="16"/>
-      <c r="AD2" s="16"/>
-      <c r="AE2" s="16"/>
-      <c r="AF2" s="16"/>
-      <c r="AG2" s="16"/>
-      <c r="AH2" s="16"/>
-      <c r="AI2" s="16"/>
-      <c r="AJ2" s="16"/>
-      <c r="AK2" s="16"/>
-      <c r="AL2" s="16"/>
-      <c r="AM2" s="16"/>
-      <c r="AN2" s="16"/>
-      <c r="AO2" s="16"/>
-      <c r="AP2" s="16"/>
-      <c r="AQ2" s="16"/>
-      <c r="AR2" s="16"/>
-      <c r="AS2" s="16"/>
-      <c r="AT2" s="16"/>
-      <c r="AU2" s="16"/>
-      <c r="AV2" s="16"/>
-      <c r="AW2" s="16"/>
-      <c r="AX2" s="16"/>
-      <c r="AY2" s="16"/>
-      <c r="AZ2" s="16"/>
-      <c r="BA2" s="16"/>
-      <c r="BB2" s="16"/>
-      <c r="BC2" s="16"/>
-      <c r="BD2" s="16"/>
-      <c r="BE2" s="16"/>
-      <c r="BF2" s="16"/>
-      <c r="BG2" s="16"/>
-      <c r="BH2" s="16"/>
-      <c r="BI2" s="16"/>
-      <c r="BJ2" s="16"/>
-      <c r="BK2" s="16"/>
-      <c r="BL2" s="16"/>
-      <c r="BM2" s="16"/>
-      <c r="BN2" s="16"/>
-      <c r="BO2" s="16"/>
-      <c r="BP2" s="16"/>
-      <c r="BQ2" s="16"/>
-      <c r="BR2" s="16"/>
-      <c r="BS2" s="16"/>
-      <c r="BT2" s="16"/>
-      <c r="BU2" s="16"/>
-      <c r="BV2" s="16"/>
-      <c r="BW2" s="16"/>
-      <c r="BX2" s="16"/>
-      <c r="BY2" s="16"/>
-      <c r="BZ2" s="16"/>
-      <c r="CA2" s="16"/>
-      <c r="CB2" s="16"/>
-      <c r="CC2" s="16"/>
-      <c r="CD2" s="16"/>
-      <c r="CE2" s="16"/>
-      <c r="CF2" s="16"/>
-      <c r="CG2" s="16"/>
-      <c r="CH2" s="16"/>
-      <c r="CI2" s="16"/>
-      <c r="CJ2" s="16"/>
-      <c r="CK2" s="16"/>
-      <c r="CL2" s="16"/>
-      <c r="CM2" s="16"/>
-      <c r="CN2" s="16"/>
-      <c r="CO2" s="16"/>
-      <c r="CP2" s="16"/>
-      <c r="CQ2" s="16"/>
-      <c r="CR2" s="16"/>
-      <c r="CS2" s="16"/>
-      <c r="CT2" s="16"/>
-      <c r="CU2" s="16"/>
-      <c r="CV2" s="16"/>
-      <c r="CW2" s="16"/>
-      <c r="CX2" s="16"/>
-      <c r="CY2" s="16"/>
-      <c r="CZ2" s="16"/>
-      <c r="DA2" s="16"/>
-      <c r="DB2" s="16"/>
-      <c r="DC2" s="16"/>
-      <c r="DD2" s="16"/>
-      <c r="DE2" s="16"/>
-      <c r="DF2" s="16"/>
-      <c r="DG2" s="16"/>
-      <c r="DH2" s="16"/>
-      <c r="DI2" s="16"/>
-      <c r="DJ2" s="16"/>
-      <c r="DK2" s="16"/>
-      <c r="DL2" s="16"/>
-      <c r="DM2" s="16"/>
-      <c r="DN2" s="16"/>
-      <c r="DO2" s="16"/>
-      <c r="DP2" s="16"/>
-      <c r="DQ2" s="16"/>
-      <c r="DR2" s="16"/>
-      <c r="DS2" s="16"/>
-      <c r="DT2" s="16"/>
-      <c r="DU2" s="16"/>
-      <c r="DV2" s="16"/>
-      <c r="DW2" s="16"/>
-      <c r="DX2" s="17"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+      <c r="AM2" s="20"/>
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="20"/>
+      <c r="AQ2" s="20"/>
+      <c r="AR2" s="20"/>
+      <c r="AS2" s="20"/>
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="20"/>
+      <c r="AZ2" s="20"/>
+      <c r="BA2" s="20"/>
+      <c r="BB2" s="20"/>
+      <c r="BC2" s="20"/>
+      <c r="BD2" s="20"/>
+      <c r="BE2" s="20"/>
+      <c r="BF2" s="20"/>
+      <c r="BG2" s="20"/>
+      <c r="BH2" s="20"/>
+      <c r="BI2" s="20"/>
+      <c r="BJ2" s="20"/>
+      <c r="BK2" s="20"/>
+      <c r="BL2" s="20"/>
+      <c r="BM2" s="20"/>
+      <c r="BN2" s="20"/>
+      <c r="BO2" s="20"/>
+      <c r="BP2" s="20"/>
+      <c r="BQ2" s="20"/>
+      <c r="BR2" s="20"/>
+      <c r="BS2" s="20"/>
+      <c r="BT2" s="20"/>
+      <c r="BU2" s="20"/>
+      <c r="BV2" s="20"/>
+      <c r="BW2" s="20"/>
+      <c r="BX2" s="20"/>
+      <c r="BY2" s="20"/>
+      <c r="BZ2" s="20"/>
+      <c r="CA2" s="20"/>
+      <c r="CB2" s="20"/>
+      <c r="CC2" s="20"/>
+      <c r="CD2" s="20"/>
+      <c r="CE2" s="20"/>
+      <c r="CF2" s="20"/>
+      <c r="CG2" s="20"/>
+      <c r="CH2" s="20"/>
+      <c r="CI2" s="20"/>
+      <c r="CJ2" s="20"/>
+      <c r="CK2" s="20"/>
+      <c r="CL2" s="20"/>
+      <c r="CM2" s="20"/>
+      <c r="CN2" s="20"/>
+      <c r="CO2" s="20"/>
+      <c r="CP2" s="20"/>
+      <c r="CQ2" s="20"/>
+      <c r="CR2" s="20"/>
+      <c r="CS2" s="20"/>
+      <c r="CT2" s="20"/>
+      <c r="CU2" s="20"/>
+      <c r="CV2" s="20"/>
+      <c r="CW2" s="20"/>
+      <c r="CX2" s="20"/>
+      <c r="CY2" s="20"/>
+      <c r="CZ2" s="20"/>
+      <c r="DA2" s="20"/>
+      <c r="DB2" s="20"/>
+      <c r="DC2" s="20"/>
+      <c r="DD2" s="20"/>
+      <c r="DE2" s="20"/>
+      <c r="DF2" s="20"/>
+      <c r="DG2" s="20"/>
+      <c r="DH2" s="20"/>
+      <c r="DI2" s="20"/>
+      <c r="DJ2" s="20"/>
+      <c r="DK2" s="20"/>
+      <c r="DL2" s="20"/>
+      <c r="DM2" s="20"/>
+      <c r="DN2" s="20"/>
+      <c r="DO2" s="20"/>
+      <c r="DP2" s="20"/>
+      <c r="DQ2" s="20"/>
+      <c r="DR2" s="20"/>
+      <c r="DS2" s="20"/>
+      <c r="DT2" s="20"/>
+      <c r="DU2" s="20"/>
+      <c r="DV2" s="20"/>
+      <c r="DW2" s="20"/>
+      <c r="DX2" s="21"/>
     </row>
     <row r="3" spans="1:157" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1639,266 +1743,297 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="5" t="s">
+      <c r="B4" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="5"/>
-      <c r="I4" s="6" t="s">
+      <c r="C4" s="14"/>
+      <c r="D4" s="14"/>
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6" t="s">
+      <c r="J4" s="10"/>
+      <c r="K4" s="10"/>
+      <c r="L4" s="10"/>
+      <c r="M4" s="10"/>
+      <c r="N4" s="10"/>
+      <c r="O4" s="10"/>
+      <c r="P4" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="6"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="7" t="s">
+      <c r="Q4" s="10"/>
+      <c r="R4" s="10"/>
+      <c r="S4" s="10"/>
+      <c r="T4" s="10"/>
+      <c r="U4" s="10"/>
+      <c r="V4" s="10"/>
+      <c r="W4" s="11" t="s">
+        <v>15</v>
+      </c>
+      <c r="X4" s="11"/>
+      <c r="Y4" s="11"/>
+      <c r="Z4" s="11"/>
+      <c r="AA4" s="11"/>
+      <c r="AB4" s="11"/>
+      <c r="AC4" s="11"/>
+      <c r="AD4" s="11"/>
+      <c r="AE4" s="11"/>
+      <c r="AF4" s="11"/>
+      <c r="AG4" s="11"/>
+      <c r="AH4" s="11"/>
+      <c r="AI4" s="11"/>
+      <c r="AJ4" s="11"/>
+      <c r="AK4" s="11"/>
+      <c r="AL4" s="11"/>
+      <c r="AM4" s="11"/>
+      <c r="AN4" s="11"/>
+      <c r="AO4" s="11"/>
+      <c r="AP4" s="11"/>
+      <c r="AQ4" s="11"/>
+      <c r="AR4" s="11"/>
+      <c r="AS4" s="11"/>
+      <c r="AT4" s="11"/>
+      <c r="AU4" s="11"/>
+      <c r="AV4" s="11"/>
+      <c r="AW4" s="11"/>
+      <c r="AX4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="X4" s="7"/>
-      <c r="Y4" s="7"/>
-      <c r="Z4" s="7"/>
-      <c r="AA4" s="7"/>
-      <c r="AB4" s="7"/>
-      <c r="AC4" s="7"/>
-      <c r="AD4" s="7"/>
-      <c r="AE4" s="7"/>
-      <c r="AF4" s="7"/>
-      <c r="AG4" s="7"/>
-      <c r="AH4" s="7"/>
-      <c r="AI4" s="7"/>
-      <c r="AJ4" s="7"/>
-      <c r="AK4" s="7"/>
-      <c r="AL4" s="7"/>
-      <c r="AM4" s="7"/>
-      <c r="AN4" s="7"/>
-      <c r="AO4" s="7"/>
-      <c r="AP4" s="7"/>
-      <c r="AQ4" s="7"/>
-      <c r="AR4" s="7"/>
-      <c r="AS4" s="7"/>
-      <c r="AT4" s="7"/>
-      <c r="AU4" s="7"/>
-      <c r="AV4" s="7"/>
-      <c r="AW4" s="7"/>
-      <c r="AX4" s="21" t="s">
+      <c r="AY4" s="13"/>
+      <c r="AZ4" s="13"/>
+      <c r="BA4" s="13"/>
+      <c r="BB4" s="13"/>
+      <c r="BC4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="AY4" s="21"/>
-      <c r="AZ4" s="21"/>
-      <c r="BA4" s="21"/>
-      <c r="BB4" s="21"/>
-      <c r="BC4" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="BD4" s="22"/>
-      <c r="BE4" s="8" t="s">
+      <c r="BD4" s="12"/>
+      <c r="BE4" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="BF4" s="9" t="s">
+      <c r="BF4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="BG4" s="10"/>
-      <c r="BH4" s="10"/>
-      <c r="BI4" s="10"/>
-      <c r="BJ4" s="10"/>
-      <c r="BK4" s="10"/>
-      <c r="BL4" s="10"/>
-      <c r="BM4" s="10"/>
-      <c r="BN4" s="10"/>
-      <c r="BO4" s="10"/>
-      <c r="BP4" s="10"/>
-      <c r="BQ4" s="10"/>
-      <c r="BR4" s="10"/>
-      <c r="BS4" s="10"/>
-      <c r="BT4" s="10"/>
-      <c r="BU4" s="10"/>
-      <c r="BV4" s="10"/>
-      <c r="BW4" s="10"/>
-      <c r="BX4" s="10"/>
-      <c r="BY4" s="10"/>
-      <c r="BZ4" s="10"/>
-      <c r="CA4" s="10"/>
-      <c r="CB4" s="10"/>
-      <c r="CC4" s="10"/>
-      <c r="CD4" s="10"/>
-      <c r="CE4" s="10"/>
-      <c r="CF4" s="10"/>
-      <c r="CG4" s="10"/>
-      <c r="CH4" s="10"/>
-      <c r="CI4" s="10"/>
-      <c r="CJ4" s="10"/>
-      <c r="CK4" s="10"/>
-      <c r="CL4" s="10"/>
-      <c r="CM4" s="10"/>
-      <c r="CN4" s="10"/>
-      <c r="CO4" s="10"/>
-      <c r="CP4" s="10"/>
-      <c r="CQ4" s="10"/>
-      <c r="CR4" s="10"/>
-      <c r="CS4" s="10"/>
-      <c r="CT4" s="10"/>
-      <c r="CU4" s="10"/>
-      <c r="CV4" s="10"/>
-      <c r="CW4" s="10"/>
-      <c r="CX4" s="10"/>
-      <c r="CY4" s="10"/>
-      <c r="CZ4" s="10"/>
-      <c r="DA4" s="10"/>
-      <c r="DB4" s="10"/>
-      <c r="DC4" s="10"/>
-      <c r="DD4" s="10"/>
-      <c r="DE4" s="10"/>
-      <c r="DF4" s="10"/>
-      <c r="DG4" s="10"/>
-      <c r="DH4" s="10"/>
-      <c r="DI4" s="10"/>
-      <c r="DJ4" s="10"/>
-      <c r="DK4" s="10"/>
-      <c r="DL4" s="10"/>
-      <c r="DM4" s="10"/>
-      <c r="DN4" s="10"/>
-      <c r="DO4" s="10"/>
-      <c r="DP4" s="10"/>
-      <c r="DQ4" s="10"/>
-      <c r="DR4" s="10"/>
-      <c r="DS4" s="10"/>
-      <c r="DT4" s="10"/>
-      <c r="DU4" s="10"/>
-      <c r="DV4" s="10"/>
-      <c r="DW4" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="DX4" s="9" t="s">
+      <c r="BG4" s="5"/>
+      <c r="BH4" s="5"/>
+      <c r="BI4" s="5"/>
+      <c r="BJ4" s="5"/>
+      <c r="BK4" s="5"/>
+      <c r="BL4" s="5"/>
+      <c r="BM4" s="5"/>
+      <c r="BN4" s="5"/>
+      <c r="BO4" s="5"/>
+      <c r="BP4" s="5"/>
+      <c r="BQ4" s="5"/>
+      <c r="BR4" s="5"/>
+      <c r="BS4" s="5"/>
+      <c r="BT4" s="5"/>
+      <c r="BU4" s="5"/>
+      <c r="BV4" s="5"/>
+      <c r="BW4" s="5"/>
+      <c r="BX4" s="5"/>
+      <c r="BY4" s="5"/>
+      <c r="BZ4" s="5"/>
+      <c r="CA4" s="5"/>
+      <c r="CB4" s="5"/>
+      <c r="CC4" s="5"/>
+      <c r="CD4" s="5"/>
+      <c r="CE4" s="5"/>
+      <c r="CF4" s="5"/>
+      <c r="CG4" s="5"/>
+      <c r="CH4" s="5"/>
+      <c r="CI4" s="5"/>
+      <c r="CJ4" s="5"/>
+      <c r="CK4" s="5"/>
+      <c r="CL4" s="5"/>
+      <c r="CM4" s="5"/>
+      <c r="CN4" s="5"/>
+      <c r="CO4" s="5"/>
+      <c r="CP4" s="5"/>
+      <c r="CQ4" s="5"/>
+      <c r="CR4" s="5"/>
+      <c r="CS4" s="5"/>
+      <c r="CT4" s="5"/>
+      <c r="CU4" s="5"/>
+      <c r="CV4" s="5"/>
+      <c r="CW4" s="5"/>
+      <c r="CX4" s="5"/>
+      <c r="CY4" s="5"/>
+      <c r="CZ4" s="5"/>
+      <c r="DA4" s="5"/>
+      <c r="DB4" s="5"/>
+      <c r="DC4" s="5"/>
+      <c r="DD4" s="5"/>
+      <c r="DE4" s="5"/>
+      <c r="DF4" s="5"/>
+      <c r="DG4" s="5"/>
+      <c r="DH4" s="5"/>
+      <c r="DI4" s="5"/>
+      <c r="DJ4" s="5"/>
+      <c r="DK4" s="5"/>
+      <c r="DL4" s="5"/>
+      <c r="DM4" s="5"/>
+      <c r="DN4" s="5"/>
+      <c r="DO4" s="5"/>
+      <c r="DP4" s="5"/>
+      <c r="DQ4" s="5"/>
+      <c r="DR4" s="5"/>
+      <c r="DS4" s="5"/>
+      <c r="DT4" s="5"/>
+      <c r="DU4" s="5"/>
+      <c r="DV4" s="5"/>
+      <c r="DW4" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="DY4" s="10"/>
-      <c r="DZ4" s="10"/>
-      <c r="EA4" s="10"/>
-      <c r="EB4" s="10"/>
-      <c r="EC4" s="10"/>
-      <c r="ED4" s="10"/>
-      <c r="EE4" s="10"/>
-      <c r="EF4" s="10"/>
-      <c r="EG4" s="10"/>
-      <c r="EH4" s="10"/>
-      <c r="EI4" s="10"/>
-      <c r="EJ4" s="10"/>
-      <c r="EK4" s="10"/>
-      <c r="EL4" s="10"/>
-      <c r="EM4" s="10"/>
-      <c r="EN4" s="10"/>
-      <c r="EO4" s="10"/>
-      <c r="EP4" s="10"/>
-      <c r="EQ4" s="10"/>
-      <c r="ER4" s="10"/>
-      <c r="ES4" s="10"/>
-      <c r="ET4" s="10"/>
-      <c r="EU4" s="10"/>
-      <c r="EV4" s="10"/>
-      <c r="EW4" s="10"/>
-      <c r="EX4" s="10"/>
-      <c r="EY4" s="10"/>
-      <c r="EZ4" s="10"/>
-      <c r="FA4" s="10"/>
+      <c r="DX4" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="DY4" s="5"/>
+      <c r="DZ4" s="5"/>
+      <c r="EA4" s="5"/>
+      <c r="EB4" s="5"/>
+      <c r="EC4" s="5"/>
+      <c r="ED4" s="5"/>
+      <c r="EE4" s="5"/>
+      <c r="EF4" s="5"/>
+      <c r="EG4" s="5"/>
+      <c r="EH4" s="5"/>
+      <c r="EI4" s="5"/>
+      <c r="EJ4" s="5"/>
+      <c r="EK4" s="5"/>
+      <c r="EL4" s="5"/>
+      <c r="EM4" s="5"/>
+      <c r="EN4" s="5"/>
+      <c r="EO4" s="5"/>
+      <c r="EP4" s="5"/>
+      <c r="EQ4" s="5"/>
+      <c r="ER4" s="5"/>
+      <c r="ES4" s="5"/>
+      <c r="ET4" s="5"/>
+      <c r="EU4" s="5"/>
+      <c r="EV4" s="5"/>
+      <c r="EW4" s="5"/>
+      <c r="EX4" s="5"/>
+      <c r="EY4" s="5"/>
+      <c r="EZ4" s="5"/>
+      <c r="FA4" s="5"/>
     </row>
     <row r="5" spans="1:157" s="4" customFormat="1" ht="223" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="11" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+      <c r="G5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="18" t="s">
-        <v>20</v>
-      </c>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="20"/>
+      <c r="I5" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
       <c r="N5" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="BE5" s="8"/>
-      <c r="BF5" s="9"/>
-      <c r="DW5" s="8"/>
-      <c r="DX5" s="9"/>
+        <v>22</v>
+      </c>
+      <c r="O5" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="24"/>
+      <c r="V5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="W5" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="24"/>
+      <c r="AC5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="BE5" s="9"/>
+      <c r="BF5" s="8"/>
+      <c r="DW5" s="9"/>
+      <c r="DX5" s="8"/>
     </row>
-    <row r="6" spans="1:157" s="4" customFormat="1" ht="244" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="BE6" s="8"/>
-      <c r="BF6" s="9"/>
-      <c r="DW6" s="8"/>
-      <c r="DX6" s="9"/>
+        <v>20</v>
+      </c>
+      <c r="V6" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="BE6" s="9"/>
+      <c r="BF6" s="8"/>
+      <c r="DW6" s="9"/>
+      <c r="DX6" s="8"/>
     </row>
-    <row r="7" spans="1:157" s="4" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="BF7" s="9"/>
-      <c r="DX7" s="9"/>
+    <row r="7" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="V7" s="28"/>
+      <c r="BF7" s="8"/>
+      <c r="DX7" s="8"/>
     </row>
-    <row r="8" spans="1:157" s="4" customFormat="1" ht="17" x14ac:dyDescent="0.2">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:157" s="4" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="24">
+      <c r="B8" s="7">
         <f ca="1">TODAY()</f>
-        <v>44693</v>
-      </c>
+        <v>44703</v>
+      </c>
+      <c r="V8" s="27"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
+    <mergeCell ref="A1:DX2"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="O5:U5"/>
+    <mergeCell ref="W5:AB5"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="BF4:BF7"/>
+    <mergeCell ref="BE4:BE6"/>
+    <mergeCell ref="V6:V8"/>
     <mergeCell ref="DX4:DX7"/>
     <mergeCell ref="DW4:DW6"/>
     <mergeCell ref="P4:V4"/>
     <mergeCell ref="W4:AW4"/>
     <mergeCell ref="BC4:BD4"/>
     <mergeCell ref="AX4:BB4"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="BF4:BF7"/>
-    <mergeCell ref="BE4:BE6"/>
-    <mergeCell ref="A1:DX2"/>
-    <mergeCell ref="I5:M5"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:XFD3">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
       <formula>$B$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>$B$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>$B$8</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Uodated meeting log and timeline following meeting 29 May 22
</commit_message>
<xml_diff>
--- a/Timeline/Project_Timeline.xlsx
+++ b/Timeline/Project_Timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10507"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Desktop/agile/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86357510-2C0A-6940-8B68-A5FC3546FF2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EAFB68-A829-0747-BF5A-840430574620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="500" windowWidth="48860" windowHeight="16660" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
   <si>
     <t>ASP - Group Project</t>
   </si>
@@ -215,30 +215,6 @@
       </rPr>
       <t xml:space="preserve">
 Determine collective project requirements</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Team Meeting 4 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">- scheduled for 1400 GMT - link to be provided on Slack
-Initial design updates </t>
     </r>
   </si>
   <si>
@@ -372,6 +348,203 @@
 - Start to design the wireframes for the individual functionality and design of the project.</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Team Meeting 4 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Design</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Initial design updates </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Team Meeting 5 - Design</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Collating all the design updates</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Team Meeting 6 - Finalising Design</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Collating the team's voted ideas for the final design - this will be from a vote (likely on Slack)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Team Meeting 7 - Proposal </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Distributing the tasks required for the Proposal submission</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">
+- Team is progressing well with initial designs. 
+- The team will now produce the the opposite of the design they produced last week 
+(wireframes -&gt; pseudocode // pseudocode -&gt; wireframes)
+- Team decided to have the project hosted on a web server once compelete</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">To review the following for presentation at the next team meeting
+Connor, Kashka, David
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Start to design the wireframes for the individual functionality and design of the project.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Ben, Thavelarn</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Start to scope pseudocode for certain functions that may be required in the project
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">**IF TIME PERMITS**
+All team members
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Update the Requirements-&gt;Final_Requirements files within the GitHub repo.
+</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -380,7 +553,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -430,8 +603,16 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -480,6 +661,30 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="14">
     <border>
@@ -644,7 +849,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -667,13 +872,55 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -685,50 +932,20 @@
     <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1082,8 +1299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3400B0-A312-474B-BDD8-7EBBB1942BA5}">
   <dimension ref="A1:FA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R2" workbookViewId="0">
-      <selection activeCell="AC5" sqref="AC5"/>
+    <sheetView tabSelected="1" topLeftCell="X6" workbookViewId="0">
+      <selection activeCell="AH6" sqref="AH6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1092,266 +1309,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="17"/>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="17"/>
-      <c r="AM1" s="17"/>
-      <c r="AN1" s="17"/>
-      <c r="AO1" s="17"/>
-      <c r="AP1" s="17"/>
-      <c r="AQ1" s="17"/>
-      <c r="AR1" s="17"/>
-      <c r="AS1" s="17"/>
-      <c r="AT1" s="17"/>
-      <c r="AU1" s="17"/>
-      <c r="AV1" s="17"/>
-      <c r="AW1" s="17"/>
-      <c r="AX1" s="17"/>
-      <c r="AY1" s="17"/>
-      <c r="AZ1" s="17"/>
-      <c r="BA1" s="17"/>
-      <c r="BB1" s="17"/>
-      <c r="BC1" s="17"/>
-      <c r="BD1" s="17"/>
-      <c r="BE1" s="17"/>
-      <c r="BF1" s="17"/>
-      <c r="BG1" s="17"/>
-      <c r="BH1" s="17"/>
-      <c r="BI1" s="17"/>
-      <c r="BJ1" s="17"/>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="17"/>
-      <c r="BM1" s="17"/>
-      <c r="BN1" s="17"/>
-      <c r="BO1" s="17"/>
-      <c r="BP1" s="17"/>
-      <c r="BQ1" s="17"/>
-      <c r="BR1" s="17"/>
-      <c r="BS1" s="17"/>
-      <c r="BT1" s="17"/>
-      <c r="BU1" s="17"/>
-      <c r="BV1" s="17"/>
-      <c r="BW1" s="17"/>
-      <c r="BX1" s="17"/>
-      <c r="BY1" s="17"/>
-      <c r="BZ1" s="17"/>
-      <c r="CA1" s="17"/>
-      <c r="CB1" s="17"/>
-      <c r="CC1" s="17"/>
-      <c r="CD1" s="17"/>
-      <c r="CE1" s="17"/>
-      <c r="CF1" s="17"/>
-      <c r="CG1" s="17"/>
-      <c r="CH1" s="17"/>
-      <c r="CI1" s="17"/>
-      <c r="CJ1" s="17"/>
-      <c r="CK1" s="17"/>
-      <c r="CL1" s="17"/>
-      <c r="CM1" s="17"/>
-      <c r="CN1" s="17"/>
-      <c r="CO1" s="17"/>
-      <c r="CP1" s="17"/>
-      <c r="CQ1" s="17"/>
-      <c r="CR1" s="17"/>
-      <c r="CS1" s="17"/>
-      <c r="CT1" s="17"/>
-      <c r="CU1" s="17"/>
-      <c r="CV1" s="17"/>
-      <c r="CW1" s="17"/>
-      <c r="CX1" s="17"/>
-      <c r="CY1" s="17"/>
-      <c r="CZ1" s="17"/>
-      <c r="DA1" s="17"/>
-      <c r="DB1" s="17"/>
-      <c r="DC1" s="17"/>
-      <c r="DD1" s="17"/>
-      <c r="DE1" s="17"/>
-      <c r="DF1" s="17"/>
-      <c r="DG1" s="17"/>
-      <c r="DH1" s="17"/>
-      <c r="DI1" s="17"/>
-      <c r="DJ1" s="17"/>
-      <c r="DK1" s="17"/>
-      <c r="DL1" s="17"/>
-      <c r="DM1" s="17"/>
-      <c r="DN1" s="17"/>
-      <c r="DO1" s="17"/>
-      <c r="DP1" s="17"/>
-      <c r="DQ1" s="17"/>
-      <c r="DR1" s="17"/>
-      <c r="DS1" s="17"/>
-      <c r="DT1" s="17"/>
-      <c r="DU1" s="17"/>
-      <c r="DV1" s="17"/>
-      <c r="DW1" s="17"/>
-      <c r="DX1" s="18"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="9"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+      <c r="T1" s="9"/>
+      <c r="U1" s="9"/>
+      <c r="V1" s="9"/>
+      <c r="W1" s="9"/>
+      <c r="X1" s="9"/>
+      <c r="Y1" s="9"/>
+      <c r="Z1" s="9"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
+      <c r="AG1" s="9"/>
+      <c r="AH1" s="9"/>
+      <c r="AI1" s="9"/>
+      <c r="AJ1" s="9"/>
+      <c r="AK1" s="9"/>
+      <c r="AL1" s="9"/>
+      <c r="AM1" s="9"/>
+      <c r="AN1" s="9"/>
+      <c r="AO1" s="9"/>
+      <c r="AP1" s="9"/>
+      <c r="AQ1" s="9"/>
+      <c r="AR1" s="9"/>
+      <c r="AS1" s="9"/>
+      <c r="AT1" s="9"/>
+      <c r="AU1" s="9"/>
+      <c r="AV1" s="9"/>
+      <c r="AW1" s="9"/>
+      <c r="AX1" s="9"/>
+      <c r="AY1" s="9"/>
+      <c r="AZ1" s="9"/>
+      <c r="BA1" s="9"/>
+      <c r="BB1" s="9"/>
+      <c r="BC1" s="9"/>
+      <c r="BD1" s="9"/>
+      <c r="BE1" s="9"/>
+      <c r="BF1" s="9"/>
+      <c r="BG1" s="9"/>
+      <c r="BH1" s="9"/>
+      <c r="BI1" s="9"/>
+      <c r="BJ1" s="9"/>
+      <c r="BK1" s="9"/>
+      <c r="BL1" s="9"/>
+      <c r="BM1" s="9"/>
+      <c r="BN1" s="9"/>
+      <c r="BO1" s="9"/>
+      <c r="BP1" s="9"/>
+      <c r="BQ1" s="9"/>
+      <c r="BR1" s="9"/>
+      <c r="BS1" s="9"/>
+      <c r="BT1" s="9"/>
+      <c r="BU1" s="9"/>
+      <c r="BV1" s="9"/>
+      <c r="BW1" s="9"/>
+      <c r="BX1" s="9"/>
+      <c r="BY1" s="9"/>
+      <c r="BZ1" s="9"/>
+      <c r="CA1" s="9"/>
+      <c r="CB1" s="9"/>
+      <c r="CC1" s="9"/>
+      <c r="CD1" s="9"/>
+      <c r="CE1" s="9"/>
+      <c r="CF1" s="9"/>
+      <c r="CG1" s="9"/>
+      <c r="CH1" s="9"/>
+      <c r="CI1" s="9"/>
+      <c r="CJ1" s="9"/>
+      <c r="CK1" s="9"/>
+      <c r="CL1" s="9"/>
+      <c r="CM1" s="9"/>
+      <c r="CN1" s="9"/>
+      <c r="CO1" s="9"/>
+      <c r="CP1" s="9"/>
+      <c r="CQ1" s="9"/>
+      <c r="CR1" s="9"/>
+      <c r="CS1" s="9"/>
+      <c r="CT1" s="9"/>
+      <c r="CU1" s="9"/>
+      <c r="CV1" s="9"/>
+      <c r="CW1" s="9"/>
+      <c r="CX1" s="9"/>
+      <c r="CY1" s="9"/>
+      <c r="CZ1" s="9"/>
+      <c r="DA1" s="9"/>
+      <c r="DB1" s="9"/>
+      <c r="DC1" s="9"/>
+      <c r="DD1" s="9"/>
+      <c r="DE1" s="9"/>
+      <c r="DF1" s="9"/>
+      <c r="DG1" s="9"/>
+      <c r="DH1" s="9"/>
+      <c r="DI1" s="9"/>
+      <c r="DJ1" s="9"/>
+      <c r="DK1" s="9"/>
+      <c r="DL1" s="9"/>
+      <c r="DM1" s="9"/>
+      <c r="DN1" s="9"/>
+      <c r="DO1" s="9"/>
+      <c r="DP1" s="9"/>
+      <c r="DQ1" s="9"/>
+      <c r="DR1" s="9"/>
+      <c r="DS1" s="9"/>
+      <c r="DT1" s="9"/>
+      <c r="DU1" s="9"/>
+      <c r="DV1" s="9"/>
+      <c r="DW1" s="9"/>
+      <c r="DX1" s="10"/>
     </row>
     <row r="2" spans="1:157" s="4" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-      <c r="AQ2" s="20"/>
-      <c r="AR2" s="20"/>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AU2" s="20"/>
-      <c r="AV2" s="20"/>
-      <c r="AW2" s="20"/>
-      <c r="AX2" s="20"/>
-      <c r="AY2" s="20"/>
-      <c r="AZ2" s="20"/>
-      <c r="BA2" s="20"/>
-      <c r="BB2" s="20"/>
-      <c r="BC2" s="20"/>
-      <c r="BD2" s="20"/>
-      <c r="BE2" s="20"/>
-      <c r="BF2" s="20"/>
-      <c r="BG2" s="20"/>
-      <c r="BH2" s="20"/>
-      <c r="BI2" s="20"/>
-      <c r="BJ2" s="20"/>
-      <c r="BK2" s="20"/>
-      <c r="BL2" s="20"/>
-      <c r="BM2" s="20"/>
-      <c r="BN2" s="20"/>
-      <c r="BO2" s="20"/>
-      <c r="BP2" s="20"/>
-      <c r="BQ2" s="20"/>
-      <c r="BR2" s="20"/>
-      <c r="BS2" s="20"/>
-      <c r="BT2" s="20"/>
-      <c r="BU2" s="20"/>
-      <c r="BV2" s="20"/>
-      <c r="BW2" s="20"/>
-      <c r="BX2" s="20"/>
-      <c r="BY2" s="20"/>
-      <c r="BZ2" s="20"/>
-      <c r="CA2" s="20"/>
-      <c r="CB2" s="20"/>
-      <c r="CC2" s="20"/>
-      <c r="CD2" s="20"/>
-      <c r="CE2" s="20"/>
-      <c r="CF2" s="20"/>
-      <c r="CG2" s="20"/>
-      <c r="CH2" s="20"/>
-      <c r="CI2" s="20"/>
-      <c r="CJ2" s="20"/>
-      <c r="CK2" s="20"/>
-      <c r="CL2" s="20"/>
-      <c r="CM2" s="20"/>
-      <c r="CN2" s="20"/>
-      <c r="CO2" s="20"/>
-      <c r="CP2" s="20"/>
-      <c r="CQ2" s="20"/>
-      <c r="CR2" s="20"/>
-      <c r="CS2" s="20"/>
-      <c r="CT2" s="20"/>
-      <c r="CU2" s="20"/>
-      <c r="CV2" s="20"/>
-      <c r="CW2" s="20"/>
-      <c r="CX2" s="20"/>
-      <c r="CY2" s="20"/>
-      <c r="CZ2" s="20"/>
-      <c r="DA2" s="20"/>
-      <c r="DB2" s="20"/>
-      <c r="DC2" s="20"/>
-      <c r="DD2" s="20"/>
-      <c r="DE2" s="20"/>
-      <c r="DF2" s="20"/>
-      <c r="DG2" s="20"/>
-      <c r="DH2" s="20"/>
-      <c r="DI2" s="20"/>
-      <c r="DJ2" s="20"/>
-      <c r="DK2" s="20"/>
-      <c r="DL2" s="20"/>
-      <c r="DM2" s="20"/>
-      <c r="DN2" s="20"/>
-      <c r="DO2" s="20"/>
-      <c r="DP2" s="20"/>
-      <c r="DQ2" s="20"/>
-      <c r="DR2" s="20"/>
-      <c r="DS2" s="20"/>
-      <c r="DT2" s="20"/>
-      <c r="DU2" s="20"/>
-      <c r="DV2" s="20"/>
-      <c r="DW2" s="20"/>
-      <c r="DX2" s="21"/>
+      <c r="A2" s="11"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="12"/>
+      <c r="H2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="12"/>
+      <c r="O2" s="12"/>
+      <c r="P2" s="12"/>
+      <c r="Q2" s="12"/>
+      <c r="R2" s="12"/>
+      <c r="S2" s="12"/>
+      <c r="T2" s="12"/>
+      <c r="U2" s="12"/>
+      <c r="V2" s="12"/>
+      <c r="W2" s="12"/>
+      <c r="X2" s="12"/>
+      <c r="Y2" s="12"/>
+      <c r="Z2" s="12"/>
+      <c r="AA2" s="12"/>
+      <c r="AB2" s="12"/>
+      <c r="AC2" s="12"/>
+      <c r="AD2" s="12"/>
+      <c r="AE2" s="12"/>
+      <c r="AF2" s="12"/>
+      <c r="AG2" s="12"/>
+      <c r="AH2" s="12"/>
+      <c r="AI2" s="12"/>
+      <c r="AJ2" s="12"/>
+      <c r="AK2" s="12"/>
+      <c r="AL2" s="12"/>
+      <c r="AM2" s="12"/>
+      <c r="AN2" s="12"/>
+      <c r="AO2" s="12"/>
+      <c r="AP2" s="12"/>
+      <c r="AQ2" s="12"/>
+      <c r="AR2" s="12"/>
+      <c r="AS2" s="12"/>
+      <c r="AT2" s="12"/>
+      <c r="AU2" s="12"/>
+      <c r="AV2" s="12"/>
+      <c r="AW2" s="12"/>
+      <c r="AX2" s="12"/>
+      <c r="AY2" s="12"/>
+      <c r="AZ2" s="12"/>
+      <c r="BA2" s="12"/>
+      <c r="BB2" s="12"/>
+      <c r="BC2" s="12"/>
+      <c r="BD2" s="12"/>
+      <c r="BE2" s="12"/>
+      <c r="BF2" s="12"/>
+      <c r="BG2" s="12"/>
+      <c r="BH2" s="12"/>
+      <c r="BI2" s="12"/>
+      <c r="BJ2" s="12"/>
+      <c r="BK2" s="12"/>
+      <c r="BL2" s="12"/>
+      <c r="BM2" s="12"/>
+      <c r="BN2" s="12"/>
+      <c r="BO2" s="12"/>
+      <c r="BP2" s="12"/>
+      <c r="BQ2" s="12"/>
+      <c r="BR2" s="12"/>
+      <c r="BS2" s="12"/>
+      <c r="BT2" s="12"/>
+      <c r="BU2" s="12"/>
+      <c r="BV2" s="12"/>
+      <c r="BW2" s="12"/>
+      <c r="BX2" s="12"/>
+      <c r="BY2" s="12"/>
+      <c r="BZ2" s="12"/>
+      <c r="CA2" s="12"/>
+      <c r="CB2" s="12"/>
+      <c r="CC2" s="12"/>
+      <c r="CD2" s="12"/>
+      <c r="CE2" s="12"/>
+      <c r="CF2" s="12"/>
+      <c r="CG2" s="12"/>
+      <c r="CH2" s="12"/>
+      <c r="CI2" s="12"/>
+      <c r="CJ2" s="12"/>
+      <c r="CK2" s="12"/>
+      <c r="CL2" s="12"/>
+      <c r="CM2" s="12"/>
+      <c r="CN2" s="12"/>
+      <c r="CO2" s="12"/>
+      <c r="CP2" s="12"/>
+      <c r="CQ2" s="12"/>
+      <c r="CR2" s="12"/>
+      <c r="CS2" s="12"/>
+      <c r="CT2" s="12"/>
+      <c r="CU2" s="12"/>
+      <c r="CV2" s="12"/>
+      <c r="CW2" s="12"/>
+      <c r="CX2" s="12"/>
+      <c r="CY2" s="12"/>
+      <c r="CZ2" s="12"/>
+      <c r="DA2" s="12"/>
+      <c r="DB2" s="12"/>
+      <c r="DC2" s="12"/>
+      <c r="DD2" s="12"/>
+      <c r="DE2" s="12"/>
+      <c r="DF2" s="12"/>
+      <c r="DG2" s="12"/>
+      <c r="DH2" s="12"/>
+      <c r="DI2" s="12"/>
+      <c r="DJ2" s="12"/>
+      <c r="DK2" s="12"/>
+      <c r="DL2" s="12"/>
+      <c r="DM2" s="12"/>
+      <c r="DN2" s="12"/>
+      <c r="DO2" s="12"/>
+      <c r="DP2" s="12"/>
+      <c r="DQ2" s="12"/>
+      <c r="DR2" s="12"/>
+      <c r="DS2" s="12"/>
+      <c r="DT2" s="12"/>
+      <c r="DU2" s="12"/>
+      <c r="DV2" s="12"/>
+      <c r="DW2" s="12"/>
+      <c r="DX2" s="13"/>
     </row>
     <row r="3" spans="1:157" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1743,77 +1960,77 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="14"/>
-      <c r="G4" s="14"/>
-      <c r="H4" s="14"/>
-      <c r="I4" s="10" t="s">
+      <c r="C4" s="17"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="17"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="17"/>
+      <c r="I4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="10"/>
-      <c r="O4" s="10"/>
-      <c r="P4" s="10" t="s">
+      <c r="J4" s="19"/>
+      <c r="K4" s="19"/>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
+      <c r="O4" s="19"/>
+      <c r="P4" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="10"/>
-      <c r="R4" s="10"/>
-      <c r="S4" s="10"/>
-      <c r="T4" s="10"/>
-      <c r="U4" s="10"/>
-      <c r="V4" s="10"/>
-      <c r="W4" s="11" t="s">
+      <c r="Q4" s="19"/>
+      <c r="R4" s="19"/>
+      <c r="S4" s="19"/>
+      <c r="T4" s="19"/>
+      <c r="U4" s="19"/>
+      <c r="V4" s="19"/>
+      <c r="W4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
-      <c r="AB4" s="11"/>
-      <c r="AC4" s="11"/>
-      <c r="AD4" s="11"/>
-      <c r="AE4" s="11"/>
-      <c r="AF4" s="11"/>
-      <c r="AG4" s="11"/>
-      <c r="AH4" s="11"/>
-      <c r="AI4" s="11"/>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="11"/>
-      <c r="AL4" s="11"/>
-      <c r="AM4" s="11"/>
-      <c r="AN4" s="11"/>
-      <c r="AO4" s="11"/>
-      <c r="AP4" s="11"/>
-      <c r="AQ4" s="11"/>
-      <c r="AR4" s="11"/>
-      <c r="AS4" s="11"/>
-      <c r="AT4" s="11"/>
-      <c r="AU4" s="11"/>
-      <c r="AV4" s="11"/>
-      <c r="AW4" s="11"/>
-      <c r="AX4" s="13" t="s">
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="25"/>
+      <c r="AH4" s="25"/>
+      <c r="AI4" s="25"/>
+      <c r="AJ4" s="25"/>
+      <c r="AK4" s="25"/>
+      <c r="AL4" s="25"/>
+      <c r="AM4" s="25"/>
+      <c r="AN4" s="25"/>
+      <c r="AO4" s="25"/>
+      <c r="AP4" s="25"/>
+      <c r="AQ4" s="25"/>
+      <c r="AR4" s="25"/>
+      <c r="AS4" s="25"/>
+      <c r="AT4" s="25"/>
+      <c r="AU4" s="25"/>
+      <c r="AV4" s="25"/>
+      <c r="AW4" s="25"/>
+      <c r="AX4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AY4" s="13"/>
-      <c r="AZ4" s="13"/>
-      <c r="BA4" s="13"/>
-      <c r="BB4" s="13"/>
-      <c r="BC4" s="12" t="s">
+      <c r="AY4" s="27"/>
+      <c r="AZ4" s="27"/>
+      <c r="BA4" s="27"/>
+      <c r="BB4" s="27"/>
+      <c r="BC4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="BD4" s="12"/>
-      <c r="BE4" s="9" t="s">
+      <c r="BD4" s="26"/>
+      <c r="BE4" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="BF4" s="8" t="s">
+      <c r="BF4" s="20" t="s">
         <v>9</v>
       </c>
       <c r="BG4" s="5"/>
@@ -1884,10 +2101,10 @@
       <c r="DT4" s="5"/>
       <c r="DU4" s="5"/>
       <c r="DV4" s="5"/>
-      <c r="DW4" s="9" t="s">
+      <c r="DW4" s="21" t="s">
         <v>13</v>
       </c>
-      <c r="DX4" s="8" t="s">
+      <c r="DX4" s="20" t="s">
         <v>12</v>
       </c>
       <c r="DY4" s="5"/>
@@ -1924,55 +2141,84 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15"/>
-      <c r="F5" s="15"/>
-      <c r="G5" s="25" t="s">
+      <c r="D5" s="18"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
-      <c r="N5" s="4" t="s">
+      <c r="J5" s="15"/>
+      <c r="K5" s="15"/>
+      <c r="L5" s="15"/>
+      <c r="M5" s="16"/>
+      <c r="N5" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="24"/>
-      <c r="V5" s="4" t="s">
+      <c r="O5" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="16"/>
+      <c r="V5" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="22" t="s">
+      <c r="W5" s="14" t="s">
+        <v>25</v>
+      </c>
+      <c r="X5" s="15"/>
+      <c r="Y5" s="15"/>
+      <c r="Z5" s="15"/>
+      <c r="AA5" s="15"/>
+      <c r="AB5" s="16"/>
+      <c r="AC5" s="31" t="s">
         <v>26</v>
       </c>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="24"/>
-      <c r="AC5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="BE5" s="9"/>
-      <c r="BF5" s="8"/>
-      <c r="DW5" s="9"/>
-      <c r="DX5" s="8"/>
+      <c r="AD5" s="14" t="s">
+        <v>31</v>
+      </c>
+      <c r="AE5" s="15"/>
+      <c r="AF5" s="15"/>
+      <c r="AG5" s="15"/>
+      <c r="AH5" s="15"/>
+      <c r="AI5" s="16"/>
+      <c r="AJ5" s="31" t="s">
+        <v>27</v>
+      </c>
+      <c r="AK5" s="14"/>
+      <c r="AL5" s="15"/>
+      <c r="AM5" s="15"/>
+      <c r="AN5" s="15"/>
+      <c r="AO5" s="15"/>
+      <c r="AP5" s="16"/>
+      <c r="AQ5" s="31" t="s">
+        <v>28</v>
+      </c>
+      <c r="AR5" s="14"/>
+      <c r="AS5" s="15"/>
+      <c r="AT5" s="15"/>
+      <c r="AU5" s="15"/>
+      <c r="AV5" s="15"/>
+      <c r="AW5" s="16"/>
+      <c r="AX5" s="28" t="s">
+        <v>29</v>
+      </c>
+      <c r="BE5" s="21"/>
+      <c r="BF5" s="20"/>
+      <c r="DW5" s="21"/>
+      <c r="DX5" s="20"/>
     </row>
     <row r="6" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -1984,18 +2230,21 @@
       <c r="N6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="26" t="s">
-        <v>25</v>
-      </c>
-      <c r="BE6" s="9"/>
-      <c r="BF6" s="8"/>
-      <c r="DW6" s="9"/>
-      <c r="DX6" s="8"/>
+      <c r="V6" s="22" t="s">
+        <v>24</v>
+      </c>
+      <c r="AC6" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="BE6" s="21"/>
+      <c r="BF6" s="20"/>
+      <c r="DW6" s="21"/>
+      <c r="DX6" s="20"/>
     </row>
     <row r="7" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V7" s="28"/>
-      <c r="BF7" s="8"/>
-      <c r="DX7" s="8"/>
+      <c r="V7" s="23"/>
+      <c r="BF7" s="20"/>
+      <c r="DX7" s="20"/>
     </row>
     <row r="8" spans="1:157" s="4" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -2003,12 +2252,15 @@
       </c>
       <c r="B8" s="7">
         <f ca="1">TODAY()</f>
-        <v>44703</v>
-      </c>
-      <c r="V8" s="27"/>
+        <v>44710</v>
+      </c>
+      <c r="V8" s="24"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="19">
+    <mergeCell ref="AD5:AI5"/>
+    <mergeCell ref="AK5:AP5"/>
+    <mergeCell ref="AR5:AW5"/>
     <mergeCell ref="A1:DX2"/>
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="O5:U5"/>

</xml_diff>

<commit_message>
Wireframes uploaded by Connor // Admin file added to hold the midterm question paper and other admin from UoL // Further work on the Requirments files needed for the midterm
</commit_message>
<xml_diff>
--- a/Timeline/Project_Timeline.xlsx
+++ b/Timeline/Project_Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Desktop/agile/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5EAFB68-A829-0747-BF5A-840430574620}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C484E8D-6A78-4247-B215-53380427CC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="500" windowWidth="48860" windowHeight="16660" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
   <si>
     <t>ASP - Group Project</t>
   </si>
@@ -542,6 +542,88 @@
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">Update the Requirements-&gt;Final_Requirements files within the GitHub repo.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>PROPOSAL CONTINGENCY PERIOD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Ensure Proposal meets the requirements of the Rubric
+- Peer review each individual submission
+- Ensure all submissions cover the correct material</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">** IF REQUIRED **
+REQUIREMENTS CONTINGENCY PERIOD
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>- Ensure Requirements are fit for purpose against Midterm Rubric</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+DESIGN CONTINGENCY PERIOD
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Ensure all pseudocode elements are fit for purpose
+- Ensure all wireframes are fit for purpose
+- Ensure initial prototypes are viable 
+- Ensure all intended technology is viable 
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
 </t>
     </r>
   </si>
@@ -849,7 +931,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -872,6 +954,30 @@
     <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -890,15 +996,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -932,20 +1029,14 @@
     <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1299,8 +1390,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3400B0-A312-474B-BDD8-7EBBB1942BA5}">
   <dimension ref="A1:FA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X6" workbookViewId="0">
-      <selection activeCell="AH6" sqref="AH6"/>
+    <sheetView tabSelected="1" topLeftCell="T5" workbookViewId="0">
+      <selection activeCell="AK7" sqref="AK7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1309,266 +1400,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
+      <c r="A1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
-      <c r="R1" s="9"/>
-      <c r="S1" s="9"/>
-      <c r="T1" s="9"/>
-      <c r="U1" s="9"/>
-      <c r="V1" s="9"/>
-      <c r="W1" s="9"/>
-      <c r="X1" s="9"/>
-      <c r="Y1" s="9"/>
-      <c r="Z1" s="9"/>
-      <c r="AA1" s="9"/>
-      <c r="AB1" s="9"/>
-      <c r="AC1" s="9"/>
-      <c r="AD1" s="9"/>
-      <c r="AE1" s="9"/>
-      <c r="AF1" s="9"/>
-      <c r="AG1" s="9"/>
-      <c r="AH1" s="9"/>
-      <c r="AI1" s="9"/>
-      <c r="AJ1" s="9"/>
-      <c r="AK1" s="9"/>
-      <c r="AL1" s="9"/>
-      <c r="AM1" s="9"/>
-      <c r="AN1" s="9"/>
-      <c r="AO1" s="9"/>
-      <c r="AP1" s="9"/>
-      <c r="AQ1" s="9"/>
-      <c r="AR1" s="9"/>
-      <c r="AS1" s="9"/>
-      <c r="AT1" s="9"/>
-      <c r="AU1" s="9"/>
-      <c r="AV1" s="9"/>
-      <c r="AW1" s="9"/>
-      <c r="AX1" s="9"/>
-      <c r="AY1" s="9"/>
-      <c r="AZ1" s="9"/>
-      <c r="BA1" s="9"/>
-      <c r="BB1" s="9"/>
-      <c r="BC1" s="9"/>
-      <c r="BD1" s="9"/>
-      <c r="BE1" s="9"/>
-      <c r="BF1" s="9"/>
-      <c r="BG1" s="9"/>
-      <c r="BH1" s="9"/>
-      <c r="BI1" s="9"/>
-      <c r="BJ1" s="9"/>
-      <c r="BK1" s="9"/>
-      <c r="BL1" s="9"/>
-      <c r="BM1" s="9"/>
-      <c r="BN1" s="9"/>
-      <c r="BO1" s="9"/>
-      <c r="BP1" s="9"/>
-      <c r="BQ1" s="9"/>
-      <c r="BR1" s="9"/>
-      <c r="BS1" s="9"/>
-      <c r="BT1" s="9"/>
-      <c r="BU1" s="9"/>
-      <c r="BV1" s="9"/>
-      <c r="BW1" s="9"/>
-      <c r="BX1" s="9"/>
-      <c r="BY1" s="9"/>
-      <c r="BZ1" s="9"/>
-      <c r="CA1" s="9"/>
-      <c r="CB1" s="9"/>
-      <c r="CC1" s="9"/>
-      <c r="CD1" s="9"/>
-      <c r="CE1" s="9"/>
-      <c r="CF1" s="9"/>
-      <c r="CG1" s="9"/>
-      <c r="CH1" s="9"/>
-      <c r="CI1" s="9"/>
-      <c r="CJ1" s="9"/>
-      <c r="CK1" s="9"/>
-      <c r="CL1" s="9"/>
-      <c r="CM1" s="9"/>
-      <c r="CN1" s="9"/>
-      <c r="CO1" s="9"/>
-      <c r="CP1" s="9"/>
-      <c r="CQ1" s="9"/>
-      <c r="CR1" s="9"/>
-      <c r="CS1" s="9"/>
-      <c r="CT1" s="9"/>
-      <c r="CU1" s="9"/>
-      <c r="CV1" s="9"/>
-      <c r="CW1" s="9"/>
-      <c r="CX1" s="9"/>
-      <c r="CY1" s="9"/>
-      <c r="CZ1" s="9"/>
-      <c r="DA1" s="9"/>
-      <c r="DB1" s="9"/>
-      <c r="DC1" s="9"/>
-      <c r="DD1" s="9"/>
-      <c r="DE1" s="9"/>
-      <c r="DF1" s="9"/>
-      <c r="DG1" s="9"/>
-      <c r="DH1" s="9"/>
-      <c r="DI1" s="9"/>
-      <c r="DJ1" s="9"/>
-      <c r="DK1" s="9"/>
-      <c r="DL1" s="9"/>
-      <c r="DM1" s="9"/>
-      <c r="DN1" s="9"/>
-      <c r="DO1" s="9"/>
-      <c r="DP1" s="9"/>
-      <c r="DQ1" s="9"/>
-      <c r="DR1" s="9"/>
-      <c r="DS1" s="9"/>
-      <c r="DT1" s="9"/>
-      <c r="DU1" s="9"/>
-      <c r="DV1" s="9"/>
-      <c r="DW1" s="9"/>
-      <c r="DX1" s="10"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="17"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="17"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="17"/>
+      <c r="AZ1" s="17"/>
+      <c r="BA1" s="17"/>
+      <c r="BB1" s="17"/>
+      <c r="BC1" s="17"/>
+      <c r="BD1" s="17"/>
+      <c r="BE1" s="17"/>
+      <c r="BF1" s="17"/>
+      <c r="BG1" s="17"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
+      <c r="BM1" s="17"/>
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="17"/>
+      <c r="BP1" s="17"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
+      <c r="BS1" s="17"/>
+      <c r="BT1" s="17"/>
+      <c r="BU1" s="17"/>
+      <c r="BV1" s="17"/>
+      <c r="BW1" s="17"/>
+      <c r="BX1" s="17"/>
+      <c r="BY1" s="17"/>
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="17"/>
+      <c r="CB1" s="17"/>
+      <c r="CC1" s="17"/>
+      <c r="CD1" s="17"/>
+      <c r="CE1" s="17"/>
+      <c r="CF1" s="17"/>
+      <c r="CG1" s="17"/>
+      <c r="CH1" s="17"/>
+      <c r="CI1" s="17"/>
+      <c r="CJ1" s="17"/>
+      <c r="CK1" s="17"/>
+      <c r="CL1" s="17"/>
+      <c r="CM1" s="17"/>
+      <c r="CN1" s="17"/>
+      <c r="CO1" s="17"/>
+      <c r="CP1" s="17"/>
+      <c r="CQ1" s="17"/>
+      <c r="CR1" s="17"/>
+      <c r="CS1" s="17"/>
+      <c r="CT1" s="17"/>
+      <c r="CU1" s="17"/>
+      <c r="CV1" s="17"/>
+      <c r="CW1" s="17"/>
+      <c r="CX1" s="17"/>
+      <c r="CY1" s="17"/>
+      <c r="CZ1" s="17"/>
+      <c r="DA1" s="17"/>
+      <c r="DB1" s="17"/>
+      <c r="DC1" s="17"/>
+      <c r="DD1" s="17"/>
+      <c r="DE1" s="17"/>
+      <c r="DF1" s="17"/>
+      <c r="DG1" s="17"/>
+      <c r="DH1" s="17"/>
+      <c r="DI1" s="17"/>
+      <c r="DJ1" s="17"/>
+      <c r="DK1" s="17"/>
+      <c r="DL1" s="17"/>
+      <c r="DM1" s="17"/>
+      <c r="DN1" s="17"/>
+      <c r="DO1" s="17"/>
+      <c r="DP1" s="17"/>
+      <c r="DQ1" s="17"/>
+      <c r="DR1" s="17"/>
+      <c r="DS1" s="17"/>
+      <c r="DT1" s="17"/>
+      <c r="DU1" s="17"/>
+      <c r="DV1" s="17"/>
+      <c r="DW1" s="17"/>
+      <c r="DX1" s="18"/>
     </row>
     <row r="2" spans="1:157" s="4" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11"/>
-      <c r="B2" s="12"/>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="12"/>
-      <c r="K2" s="12"/>
-      <c r="L2" s="12"/>
-      <c r="M2" s="12"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="12"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="12"/>
-      <c r="R2" s="12"/>
-      <c r="S2" s="12"/>
-      <c r="T2" s="12"/>
-      <c r="U2" s="12"/>
-      <c r="V2" s="12"/>
-      <c r="W2" s="12"/>
-      <c r="X2" s="12"/>
-      <c r="Y2" s="12"/>
-      <c r="Z2" s="12"/>
-      <c r="AA2" s="12"/>
-      <c r="AB2" s="12"/>
-      <c r="AC2" s="12"/>
-      <c r="AD2" s="12"/>
-      <c r="AE2" s="12"/>
-      <c r="AF2" s="12"/>
-      <c r="AG2" s="12"/>
-      <c r="AH2" s="12"/>
-      <c r="AI2" s="12"/>
-      <c r="AJ2" s="12"/>
-      <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
-      <c r="AM2" s="12"/>
-      <c r="AN2" s="12"/>
-      <c r="AO2" s="12"/>
-      <c r="AP2" s="12"/>
-      <c r="AQ2" s="12"/>
-      <c r="AR2" s="12"/>
-      <c r="AS2" s="12"/>
-      <c r="AT2" s="12"/>
-      <c r="AU2" s="12"/>
-      <c r="AV2" s="12"/>
-      <c r="AW2" s="12"/>
-      <c r="AX2" s="12"/>
-      <c r="AY2" s="12"/>
-      <c r="AZ2" s="12"/>
-      <c r="BA2" s="12"/>
-      <c r="BB2" s="12"/>
-      <c r="BC2" s="12"/>
-      <c r="BD2" s="12"/>
-      <c r="BE2" s="12"/>
-      <c r="BF2" s="12"/>
-      <c r="BG2" s="12"/>
-      <c r="BH2" s="12"/>
-      <c r="BI2" s="12"/>
-      <c r="BJ2" s="12"/>
-      <c r="BK2" s="12"/>
-      <c r="BL2" s="12"/>
-      <c r="BM2" s="12"/>
-      <c r="BN2" s="12"/>
-      <c r="BO2" s="12"/>
-      <c r="BP2" s="12"/>
-      <c r="BQ2" s="12"/>
-      <c r="BR2" s="12"/>
-      <c r="BS2" s="12"/>
-      <c r="BT2" s="12"/>
-      <c r="BU2" s="12"/>
-      <c r="BV2" s="12"/>
-      <c r="BW2" s="12"/>
-      <c r="BX2" s="12"/>
-      <c r="BY2" s="12"/>
-      <c r="BZ2" s="12"/>
-      <c r="CA2" s="12"/>
-      <c r="CB2" s="12"/>
-      <c r="CC2" s="12"/>
-      <c r="CD2" s="12"/>
-      <c r="CE2" s="12"/>
-      <c r="CF2" s="12"/>
-      <c r="CG2" s="12"/>
-      <c r="CH2" s="12"/>
-      <c r="CI2" s="12"/>
-      <c r="CJ2" s="12"/>
-      <c r="CK2" s="12"/>
-      <c r="CL2" s="12"/>
-      <c r="CM2" s="12"/>
-      <c r="CN2" s="12"/>
-      <c r="CO2" s="12"/>
-      <c r="CP2" s="12"/>
-      <c r="CQ2" s="12"/>
-      <c r="CR2" s="12"/>
-      <c r="CS2" s="12"/>
-      <c r="CT2" s="12"/>
-      <c r="CU2" s="12"/>
-      <c r="CV2" s="12"/>
-      <c r="CW2" s="12"/>
-      <c r="CX2" s="12"/>
-      <c r="CY2" s="12"/>
-      <c r="CZ2" s="12"/>
-      <c r="DA2" s="12"/>
-      <c r="DB2" s="12"/>
-      <c r="DC2" s="12"/>
-      <c r="DD2" s="12"/>
-      <c r="DE2" s="12"/>
-      <c r="DF2" s="12"/>
-      <c r="DG2" s="12"/>
-      <c r="DH2" s="12"/>
-      <c r="DI2" s="12"/>
-      <c r="DJ2" s="12"/>
-      <c r="DK2" s="12"/>
-      <c r="DL2" s="12"/>
-      <c r="DM2" s="12"/>
-      <c r="DN2" s="12"/>
-      <c r="DO2" s="12"/>
-      <c r="DP2" s="12"/>
-      <c r="DQ2" s="12"/>
-      <c r="DR2" s="12"/>
-      <c r="DS2" s="12"/>
-      <c r="DT2" s="12"/>
-      <c r="DU2" s="12"/>
-      <c r="DV2" s="12"/>
-      <c r="DW2" s="12"/>
-      <c r="DX2" s="13"/>
+      <c r="A2" s="19"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="20"/>
+      <c r="L2" s="20"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="20"/>
+      <c r="Q2" s="20"/>
+      <c r="R2" s="20"/>
+      <c r="S2" s="20"/>
+      <c r="T2" s="20"/>
+      <c r="U2" s="20"/>
+      <c r="V2" s="20"/>
+      <c r="W2" s="20"/>
+      <c r="X2" s="20"/>
+      <c r="Y2" s="20"/>
+      <c r="Z2" s="20"/>
+      <c r="AA2" s="20"/>
+      <c r="AB2" s="20"/>
+      <c r="AC2" s="20"/>
+      <c r="AD2" s="20"/>
+      <c r="AE2" s="20"/>
+      <c r="AF2" s="20"/>
+      <c r="AG2" s="20"/>
+      <c r="AH2" s="20"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="20"/>
+      <c r="AK2" s="20"/>
+      <c r="AL2" s="20"/>
+      <c r="AM2" s="20"/>
+      <c r="AN2" s="20"/>
+      <c r="AO2" s="20"/>
+      <c r="AP2" s="20"/>
+      <c r="AQ2" s="20"/>
+      <c r="AR2" s="20"/>
+      <c r="AS2" s="20"/>
+      <c r="AT2" s="20"/>
+      <c r="AU2" s="20"/>
+      <c r="AV2" s="20"/>
+      <c r="AW2" s="20"/>
+      <c r="AX2" s="20"/>
+      <c r="AY2" s="20"/>
+      <c r="AZ2" s="20"/>
+      <c r="BA2" s="20"/>
+      <c r="BB2" s="20"/>
+      <c r="BC2" s="20"/>
+      <c r="BD2" s="20"/>
+      <c r="BE2" s="20"/>
+      <c r="BF2" s="20"/>
+      <c r="BG2" s="20"/>
+      <c r="BH2" s="20"/>
+      <c r="BI2" s="20"/>
+      <c r="BJ2" s="20"/>
+      <c r="BK2" s="20"/>
+      <c r="BL2" s="20"/>
+      <c r="BM2" s="20"/>
+      <c r="BN2" s="20"/>
+      <c r="BO2" s="20"/>
+      <c r="BP2" s="20"/>
+      <c r="BQ2" s="20"/>
+      <c r="BR2" s="20"/>
+      <c r="BS2" s="20"/>
+      <c r="BT2" s="20"/>
+      <c r="BU2" s="20"/>
+      <c r="BV2" s="20"/>
+      <c r="BW2" s="20"/>
+      <c r="BX2" s="20"/>
+      <c r="BY2" s="20"/>
+      <c r="BZ2" s="20"/>
+      <c r="CA2" s="20"/>
+      <c r="CB2" s="20"/>
+      <c r="CC2" s="20"/>
+      <c r="CD2" s="20"/>
+      <c r="CE2" s="20"/>
+      <c r="CF2" s="20"/>
+      <c r="CG2" s="20"/>
+      <c r="CH2" s="20"/>
+      <c r="CI2" s="20"/>
+      <c r="CJ2" s="20"/>
+      <c r="CK2" s="20"/>
+      <c r="CL2" s="20"/>
+      <c r="CM2" s="20"/>
+      <c r="CN2" s="20"/>
+      <c r="CO2" s="20"/>
+      <c r="CP2" s="20"/>
+      <c r="CQ2" s="20"/>
+      <c r="CR2" s="20"/>
+      <c r="CS2" s="20"/>
+      <c r="CT2" s="20"/>
+      <c r="CU2" s="20"/>
+      <c r="CV2" s="20"/>
+      <c r="CW2" s="20"/>
+      <c r="CX2" s="20"/>
+      <c r="CY2" s="20"/>
+      <c r="CZ2" s="20"/>
+      <c r="DA2" s="20"/>
+      <c r="DB2" s="20"/>
+      <c r="DC2" s="20"/>
+      <c r="DD2" s="20"/>
+      <c r="DE2" s="20"/>
+      <c r="DF2" s="20"/>
+      <c r="DG2" s="20"/>
+      <c r="DH2" s="20"/>
+      <c r="DI2" s="20"/>
+      <c r="DJ2" s="20"/>
+      <c r="DK2" s="20"/>
+      <c r="DL2" s="20"/>
+      <c r="DM2" s="20"/>
+      <c r="DN2" s="20"/>
+      <c r="DO2" s="20"/>
+      <c r="DP2" s="20"/>
+      <c r="DQ2" s="20"/>
+      <c r="DR2" s="20"/>
+      <c r="DS2" s="20"/>
+      <c r="DT2" s="20"/>
+      <c r="DU2" s="20"/>
+      <c r="DV2" s="20"/>
+      <c r="DW2" s="20"/>
+      <c r="DX2" s="21"/>
     </row>
     <row r="3" spans="1:157" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1960,77 +2051,77 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="22" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
-      <c r="I4" s="19" t="s">
+      <c r="C4" s="22"/>
+      <c r="D4" s="22"/>
+      <c r="E4" s="22"/>
+      <c r="F4" s="22"/>
+      <c r="G4" s="22"/>
+      <c r="H4" s="22"/>
+      <c r="I4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19" t="s">
+      <c r="J4" s="24"/>
+      <c r="K4" s="24"/>
+      <c r="L4" s="24"/>
+      <c r="M4" s="24"/>
+      <c r="N4" s="24"/>
+      <c r="O4" s="24"/>
+      <c r="P4" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19"/>
-      <c r="T4" s="19"/>
-      <c r="U4" s="19"/>
-      <c r="V4" s="19"/>
-      <c r="W4" s="25" t="s">
+      <c r="Q4" s="24"/>
+      <c r="R4" s="24"/>
+      <c r="S4" s="24"/>
+      <c r="T4" s="24"/>
+      <c r="U4" s="24"/>
+      <c r="V4" s="24"/>
+      <c r="W4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="25"/>
-      <c r="AE4" s="25"/>
-      <c r="AF4" s="25"/>
-      <c r="AG4" s="25"/>
-      <c r="AH4" s="25"/>
-      <c r="AI4" s="25"/>
-      <c r="AJ4" s="25"/>
-      <c r="AK4" s="25"/>
-      <c r="AL4" s="25"/>
-      <c r="AM4" s="25"/>
-      <c r="AN4" s="25"/>
-      <c r="AO4" s="25"/>
-      <c r="AP4" s="25"/>
-      <c r="AQ4" s="25"/>
-      <c r="AR4" s="25"/>
-      <c r="AS4" s="25"/>
-      <c r="AT4" s="25"/>
-      <c r="AU4" s="25"/>
-      <c r="AV4" s="25"/>
-      <c r="AW4" s="25"/>
-      <c r="AX4" s="27" t="s">
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="30"/>
+      <c r="AF4" s="30"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="30"/>
+      <c r="AJ4" s="30"/>
+      <c r="AK4" s="30"/>
+      <c r="AL4" s="30"/>
+      <c r="AM4" s="30"/>
+      <c r="AN4" s="30"/>
+      <c r="AO4" s="30"/>
+      <c r="AP4" s="30"/>
+      <c r="AQ4" s="30"/>
+      <c r="AR4" s="30"/>
+      <c r="AS4" s="30"/>
+      <c r="AT4" s="30"/>
+      <c r="AU4" s="30"/>
+      <c r="AV4" s="30"/>
+      <c r="AW4" s="30"/>
+      <c r="AX4" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="AY4" s="27"/>
-      <c r="AZ4" s="27"/>
-      <c r="BA4" s="27"/>
-      <c r="BB4" s="27"/>
-      <c r="BC4" s="26" t="s">
+      <c r="AY4" s="32"/>
+      <c r="AZ4" s="32"/>
+      <c r="BA4" s="32"/>
+      <c r="BB4" s="32"/>
+      <c r="BC4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="BD4" s="26"/>
-      <c r="BE4" s="21" t="s">
+      <c r="BD4" s="31"/>
+      <c r="BE4" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="BF4" s="20" t="s">
+      <c r="BF4" s="25" t="s">
         <v>9</v>
       </c>
       <c r="BG4" s="5"/>
@@ -2101,10 +2192,10 @@
       <c r="DT4" s="5"/>
       <c r="DU4" s="5"/>
       <c r="DV4" s="5"/>
-      <c r="DW4" s="21" t="s">
+      <c r="DW4" s="26" t="s">
         <v>13</v>
       </c>
-      <c r="DX4" s="20" t="s">
+      <c r="DX4" s="25" t="s">
         <v>12</v>
       </c>
       <c r="DY4" s="5"/>
@@ -2141,84 +2232,84 @@
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="18"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="29" t="s">
+      <c r="D5" s="23"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="15"/>
-      <c r="K5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="M5" s="16"/>
-      <c r="N5" s="30" t="s">
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="14" t="s">
+      <c r="O5" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="15"/>
-      <c r="Q5" s="15"/>
-      <c r="R5" s="15"/>
-      <c r="S5" s="15"/>
-      <c r="T5" s="15"/>
-      <c r="U5" s="16"/>
-      <c r="V5" s="30" t="s">
+      <c r="P5" s="14"/>
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="15"/>
+      <c r="V5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="14" t="s">
+      <c r="W5" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="X5" s="15"/>
-      <c r="Y5" s="15"/>
-      <c r="Z5" s="15"/>
-      <c r="AA5" s="15"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="31" t="s">
+      <c r="X5" s="14"/>
+      <c r="Y5" s="14"/>
+      <c r="Z5" s="14"/>
+      <c r="AA5" s="14"/>
+      <c r="AB5" s="15"/>
+      <c r="AC5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="14" t="s">
+      <c r="AD5" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="AE5" s="15"/>
-      <c r="AF5" s="15"/>
-      <c r="AG5" s="15"/>
-      <c r="AH5" s="15"/>
-      <c r="AI5" s="16"/>
-      <c r="AJ5" s="31" t="s">
+      <c r="AE5" s="14"/>
+      <c r="AF5" s="14"/>
+      <c r="AG5" s="14"/>
+      <c r="AH5" s="14"/>
+      <c r="AI5" s="15"/>
+      <c r="AJ5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AK5" s="14"/>
-      <c r="AL5" s="15"/>
-      <c r="AM5" s="15"/>
-      <c r="AN5" s="15"/>
-      <c r="AO5" s="15"/>
-      <c r="AP5" s="16"/>
-      <c r="AQ5" s="31" t="s">
+      <c r="AK5" s="13"/>
+      <c r="AL5" s="14"/>
+      <c r="AM5" s="14"/>
+      <c r="AN5" s="14"/>
+      <c r="AO5" s="14"/>
+      <c r="AP5" s="15"/>
+      <c r="AQ5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AR5" s="14"/>
-      <c r="AS5" s="15"/>
-      <c r="AT5" s="15"/>
-      <c r="AU5" s="15"/>
-      <c r="AV5" s="15"/>
-      <c r="AW5" s="16"/>
-      <c r="AX5" s="28" t="s">
+      <c r="AR5" s="13"/>
+      <c r="AS5" s="14"/>
+      <c r="AT5" s="14"/>
+      <c r="AU5" s="14"/>
+      <c r="AV5" s="14"/>
+      <c r="AW5" s="15"/>
+      <c r="AX5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="BE5" s="21"/>
-      <c r="BF5" s="20"/>
-      <c r="DW5" s="21"/>
-      <c r="DX5" s="20"/>
+      <c r="BE5" s="26"/>
+      <c r="BF5" s="25"/>
+      <c r="DW5" s="26"/>
+      <c r="DX5" s="25"/>
     </row>
     <row r="6" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -2230,21 +2321,33 @@
       <c r="N6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="22" t="s">
+      <c r="V6" s="27" t="s">
         <v>24</v>
       </c>
       <c r="AC6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="BE6" s="21"/>
-      <c r="BF6" s="20"/>
-      <c r="DW6" s="21"/>
-      <c r="DX6" s="20"/>
+      <c r="AK6" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="AL6" s="34"/>
+      <c r="AM6" s="34"/>
+      <c r="AN6" s="34"/>
+      <c r="AO6" s="34"/>
+      <c r="AP6" s="35"/>
+      <c r="BC6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="BD6" s="15"/>
+      <c r="BE6" s="26"/>
+      <c r="BF6" s="25"/>
+      <c r="DW6" s="26"/>
+      <c r="DX6" s="25"/>
     </row>
     <row r="7" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V7" s="23"/>
-      <c r="BF7" s="20"/>
-      <c r="DX7" s="20"/>
+      <c r="V7" s="28"/>
+      <c r="BF7" s="25"/>
+      <c r="DX7" s="25"/>
     </row>
     <row r="8" spans="1:157" s="4" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -2252,12 +2355,17 @@
       </c>
       <c r="B8" s="7">
         <f ca="1">TODAY()</f>
-        <v>44710</v>
-      </c>
-      <c r="V8" s="24"/>
+        <v>44716</v>
+      </c>
+      <c r="V8" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="19">
+  <mergeCells count="21">
+    <mergeCell ref="W4:AW4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="AX4:BB4"/>
+    <mergeCell ref="AK6:AP6"/>
+    <mergeCell ref="BC6:BD6"/>
     <mergeCell ref="AD5:AI5"/>
     <mergeCell ref="AK5:AP5"/>
     <mergeCell ref="AR5:AW5"/>
@@ -2274,9 +2382,6 @@
     <mergeCell ref="DX4:DX7"/>
     <mergeCell ref="DW4:DW6"/>
     <mergeCell ref="P4:V4"/>
-    <mergeCell ref="W4:AW4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="AX4:BB4"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:XFD3">
     <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">

</xml_diff>

<commit_message>
Meeting log from 5 Jun 2022 // Timeline update to include 7 Sprints for the software development post midterm // 19 June 2022 deadline added to objectives for edits to the Requirements
</commit_message>
<xml_diff>
--- a/Timeline/Project_Timeline.xlsx
+++ b/Timeline/Project_Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Desktop/agile/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C484E8D-6A78-4247-B215-53380427CC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9469DA6E-381F-254E-9AA6-3E8AA7CD3DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16640" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
+    <workbookView xWindow="19820" yWindow="2240" windowWidth="28800" windowHeight="22140" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
   <si>
     <t>ASP - Group Project</t>
   </si>
@@ -627,6 +627,310 @@
 </t>
     </r>
   </si>
+  <si>
+    <t>Final Requirements updates/submissions/edits before the midterm</t>
+  </si>
+  <si>
+    <t>Requirements deadline</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Connor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Create voting options for the final Designs </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+All team members </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Update the files within the Github repo under Requirements
+(Github/agile/Requirements/Final_Requirements)
+- Vote on final designs once uploaded to the Slack channel </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">All team members </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Update the files within the Github repo under Requirements
+(Github/agile/Requirements/Final_Requirements)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>All Team members</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Create midterm submission from the information contained within the Github/Requirements/Final_Requirements folder
+-&gt; All information required to successfully answer the questions should be contained within these folders.</t>
+    </r>
+  </si>
+  <si>
+    <t>All team members
+- Review midterm submissions</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team Meeting 15 - Development Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Update on the project build</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team Meeting 16 - Development Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Update on the project build</t>
+    </r>
+  </si>
+  <si>
+    <t>Testing &amp; Evaluation</t>
+  </si>
+  <si>
+    <t>Sprint 1 - Software Development</t>
+  </si>
+  <si>
+    <t>Sprint 2 - Software Development</t>
+  </si>
+  <si>
+    <t>Sprint 3 - Software Development</t>
+  </si>
+  <si>
+    <t>Sprint 4 - Software Development</t>
+  </si>
+  <si>
+    <t>Sprint 5 - Software Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Analysis </t>
+  </si>
+  <si>
+    <t>Sprint 6 - Software Development</t>
+  </si>
+  <si>
+    <t>Sprint 7 - Software Development</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Team Meeting 9 - Development Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Update on the project build</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Team Meeting 10 - Development Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Update on the project build</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Team Meeting 11 - Development Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Update on the project build</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team Meeting 12 - Development Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Update on the project build</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team Meeting 13 - Development Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Update on the project build</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team Meeting 14 - Development Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Update on the project build</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Team Meeting 15 - Development Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Update on the project build</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -635,7 +939,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -693,8 +997,37 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -764,6 +1097,78 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF6D3E00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF814C00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA649EF"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -931,7 +1336,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -969,15 +1374,33 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1020,22 +1443,106 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1045,11 +1552,11 @@
   <dxfs count="3">
     <dxf>
       <font>
-        <color theme="0" tint="-0.24994659260841701"/>
+        <color rgb="FF006100"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor theme="1" tint="0.34998626667073579"/>
+          <bgColor rgb="FFC6EFCE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1065,11 +1572,11 @@
     </dxf>
     <dxf>
       <font>
-        <color rgb="FF006100"/>
+        <color theme="0" tint="-0.24994659260841701"/>
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
+          <bgColor theme="1" tint="0.34998626667073579"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1077,6 +1584,9 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFA649EF"/>
+      <color rgb="FF814C00"/>
+      <color rgb="FF6D3E00"/>
       <color rgb="FFFF4818"/>
     </mruColors>
   </colors>
@@ -1390,8 +1900,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3400B0-A312-474B-BDD8-7EBBB1942BA5}">
   <dimension ref="A1:FA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T5" workbookViewId="0">
-      <selection activeCell="AK7" sqref="AK7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:DX2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1400,266 +1910,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="22" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="17"/>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
-      <c r="E1" s="17"/>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
-      <c r="H1" s="17"/>
-      <c r="I1" s="17"/>
-      <c r="J1" s="17"/>
-      <c r="K1" s="17"/>
-      <c r="L1" s="17"/>
-      <c r="M1" s="17"/>
-      <c r="N1" s="17"/>
-      <c r="O1" s="17"/>
-      <c r="P1" s="17"/>
-      <c r="Q1" s="17"/>
-      <c r="R1" s="17"/>
-      <c r="S1" s="17"/>
-      <c r="T1" s="17"/>
-      <c r="U1" s="17"/>
-      <c r="V1" s="17"/>
-      <c r="W1" s="17"/>
-      <c r="X1" s="17"/>
-      <c r="Y1" s="17"/>
-      <c r="Z1" s="17"/>
-      <c r="AA1" s="17"/>
-      <c r="AB1" s="17"/>
-      <c r="AC1" s="17"/>
-      <c r="AD1" s="17"/>
-      <c r="AE1" s="17"/>
-      <c r="AF1" s="17"/>
-      <c r="AG1" s="17"/>
-      <c r="AH1" s="17"/>
-      <c r="AI1" s="17"/>
-      <c r="AJ1" s="17"/>
-      <c r="AK1" s="17"/>
-      <c r="AL1" s="17"/>
-      <c r="AM1" s="17"/>
-      <c r="AN1" s="17"/>
-      <c r="AO1" s="17"/>
-      <c r="AP1" s="17"/>
-      <c r="AQ1" s="17"/>
-      <c r="AR1" s="17"/>
-      <c r="AS1" s="17"/>
-      <c r="AT1" s="17"/>
-      <c r="AU1" s="17"/>
-      <c r="AV1" s="17"/>
-      <c r="AW1" s="17"/>
-      <c r="AX1" s="17"/>
-      <c r="AY1" s="17"/>
-      <c r="AZ1" s="17"/>
-      <c r="BA1" s="17"/>
-      <c r="BB1" s="17"/>
-      <c r="BC1" s="17"/>
-      <c r="BD1" s="17"/>
-      <c r="BE1" s="17"/>
-      <c r="BF1" s="17"/>
-      <c r="BG1" s="17"/>
-      <c r="BH1" s="17"/>
-      <c r="BI1" s="17"/>
-      <c r="BJ1" s="17"/>
-      <c r="BK1" s="17"/>
-      <c r="BL1" s="17"/>
-      <c r="BM1" s="17"/>
-      <c r="BN1" s="17"/>
-      <c r="BO1" s="17"/>
-      <c r="BP1" s="17"/>
-      <c r="BQ1" s="17"/>
-      <c r="BR1" s="17"/>
-      <c r="BS1" s="17"/>
-      <c r="BT1" s="17"/>
-      <c r="BU1" s="17"/>
-      <c r="BV1" s="17"/>
-      <c r="BW1" s="17"/>
-      <c r="BX1" s="17"/>
-      <c r="BY1" s="17"/>
-      <c r="BZ1" s="17"/>
-      <c r="CA1" s="17"/>
-      <c r="CB1" s="17"/>
-      <c r="CC1" s="17"/>
-      <c r="CD1" s="17"/>
-      <c r="CE1" s="17"/>
-      <c r="CF1" s="17"/>
-      <c r="CG1" s="17"/>
-      <c r="CH1" s="17"/>
-      <c r="CI1" s="17"/>
-      <c r="CJ1" s="17"/>
-      <c r="CK1" s="17"/>
-      <c r="CL1" s="17"/>
-      <c r="CM1" s="17"/>
-      <c r="CN1" s="17"/>
-      <c r="CO1" s="17"/>
-      <c r="CP1" s="17"/>
-      <c r="CQ1" s="17"/>
-      <c r="CR1" s="17"/>
-      <c r="CS1" s="17"/>
-      <c r="CT1" s="17"/>
-      <c r="CU1" s="17"/>
-      <c r="CV1" s="17"/>
-      <c r="CW1" s="17"/>
-      <c r="CX1" s="17"/>
-      <c r="CY1" s="17"/>
-      <c r="CZ1" s="17"/>
-      <c r="DA1" s="17"/>
-      <c r="DB1" s="17"/>
-      <c r="DC1" s="17"/>
-      <c r="DD1" s="17"/>
-      <c r="DE1" s="17"/>
-      <c r="DF1" s="17"/>
-      <c r="DG1" s="17"/>
-      <c r="DH1" s="17"/>
-      <c r="DI1" s="17"/>
-      <c r="DJ1" s="17"/>
-      <c r="DK1" s="17"/>
-      <c r="DL1" s="17"/>
-      <c r="DM1" s="17"/>
-      <c r="DN1" s="17"/>
-      <c r="DO1" s="17"/>
-      <c r="DP1" s="17"/>
-      <c r="DQ1" s="17"/>
-      <c r="DR1" s="17"/>
-      <c r="DS1" s="17"/>
-      <c r="DT1" s="17"/>
-      <c r="DU1" s="17"/>
-      <c r="DV1" s="17"/>
-      <c r="DW1" s="17"/>
-      <c r="DX1" s="18"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="23"/>
+      <c r="H1" s="23"/>
+      <c r="I1" s="23"/>
+      <c r="J1" s="23"/>
+      <c r="K1" s="23"/>
+      <c r="L1" s="23"/>
+      <c r="M1" s="23"/>
+      <c r="N1" s="23"/>
+      <c r="O1" s="23"/>
+      <c r="P1" s="23"/>
+      <c r="Q1" s="23"/>
+      <c r="R1" s="23"/>
+      <c r="S1" s="23"/>
+      <c r="T1" s="23"/>
+      <c r="U1" s="23"/>
+      <c r="V1" s="23"/>
+      <c r="W1" s="23"/>
+      <c r="X1" s="23"/>
+      <c r="Y1" s="23"/>
+      <c r="Z1" s="23"/>
+      <c r="AA1" s="23"/>
+      <c r="AB1" s="23"/>
+      <c r="AC1" s="23"/>
+      <c r="AD1" s="23"/>
+      <c r="AE1" s="23"/>
+      <c r="AF1" s="23"/>
+      <c r="AG1" s="23"/>
+      <c r="AH1" s="23"/>
+      <c r="AI1" s="23"/>
+      <c r="AJ1" s="23"/>
+      <c r="AK1" s="23"/>
+      <c r="AL1" s="23"/>
+      <c r="AM1" s="23"/>
+      <c r="AN1" s="23"/>
+      <c r="AO1" s="23"/>
+      <c r="AP1" s="23"/>
+      <c r="AQ1" s="23"/>
+      <c r="AR1" s="23"/>
+      <c r="AS1" s="23"/>
+      <c r="AT1" s="23"/>
+      <c r="AU1" s="23"/>
+      <c r="AV1" s="23"/>
+      <c r="AW1" s="23"/>
+      <c r="AX1" s="23"/>
+      <c r="AY1" s="23"/>
+      <c r="AZ1" s="23"/>
+      <c r="BA1" s="23"/>
+      <c r="BB1" s="23"/>
+      <c r="BC1" s="23"/>
+      <c r="BD1" s="23"/>
+      <c r="BE1" s="23"/>
+      <c r="BF1" s="23"/>
+      <c r="BG1" s="23"/>
+      <c r="BH1" s="23"/>
+      <c r="BI1" s="23"/>
+      <c r="BJ1" s="23"/>
+      <c r="BK1" s="23"/>
+      <c r="BL1" s="23"/>
+      <c r="BM1" s="23"/>
+      <c r="BN1" s="23"/>
+      <c r="BO1" s="23"/>
+      <c r="BP1" s="23"/>
+      <c r="BQ1" s="23"/>
+      <c r="BR1" s="23"/>
+      <c r="BS1" s="23"/>
+      <c r="BT1" s="23"/>
+      <c r="BU1" s="23"/>
+      <c r="BV1" s="23"/>
+      <c r="BW1" s="23"/>
+      <c r="BX1" s="23"/>
+      <c r="BY1" s="23"/>
+      <c r="BZ1" s="23"/>
+      <c r="CA1" s="23"/>
+      <c r="CB1" s="23"/>
+      <c r="CC1" s="23"/>
+      <c r="CD1" s="23"/>
+      <c r="CE1" s="23"/>
+      <c r="CF1" s="23"/>
+      <c r="CG1" s="23"/>
+      <c r="CH1" s="23"/>
+      <c r="CI1" s="23"/>
+      <c r="CJ1" s="23"/>
+      <c r="CK1" s="23"/>
+      <c r="CL1" s="23"/>
+      <c r="CM1" s="23"/>
+      <c r="CN1" s="23"/>
+      <c r="CO1" s="23"/>
+      <c r="CP1" s="23"/>
+      <c r="CQ1" s="23"/>
+      <c r="CR1" s="23"/>
+      <c r="CS1" s="23"/>
+      <c r="CT1" s="23"/>
+      <c r="CU1" s="23"/>
+      <c r="CV1" s="23"/>
+      <c r="CW1" s="23"/>
+      <c r="CX1" s="23"/>
+      <c r="CY1" s="23"/>
+      <c r="CZ1" s="23"/>
+      <c r="DA1" s="23"/>
+      <c r="DB1" s="23"/>
+      <c r="DC1" s="23"/>
+      <c r="DD1" s="23"/>
+      <c r="DE1" s="23"/>
+      <c r="DF1" s="23"/>
+      <c r="DG1" s="23"/>
+      <c r="DH1" s="23"/>
+      <c r="DI1" s="23"/>
+      <c r="DJ1" s="23"/>
+      <c r="DK1" s="23"/>
+      <c r="DL1" s="23"/>
+      <c r="DM1" s="23"/>
+      <c r="DN1" s="23"/>
+      <c r="DO1" s="23"/>
+      <c r="DP1" s="23"/>
+      <c r="DQ1" s="23"/>
+      <c r="DR1" s="23"/>
+      <c r="DS1" s="23"/>
+      <c r="DT1" s="23"/>
+      <c r="DU1" s="23"/>
+      <c r="DV1" s="23"/>
+      <c r="DW1" s="23"/>
+      <c r="DX1" s="24"/>
     </row>
     <row r="2" spans="1:157" s="4" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="20"/>
-      <c r="C2" s="20"/>
-      <c r="D2" s="20"/>
-      <c r="E2" s="20"/>
-      <c r="F2" s="20"/>
-      <c r="G2" s="20"/>
-      <c r="H2" s="20"/>
-      <c r="I2" s="20"/>
-      <c r="J2" s="20"/>
-      <c r="K2" s="20"/>
-      <c r="L2" s="20"/>
-      <c r="M2" s="20"/>
-      <c r="N2" s="20"/>
-      <c r="O2" s="20"/>
-      <c r="P2" s="20"/>
-      <c r="Q2" s="20"/>
-      <c r="R2" s="20"/>
-      <c r="S2" s="20"/>
-      <c r="T2" s="20"/>
-      <c r="U2" s="20"/>
-      <c r="V2" s="20"/>
-      <c r="W2" s="20"/>
-      <c r="X2" s="20"/>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="20"/>
-      <c r="AA2" s="20"/>
-      <c r="AB2" s="20"/>
-      <c r="AC2" s="20"/>
-      <c r="AD2" s="20"/>
-      <c r="AE2" s="20"/>
-      <c r="AF2" s="20"/>
-      <c r="AG2" s="20"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="20"/>
-      <c r="AJ2" s="20"/>
-      <c r="AK2" s="20"/>
-      <c r="AL2" s="20"/>
-      <c r="AM2" s="20"/>
-      <c r="AN2" s="20"/>
-      <c r="AO2" s="20"/>
-      <c r="AP2" s="20"/>
-      <c r="AQ2" s="20"/>
-      <c r="AR2" s="20"/>
-      <c r="AS2" s="20"/>
-      <c r="AT2" s="20"/>
-      <c r="AU2" s="20"/>
-      <c r="AV2" s="20"/>
-      <c r="AW2" s="20"/>
-      <c r="AX2" s="20"/>
-      <c r="AY2" s="20"/>
-      <c r="AZ2" s="20"/>
-      <c r="BA2" s="20"/>
-      <c r="BB2" s="20"/>
-      <c r="BC2" s="20"/>
-      <c r="BD2" s="20"/>
-      <c r="BE2" s="20"/>
-      <c r="BF2" s="20"/>
-      <c r="BG2" s="20"/>
-      <c r="BH2" s="20"/>
-      <c r="BI2" s="20"/>
-      <c r="BJ2" s="20"/>
-      <c r="BK2" s="20"/>
-      <c r="BL2" s="20"/>
-      <c r="BM2" s="20"/>
-      <c r="BN2" s="20"/>
-      <c r="BO2" s="20"/>
-      <c r="BP2" s="20"/>
-      <c r="BQ2" s="20"/>
-      <c r="BR2" s="20"/>
-      <c r="BS2" s="20"/>
-      <c r="BT2" s="20"/>
-      <c r="BU2" s="20"/>
-      <c r="BV2" s="20"/>
-      <c r="BW2" s="20"/>
-      <c r="BX2" s="20"/>
-      <c r="BY2" s="20"/>
-      <c r="BZ2" s="20"/>
-      <c r="CA2" s="20"/>
-      <c r="CB2" s="20"/>
-      <c r="CC2" s="20"/>
-      <c r="CD2" s="20"/>
-      <c r="CE2" s="20"/>
-      <c r="CF2" s="20"/>
-      <c r="CG2" s="20"/>
-      <c r="CH2" s="20"/>
-      <c r="CI2" s="20"/>
-      <c r="CJ2" s="20"/>
-      <c r="CK2" s="20"/>
-      <c r="CL2" s="20"/>
-      <c r="CM2" s="20"/>
-      <c r="CN2" s="20"/>
-      <c r="CO2" s="20"/>
-      <c r="CP2" s="20"/>
-      <c r="CQ2" s="20"/>
-      <c r="CR2" s="20"/>
-      <c r="CS2" s="20"/>
-      <c r="CT2" s="20"/>
-      <c r="CU2" s="20"/>
-      <c r="CV2" s="20"/>
-      <c r="CW2" s="20"/>
-      <c r="CX2" s="20"/>
-      <c r="CY2" s="20"/>
-      <c r="CZ2" s="20"/>
-      <c r="DA2" s="20"/>
-      <c r="DB2" s="20"/>
-      <c r="DC2" s="20"/>
-      <c r="DD2" s="20"/>
-      <c r="DE2" s="20"/>
-      <c r="DF2" s="20"/>
-      <c r="DG2" s="20"/>
-      <c r="DH2" s="20"/>
-      <c r="DI2" s="20"/>
-      <c r="DJ2" s="20"/>
-      <c r="DK2" s="20"/>
-      <c r="DL2" s="20"/>
-      <c r="DM2" s="20"/>
-      <c r="DN2" s="20"/>
-      <c r="DO2" s="20"/>
-      <c r="DP2" s="20"/>
-      <c r="DQ2" s="20"/>
-      <c r="DR2" s="20"/>
-      <c r="DS2" s="20"/>
-      <c r="DT2" s="20"/>
-      <c r="DU2" s="20"/>
-      <c r="DV2" s="20"/>
-      <c r="DW2" s="20"/>
-      <c r="DX2" s="21"/>
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
+      <c r="I2" s="26"/>
+      <c r="J2" s="26"/>
+      <c r="K2" s="26"/>
+      <c r="L2" s="26"/>
+      <c r="M2" s="26"/>
+      <c r="N2" s="26"/>
+      <c r="O2" s="26"/>
+      <c r="P2" s="26"/>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="26"/>
+      <c r="T2" s="26"/>
+      <c r="U2" s="26"/>
+      <c r="V2" s="26"/>
+      <c r="W2" s="26"/>
+      <c r="X2" s="26"/>
+      <c r="Y2" s="26"/>
+      <c r="Z2" s="26"/>
+      <c r="AA2" s="26"/>
+      <c r="AB2" s="26"/>
+      <c r="AC2" s="26"/>
+      <c r="AD2" s="26"/>
+      <c r="AE2" s="26"/>
+      <c r="AF2" s="26"/>
+      <c r="AG2" s="26"/>
+      <c r="AH2" s="26"/>
+      <c r="AI2" s="26"/>
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="26"/>
+      <c r="AL2" s="26"/>
+      <c r="AM2" s="26"/>
+      <c r="AN2" s="26"/>
+      <c r="AO2" s="26"/>
+      <c r="AP2" s="26"/>
+      <c r="AQ2" s="26"/>
+      <c r="AR2" s="26"/>
+      <c r="AS2" s="26"/>
+      <c r="AT2" s="26"/>
+      <c r="AU2" s="26"/>
+      <c r="AV2" s="26"/>
+      <c r="AW2" s="26"/>
+      <c r="AX2" s="26"/>
+      <c r="AY2" s="26"/>
+      <c r="AZ2" s="26"/>
+      <c r="BA2" s="26"/>
+      <c r="BB2" s="26"/>
+      <c r="BC2" s="26"/>
+      <c r="BD2" s="26"/>
+      <c r="BE2" s="26"/>
+      <c r="BF2" s="26"/>
+      <c r="BG2" s="26"/>
+      <c r="BH2" s="26"/>
+      <c r="BI2" s="26"/>
+      <c r="BJ2" s="26"/>
+      <c r="BK2" s="26"/>
+      <c r="BL2" s="26"/>
+      <c r="BM2" s="26"/>
+      <c r="BN2" s="26"/>
+      <c r="BO2" s="26"/>
+      <c r="BP2" s="26"/>
+      <c r="BQ2" s="26"/>
+      <c r="BR2" s="26"/>
+      <c r="BS2" s="26"/>
+      <c r="BT2" s="26"/>
+      <c r="BU2" s="26"/>
+      <c r="BV2" s="26"/>
+      <c r="BW2" s="26"/>
+      <c r="BX2" s="26"/>
+      <c r="BY2" s="26"/>
+      <c r="BZ2" s="26"/>
+      <c r="CA2" s="26"/>
+      <c r="CB2" s="26"/>
+      <c r="CC2" s="26"/>
+      <c r="CD2" s="26"/>
+      <c r="CE2" s="26"/>
+      <c r="CF2" s="26"/>
+      <c r="CG2" s="26"/>
+      <c r="CH2" s="26"/>
+      <c r="CI2" s="26"/>
+      <c r="CJ2" s="26"/>
+      <c r="CK2" s="26"/>
+      <c r="CL2" s="26"/>
+      <c r="CM2" s="26"/>
+      <c r="CN2" s="26"/>
+      <c r="CO2" s="26"/>
+      <c r="CP2" s="26"/>
+      <c r="CQ2" s="26"/>
+      <c r="CR2" s="26"/>
+      <c r="CS2" s="26"/>
+      <c r="CT2" s="26"/>
+      <c r="CU2" s="26"/>
+      <c r="CV2" s="26"/>
+      <c r="CW2" s="26"/>
+      <c r="CX2" s="26"/>
+      <c r="CY2" s="26"/>
+      <c r="CZ2" s="26"/>
+      <c r="DA2" s="26"/>
+      <c r="DB2" s="26"/>
+      <c r="DC2" s="26"/>
+      <c r="DD2" s="26"/>
+      <c r="DE2" s="26"/>
+      <c r="DF2" s="26"/>
+      <c r="DG2" s="26"/>
+      <c r="DH2" s="26"/>
+      <c r="DI2" s="26"/>
+      <c r="DJ2" s="26"/>
+      <c r="DK2" s="26"/>
+      <c r="DL2" s="26"/>
+      <c r="DM2" s="26"/>
+      <c r="DN2" s="26"/>
+      <c r="DO2" s="26"/>
+      <c r="DP2" s="26"/>
+      <c r="DQ2" s="26"/>
+      <c r="DR2" s="26"/>
+      <c r="DS2" s="26"/>
+      <c r="DT2" s="26"/>
+      <c r="DU2" s="26"/>
+      <c r="DV2" s="26"/>
+      <c r="DW2" s="26"/>
+      <c r="DX2" s="27"/>
     </row>
     <row r="3" spans="1:157" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2047,155 +2557,173 @@
         <v>44809</v>
       </c>
     </row>
-    <row r="4" spans="1:157" s="4" customFormat="1" ht="22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:157" s="4" customFormat="1" ht="26" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="24" t="s">
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="24"/>
-      <c r="K4" s="24"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="24"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="24"/>
-      <c r="P4" s="24" t="s">
+      <c r="J4" s="30"/>
+      <c r="K4" s="30"/>
+      <c r="L4" s="30"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="30"/>
+      <c r="O4" s="30"/>
+      <c r="P4" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="24"/>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24"/>
-      <c r="T4" s="24"/>
-      <c r="U4" s="24"/>
-      <c r="V4" s="24"/>
-      <c r="W4" s="30" t="s">
+      <c r="Q4" s="30"/>
+      <c r="R4" s="30"/>
+      <c r="S4" s="30"/>
+      <c r="T4" s="30"/>
+      <c r="U4" s="30"/>
+      <c r="V4" s="30"/>
+      <c r="W4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="30"/>
-      <c r="AF4" s="30"/>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="30"/>
-      <c r="AJ4" s="30"/>
-      <c r="AK4" s="30"/>
-      <c r="AL4" s="30"/>
-      <c r="AM4" s="30"/>
-      <c r="AN4" s="30"/>
-      <c r="AO4" s="30"/>
-      <c r="AP4" s="30"/>
-      <c r="AQ4" s="30"/>
-      <c r="AR4" s="30"/>
-      <c r="AS4" s="30"/>
-      <c r="AT4" s="30"/>
-      <c r="AU4" s="30"/>
-      <c r="AV4" s="30"/>
-      <c r="AW4" s="30"/>
-      <c r="AX4" s="32" t="s">
+      <c r="X4" s="13"/>
+      <c r="Y4" s="13"/>
+      <c r="Z4" s="13"/>
+      <c r="AA4" s="13"/>
+      <c r="AB4" s="13"/>
+      <c r="AC4" s="13"/>
+      <c r="AD4" s="13"/>
+      <c r="AE4" s="13"/>
+      <c r="AF4" s="13"/>
+      <c r="AG4" s="13"/>
+      <c r="AH4" s="13"/>
+      <c r="AI4" s="13"/>
+      <c r="AJ4" s="13"/>
+      <c r="AK4" s="13"/>
+      <c r="AL4" s="13"/>
+      <c r="AM4" s="13"/>
+      <c r="AN4" s="13"/>
+      <c r="AO4" s="13"/>
+      <c r="AP4" s="13"/>
+      <c r="AQ4" s="13"/>
+      <c r="AR4" s="13"/>
+      <c r="AS4" s="13"/>
+      <c r="AT4" s="13"/>
+      <c r="AU4" s="13"/>
+      <c r="AV4" s="13"/>
+      <c r="AW4" s="13"/>
+      <c r="AX4" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AY4" s="32"/>
-      <c r="AZ4" s="32"/>
-      <c r="BA4" s="32"/>
-      <c r="BB4" s="32"/>
-      <c r="BC4" s="31" t="s">
+      <c r="AY4" s="15"/>
+      <c r="AZ4" s="15"/>
+      <c r="BA4" s="15"/>
+      <c r="BB4" s="15"/>
+      <c r="BC4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="BD4" s="31"/>
-      <c r="BE4" s="26" t="s">
+      <c r="BD4" s="14"/>
+      <c r="BE4" s="32" t="s">
         <v>10</v>
       </c>
-      <c r="BF4" s="25" t="s">
+      <c r="BF4" s="31" t="s">
         <v>9</v>
       </c>
-      <c r="BG4" s="5"/>
-      <c r="BH4" s="5"/>
-      <c r="BI4" s="5"/>
-      <c r="BJ4" s="5"/>
-      <c r="BK4" s="5"/>
-      <c r="BL4" s="5"/>
-      <c r="BM4" s="5"/>
-      <c r="BN4" s="5"/>
-      <c r="BO4" s="5"/>
-      <c r="BP4" s="5"/>
-      <c r="BQ4" s="5"/>
-      <c r="BR4" s="5"/>
-      <c r="BS4" s="5"/>
-      <c r="BT4" s="5"/>
-      <c r="BU4" s="5"/>
-      <c r="BV4" s="5"/>
-      <c r="BW4" s="5"/>
-      <c r="BX4" s="5"/>
-      <c r="BY4" s="5"/>
-      <c r="BZ4" s="5"/>
-      <c r="CA4" s="5"/>
-      <c r="CB4" s="5"/>
-      <c r="CC4" s="5"/>
-      <c r="CD4" s="5"/>
-      <c r="CE4" s="5"/>
-      <c r="CF4" s="5"/>
-      <c r="CG4" s="5"/>
-      <c r="CH4" s="5"/>
-      <c r="CI4" s="5"/>
-      <c r="CJ4" s="5"/>
-      <c r="CK4" s="5"/>
-      <c r="CL4" s="5"/>
-      <c r="CM4" s="5"/>
-      <c r="CN4" s="5"/>
-      <c r="CO4" s="5"/>
-      <c r="CP4" s="5"/>
-      <c r="CQ4" s="5"/>
-      <c r="CR4" s="5"/>
-      <c r="CS4" s="5"/>
-      <c r="CT4" s="5"/>
-      <c r="CU4" s="5"/>
-      <c r="CV4" s="5"/>
-      <c r="CW4" s="5"/>
-      <c r="CX4" s="5"/>
-      <c r="CY4" s="5"/>
-      <c r="CZ4" s="5"/>
-      <c r="DA4" s="5"/>
-      <c r="DB4" s="5"/>
-      <c r="DC4" s="5"/>
-      <c r="DD4" s="5"/>
-      <c r="DE4" s="5"/>
-      <c r="DF4" s="5"/>
-      <c r="DG4" s="5"/>
-      <c r="DH4" s="5"/>
-      <c r="DI4" s="5"/>
-      <c r="DJ4" s="5"/>
-      <c r="DK4" s="5"/>
-      <c r="DL4" s="5"/>
-      <c r="DM4" s="5"/>
-      <c r="DN4" s="5"/>
-      <c r="DO4" s="5"/>
-      <c r="DP4" s="5"/>
-      <c r="DQ4" s="5"/>
-      <c r="DR4" s="5"/>
-      <c r="DS4" s="5"/>
-      <c r="DT4" s="5"/>
-      <c r="DU4" s="5"/>
-      <c r="DV4" s="5"/>
-      <c r="DW4" s="26" t="s">
+      <c r="BG4" s="39" t="s">
+        <v>43</v>
+      </c>
+      <c r="BH4" s="40"/>
+      <c r="BI4" s="40"/>
+      <c r="BJ4" s="40"/>
+      <c r="BK4" s="40"/>
+      <c r="BL4" s="41"/>
+      <c r="BM4" s="42" t="s">
+        <v>44</v>
+      </c>
+      <c r="BN4" s="43"/>
+      <c r="BO4" s="43"/>
+      <c r="BP4" s="43"/>
+      <c r="BQ4" s="43"/>
+      <c r="BR4" s="43"/>
+      <c r="BS4" s="44"/>
+      <c r="BT4" s="45" t="s">
+        <v>45</v>
+      </c>
+      <c r="BU4" s="46"/>
+      <c r="BV4" s="46"/>
+      <c r="BW4" s="46"/>
+      <c r="BX4" s="46"/>
+      <c r="BY4" s="46"/>
+      <c r="BZ4" s="47"/>
+      <c r="CA4" s="67" t="s">
+        <v>46</v>
+      </c>
+      <c r="CB4" s="68"/>
+      <c r="CC4" s="68"/>
+      <c r="CD4" s="68"/>
+      <c r="CE4" s="68"/>
+      <c r="CF4" s="68"/>
+      <c r="CG4" s="69"/>
+      <c r="CH4" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="CI4" s="49"/>
+      <c r="CJ4" s="49"/>
+      <c r="CK4" s="49"/>
+      <c r="CL4" s="49"/>
+      <c r="CM4" s="49"/>
+      <c r="CN4" s="50"/>
+      <c r="CO4" s="54" t="s">
+        <v>49</v>
+      </c>
+      <c r="CP4" s="55"/>
+      <c r="CQ4" s="55"/>
+      <c r="CR4" s="55"/>
+      <c r="CS4" s="55"/>
+      <c r="CT4" s="56"/>
+      <c r="CU4" s="57" t="s">
+        <v>50</v>
+      </c>
+      <c r="CV4" s="58"/>
+      <c r="CW4" s="58"/>
+      <c r="CX4" s="58"/>
+      <c r="CY4" s="58"/>
+      <c r="CZ4" s="58"/>
+      <c r="DA4" s="59"/>
+      <c r="DB4" s="63" t="s">
+        <v>42</v>
+      </c>
+      <c r="DC4" s="64"/>
+      <c r="DD4" s="64"/>
+      <c r="DE4" s="64"/>
+      <c r="DF4" s="64"/>
+      <c r="DG4" s="64"/>
+      <c r="DH4" s="64"/>
+      <c r="DI4" s="64"/>
+      <c r="DJ4" s="64"/>
+      <c r="DK4" s="64"/>
+      <c r="DL4" s="64"/>
+      <c r="DM4" s="64"/>
+      <c r="DN4" s="64"/>
+      <c r="DO4" s="64"/>
+      <c r="DP4" s="65"/>
+      <c r="DQ4" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="DR4" s="52"/>
+      <c r="DS4" s="52"/>
+      <c r="DT4" s="52"/>
+      <c r="DU4" s="52"/>
+      <c r="DV4" s="53"/>
+      <c r="DW4" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="DX4" s="25" t="s">
+      <c r="DX4" s="31" t="s">
         <v>12</v>
       </c>
       <c r="DY4" s="5"/>
@@ -2235,81 +2763,122 @@
       <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="23"/>
-      <c r="E5" s="23"/>
-      <c r="F5" s="23"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="29"/>
+      <c r="F5" s="29"/>
       <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="13" t="s">
+      <c r="I5" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="14"/>
-      <c r="K5" s="14"/>
-      <c r="L5" s="14"/>
-      <c r="M5" s="15"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="20"/>
       <c r="N5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="13" t="s">
+      <c r="O5" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="14"/>
-      <c r="Q5" s="14"/>
-      <c r="R5" s="14"/>
-      <c r="S5" s="14"/>
-      <c r="T5" s="14"/>
-      <c r="U5" s="15"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="20"/>
       <c r="V5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="13" t="s">
+      <c r="W5" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="X5" s="14"/>
-      <c r="Y5" s="14"/>
-      <c r="Z5" s="14"/>
-      <c r="AA5" s="14"/>
-      <c r="AB5" s="15"/>
+      <c r="X5" s="21"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="21"/>
+      <c r="AB5" s="20"/>
       <c r="AC5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="13" t="s">
+      <c r="AD5" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="AE5" s="14"/>
-      <c r="AF5" s="14"/>
-      <c r="AG5" s="14"/>
-      <c r="AH5" s="14"/>
-      <c r="AI5" s="15"/>
+      <c r="AE5" s="21"/>
+      <c r="AF5" s="21"/>
+      <c r="AG5" s="21"/>
+      <c r="AH5" s="21"/>
+      <c r="AI5" s="20"/>
       <c r="AJ5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AK5" s="13"/>
-      <c r="AL5" s="14"/>
-      <c r="AM5" s="14"/>
-      <c r="AN5" s="14"/>
-      <c r="AO5" s="14"/>
-      <c r="AP5" s="15"/>
+      <c r="AK5" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL5" s="21"/>
+      <c r="AM5" s="21"/>
+      <c r="AN5" s="21"/>
+      <c r="AO5" s="21"/>
+      <c r="AP5" s="20"/>
       <c r="AQ5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AR5" s="13"/>
-      <c r="AS5" s="14"/>
-      <c r="AT5" s="14"/>
-      <c r="AU5" s="14"/>
-      <c r="AV5" s="14"/>
-      <c r="AW5" s="15"/>
+      <c r="AR5" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="AS5" s="21"/>
+      <c r="AT5" s="21"/>
+      <c r="AU5" s="21"/>
+      <c r="AV5" s="21"/>
+      <c r="AW5" s="20"/>
       <c r="AX5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="BE5" s="26"/>
-      <c r="BF5" s="25"/>
-      <c r="DW5" s="26"/>
-      <c r="DX5" s="25"/>
+      <c r="AY5" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="AZ5" s="21"/>
+      <c r="BA5" s="21"/>
+      <c r="BB5" s="20"/>
+      <c r="BC5" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="BD5" s="20"/>
+      <c r="BE5" s="32"/>
+      <c r="BF5" s="31"/>
+      <c r="BL5" s="60" t="s">
+        <v>51</v>
+      </c>
+      <c r="BS5" s="60" t="s">
+        <v>52</v>
+      </c>
+      <c r="BZ5" s="60" t="s">
+        <v>53</v>
+      </c>
+      <c r="CG5" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="CN5" s="61" t="s">
+        <v>55</v>
+      </c>
+      <c r="CU5" s="61" t="s">
+        <v>56</v>
+      </c>
+      <c r="DB5" s="62" t="s">
+        <v>57</v>
+      </c>
+      <c r="DI5" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="DP5" s="66" t="s">
+        <v>41</v>
+      </c>
+      <c r="DW5" s="32"/>
+      <c r="DX5" s="31"/>
     </row>
     <row r="6" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -2321,33 +2890,44 @@
       <c r="N6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="27" t="s">
+      <c r="V6" s="33" t="s">
         <v>24</v>
       </c>
       <c r="AC6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="AK6" s="33" t="s">
+      <c r="AK6" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="AL6" s="34"/>
-      <c r="AM6" s="34"/>
-      <c r="AN6" s="34"/>
-      <c r="AO6" s="34"/>
-      <c r="AP6" s="35"/>
-      <c r="BC6" s="13" t="s">
+      <c r="AL6" s="17"/>
+      <c r="AM6" s="17"/>
+      <c r="AN6" s="17"/>
+      <c r="AO6" s="17"/>
+      <c r="AP6" s="18"/>
+      <c r="AV6" s="36" t="s">
+        <v>34</v>
+      </c>
+      <c r="AW6" s="37"/>
+      <c r="AX6" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="AY6" s="19"/>
+      <c r="AZ6" s="21"/>
+      <c r="BA6" s="21"/>
+      <c r="BB6" s="20"/>
+      <c r="BC6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="BD6" s="15"/>
-      <c r="BE6" s="26"/>
-      <c r="BF6" s="25"/>
-      <c r="DW6" s="26"/>
-      <c r="DX6" s="25"/>
+      <c r="BD6" s="20"/>
+      <c r="BE6" s="32"/>
+      <c r="BF6" s="31"/>
+      <c r="DW6" s="32"/>
+      <c r="DX6" s="31"/>
     </row>
     <row r="7" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V7" s="28"/>
-      <c r="BF7" s="25"/>
-      <c r="DX7" s="25"/>
+      <c r="V7" s="34"/>
+      <c r="BF7" s="31"/>
+      <c r="DX7" s="31"/>
     </row>
     <row r="8" spans="1:157" s="4" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -2355,20 +2935,21 @@
       </c>
       <c r="B8" s="7">
         <f ca="1">TODAY()</f>
-        <v>44716</v>
-      </c>
-      <c r="V8" s="29"/>
+        <v>44717</v>
+      </c>
+      <c r="V8" s="35"/>
     </row>
   </sheetData>
-  <mergeCells count="21">
-    <mergeCell ref="W4:AW4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="AX4:BB4"/>
-    <mergeCell ref="AK6:AP6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="AD5:AI5"/>
-    <mergeCell ref="AK5:AP5"/>
-    <mergeCell ref="AR5:AW5"/>
+  <mergeCells count="34">
+    <mergeCell ref="DQ4:DV4"/>
+    <mergeCell ref="CO4:CT4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="BG4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="DB4:DP4"/>
     <mergeCell ref="A1:DX2"/>
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="O5:U5"/>
@@ -2382,15 +2963,27 @@
     <mergeCell ref="DX4:DX7"/>
     <mergeCell ref="DW4:DW6"/>
     <mergeCell ref="P4:V4"/>
+    <mergeCell ref="AY6:BB6"/>
+    <mergeCell ref="AV6:AW6"/>
+    <mergeCell ref="AY5:BB5"/>
+    <mergeCell ref="W4:AW4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="AX4:BB4"/>
+    <mergeCell ref="AK6:AP6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="AD5:AI5"/>
+    <mergeCell ref="AK5:AP5"/>
+    <mergeCell ref="AR5:AW5"/>
+    <mergeCell ref="BC5:BD5"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:XFD3">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">
       <formula>$B$8</formula>
     </cfRule>
     <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>$B$8</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="3" operator="greaterThan">
       <formula>$B$8</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Meeting log from 3 Jul 22 // timeline update
</commit_message>
<xml_diff>
--- a/Timeline/Project_Timeline.xlsx
+++ b/Timeline/Project_Timeline.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10520"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Desktop/agile/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9469DA6E-381F-254E-9AA6-3E8AA7CD3DDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3216790F-FA9C-364D-A073-8D8C6AF6DFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19820" yWindow="2240" windowWidth="28800" windowHeight="22140" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
+    <workbookView xWindow="15920" yWindow="4020" windowWidth="28800" windowHeight="22140" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
   <si>
     <t>ASP - Group Project</t>
   </si>
@@ -442,30 +442,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Team Meeting 7 - Proposal </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Distributing the tasks required for the Proposal submission</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">
 - Team is progressing well with initial designs. 
 - The team will now produce the the opposite of the design they produced last week 
@@ -737,13 +713,48 @@
 - Review midterm submissions</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Team Meeting 15 - Development Update </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
+    <t>Testing &amp; Evaluation</t>
+  </si>
+  <si>
+    <t>Sprint 1 - Software Development</t>
+  </si>
+  <si>
+    <t>Sprint 2 - Software Development</t>
+  </si>
+  <si>
+    <t>Sprint 3 - Software Development</t>
+  </si>
+  <si>
+    <t>Sprint 4 - Software Development</t>
+  </si>
+  <si>
+    <t>Sprint 5 - Software Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Final Analysis </t>
+  </si>
+  <si>
+    <t>Sprint 6 - Software Development</t>
+  </si>
+  <si>
+    <t>Sprint 7 - Software Development</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Team Meeting 9 - Development Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -754,12 +765,12 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Team Meeting 16 - Development Update </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFFFFFF"/>
+      <t xml:space="preserve">Team Meeting 14 - Development Update </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -769,33 +780,6 @@
     </r>
   </si>
   <si>
-    <t>Testing &amp; Evaluation</t>
-  </si>
-  <si>
-    <t>Sprint 1 - Software Development</t>
-  </si>
-  <si>
-    <t>Sprint 2 - Software Development</t>
-  </si>
-  <si>
-    <t>Sprint 3 - Software Development</t>
-  </si>
-  <si>
-    <t>Sprint 4 - Software Development</t>
-  </si>
-  <si>
-    <t>Sprint 5 - Software Development</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Final Analysis </t>
-  </si>
-  <si>
-    <t>Sprint 6 - Software Development</t>
-  </si>
-  <si>
-    <t>Sprint 7 - Software Development</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <b/>
@@ -805,7 +789,130 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Team Meeting 9 - Development Update </t>
+      <t xml:space="preserve">Ben &amp; Thavelarn
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Develop basic HTML skeleton for the navigation bar / other areas of the program
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">David, Kashka, Connor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Develop code for a reactive navigation bar (to be implemented later)
+- Develop code to utilise the host OS to select and load a specific file 
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Ben &amp; Thavelarn
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Develop the HTML skeleton further
+- Add basic CSS to the design
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">David, Kashka, Connor
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Develop code implemeting charts.js 
+- Develop code to implement a menu button
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Proposal Meeting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Distributing the tasks required for the Proposal submission</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Team Meeting 7 - Development Update </t>
     </r>
     <r>
       <rPr>
@@ -829,7 +936,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve">Team Meeting 10 - Development Update </t>
+      <t xml:space="preserve">Team Meeting 8 - Development Update </t>
     </r>
     <r>
       <rPr>
@@ -845,15 +952,7 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Team Meeting 11 - Development Update </t>
+      <t xml:space="preserve">Team Meeting 10 - Development Update </t>
     </r>
     <r>
       <rPr>
@@ -869,7 +968,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Team Meeting 12 - Development Update </t>
+      <t xml:space="preserve">Team Meeting 11 - Development Update </t>
     </r>
     <r>
       <rPr>
@@ -884,13 +983,76 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Team Meeting 13 - Development Update </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
+    <t>Intended MVP deadline</t>
+  </si>
+  <si>
+    <t>THIS WEEK MAY BE CONTINGENCY DEVELOPMENT TIME AS SPRINT 8 IF REQUIRED</t>
+  </si>
+  <si>
+    <t>DEVELOPMENT DEADLINE</t>
+  </si>
+  <si>
+    <t>TBC</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DEVELOPMENT CONTINGENCY PERIOD
+IF TIME PERMITS … </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Add in more features to the software
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If MVP NOT CREATED</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Continue with MVP development as a contingency period</t>
+    </r>
+  </si>
+  <si>
+    <t>OPTIONAL DEVELOPMENT CONTINGENCY PERIOD IF FURTHER DEVELOPEMT IS NEEDED</t>
+  </si>
+  <si>
+    <r>
+      <t>Team Meeting 15 - T&amp;E meeting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -901,12 +1063,12 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Team Meeting 14 - Development Update </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
+      <t>Team Meeting 15 - T&amp;E meeting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -917,12 +1079,12 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Team Meeting 15 - Development Update </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0"/>
+      <t>Team Meeting 16 - Final T&amp;E meeting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFFFFFF"/>
         <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
@@ -930,6 +1092,9 @@
       <t xml:space="preserve">
 Update on the project build</t>
     </r>
+  </si>
+  <si>
+    <t>Prepare group submission</t>
   </si>
 </sst>
 </file>
@@ -939,7 +1104,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -993,13 +1158,6 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1336,7 +1494,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1374,147 +1532,9 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="21" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -1524,6 +1544,81 @@
     <xf numFmtId="0" fontId="7" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1533,17 +1628,83 @@
     <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1900,8 +2061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3400B0-A312-474B-BDD8-7EBBB1942BA5}">
   <dimension ref="A1:FA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:DX2"/>
+    <sheetView tabSelected="1" topLeftCell="BD4" workbookViewId="0">
+      <selection activeCell="DQ6" sqref="DQ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1910,266 +2071,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="22" t="s">
+      <c r="A1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="23"/>
-      <c r="F1" s="23"/>
-      <c r="G1" s="23"/>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="23"/>
-      <c r="N1" s="23"/>
-      <c r="O1" s="23"/>
-      <c r="P1" s="23"/>
-      <c r="Q1" s="23"/>
-      <c r="R1" s="23"/>
-      <c r="S1" s="23"/>
-      <c r="T1" s="23"/>
-      <c r="U1" s="23"/>
-      <c r="V1" s="23"/>
-      <c r="W1" s="23"/>
-      <c r="X1" s="23"/>
-      <c r="Y1" s="23"/>
-      <c r="Z1" s="23"/>
-      <c r="AA1" s="23"/>
-      <c r="AB1" s="23"/>
-      <c r="AC1" s="23"/>
-      <c r="AD1" s="23"/>
-      <c r="AE1" s="23"/>
-      <c r="AF1" s="23"/>
-      <c r="AG1" s="23"/>
-      <c r="AH1" s="23"/>
-      <c r="AI1" s="23"/>
-      <c r="AJ1" s="23"/>
-      <c r="AK1" s="23"/>
-      <c r="AL1" s="23"/>
-      <c r="AM1" s="23"/>
-      <c r="AN1" s="23"/>
-      <c r="AO1" s="23"/>
-      <c r="AP1" s="23"/>
-      <c r="AQ1" s="23"/>
-      <c r="AR1" s="23"/>
-      <c r="AS1" s="23"/>
-      <c r="AT1" s="23"/>
-      <c r="AU1" s="23"/>
-      <c r="AV1" s="23"/>
-      <c r="AW1" s="23"/>
-      <c r="AX1" s="23"/>
-      <c r="AY1" s="23"/>
-      <c r="AZ1" s="23"/>
-      <c r="BA1" s="23"/>
-      <c r="BB1" s="23"/>
-      <c r="BC1" s="23"/>
-      <c r="BD1" s="23"/>
-      <c r="BE1" s="23"/>
-      <c r="BF1" s="23"/>
-      <c r="BG1" s="23"/>
-      <c r="BH1" s="23"/>
-      <c r="BI1" s="23"/>
-      <c r="BJ1" s="23"/>
-      <c r="BK1" s="23"/>
-      <c r="BL1" s="23"/>
-      <c r="BM1" s="23"/>
-      <c r="BN1" s="23"/>
-      <c r="BO1" s="23"/>
-      <c r="BP1" s="23"/>
-      <c r="BQ1" s="23"/>
-      <c r="BR1" s="23"/>
-      <c r="BS1" s="23"/>
-      <c r="BT1" s="23"/>
-      <c r="BU1" s="23"/>
-      <c r="BV1" s="23"/>
-      <c r="BW1" s="23"/>
-      <c r="BX1" s="23"/>
-      <c r="BY1" s="23"/>
-      <c r="BZ1" s="23"/>
-      <c r="CA1" s="23"/>
-      <c r="CB1" s="23"/>
-      <c r="CC1" s="23"/>
-      <c r="CD1" s="23"/>
-      <c r="CE1" s="23"/>
-      <c r="CF1" s="23"/>
-      <c r="CG1" s="23"/>
-      <c r="CH1" s="23"/>
-      <c r="CI1" s="23"/>
-      <c r="CJ1" s="23"/>
-      <c r="CK1" s="23"/>
-      <c r="CL1" s="23"/>
-      <c r="CM1" s="23"/>
-      <c r="CN1" s="23"/>
-      <c r="CO1" s="23"/>
-      <c r="CP1" s="23"/>
-      <c r="CQ1" s="23"/>
-      <c r="CR1" s="23"/>
-      <c r="CS1" s="23"/>
-      <c r="CT1" s="23"/>
-      <c r="CU1" s="23"/>
-      <c r="CV1" s="23"/>
-      <c r="CW1" s="23"/>
-      <c r="CX1" s="23"/>
-      <c r="CY1" s="23"/>
-      <c r="CZ1" s="23"/>
-      <c r="DA1" s="23"/>
-      <c r="DB1" s="23"/>
-      <c r="DC1" s="23"/>
-      <c r="DD1" s="23"/>
-      <c r="DE1" s="23"/>
-      <c r="DF1" s="23"/>
-      <c r="DG1" s="23"/>
-      <c r="DH1" s="23"/>
-      <c r="DI1" s="23"/>
-      <c r="DJ1" s="23"/>
-      <c r="DK1" s="23"/>
-      <c r="DL1" s="23"/>
-      <c r="DM1" s="23"/>
-      <c r="DN1" s="23"/>
-      <c r="DO1" s="23"/>
-      <c r="DP1" s="23"/>
-      <c r="DQ1" s="23"/>
-      <c r="DR1" s="23"/>
-      <c r="DS1" s="23"/>
-      <c r="DT1" s="23"/>
-      <c r="DU1" s="23"/>
-      <c r="DV1" s="23"/>
-      <c r="DW1" s="23"/>
-      <c r="DX1" s="24"/>
+      <c r="B1" s="46"/>
+      <c r="C1" s="46"/>
+      <c r="D1" s="46"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="46"/>
+      <c r="I1" s="46"/>
+      <c r="J1" s="46"/>
+      <c r="K1" s="46"/>
+      <c r="L1" s="46"/>
+      <c r="M1" s="46"/>
+      <c r="N1" s="46"/>
+      <c r="O1" s="46"/>
+      <c r="P1" s="46"/>
+      <c r="Q1" s="46"/>
+      <c r="R1" s="46"/>
+      <c r="S1" s="46"/>
+      <c r="T1" s="46"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="46"/>
+      <c r="W1" s="46"/>
+      <c r="X1" s="46"/>
+      <c r="Y1" s="46"/>
+      <c r="Z1" s="46"/>
+      <c r="AA1" s="46"/>
+      <c r="AB1" s="46"/>
+      <c r="AC1" s="46"/>
+      <c r="AD1" s="46"/>
+      <c r="AE1" s="46"/>
+      <c r="AF1" s="46"/>
+      <c r="AG1" s="46"/>
+      <c r="AH1" s="46"/>
+      <c r="AI1" s="46"/>
+      <c r="AJ1" s="46"/>
+      <c r="AK1" s="46"/>
+      <c r="AL1" s="46"/>
+      <c r="AM1" s="46"/>
+      <c r="AN1" s="46"/>
+      <c r="AO1" s="46"/>
+      <c r="AP1" s="46"/>
+      <c r="AQ1" s="46"/>
+      <c r="AR1" s="46"/>
+      <c r="AS1" s="46"/>
+      <c r="AT1" s="46"/>
+      <c r="AU1" s="46"/>
+      <c r="AV1" s="46"/>
+      <c r="AW1" s="46"/>
+      <c r="AX1" s="46"/>
+      <c r="AY1" s="46"/>
+      <c r="AZ1" s="46"/>
+      <c r="BA1" s="46"/>
+      <c r="BB1" s="46"/>
+      <c r="BC1" s="46"/>
+      <c r="BD1" s="46"/>
+      <c r="BE1" s="46"/>
+      <c r="BF1" s="46"/>
+      <c r="BG1" s="46"/>
+      <c r="BH1" s="46"/>
+      <c r="BI1" s="46"/>
+      <c r="BJ1" s="46"/>
+      <c r="BK1" s="46"/>
+      <c r="BL1" s="46"/>
+      <c r="BM1" s="46"/>
+      <c r="BN1" s="46"/>
+      <c r="BO1" s="46"/>
+      <c r="BP1" s="46"/>
+      <c r="BQ1" s="46"/>
+      <c r="BR1" s="46"/>
+      <c r="BS1" s="46"/>
+      <c r="BT1" s="46"/>
+      <c r="BU1" s="46"/>
+      <c r="BV1" s="46"/>
+      <c r="BW1" s="46"/>
+      <c r="BX1" s="46"/>
+      <c r="BY1" s="46"/>
+      <c r="BZ1" s="46"/>
+      <c r="CA1" s="46"/>
+      <c r="CB1" s="46"/>
+      <c r="CC1" s="46"/>
+      <c r="CD1" s="46"/>
+      <c r="CE1" s="46"/>
+      <c r="CF1" s="46"/>
+      <c r="CG1" s="46"/>
+      <c r="CH1" s="46"/>
+      <c r="CI1" s="46"/>
+      <c r="CJ1" s="46"/>
+      <c r="CK1" s="46"/>
+      <c r="CL1" s="46"/>
+      <c r="CM1" s="46"/>
+      <c r="CN1" s="46"/>
+      <c r="CO1" s="46"/>
+      <c r="CP1" s="46"/>
+      <c r="CQ1" s="46"/>
+      <c r="CR1" s="46"/>
+      <c r="CS1" s="46"/>
+      <c r="CT1" s="46"/>
+      <c r="CU1" s="46"/>
+      <c r="CV1" s="46"/>
+      <c r="CW1" s="46"/>
+      <c r="CX1" s="46"/>
+      <c r="CY1" s="46"/>
+      <c r="CZ1" s="46"/>
+      <c r="DA1" s="46"/>
+      <c r="DB1" s="46"/>
+      <c r="DC1" s="46"/>
+      <c r="DD1" s="46"/>
+      <c r="DE1" s="46"/>
+      <c r="DF1" s="46"/>
+      <c r="DG1" s="46"/>
+      <c r="DH1" s="46"/>
+      <c r="DI1" s="46"/>
+      <c r="DJ1" s="46"/>
+      <c r="DK1" s="46"/>
+      <c r="DL1" s="46"/>
+      <c r="DM1" s="46"/>
+      <c r="DN1" s="46"/>
+      <c r="DO1" s="46"/>
+      <c r="DP1" s="46"/>
+      <c r="DQ1" s="46"/>
+      <c r="DR1" s="46"/>
+      <c r="DS1" s="46"/>
+      <c r="DT1" s="46"/>
+      <c r="DU1" s="46"/>
+      <c r="DV1" s="46"/>
+      <c r="DW1" s="46"/>
+      <c r="DX1" s="47"/>
     </row>
     <row r="2" spans="1:157" s="4" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="26"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="26"/>
-      <c r="G2" s="26"/>
-      <c r="H2" s="26"/>
-      <c r="I2" s="26"/>
-      <c r="J2" s="26"/>
-      <c r="K2" s="26"/>
-      <c r="L2" s="26"/>
-      <c r="M2" s="26"/>
-      <c r="N2" s="26"/>
-      <c r="O2" s="26"/>
-      <c r="P2" s="26"/>
-      <c r="Q2" s="26"/>
-      <c r="R2" s="26"/>
-      <c r="S2" s="26"/>
-      <c r="T2" s="26"/>
-      <c r="U2" s="26"/>
-      <c r="V2" s="26"/>
-      <c r="W2" s="26"/>
-      <c r="X2" s="26"/>
-      <c r="Y2" s="26"/>
-      <c r="Z2" s="26"/>
-      <c r="AA2" s="26"/>
-      <c r="AB2" s="26"/>
-      <c r="AC2" s="26"/>
-      <c r="AD2" s="26"/>
-      <c r="AE2" s="26"/>
-      <c r="AF2" s="26"/>
-      <c r="AG2" s="26"/>
-      <c r="AH2" s="26"/>
-      <c r="AI2" s="26"/>
-      <c r="AJ2" s="26"/>
-      <c r="AK2" s="26"/>
-      <c r="AL2" s="26"/>
-      <c r="AM2" s="26"/>
-      <c r="AN2" s="26"/>
-      <c r="AO2" s="26"/>
-      <c r="AP2" s="26"/>
-      <c r="AQ2" s="26"/>
-      <c r="AR2" s="26"/>
-      <c r="AS2" s="26"/>
-      <c r="AT2" s="26"/>
-      <c r="AU2" s="26"/>
-      <c r="AV2" s="26"/>
-      <c r="AW2" s="26"/>
-      <c r="AX2" s="26"/>
-      <c r="AY2" s="26"/>
-      <c r="AZ2" s="26"/>
-      <c r="BA2" s="26"/>
-      <c r="BB2" s="26"/>
-      <c r="BC2" s="26"/>
-      <c r="BD2" s="26"/>
-      <c r="BE2" s="26"/>
-      <c r="BF2" s="26"/>
-      <c r="BG2" s="26"/>
-      <c r="BH2" s="26"/>
-      <c r="BI2" s="26"/>
-      <c r="BJ2" s="26"/>
-      <c r="BK2" s="26"/>
-      <c r="BL2" s="26"/>
-      <c r="BM2" s="26"/>
-      <c r="BN2" s="26"/>
-      <c r="BO2" s="26"/>
-      <c r="BP2" s="26"/>
-      <c r="BQ2" s="26"/>
-      <c r="BR2" s="26"/>
-      <c r="BS2" s="26"/>
-      <c r="BT2" s="26"/>
-      <c r="BU2" s="26"/>
-      <c r="BV2" s="26"/>
-      <c r="BW2" s="26"/>
-      <c r="BX2" s="26"/>
-      <c r="BY2" s="26"/>
-      <c r="BZ2" s="26"/>
-      <c r="CA2" s="26"/>
-      <c r="CB2" s="26"/>
-      <c r="CC2" s="26"/>
-      <c r="CD2" s="26"/>
-      <c r="CE2" s="26"/>
-      <c r="CF2" s="26"/>
-      <c r="CG2" s="26"/>
-      <c r="CH2" s="26"/>
-      <c r="CI2" s="26"/>
-      <c r="CJ2" s="26"/>
-      <c r="CK2" s="26"/>
-      <c r="CL2" s="26"/>
-      <c r="CM2" s="26"/>
-      <c r="CN2" s="26"/>
-      <c r="CO2" s="26"/>
-      <c r="CP2" s="26"/>
-      <c r="CQ2" s="26"/>
-      <c r="CR2" s="26"/>
-      <c r="CS2" s="26"/>
-      <c r="CT2" s="26"/>
-      <c r="CU2" s="26"/>
-      <c r="CV2" s="26"/>
-      <c r="CW2" s="26"/>
-      <c r="CX2" s="26"/>
-      <c r="CY2" s="26"/>
-      <c r="CZ2" s="26"/>
-      <c r="DA2" s="26"/>
-      <c r="DB2" s="26"/>
-      <c r="DC2" s="26"/>
-      <c r="DD2" s="26"/>
-      <c r="DE2" s="26"/>
-      <c r="DF2" s="26"/>
-      <c r="DG2" s="26"/>
-      <c r="DH2" s="26"/>
-      <c r="DI2" s="26"/>
-      <c r="DJ2" s="26"/>
-      <c r="DK2" s="26"/>
-      <c r="DL2" s="26"/>
-      <c r="DM2" s="26"/>
-      <c r="DN2" s="26"/>
-      <c r="DO2" s="26"/>
-      <c r="DP2" s="26"/>
-      <c r="DQ2" s="26"/>
-      <c r="DR2" s="26"/>
-      <c r="DS2" s="26"/>
-      <c r="DT2" s="26"/>
-      <c r="DU2" s="26"/>
-      <c r="DV2" s="26"/>
-      <c r="DW2" s="26"/>
-      <c r="DX2" s="27"/>
+      <c r="A2" s="48"/>
+      <c r="B2" s="49"/>
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="M2" s="49"/>
+      <c r="N2" s="49"/>
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Y2" s="49"/>
+      <c r="Z2" s="49"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
+      <c r="AI2" s="49"/>
+      <c r="AJ2" s="49"/>
+      <c r="AK2" s="49"/>
+      <c r="AL2" s="49"/>
+      <c r="AM2" s="49"/>
+      <c r="AN2" s="49"/>
+      <c r="AO2" s="49"/>
+      <c r="AP2" s="49"/>
+      <c r="AQ2" s="49"/>
+      <c r="AR2" s="49"/>
+      <c r="AS2" s="49"/>
+      <c r="AT2" s="49"/>
+      <c r="AU2" s="49"/>
+      <c r="AV2" s="49"/>
+      <c r="AW2" s="49"/>
+      <c r="AX2" s="49"/>
+      <c r="AY2" s="49"/>
+      <c r="AZ2" s="49"/>
+      <c r="BA2" s="49"/>
+      <c r="BB2" s="49"/>
+      <c r="BC2" s="49"/>
+      <c r="BD2" s="49"/>
+      <c r="BE2" s="49"/>
+      <c r="BF2" s="49"/>
+      <c r="BG2" s="49"/>
+      <c r="BH2" s="49"/>
+      <c r="BI2" s="49"/>
+      <c r="BJ2" s="49"/>
+      <c r="BK2" s="49"/>
+      <c r="BL2" s="49"/>
+      <c r="BM2" s="49"/>
+      <c r="BN2" s="49"/>
+      <c r="BO2" s="49"/>
+      <c r="BP2" s="49"/>
+      <c r="BQ2" s="49"/>
+      <c r="BR2" s="49"/>
+      <c r="BS2" s="49"/>
+      <c r="BT2" s="49"/>
+      <c r="BU2" s="49"/>
+      <c r="BV2" s="49"/>
+      <c r="BW2" s="49"/>
+      <c r="BX2" s="49"/>
+      <c r="BY2" s="49"/>
+      <c r="BZ2" s="49"/>
+      <c r="CA2" s="49"/>
+      <c r="CB2" s="49"/>
+      <c r="CC2" s="49"/>
+      <c r="CD2" s="49"/>
+      <c r="CE2" s="49"/>
+      <c r="CF2" s="49"/>
+      <c r="CG2" s="49"/>
+      <c r="CH2" s="49"/>
+      <c r="CI2" s="49"/>
+      <c r="CJ2" s="49"/>
+      <c r="CK2" s="49"/>
+      <c r="CL2" s="49"/>
+      <c r="CM2" s="49"/>
+      <c r="CN2" s="49"/>
+      <c r="CO2" s="49"/>
+      <c r="CP2" s="49"/>
+      <c r="CQ2" s="49"/>
+      <c r="CR2" s="49"/>
+      <c r="CS2" s="49"/>
+      <c r="CT2" s="49"/>
+      <c r="CU2" s="49"/>
+      <c r="CV2" s="49"/>
+      <c r="CW2" s="49"/>
+      <c r="CX2" s="49"/>
+      <c r="CY2" s="49"/>
+      <c r="CZ2" s="49"/>
+      <c r="DA2" s="49"/>
+      <c r="DB2" s="49"/>
+      <c r="DC2" s="49"/>
+      <c r="DD2" s="49"/>
+      <c r="DE2" s="49"/>
+      <c r="DF2" s="49"/>
+      <c r="DG2" s="49"/>
+      <c r="DH2" s="49"/>
+      <c r="DI2" s="49"/>
+      <c r="DJ2" s="49"/>
+      <c r="DK2" s="49"/>
+      <c r="DL2" s="49"/>
+      <c r="DM2" s="49"/>
+      <c r="DN2" s="49"/>
+      <c r="DO2" s="49"/>
+      <c r="DP2" s="49"/>
+      <c r="DQ2" s="49"/>
+      <c r="DR2" s="49"/>
+      <c r="DS2" s="49"/>
+      <c r="DT2" s="49"/>
+      <c r="DU2" s="49"/>
+      <c r="DV2" s="49"/>
+      <c r="DW2" s="49"/>
+      <c r="DX2" s="50"/>
     </row>
     <row r="3" spans="1:157" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2561,169 +2722,169 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="28" t="s">
+      <c r="B4" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-      <c r="G4" s="28"/>
-      <c r="H4" s="28"/>
-      <c r="I4" s="30" t="s">
+      <c r="C4" s="54"/>
+      <c r="D4" s="54"/>
+      <c r="E4" s="54"/>
+      <c r="F4" s="54"/>
+      <c r="G4" s="54"/>
+      <c r="H4" s="54"/>
+      <c r="I4" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="30"/>
-      <c r="K4" s="30"/>
-      <c r="L4" s="30"/>
-      <c r="M4" s="30"/>
-      <c r="N4" s="30"/>
-      <c r="O4" s="30"/>
-      <c r="P4" s="30" t="s">
+      <c r="J4" s="56"/>
+      <c r="K4" s="56"/>
+      <c r="L4" s="56"/>
+      <c r="M4" s="56"/>
+      <c r="N4" s="56"/>
+      <c r="O4" s="56"/>
+      <c r="P4" s="56" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="30"/>
-      <c r="R4" s="30"/>
-      <c r="S4" s="30"/>
-      <c r="T4" s="30"/>
-      <c r="U4" s="30"/>
-      <c r="V4" s="30"/>
-      <c r="W4" s="13" t="s">
+      <c r="Q4" s="56"/>
+      <c r="R4" s="56"/>
+      <c r="S4" s="56"/>
+      <c r="T4" s="56"/>
+      <c r="U4" s="56"/>
+      <c r="V4" s="56"/>
+      <c r="W4" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="13"/>
-      <c r="Y4" s="13"/>
-      <c r="Z4" s="13"/>
-      <c r="AA4" s="13"/>
-      <c r="AB4" s="13"/>
-      <c r="AC4" s="13"/>
-      <c r="AD4" s="13"/>
-      <c r="AE4" s="13"/>
-      <c r="AF4" s="13"/>
-      <c r="AG4" s="13"/>
-      <c r="AH4" s="13"/>
-      <c r="AI4" s="13"/>
-      <c r="AJ4" s="13"/>
-      <c r="AK4" s="13"/>
-      <c r="AL4" s="13"/>
-      <c r="AM4" s="13"/>
-      <c r="AN4" s="13"/>
-      <c r="AO4" s="13"/>
-      <c r="AP4" s="13"/>
-      <c r="AQ4" s="13"/>
-      <c r="AR4" s="13"/>
-      <c r="AS4" s="13"/>
-      <c r="AT4" s="13"/>
-      <c r="AU4" s="13"/>
-      <c r="AV4" s="13"/>
-      <c r="AW4" s="13"/>
-      <c r="AX4" s="15" t="s">
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64"/>
+      <c r="Z4" s="64"/>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="64"/>
+      <c r="AC4" s="64"/>
+      <c r="AD4" s="64"/>
+      <c r="AE4" s="64"/>
+      <c r="AF4" s="64"/>
+      <c r="AG4" s="64"/>
+      <c r="AH4" s="64"/>
+      <c r="AI4" s="64"/>
+      <c r="AJ4" s="64"/>
+      <c r="AK4" s="64"/>
+      <c r="AL4" s="64"/>
+      <c r="AM4" s="64"/>
+      <c r="AN4" s="64"/>
+      <c r="AO4" s="64"/>
+      <c r="AP4" s="64"/>
+      <c r="AQ4" s="64"/>
+      <c r="AR4" s="64"/>
+      <c r="AS4" s="64"/>
+      <c r="AT4" s="64"/>
+      <c r="AU4" s="64"/>
+      <c r="AV4" s="64"/>
+      <c r="AW4" s="64"/>
+      <c r="AX4" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="AY4" s="15"/>
-      <c r="AZ4" s="15"/>
-      <c r="BA4" s="15"/>
-      <c r="BB4" s="15"/>
-      <c r="BC4" s="14" t="s">
+      <c r="AY4" s="66"/>
+      <c r="AZ4" s="66"/>
+      <c r="BA4" s="66"/>
+      <c r="BB4" s="66"/>
+      <c r="BC4" s="65" t="s">
         <v>17</v>
       </c>
-      <c r="BD4" s="14"/>
-      <c r="BE4" s="32" t="s">
+      <c r="BD4" s="65"/>
+      <c r="BE4" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="BF4" s="31" t="s">
+      <c r="BF4" s="57" t="s">
         <v>9</v>
       </c>
-      <c r="BG4" s="39" t="s">
+      <c r="BG4" s="27" t="s">
+        <v>40</v>
+      </c>
+      <c r="BH4" s="28"/>
+      <c r="BI4" s="28"/>
+      <c r="BJ4" s="28"/>
+      <c r="BK4" s="28"/>
+      <c r="BL4" s="29"/>
+      <c r="BM4" s="30" t="s">
+        <v>41</v>
+      </c>
+      <c r="BN4" s="31"/>
+      <c r="BO4" s="31"/>
+      <c r="BP4" s="31"/>
+      <c r="BQ4" s="31"/>
+      <c r="BR4" s="31"/>
+      <c r="BS4" s="32"/>
+      <c r="BT4" s="33" t="s">
+        <v>42</v>
+      </c>
+      <c r="BU4" s="34"/>
+      <c r="BV4" s="34"/>
+      <c r="BW4" s="34"/>
+      <c r="BX4" s="34"/>
+      <c r="BY4" s="34"/>
+      <c r="BZ4" s="35"/>
+      <c r="CA4" s="36" t="s">
         <v>43</v>
       </c>
-      <c r="BH4" s="40"/>
-      <c r="BI4" s="40"/>
-      <c r="BJ4" s="40"/>
-      <c r="BK4" s="40"/>
-      <c r="BL4" s="41"/>
-      <c r="BM4" s="42" t="s">
+      <c r="CB4" s="37"/>
+      <c r="CC4" s="37"/>
+      <c r="CD4" s="37"/>
+      <c r="CE4" s="37"/>
+      <c r="CF4" s="37"/>
+      <c r="CG4" s="38"/>
+      <c r="CH4" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="BN4" s="43"/>
-      <c r="BO4" s="43"/>
-      <c r="BP4" s="43"/>
-      <c r="BQ4" s="43"/>
-      <c r="BR4" s="43"/>
-      <c r="BS4" s="44"/>
-      <c r="BT4" s="45" t="s">
+      <c r="CI4" s="40"/>
+      <c r="CJ4" s="40"/>
+      <c r="CK4" s="40"/>
+      <c r="CL4" s="40"/>
+      <c r="CM4" s="40"/>
+      <c r="CN4" s="41"/>
+      <c r="CO4" s="21" t="s">
+        <v>46</v>
+      </c>
+      <c r="CP4" s="22"/>
+      <c r="CQ4" s="22"/>
+      <c r="CR4" s="22"/>
+      <c r="CS4" s="22"/>
+      <c r="CT4" s="23"/>
+      <c r="CU4" s="24" t="s">
+        <v>47</v>
+      </c>
+      <c r="CV4" s="25"/>
+      <c r="CW4" s="25"/>
+      <c r="CX4" s="25"/>
+      <c r="CY4" s="25"/>
+      <c r="CZ4" s="25"/>
+      <c r="DA4" s="26"/>
+      <c r="DB4" s="42" t="s">
+        <v>39</v>
+      </c>
+      <c r="DC4" s="43"/>
+      <c r="DD4" s="43"/>
+      <c r="DE4" s="43"/>
+      <c r="DF4" s="43"/>
+      <c r="DG4" s="43"/>
+      <c r="DH4" s="43"/>
+      <c r="DI4" s="43"/>
+      <c r="DJ4" s="43"/>
+      <c r="DK4" s="43"/>
+      <c r="DL4" s="43"/>
+      <c r="DM4" s="43"/>
+      <c r="DN4" s="43"/>
+      <c r="DO4" s="43"/>
+      <c r="DP4" s="44"/>
+      <c r="DQ4" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="BU4" s="46"/>
-      <c r="BV4" s="46"/>
-      <c r="BW4" s="46"/>
-      <c r="BX4" s="46"/>
-      <c r="BY4" s="46"/>
-      <c r="BZ4" s="47"/>
-      <c r="CA4" s="67" t="s">
-        <v>46</v>
-      </c>
-      <c r="CB4" s="68"/>
-      <c r="CC4" s="68"/>
-      <c r="CD4" s="68"/>
-      <c r="CE4" s="68"/>
-      <c r="CF4" s="68"/>
-      <c r="CG4" s="69"/>
-      <c r="CH4" s="48" t="s">
-        <v>47</v>
-      </c>
-      <c r="CI4" s="49"/>
-      <c r="CJ4" s="49"/>
-      <c r="CK4" s="49"/>
-      <c r="CL4" s="49"/>
-      <c r="CM4" s="49"/>
-      <c r="CN4" s="50"/>
-      <c r="CO4" s="54" t="s">
-        <v>49</v>
-      </c>
-      <c r="CP4" s="55"/>
-      <c r="CQ4" s="55"/>
-      <c r="CR4" s="55"/>
-      <c r="CS4" s="55"/>
-      <c r="CT4" s="56"/>
-      <c r="CU4" s="57" t="s">
-        <v>50</v>
-      </c>
-      <c r="CV4" s="58"/>
-      <c r="CW4" s="58"/>
-      <c r="CX4" s="58"/>
-      <c r="CY4" s="58"/>
-      <c r="CZ4" s="58"/>
-      <c r="DA4" s="59"/>
-      <c r="DB4" s="63" t="s">
-        <v>42</v>
-      </c>
-      <c r="DC4" s="64"/>
-      <c r="DD4" s="64"/>
-      <c r="DE4" s="64"/>
-      <c r="DF4" s="64"/>
-      <c r="DG4" s="64"/>
-      <c r="DH4" s="64"/>
-      <c r="DI4" s="64"/>
-      <c r="DJ4" s="64"/>
-      <c r="DK4" s="64"/>
-      <c r="DL4" s="64"/>
-      <c r="DM4" s="64"/>
-      <c r="DN4" s="64"/>
-      <c r="DO4" s="64"/>
-      <c r="DP4" s="65"/>
-      <c r="DQ4" s="51" t="s">
-        <v>48</v>
-      </c>
-      <c r="DR4" s="52"/>
-      <c r="DS4" s="52"/>
-      <c r="DT4" s="52"/>
-      <c r="DU4" s="52"/>
-      <c r="DV4" s="53"/>
-      <c r="DW4" s="32" t="s">
+      <c r="DR4" s="19"/>
+      <c r="DS4" s="19"/>
+      <c r="DT4" s="19"/>
+      <c r="DU4" s="19"/>
+      <c r="DV4" s="20"/>
+      <c r="DW4" s="58" t="s">
         <v>13</v>
       </c>
-      <c r="DX4" s="31" t="s">
+      <c r="DX4" s="57" t="s">
         <v>12</v>
       </c>
       <c r="DY4" s="5"/>
@@ -2763,122 +2924,193 @@
       <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="E5" s="29"/>
-      <c r="F5" s="29"/>
+      <c r="D5" s="55"/>
+      <c r="E5" s="55"/>
+      <c r="F5" s="55"/>
       <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="19" t="s">
+      <c r="I5" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="21"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="21"/>
-      <c r="M5" s="20"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="53"/>
       <c r="N5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="19" t="s">
+      <c r="O5" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="21"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="21"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="20"/>
+      <c r="P5" s="52"/>
+      <c r="Q5" s="52"/>
+      <c r="R5" s="52"/>
+      <c r="S5" s="52"/>
+      <c r="T5" s="52"/>
+      <c r="U5" s="53"/>
       <c r="V5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="19" t="s">
+      <c r="W5" s="51" t="s">
         <v>25</v>
       </c>
-      <c r="X5" s="21"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="21"/>
-      <c r="AA5" s="21"/>
-      <c r="AB5" s="20"/>
+      <c r="X5" s="52"/>
+      <c r="Y5" s="52"/>
+      <c r="Z5" s="52"/>
+      <c r="AA5" s="52"/>
+      <c r="AB5" s="53"/>
       <c r="AC5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="19" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE5" s="21"/>
-      <c r="AF5" s="21"/>
-      <c r="AG5" s="21"/>
-      <c r="AH5" s="21"/>
-      <c r="AI5" s="20"/>
+      <c r="AD5" s="51" t="s">
+        <v>30</v>
+      </c>
+      <c r="AE5" s="52"/>
+      <c r="AF5" s="52"/>
+      <c r="AG5" s="52"/>
+      <c r="AH5" s="52"/>
+      <c r="AI5" s="53"/>
       <c r="AJ5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AK5" s="19" t="s">
-        <v>36</v>
-      </c>
-      <c r="AL5" s="21"/>
-      <c r="AM5" s="21"/>
-      <c r="AN5" s="21"/>
-      <c r="AO5" s="21"/>
-      <c r="AP5" s="20"/>
+      <c r="AK5" s="51" t="s">
+        <v>35</v>
+      </c>
+      <c r="AL5" s="52"/>
+      <c r="AM5" s="52"/>
+      <c r="AN5" s="52"/>
+      <c r="AO5" s="52"/>
+      <c r="AP5" s="53"/>
       <c r="AQ5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AR5" s="19" t="s">
+      <c r="AR5" s="51" t="s">
+        <v>36</v>
+      </c>
+      <c r="AS5" s="52"/>
+      <c r="AT5" s="52"/>
+      <c r="AU5" s="52"/>
+      <c r="AV5" s="52"/>
+      <c r="AW5" s="53"/>
+      <c r="AX5" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="AY5" s="51" t="s">
         <v>37</v>
       </c>
-      <c r="AS5" s="21"/>
-      <c r="AT5" s="21"/>
-      <c r="AU5" s="21"/>
-      <c r="AV5" s="21"/>
-      <c r="AW5" s="20"/>
-      <c r="AX5" s="8" t="s">
-        <v>29</v>
-      </c>
-      <c r="AY5" s="19" t="s">
+      <c r="AZ5" s="52"/>
+      <c r="BA5" s="52"/>
+      <c r="BB5" s="53"/>
+      <c r="BC5" s="51" t="s">
         <v>38</v>
       </c>
-      <c r="AZ5" s="21"/>
-      <c r="BA5" s="21"/>
-      <c r="BB5" s="20"/>
-      <c r="BC5" s="19" t="s">
-        <v>39</v>
-      </c>
-      <c r="BD5" s="20"/>
-      <c r="BE5" s="32"/>
-      <c r="BF5" s="31"/>
-      <c r="BL5" s="60" t="s">
+      <c r="BD5" s="53"/>
+      <c r="BE5" s="58"/>
+      <c r="BF5" s="57"/>
+      <c r="BG5" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="BH5" s="52"/>
+      <c r="BI5" s="52"/>
+      <c r="BJ5" s="52"/>
+      <c r="BK5" s="53"/>
+      <c r="BL5" s="14" t="s">
+        <v>53</v>
+      </c>
+      <c r="BM5" s="51" t="s">
         <v>51</v>
       </c>
-      <c r="BS5" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="BZ5" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="CG5" s="61" t="s">
+      <c r="BN5" s="52"/>
+      <c r="BO5" s="52"/>
+      <c r="BP5" s="52"/>
+      <c r="BQ5" s="52"/>
+      <c r="BR5" s="53"/>
+      <c r="BS5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="CN5" s="61" t="s">
+      <c r="BT5" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="BU5" s="52"/>
+      <c r="BV5" s="52"/>
+      <c r="BW5" s="52"/>
+      <c r="BX5" s="52"/>
+      <c r="BY5" s="53"/>
+      <c r="BZ5" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="CA5" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="CB5" s="52"/>
+      <c r="CC5" s="52"/>
+      <c r="CD5" s="52"/>
+      <c r="CE5" s="52"/>
+      <c r="CF5" s="53"/>
+      <c r="CG5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="CU5" s="61" t="s">
+      <c r="CH5" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="CI5" s="52"/>
+      <c r="CJ5" s="52"/>
+      <c r="CK5" s="52"/>
+      <c r="CL5" s="52"/>
+      <c r="CM5" s="53"/>
+      <c r="CN5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="DB5" s="62" t="s">
-        <v>57</v>
-      </c>
-      <c r="DI5" s="66" t="s">
-        <v>40</v>
-      </c>
-      <c r="DP5" s="66" t="s">
-        <v>41</v>
-      </c>
-      <c r="DW5" s="32"/>
-      <c r="DX5" s="31"/>
+      <c r="CO5" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="CP5" s="52"/>
+      <c r="CQ5" s="52"/>
+      <c r="CR5" s="52"/>
+      <c r="CS5" s="52"/>
+      <c r="CT5" s="53"/>
+      <c r="CU5" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="CV5" s="51" t="s">
+        <v>60</v>
+      </c>
+      <c r="CW5" s="52"/>
+      <c r="CX5" s="52"/>
+      <c r="CY5" s="52"/>
+      <c r="CZ5" s="52"/>
+      <c r="DA5" s="53"/>
+      <c r="DB5" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="DC5" s="67" t="s">
+        <v>58</v>
+      </c>
+      <c r="DD5" s="68"/>
+      <c r="DE5" s="68"/>
+      <c r="DF5" s="68"/>
+      <c r="DG5" s="68"/>
+      <c r="DH5" s="69"/>
+      <c r="DI5" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="DP5" s="17" t="s">
+        <v>65</v>
+      </c>
+      <c r="DQ5" s="51" t="s">
+        <v>66</v>
+      </c>
+      <c r="DR5" s="52"/>
+      <c r="DS5" s="52"/>
+      <c r="DT5" s="52"/>
+      <c r="DU5" s="52"/>
+      <c r="DV5" s="53"/>
+      <c r="DW5" s="58"/>
+      <c r="DX5" s="57"/>
     </row>
     <row r="6" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -2890,44 +3122,74 @@
       <c r="N6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="33" t="s">
+      <c r="V6" s="59" t="s">
         <v>24</v>
       </c>
       <c r="AC6" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="AK6" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="AK6" s="67" t="s">
+        <v>32</v>
+      </c>
+      <c r="AL6" s="68"/>
+      <c r="AM6" s="68"/>
+      <c r="AN6" s="68"/>
+      <c r="AO6" s="68"/>
+      <c r="AP6" s="69"/>
+      <c r="AV6" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="AL6" s="17"/>
-      <c r="AM6" s="17"/>
-      <c r="AN6" s="17"/>
-      <c r="AO6" s="17"/>
-      <c r="AP6" s="18"/>
-      <c r="AV6" s="36" t="s">
+      <c r="AW6" s="63"/>
+      <c r="AX6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AW6" s="37"/>
-      <c r="AX6" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="AY6" s="19"/>
-      <c r="AZ6" s="21"/>
-      <c r="BA6" s="21"/>
-      <c r="BB6" s="20"/>
-      <c r="BC6" s="19" t="s">
-        <v>32</v>
-      </c>
-      <c r="BD6" s="20"/>
-      <c r="BE6" s="32"/>
-      <c r="BF6" s="31"/>
-      <c r="DW6" s="32"/>
-      <c r="DX6" s="31"/>
+      <c r="AY6" s="51"/>
+      <c r="AZ6" s="52"/>
+      <c r="BA6" s="52"/>
+      <c r="BB6" s="53"/>
+      <c r="BC6" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="BD6" s="53"/>
+      <c r="BE6" s="58"/>
+      <c r="BF6" s="57"/>
+      <c r="CN6" s="70" t="s">
+        <v>57</v>
+      </c>
+      <c r="CO6" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="CP6" s="52"/>
+      <c r="CQ6" s="52"/>
+      <c r="CR6" s="52"/>
+      <c r="CS6" s="52"/>
+      <c r="CT6" s="53"/>
+      <c r="CV6" s="51" t="s">
+        <v>61</v>
+      </c>
+      <c r="CW6" s="52"/>
+      <c r="CX6" s="52"/>
+      <c r="CY6" s="52"/>
+      <c r="CZ6" s="52"/>
+      <c r="DA6" s="53"/>
+      <c r="DC6" s="67" t="s">
+        <v>62</v>
+      </c>
+      <c r="DD6" s="52"/>
+      <c r="DE6" s="52"/>
+      <c r="DF6" s="52"/>
+      <c r="DG6" s="52"/>
+      <c r="DH6" s="53"/>
+      <c r="DI6" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="DW6" s="58"/>
+      <c r="DX6" s="57"/>
     </row>
     <row r="7" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V7" s="34"/>
-      <c r="BF7" s="31"/>
-      <c r="DX7" s="31"/>
+      <c r="V7" s="60"/>
+      <c r="BF7" s="57"/>
+      <c r="DX7" s="57"/>
     </row>
     <row r="8" spans="1:157" s="4" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -2935,21 +3197,33 @@
       </c>
       <c r="B8" s="7">
         <f ca="1">TODAY()</f>
-        <v>44717</v>
-      </c>
-      <c r="V8" s="35"/>
+        <v>44745</v>
+      </c>
+      <c r="V8" s="61"/>
     </row>
   </sheetData>
-  <mergeCells count="34">
-    <mergeCell ref="DQ4:DV4"/>
-    <mergeCell ref="CO4:CT4"/>
-    <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="BG4:BL4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="DB4:DP4"/>
+  <mergeCells count="46">
+    <mergeCell ref="DC6:DH6"/>
+    <mergeCell ref="DQ5:DV5"/>
+    <mergeCell ref="DC5:DH5"/>
+    <mergeCell ref="BT5:BY5"/>
+    <mergeCell ref="CA5:CF5"/>
+    <mergeCell ref="CH5:CM5"/>
+    <mergeCell ref="CO5:CT5"/>
+    <mergeCell ref="CV5:DA5"/>
+    <mergeCell ref="BG5:BK5"/>
+    <mergeCell ref="BM5:BR5"/>
+    <mergeCell ref="CO6:CT6"/>
+    <mergeCell ref="CV6:DA6"/>
+    <mergeCell ref="W4:AW4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="AX4:BB4"/>
+    <mergeCell ref="AK6:AP6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="AD5:AI5"/>
+    <mergeCell ref="AK5:AP5"/>
+    <mergeCell ref="AR5:AW5"/>
+    <mergeCell ref="BC5:BD5"/>
     <mergeCell ref="A1:DX2"/>
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="O5:U5"/>
@@ -2966,15 +3240,15 @@
     <mergeCell ref="AY6:BB6"/>
     <mergeCell ref="AV6:AW6"/>
     <mergeCell ref="AY5:BB5"/>
-    <mergeCell ref="W4:AW4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="AX4:BB4"/>
-    <mergeCell ref="AK6:AP6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="AD5:AI5"/>
-    <mergeCell ref="AK5:AP5"/>
-    <mergeCell ref="AR5:AW5"/>
-    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="DQ4:DV4"/>
+    <mergeCell ref="CO4:CT4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="BG4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="DB4:DP4"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:XFD3">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
updated meeting notes and timeline from 10 Jul 22
</commit_message>
<xml_diff>
--- a/Timeline/Project_Timeline.xlsx
+++ b/Timeline/Project_Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Desktop/agile/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3216790F-FA9C-364D-A073-8D8C6AF6DFEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A507C5E6-012E-0945-B078-BA6ACC5390B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15920" yWindow="4020" windowWidth="28800" windowHeight="22140" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
   <si>
     <t>ASP - Group Project</t>
   </si>
@@ -1095,6 +1095,71 @@
   </si>
   <si>
     <t>Prepare group submission</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Initial HMTL skeleton produced with sample code created for the backend </t>
+  </si>
+  <si>
+    <t>Front end mostly complete 
+Backend featrues added - button link to chart.js and File load complete</t>
+  </si>
+  <si>
+    <t>Accelerated MVP intended timeline - TBC following sprint 3</t>
+  </si>
+  <si>
+    <t>ADDITIONAL FEATURES IF MVP TIMELINE IS EARLY</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Ben &amp; Thavelarn
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Continue to tweak the front end 
+- Look into finding/creating the pre-built data for the system.
+- Investigate implementing Google Big Query in a future sprint
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+David &amp; Connor &amp; Kashka</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Continue integration of backend features on the system. The next focus will be chart.js implementation and error management of the data.
+- Look at implementing an export feature of charts.js once it has been successfully implemented on the system.
+</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1185,7 +1250,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="25">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1327,6 +1392,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFA649EF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1494,7 +1571,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1547,164 +1624,176 @@
     <xf numFmtId="0" fontId="10" fillId="23" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2061,8 +2150,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3400B0-A312-474B-BDD8-7EBBB1942BA5}">
   <dimension ref="A1:FA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BD4" workbookViewId="0">
-      <selection activeCell="DQ6" sqref="DQ6"/>
+    <sheetView tabSelected="1" topLeftCell="BM3" workbookViewId="0">
+      <selection activeCell="BT5" sqref="BT5:BY5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2071,266 +2160,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="46"/>
-      <c r="C1" s="46"/>
-      <c r="D1" s="46"/>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="46"/>
-      <c r="I1" s="46"/>
-      <c r="J1" s="46"/>
-      <c r="K1" s="46"/>
-      <c r="L1" s="46"/>
-      <c r="M1" s="46"/>
-      <c r="N1" s="46"/>
-      <c r="O1" s="46"/>
-      <c r="P1" s="46"/>
-      <c r="Q1" s="46"/>
-      <c r="R1" s="46"/>
-      <c r="S1" s="46"/>
-      <c r="T1" s="46"/>
-      <c r="U1" s="46"/>
-      <c r="V1" s="46"/>
-      <c r="W1" s="46"/>
-      <c r="X1" s="46"/>
-      <c r="Y1" s="46"/>
-      <c r="Z1" s="46"/>
-      <c r="AA1" s="46"/>
-      <c r="AB1" s="46"/>
-      <c r="AC1" s="46"/>
-      <c r="AD1" s="46"/>
-      <c r="AE1" s="46"/>
-      <c r="AF1" s="46"/>
-      <c r="AG1" s="46"/>
-      <c r="AH1" s="46"/>
-      <c r="AI1" s="46"/>
-      <c r="AJ1" s="46"/>
-      <c r="AK1" s="46"/>
-      <c r="AL1" s="46"/>
-      <c r="AM1" s="46"/>
-      <c r="AN1" s="46"/>
-      <c r="AO1" s="46"/>
-      <c r="AP1" s="46"/>
-      <c r="AQ1" s="46"/>
-      <c r="AR1" s="46"/>
-      <c r="AS1" s="46"/>
-      <c r="AT1" s="46"/>
-      <c r="AU1" s="46"/>
-      <c r="AV1" s="46"/>
-      <c r="AW1" s="46"/>
-      <c r="AX1" s="46"/>
-      <c r="AY1" s="46"/>
-      <c r="AZ1" s="46"/>
-      <c r="BA1" s="46"/>
-      <c r="BB1" s="46"/>
-      <c r="BC1" s="46"/>
-      <c r="BD1" s="46"/>
-      <c r="BE1" s="46"/>
-      <c r="BF1" s="46"/>
-      <c r="BG1" s="46"/>
-      <c r="BH1" s="46"/>
-      <c r="BI1" s="46"/>
-      <c r="BJ1" s="46"/>
-      <c r="BK1" s="46"/>
-      <c r="BL1" s="46"/>
-      <c r="BM1" s="46"/>
-      <c r="BN1" s="46"/>
-      <c r="BO1" s="46"/>
-      <c r="BP1" s="46"/>
-      <c r="BQ1" s="46"/>
-      <c r="BR1" s="46"/>
-      <c r="BS1" s="46"/>
-      <c r="BT1" s="46"/>
-      <c r="BU1" s="46"/>
-      <c r="BV1" s="46"/>
-      <c r="BW1" s="46"/>
-      <c r="BX1" s="46"/>
-      <c r="BY1" s="46"/>
-      <c r="BZ1" s="46"/>
-      <c r="CA1" s="46"/>
-      <c r="CB1" s="46"/>
-      <c r="CC1" s="46"/>
-      <c r="CD1" s="46"/>
-      <c r="CE1" s="46"/>
-      <c r="CF1" s="46"/>
-      <c r="CG1" s="46"/>
-      <c r="CH1" s="46"/>
-      <c r="CI1" s="46"/>
-      <c r="CJ1" s="46"/>
-      <c r="CK1" s="46"/>
-      <c r="CL1" s="46"/>
-      <c r="CM1" s="46"/>
-      <c r="CN1" s="46"/>
-      <c r="CO1" s="46"/>
-      <c r="CP1" s="46"/>
-      <c r="CQ1" s="46"/>
-      <c r="CR1" s="46"/>
-      <c r="CS1" s="46"/>
-      <c r="CT1" s="46"/>
-      <c r="CU1" s="46"/>
-      <c r="CV1" s="46"/>
-      <c r="CW1" s="46"/>
-      <c r="CX1" s="46"/>
-      <c r="CY1" s="46"/>
-      <c r="CZ1" s="46"/>
-      <c r="DA1" s="46"/>
-      <c r="DB1" s="46"/>
-      <c r="DC1" s="46"/>
-      <c r="DD1" s="46"/>
-      <c r="DE1" s="46"/>
-      <c r="DF1" s="46"/>
-      <c r="DG1" s="46"/>
-      <c r="DH1" s="46"/>
-      <c r="DI1" s="46"/>
-      <c r="DJ1" s="46"/>
-      <c r="DK1" s="46"/>
-      <c r="DL1" s="46"/>
-      <c r="DM1" s="46"/>
-      <c r="DN1" s="46"/>
-      <c r="DO1" s="46"/>
-      <c r="DP1" s="46"/>
-      <c r="DQ1" s="46"/>
-      <c r="DR1" s="46"/>
-      <c r="DS1" s="46"/>
-      <c r="DT1" s="46"/>
-      <c r="DU1" s="46"/>
-      <c r="DV1" s="46"/>
-      <c r="DW1" s="46"/>
-      <c r="DX1" s="47"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
+      <c r="AU1" s="29"/>
+      <c r="AV1" s="29"/>
+      <c r="AW1" s="29"/>
+      <c r="AX1" s="29"/>
+      <c r="AY1" s="29"/>
+      <c r="AZ1" s="29"/>
+      <c r="BA1" s="29"/>
+      <c r="BB1" s="29"/>
+      <c r="BC1" s="29"/>
+      <c r="BD1" s="29"/>
+      <c r="BE1" s="29"/>
+      <c r="BF1" s="29"/>
+      <c r="BG1" s="29"/>
+      <c r="BH1" s="29"/>
+      <c r="BI1" s="29"/>
+      <c r="BJ1" s="29"/>
+      <c r="BK1" s="29"/>
+      <c r="BL1" s="29"/>
+      <c r="BM1" s="29"/>
+      <c r="BN1" s="29"/>
+      <c r="BO1" s="29"/>
+      <c r="BP1" s="29"/>
+      <c r="BQ1" s="29"/>
+      <c r="BR1" s="29"/>
+      <c r="BS1" s="29"/>
+      <c r="BT1" s="29"/>
+      <c r="BU1" s="29"/>
+      <c r="BV1" s="29"/>
+      <c r="BW1" s="29"/>
+      <c r="BX1" s="29"/>
+      <c r="BY1" s="29"/>
+      <c r="BZ1" s="29"/>
+      <c r="CA1" s="29"/>
+      <c r="CB1" s="29"/>
+      <c r="CC1" s="29"/>
+      <c r="CD1" s="29"/>
+      <c r="CE1" s="29"/>
+      <c r="CF1" s="29"/>
+      <c r="CG1" s="29"/>
+      <c r="CH1" s="29"/>
+      <c r="CI1" s="29"/>
+      <c r="CJ1" s="29"/>
+      <c r="CK1" s="29"/>
+      <c r="CL1" s="29"/>
+      <c r="CM1" s="29"/>
+      <c r="CN1" s="29"/>
+      <c r="CO1" s="29"/>
+      <c r="CP1" s="29"/>
+      <c r="CQ1" s="29"/>
+      <c r="CR1" s="29"/>
+      <c r="CS1" s="29"/>
+      <c r="CT1" s="29"/>
+      <c r="CU1" s="29"/>
+      <c r="CV1" s="29"/>
+      <c r="CW1" s="29"/>
+      <c r="CX1" s="29"/>
+      <c r="CY1" s="29"/>
+      <c r="CZ1" s="29"/>
+      <c r="DA1" s="29"/>
+      <c r="DB1" s="29"/>
+      <c r="DC1" s="29"/>
+      <c r="DD1" s="29"/>
+      <c r="DE1" s="29"/>
+      <c r="DF1" s="29"/>
+      <c r="DG1" s="29"/>
+      <c r="DH1" s="29"/>
+      <c r="DI1" s="29"/>
+      <c r="DJ1" s="29"/>
+      <c r="DK1" s="29"/>
+      <c r="DL1" s="29"/>
+      <c r="DM1" s="29"/>
+      <c r="DN1" s="29"/>
+      <c r="DO1" s="29"/>
+      <c r="DP1" s="29"/>
+      <c r="DQ1" s="29"/>
+      <c r="DR1" s="29"/>
+      <c r="DS1" s="29"/>
+      <c r="DT1" s="29"/>
+      <c r="DU1" s="29"/>
+      <c r="DV1" s="29"/>
+      <c r="DW1" s="29"/>
+      <c r="DX1" s="30"/>
     </row>
     <row r="2" spans="1:157" s="4" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="48"/>
-      <c r="B2" s="49"/>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="M2" s="49"/>
-      <c r="N2" s="49"/>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Y2" s="49"/>
-      <c r="Z2" s="49"/>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="49"/>
-      <c r="AH2" s="49"/>
-      <c r="AI2" s="49"/>
-      <c r="AJ2" s="49"/>
-      <c r="AK2" s="49"/>
-      <c r="AL2" s="49"/>
-      <c r="AM2" s="49"/>
-      <c r="AN2" s="49"/>
-      <c r="AO2" s="49"/>
-      <c r="AP2" s="49"/>
-      <c r="AQ2" s="49"/>
-      <c r="AR2" s="49"/>
-      <c r="AS2" s="49"/>
-      <c r="AT2" s="49"/>
-      <c r="AU2" s="49"/>
-      <c r="AV2" s="49"/>
-      <c r="AW2" s="49"/>
-      <c r="AX2" s="49"/>
-      <c r="AY2" s="49"/>
-      <c r="AZ2" s="49"/>
-      <c r="BA2" s="49"/>
-      <c r="BB2" s="49"/>
-      <c r="BC2" s="49"/>
-      <c r="BD2" s="49"/>
-      <c r="BE2" s="49"/>
-      <c r="BF2" s="49"/>
-      <c r="BG2" s="49"/>
-      <c r="BH2" s="49"/>
-      <c r="BI2" s="49"/>
-      <c r="BJ2" s="49"/>
-      <c r="BK2" s="49"/>
-      <c r="BL2" s="49"/>
-      <c r="BM2" s="49"/>
-      <c r="BN2" s="49"/>
-      <c r="BO2" s="49"/>
-      <c r="BP2" s="49"/>
-      <c r="BQ2" s="49"/>
-      <c r="BR2" s="49"/>
-      <c r="BS2" s="49"/>
-      <c r="BT2" s="49"/>
-      <c r="BU2" s="49"/>
-      <c r="BV2" s="49"/>
-      <c r="BW2" s="49"/>
-      <c r="BX2" s="49"/>
-      <c r="BY2" s="49"/>
-      <c r="BZ2" s="49"/>
-      <c r="CA2" s="49"/>
-      <c r="CB2" s="49"/>
-      <c r="CC2" s="49"/>
-      <c r="CD2" s="49"/>
-      <c r="CE2" s="49"/>
-      <c r="CF2" s="49"/>
-      <c r="CG2" s="49"/>
-      <c r="CH2" s="49"/>
-      <c r="CI2" s="49"/>
-      <c r="CJ2" s="49"/>
-      <c r="CK2" s="49"/>
-      <c r="CL2" s="49"/>
-      <c r="CM2" s="49"/>
-      <c r="CN2" s="49"/>
-      <c r="CO2" s="49"/>
-      <c r="CP2" s="49"/>
-      <c r="CQ2" s="49"/>
-      <c r="CR2" s="49"/>
-      <c r="CS2" s="49"/>
-      <c r="CT2" s="49"/>
-      <c r="CU2" s="49"/>
-      <c r="CV2" s="49"/>
-      <c r="CW2" s="49"/>
-      <c r="CX2" s="49"/>
-      <c r="CY2" s="49"/>
-      <c r="CZ2" s="49"/>
-      <c r="DA2" s="49"/>
-      <c r="DB2" s="49"/>
-      <c r="DC2" s="49"/>
-      <c r="DD2" s="49"/>
-      <c r="DE2" s="49"/>
-      <c r="DF2" s="49"/>
-      <c r="DG2" s="49"/>
-      <c r="DH2" s="49"/>
-      <c r="DI2" s="49"/>
-      <c r="DJ2" s="49"/>
-      <c r="DK2" s="49"/>
-      <c r="DL2" s="49"/>
-      <c r="DM2" s="49"/>
-      <c r="DN2" s="49"/>
-      <c r="DO2" s="49"/>
-      <c r="DP2" s="49"/>
-      <c r="DQ2" s="49"/>
-      <c r="DR2" s="49"/>
-      <c r="DS2" s="49"/>
-      <c r="DT2" s="49"/>
-      <c r="DU2" s="49"/>
-      <c r="DV2" s="49"/>
-      <c r="DW2" s="49"/>
-      <c r="DX2" s="50"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32"/>
+      <c r="AS2" s="32"/>
+      <c r="AT2" s="32"/>
+      <c r="AU2" s="32"/>
+      <c r="AV2" s="32"/>
+      <c r="AW2" s="32"/>
+      <c r="AX2" s="32"/>
+      <c r="AY2" s="32"/>
+      <c r="AZ2" s="32"/>
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="32"/>
+      <c r="BD2" s="32"/>
+      <c r="BE2" s="32"/>
+      <c r="BF2" s="32"/>
+      <c r="BG2" s="32"/>
+      <c r="BH2" s="32"/>
+      <c r="BI2" s="32"/>
+      <c r="BJ2" s="32"/>
+      <c r="BK2" s="32"/>
+      <c r="BL2" s="32"/>
+      <c r="BM2" s="32"/>
+      <c r="BN2" s="32"/>
+      <c r="BO2" s="32"/>
+      <c r="BP2" s="32"/>
+      <c r="BQ2" s="32"/>
+      <c r="BR2" s="32"/>
+      <c r="BS2" s="32"/>
+      <c r="BT2" s="32"/>
+      <c r="BU2" s="32"/>
+      <c r="BV2" s="32"/>
+      <c r="BW2" s="32"/>
+      <c r="BX2" s="32"/>
+      <c r="BY2" s="32"/>
+      <c r="BZ2" s="32"/>
+      <c r="CA2" s="32"/>
+      <c r="CB2" s="32"/>
+      <c r="CC2" s="32"/>
+      <c r="CD2" s="32"/>
+      <c r="CE2" s="32"/>
+      <c r="CF2" s="32"/>
+      <c r="CG2" s="32"/>
+      <c r="CH2" s="32"/>
+      <c r="CI2" s="32"/>
+      <c r="CJ2" s="32"/>
+      <c r="CK2" s="32"/>
+      <c r="CL2" s="32"/>
+      <c r="CM2" s="32"/>
+      <c r="CN2" s="32"/>
+      <c r="CO2" s="32"/>
+      <c r="CP2" s="32"/>
+      <c r="CQ2" s="32"/>
+      <c r="CR2" s="32"/>
+      <c r="CS2" s="32"/>
+      <c r="CT2" s="32"/>
+      <c r="CU2" s="32"/>
+      <c r="CV2" s="32"/>
+      <c r="CW2" s="32"/>
+      <c r="CX2" s="32"/>
+      <c r="CY2" s="32"/>
+      <c r="CZ2" s="32"/>
+      <c r="DA2" s="32"/>
+      <c r="DB2" s="32"/>
+      <c r="DC2" s="32"/>
+      <c r="DD2" s="32"/>
+      <c r="DE2" s="32"/>
+      <c r="DF2" s="32"/>
+      <c r="DG2" s="32"/>
+      <c r="DH2" s="32"/>
+      <c r="DI2" s="32"/>
+      <c r="DJ2" s="32"/>
+      <c r="DK2" s="32"/>
+      <c r="DL2" s="32"/>
+      <c r="DM2" s="32"/>
+      <c r="DN2" s="32"/>
+      <c r="DO2" s="32"/>
+      <c r="DP2" s="32"/>
+      <c r="DQ2" s="32"/>
+      <c r="DR2" s="32"/>
+      <c r="DS2" s="32"/>
+      <c r="DT2" s="32"/>
+      <c r="DU2" s="32"/>
+      <c r="DV2" s="32"/>
+      <c r="DW2" s="32"/>
+      <c r="DX2" s="33"/>
     </row>
     <row r="3" spans="1:157" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2722,169 +2811,169 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="54" t="s">
+      <c r="B4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
-      <c r="G4" s="54"/>
-      <c r="H4" s="54"/>
-      <c r="I4" s="56" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="56"/>
-      <c r="K4" s="56"/>
-      <c r="L4" s="56"/>
-      <c r="M4" s="56"/>
-      <c r="N4" s="56"/>
-      <c r="O4" s="56"/>
-      <c r="P4" s="56" t="s">
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="56"/>
-      <c r="R4" s="56"/>
-      <c r="S4" s="56"/>
-      <c r="T4" s="56"/>
-      <c r="U4" s="56"/>
-      <c r="V4" s="56"/>
-      <c r="W4" s="64" t="s">
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
-      <c r="Z4" s="64"/>
-      <c r="AA4" s="64"/>
-      <c r="AB4" s="64"/>
-      <c r="AC4" s="64"/>
-      <c r="AD4" s="64"/>
-      <c r="AE4" s="64"/>
-      <c r="AF4" s="64"/>
-      <c r="AG4" s="64"/>
-      <c r="AH4" s="64"/>
-      <c r="AI4" s="64"/>
-      <c r="AJ4" s="64"/>
-      <c r="AK4" s="64"/>
-      <c r="AL4" s="64"/>
-      <c r="AM4" s="64"/>
-      <c r="AN4" s="64"/>
-      <c r="AO4" s="64"/>
-      <c r="AP4" s="64"/>
-      <c r="AQ4" s="64"/>
-      <c r="AR4" s="64"/>
-      <c r="AS4" s="64"/>
-      <c r="AT4" s="64"/>
-      <c r="AU4" s="64"/>
-      <c r="AV4" s="64"/>
-      <c r="AW4" s="64"/>
-      <c r="AX4" s="66" t="s">
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="25"/>
+      <c r="AH4" s="25"/>
+      <c r="AI4" s="25"/>
+      <c r="AJ4" s="25"/>
+      <c r="AK4" s="25"/>
+      <c r="AL4" s="25"/>
+      <c r="AM4" s="25"/>
+      <c r="AN4" s="25"/>
+      <c r="AO4" s="25"/>
+      <c r="AP4" s="25"/>
+      <c r="AQ4" s="25"/>
+      <c r="AR4" s="25"/>
+      <c r="AS4" s="25"/>
+      <c r="AT4" s="25"/>
+      <c r="AU4" s="25"/>
+      <c r="AV4" s="25"/>
+      <c r="AW4" s="25"/>
+      <c r="AX4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AY4" s="66"/>
-      <c r="AZ4" s="66"/>
-      <c r="BA4" s="66"/>
-      <c r="BB4" s="66"/>
-      <c r="BC4" s="65" t="s">
+      <c r="AY4" s="27"/>
+      <c r="AZ4" s="27"/>
+      <c r="BA4" s="27"/>
+      <c r="BB4" s="27"/>
+      <c r="BC4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="BD4" s="65"/>
-      <c r="BE4" s="58" t="s">
+      <c r="BD4" s="26"/>
+      <c r="BE4" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="BF4" s="57" t="s">
+      <c r="BF4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="BG4" s="27" t="s">
+      <c r="BG4" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="BH4" s="28"/>
-      <c r="BI4" s="28"/>
-      <c r="BJ4" s="28"/>
-      <c r="BK4" s="28"/>
-      <c r="BL4" s="29"/>
-      <c r="BM4" s="30" t="s">
+      <c r="BH4" s="54"/>
+      <c r="BI4" s="54"/>
+      <c r="BJ4" s="54"/>
+      <c r="BK4" s="54"/>
+      <c r="BL4" s="55"/>
+      <c r="BM4" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="BN4" s="31"/>
-      <c r="BO4" s="31"/>
-      <c r="BP4" s="31"/>
-      <c r="BQ4" s="31"/>
-      <c r="BR4" s="31"/>
-      <c r="BS4" s="32"/>
-      <c r="BT4" s="33" t="s">
+      <c r="BN4" s="57"/>
+      <c r="BO4" s="57"/>
+      <c r="BP4" s="57"/>
+      <c r="BQ4" s="57"/>
+      <c r="BR4" s="57"/>
+      <c r="BS4" s="58"/>
+      <c r="BT4" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="BU4" s="34"/>
-      <c r="BV4" s="34"/>
-      <c r="BW4" s="34"/>
-      <c r="BX4" s="34"/>
-      <c r="BY4" s="34"/>
-      <c r="BZ4" s="35"/>
-      <c r="CA4" s="36" t="s">
+      <c r="BU4" s="60"/>
+      <c r="BV4" s="60"/>
+      <c r="BW4" s="60"/>
+      <c r="BX4" s="60"/>
+      <c r="BY4" s="60"/>
+      <c r="BZ4" s="61"/>
+      <c r="CA4" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="CB4" s="37"/>
-      <c r="CC4" s="37"/>
-      <c r="CD4" s="37"/>
-      <c r="CE4" s="37"/>
-      <c r="CF4" s="37"/>
-      <c r="CG4" s="38"/>
-      <c r="CH4" s="39" t="s">
+      <c r="CB4" s="63"/>
+      <c r="CC4" s="63"/>
+      <c r="CD4" s="63"/>
+      <c r="CE4" s="63"/>
+      <c r="CF4" s="63"/>
+      <c r="CG4" s="64"/>
+      <c r="CH4" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="CI4" s="40"/>
-      <c r="CJ4" s="40"/>
-      <c r="CK4" s="40"/>
-      <c r="CL4" s="40"/>
-      <c r="CM4" s="40"/>
-      <c r="CN4" s="41"/>
-      <c r="CO4" s="21" t="s">
+      <c r="CI4" s="66"/>
+      <c r="CJ4" s="66"/>
+      <c r="CK4" s="66"/>
+      <c r="CL4" s="66"/>
+      <c r="CM4" s="66"/>
+      <c r="CN4" s="67"/>
+      <c r="CO4" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="CP4" s="22"/>
-      <c r="CQ4" s="22"/>
-      <c r="CR4" s="22"/>
-      <c r="CS4" s="22"/>
-      <c r="CT4" s="23"/>
-      <c r="CU4" s="24" t="s">
+      <c r="CP4" s="48"/>
+      <c r="CQ4" s="48"/>
+      <c r="CR4" s="48"/>
+      <c r="CS4" s="48"/>
+      <c r="CT4" s="49"/>
+      <c r="CU4" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="CV4" s="25"/>
-      <c r="CW4" s="25"/>
-      <c r="CX4" s="25"/>
-      <c r="CY4" s="25"/>
-      <c r="CZ4" s="25"/>
-      <c r="DA4" s="26"/>
-      <c r="DB4" s="42" t="s">
+      <c r="CV4" s="51"/>
+      <c r="CW4" s="51"/>
+      <c r="CX4" s="51"/>
+      <c r="CY4" s="51"/>
+      <c r="CZ4" s="51"/>
+      <c r="DA4" s="52"/>
+      <c r="DB4" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="DC4" s="43"/>
-      <c r="DD4" s="43"/>
-      <c r="DE4" s="43"/>
-      <c r="DF4" s="43"/>
-      <c r="DG4" s="43"/>
-      <c r="DH4" s="43"/>
-      <c r="DI4" s="43"/>
-      <c r="DJ4" s="43"/>
-      <c r="DK4" s="43"/>
-      <c r="DL4" s="43"/>
-      <c r="DM4" s="43"/>
-      <c r="DN4" s="43"/>
-      <c r="DO4" s="43"/>
-      <c r="DP4" s="44"/>
-      <c r="DQ4" s="18" t="s">
+      <c r="DC4" s="69"/>
+      <c r="DD4" s="69"/>
+      <c r="DE4" s="69"/>
+      <c r="DF4" s="69"/>
+      <c r="DG4" s="69"/>
+      <c r="DH4" s="69"/>
+      <c r="DI4" s="69"/>
+      <c r="DJ4" s="69"/>
+      <c r="DK4" s="69"/>
+      <c r="DL4" s="69"/>
+      <c r="DM4" s="69"/>
+      <c r="DN4" s="69"/>
+      <c r="DO4" s="69"/>
+      <c r="DP4" s="70"/>
+      <c r="DQ4" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="DR4" s="19"/>
-      <c r="DS4" s="19"/>
-      <c r="DT4" s="19"/>
-      <c r="DU4" s="19"/>
-      <c r="DV4" s="20"/>
-      <c r="DW4" s="58" t="s">
+      <c r="DR4" s="45"/>
+      <c r="DS4" s="45"/>
+      <c r="DT4" s="45"/>
+      <c r="DU4" s="45"/>
+      <c r="DV4" s="46"/>
+      <c r="DW4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="DX4" s="57" t="s">
+      <c r="DX4" s="37" t="s">
         <v>12</v>
       </c>
       <c r="DY4" s="5"/>
@@ -2924,193 +3013,193 @@
       <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="55" t="s">
+      <c r="C5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="55"/>
-      <c r="E5" s="55"/>
-      <c r="F5" s="55"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="51" t="s">
+      <c r="I5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="52"/>
-      <c r="K5" s="52"/>
-      <c r="L5" s="52"/>
-      <c r="M5" s="53"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="21"/>
       <c r="N5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="51" t="s">
+      <c r="O5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="52"/>
-      <c r="Q5" s="52"/>
-      <c r="R5" s="52"/>
-      <c r="S5" s="52"/>
-      <c r="T5" s="52"/>
-      <c r="U5" s="53"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="21"/>
       <c r="V5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="51" t="s">
+      <c r="W5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="X5" s="52"/>
-      <c r="Y5" s="52"/>
-      <c r="Z5" s="52"/>
-      <c r="AA5" s="52"/>
-      <c r="AB5" s="53"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="21"/>
       <c r="AC5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="51" t="s">
+      <c r="AD5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AE5" s="52"/>
-      <c r="AF5" s="52"/>
-      <c r="AG5" s="52"/>
-      <c r="AH5" s="52"/>
-      <c r="AI5" s="53"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="21"/>
       <c r="AJ5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AK5" s="51" t="s">
+      <c r="AK5" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="AL5" s="52"/>
-      <c r="AM5" s="52"/>
-      <c r="AN5" s="52"/>
-      <c r="AO5" s="52"/>
-      <c r="AP5" s="53"/>
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="20"/>
+      <c r="AN5" s="20"/>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="21"/>
       <c r="AQ5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AR5" s="51" t="s">
+      <c r="AR5" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="AS5" s="52"/>
-      <c r="AT5" s="52"/>
-      <c r="AU5" s="52"/>
-      <c r="AV5" s="52"/>
-      <c r="AW5" s="53"/>
+      <c r="AS5" s="20"/>
+      <c r="AT5" s="20"/>
+      <c r="AU5" s="20"/>
+      <c r="AV5" s="20"/>
+      <c r="AW5" s="21"/>
       <c r="AX5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AY5" s="51" t="s">
+      <c r="AY5" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="AZ5" s="52"/>
-      <c r="BA5" s="52"/>
-      <c r="BB5" s="53"/>
-      <c r="BC5" s="51" t="s">
+      <c r="AZ5" s="20"/>
+      <c r="BA5" s="20"/>
+      <c r="BB5" s="21"/>
+      <c r="BC5" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="BD5" s="53"/>
-      <c r="BE5" s="58"/>
-      <c r="BF5" s="57"/>
-      <c r="BG5" s="51" t="s">
+      <c r="BD5" s="21"/>
+      <c r="BE5" s="38"/>
+      <c r="BF5" s="37"/>
+      <c r="BG5" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="BH5" s="52"/>
-      <c r="BI5" s="52"/>
-      <c r="BJ5" s="52"/>
-      <c r="BK5" s="53"/>
+      <c r="BH5" s="20"/>
+      <c r="BI5" s="20"/>
+      <c r="BJ5" s="20"/>
+      <c r="BK5" s="21"/>
       <c r="BL5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="BM5" s="51" t="s">
+      <c r="BM5" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="BN5" s="52"/>
-      <c r="BO5" s="52"/>
-      <c r="BP5" s="52"/>
-      <c r="BQ5" s="52"/>
-      <c r="BR5" s="53"/>
+      <c r="BN5" s="20"/>
+      <c r="BO5" s="20"/>
+      <c r="BP5" s="20"/>
+      <c r="BQ5" s="20"/>
+      <c r="BR5" s="21"/>
       <c r="BS5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="BT5" s="51" t="s">
-        <v>60</v>
-      </c>
-      <c r="BU5" s="52"/>
-      <c r="BV5" s="52"/>
-      <c r="BW5" s="52"/>
-      <c r="BX5" s="52"/>
-      <c r="BY5" s="53"/>
+      <c r="BT5" s="22" t="s">
+        <v>71</v>
+      </c>
+      <c r="BU5" s="20"/>
+      <c r="BV5" s="20"/>
+      <c r="BW5" s="20"/>
+      <c r="BX5" s="20"/>
+      <c r="BY5" s="21"/>
       <c r="BZ5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="CA5" s="51" t="s">
+      <c r="CA5" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="CB5" s="52"/>
-      <c r="CC5" s="52"/>
-      <c r="CD5" s="52"/>
-      <c r="CE5" s="52"/>
-      <c r="CF5" s="53"/>
+      <c r="CB5" s="20"/>
+      <c r="CC5" s="20"/>
+      <c r="CD5" s="20"/>
+      <c r="CE5" s="20"/>
+      <c r="CF5" s="21"/>
       <c r="CG5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="CH5" s="51" t="s">
+      <c r="CH5" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="CI5" s="52"/>
-      <c r="CJ5" s="52"/>
-      <c r="CK5" s="52"/>
-      <c r="CL5" s="52"/>
-      <c r="CM5" s="53"/>
+      <c r="CI5" s="20"/>
+      <c r="CJ5" s="20"/>
+      <c r="CK5" s="20"/>
+      <c r="CL5" s="20"/>
+      <c r="CM5" s="21"/>
       <c r="CN5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="CO5" s="51" t="s">
+      <c r="CO5" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="CP5" s="52"/>
-      <c r="CQ5" s="52"/>
-      <c r="CR5" s="52"/>
-      <c r="CS5" s="52"/>
-      <c r="CT5" s="53"/>
+      <c r="CP5" s="20"/>
+      <c r="CQ5" s="20"/>
+      <c r="CR5" s="20"/>
+      <c r="CS5" s="20"/>
+      <c r="CT5" s="21"/>
       <c r="CU5" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="CV5" s="51" t="s">
+      <c r="CV5" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="CW5" s="52"/>
-      <c r="CX5" s="52"/>
-      <c r="CY5" s="52"/>
-      <c r="CZ5" s="52"/>
-      <c r="DA5" s="53"/>
+      <c r="CW5" s="20"/>
+      <c r="CX5" s="20"/>
+      <c r="CY5" s="20"/>
+      <c r="CZ5" s="20"/>
+      <c r="DA5" s="21"/>
       <c r="DB5" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="DC5" s="67" t="s">
+      <c r="DC5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="DD5" s="68"/>
-      <c r="DE5" s="68"/>
-      <c r="DF5" s="68"/>
-      <c r="DG5" s="68"/>
-      <c r="DH5" s="69"/>
+      <c r="DD5" s="23"/>
+      <c r="DE5" s="23"/>
+      <c r="DF5" s="23"/>
+      <c r="DG5" s="23"/>
+      <c r="DH5" s="24"/>
       <c r="DI5" s="17" t="s">
         <v>64</v>
       </c>
       <c r="DP5" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="DQ5" s="51" t="s">
+      <c r="DQ5" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="DR5" s="52"/>
-      <c r="DS5" s="52"/>
-      <c r="DT5" s="52"/>
-      <c r="DU5" s="52"/>
-      <c r="DV5" s="53"/>
-      <c r="DW5" s="58"/>
-      <c r="DX5" s="57"/>
+      <c r="DR5" s="20"/>
+      <c r="DS5" s="20"/>
+      <c r="DT5" s="20"/>
+      <c r="DU5" s="20"/>
+      <c r="DV5" s="21"/>
+      <c r="DW5" s="38"/>
+      <c r="DX5" s="37"/>
     </row>
     <row r="6" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -3122,74 +3211,107 @@
       <c r="N6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="59" t="s">
+      <c r="V6" s="39" t="s">
         <v>24</v>
       </c>
       <c r="AC6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AK6" s="67" t="s">
+      <c r="AK6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="AL6" s="68"/>
-      <c r="AM6" s="68"/>
-      <c r="AN6" s="68"/>
-      <c r="AO6" s="68"/>
-      <c r="AP6" s="69"/>
-      <c r="AV6" s="62" t="s">
+      <c r="AL6" s="23"/>
+      <c r="AM6" s="23"/>
+      <c r="AN6" s="23"/>
+      <c r="AO6" s="23"/>
+      <c r="AP6" s="24"/>
+      <c r="AV6" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="AW6" s="63"/>
+      <c r="AW6" s="43"/>
       <c r="AX6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AY6" s="51"/>
-      <c r="AZ6" s="52"/>
-      <c r="BA6" s="52"/>
-      <c r="BB6" s="53"/>
-      <c r="BC6" s="51" t="s">
+      <c r="AY6" s="22"/>
+      <c r="AZ6" s="20"/>
+      <c r="BA6" s="20"/>
+      <c r="BB6" s="21"/>
+      <c r="BC6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="BD6" s="53"/>
-      <c r="BE6" s="58"/>
-      <c r="BF6" s="57"/>
-      <c r="CN6" s="70" t="s">
+      <c r="BD6" s="21"/>
+      <c r="BE6" s="38"/>
+      <c r="BF6" s="37"/>
+      <c r="BG6" s="22" t="s">
+        <v>67</v>
+      </c>
+      <c r="BH6" s="20"/>
+      <c r="BI6" s="20"/>
+      <c r="BJ6" s="20"/>
+      <c r="BK6" s="21"/>
+      <c r="BM6" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="BN6" s="20"/>
+      <c r="BO6" s="20"/>
+      <c r="BP6" s="20"/>
+      <c r="BQ6" s="20"/>
+      <c r="BR6" s="21"/>
+      <c r="BZ6" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="CA6" s="72" t="s">
+        <v>70</v>
+      </c>
+      <c r="CB6" s="73"/>
+      <c r="CC6" s="73"/>
+      <c r="CD6" s="73"/>
+      <c r="CE6" s="73"/>
+      <c r="CF6" s="73"/>
+      <c r="CG6" s="73"/>
+      <c r="CH6" s="73"/>
+      <c r="CI6" s="73"/>
+      <c r="CJ6" s="73"/>
+      <c r="CK6" s="73"/>
+      <c r="CL6" s="73"/>
+      <c r="CM6" s="74"/>
+      <c r="CN6" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="CO6" s="51" t="s">
+      <c r="CO6" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="CP6" s="52"/>
-      <c r="CQ6" s="52"/>
-      <c r="CR6" s="52"/>
-      <c r="CS6" s="52"/>
-      <c r="CT6" s="53"/>
-      <c r="CV6" s="51" t="s">
+      <c r="CP6" s="20"/>
+      <c r="CQ6" s="20"/>
+      <c r="CR6" s="20"/>
+      <c r="CS6" s="20"/>
+      <c r="CT6" s="21"/>
+      <c r="CV6" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="CW6" s="52"/>
-      <c r="CX6" s="52"/>
-      <c r="CY6" s="52"/>
-      <c r="CZ6" s="52"/>
-      <c r="DA6" s="53"/>
-      <c r="DC6" s="67" t="s">
+      <c r="CW6" s="20"/>
+      <c r="CX6" s="20"/>
+      <c r="CY6" s="20"/>
+      <c r="CZ6" s="20"/>
+      <c r="DA6" s="21"/>
+      <c r="DC6" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="DD6" s="52"/>
-      <c r="DE6" s="52"/>
-      <c r="DF6" s="52"/>
-      <c r="DG6" s="52"/>
-      <c r="DH6" s="53"/>
+      <c r="DD6" s="20"/>
+      <c r="DE6" s="20"/>
+      <c r="DF6" s="20"/>
+      <c r="DG6" s="20"/>
+      <c r="DH6" s="21"/>
       <c r="DI6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="DW6" s="58"/>
-      <c r="DX6" s="57"/>
+      <c r="DW6" s="38"/>
+      <c r="DX6" s="37"/>
     </row>
     <row r="7" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V7" s="60"/>
-      <c r="BF7" s="57"/>
-      <c r="DX7" s="57"/>
+      <c r="V7" s="40"/>
+      <c r="BF7" s="37"/>
+      <c r="DX7" s="37"/>
     </row>
     <row r="8" spans="1:157" s="4" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -3197,33 +3319,21 @@
       </c>
       <c r="B8" s="7">
         <f ca="1">TODAY()</f>
-        <v>44745</v>
-      </c>
-      <c r="V8" s="61"/>
+        <v>44752</v>
+      </c>
+      <c r="V8" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="DC6:DH6"/>
-    <mergeCell ref="DQ5:DV5"/>
-    <mergeCell ref="DC5:DH5"/>
-    <mergeCell ref="BT5:BY5"/>
-    <mergeCell ref="CA5:CF5"/>
-    <mergeCell ref="CH5:CM5"/>
-    <mergeCell ref="CO5:CT5"/>
-    <mergeCell ref="CV5:DA5"/>
-    <mergeCell ref="BG5:BK5"/>
-    <mergeCell ref="BM5:BR5"/>
-    <mergeCell ref="CO6:CT6"/>
-    <mergeCell ref="CV6:DA6"/>
-    <mergeCell ref="W4:AW4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="AX4:BB4"/>
-    <mergeCell ref="AK6:AP6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="AD5:AI5"/>
-    <mergeCell ref="AK5:AP5"/>
-    <mergeCell ref="AR5:AW5"/>
-    <mergeCell ref="BC5:BD5"/>
+  <mergeCells count="49">
+    <mergeCell ref="DQ4:DV4"/>
+    <mergeCell ref="CO4:CT4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="BG4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="DB4:DP4"/>
     <mergeCell ref="A1:DX2"/>
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="O5:U5"/>
@@ -3240,15 +3350,30 @@
     <mergeCell ref="AY6:BB6"/>
     <mergeCell ref="AV6:AW6"/>
     <mergeCell ref="AY5:BB5"/>
-    <mergeCell ref="DQ4:DV4"/>
-    <mergeCell ref="CO4:CT4"/>
-    <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="BG4:BL4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="DB4:DP4"/>
+    <mergeCell ref="BG5:BK5"/>
+    <mergeCell ref="BM5:BR5"/>
+    <mergeCell ref="CO6:CT6"/>
+    <mergeCell ref="CV6:DA6"/>
+    <mergeCell ref="W4:AW4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="AX4:BB4"/>
+    <mergeCell ref="AK6:AP6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="AD5:AI5"/>
+    <mergeCell ref="AK5:AP5"/>
+    <mergeCell ref="AR5:AW5"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BG6:BK6"/>
+    <mergeCell ref="BM6:BR6"/>
+    <mergeCell ref="CA6:CM6"/>
+    <mergeCell ref="DC6:DH6"/>
+    <mergeCell ref="DQ5:DV5"/>
+    <mergeCell ref="DC5:DH5"/>
+    <mergeCell ref="BT5:BY5"/>
+    <mergeCell ref="CA5:CF5"/>
+    <mergeCell ref="CH5:CM5"/>
+    <mergeCell ref="CO5:CT5"/>
+    <mergeCell ref="CV5:DA5"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:XFD3">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
updated meeting log from 17 Jul 22
</commit_message>
<xml_diff>
--- a/Timeline/Project_Timeline.xlsx
+++ b/Timeline/Project_Timeline.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Desktop/agile/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A507C5E6-012E-0945-B078-BA6ACC5390B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B3BD9E-B404-6E4C-A8E5-534FA9FCA1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15920" yWindow="4020" windowWidth="28800" windowHeight="22140" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
   <si>
     <t>ASP - Group Project</t>
   </si>
@@ -1104,9 +1104,6 @@
 Backend featrues added - button link to chart.js and File load complete</t>
   </si>
   <si>
-    <t>Accelerated MVP intended timeline - TBC following sprint 3</t>
-  </si>
-  <si>
     <t>ADDITIONAL FEATURES IF MVP TIMELINE IS EARLY</t>
   </si>
   <si>
@@ -1159,6 +1156,122 @@
 - Continue integration of backend features on the system. The next focus will be chart.js implementation and error management of the data.
 - Look at implementing an export feature of charts.js once it has been successfully implemented on the system.
 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Ben &amp; Thavelarn
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">- Add all features to the front end so the backend can link them
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Kashka</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Create parsing function.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Connor</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> 
+- Create navigation bar
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>David</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+- Charts.js linking
+</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Accelerated MVP intended timeline
+</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Accelerated MVP intended timeline
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Unable to achieve this timeline, review next week</t>
     </r>
   </si>
 </sst>
@@ -1627,173 +1740,173 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2150,8 +2263,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3400B0-A312-474B-BDD8-7EBBB1942BA5}">
   <dimension ref="A1:FA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BM3" workbookViewId="0">
-      <selection activeCell="BT5" sqref="BT5:BY5"/>
+    <sheetView tabSelected="1" topLeftCell="CE2" workbookViewId="0">
+      <selection activeCell="CB6" sqref="CB6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2160,266 +2273,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="29"/>
-      <c r="AJ1" s="29"/>
-      <c r="AK1" s="29"/>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="29"/>
-      <c r="AP1" s="29"/>
-      <c r="AQ1" s="29"/>
-      <c r="AR1" s="29"/>
-      <c r="AS1" s="29"/>
-      <c r="AT1" s="29"/>
-      <c r="AU1" s="29"/>
-      <c r="AV1" s="29"/>
-      <c r="AW1" s="29"/>
-      <c r="AX1" s="29"/>
-      <c r="AY1" s="29"/>
-      <c r="AZ1" s="29"/>
-      <c r="BA1" s="29"/>
-      <c r="BB1" s="29"/>
-      <c r="BC1" s="29"/>
-      <c r="BD1" s="29"/>
-      <c r="BE1" s="29"/>
-      <c r="BF1" s="29"/>
-      <c r="BG1" s="29"/>
-      <c r="BH1" s="29"/>
-      <c r="BI1" s="29"/>
-      <c r="BJ1" s="29"/>
-      <c r="BK1" s="29"/>
-      <c r="BL1" s="29"/>
-      <c r="BM1" s="29"/>
-      <c r="BN1" s="29"/>
-      <c r="BO1" s="29"/>
-      <c r="BP1" s="29"/>
-      <c r="BQ1" s="29"/>
-      <c r="BR1" s="29"/>
-      <c r="BS1" s="29"/>
-      <c r="BT1" s="29"/>
-      <c r="BU1" s="29"/>
-      <c r="BV1" s="29"/>
-      <c r="BW1" s="29"/>
-      <c r="BX1" s="29"/>
-      <c r="BY1" s="29"/>
-      <c r="BZ1" s="29"/>
-      <c r="CA1" s="29"/>
-      <c r="CB1" s="29"/>
-      <c r="CC1" s="29"/>
-      <c r="CD1" s="29"/>
-      <c r="CE1" s="29"/>
-      <c r="CF1" s="29"/>
-      <c r="CG1" s="29"/>
-      <c r="CH1" s="29"/>
-      <c r="CI1" s="29"/>
-      <c r="CJ1" s="29"/>
-      <c r="CK1" s="29"/>
-      <c r="CL1" s="29"/>
-      <c r="CM1" s="29"/>
-      <c r="CN1" s="29"/>
-      <c r="CO1" s="29"/>
-      <c r="CP1" s="29"/>
-      <c r="CQ1" s="29"/>
-      <c r="CR1" s="29"/>
-      <c r="CS1" s="29"/>
-      <c r="CT1" s="29"/>
-      <c r="CU1" s="29"/>
-      <c r="CV1" s="29"/>
-      <c r="CW1" s="29"/>
-      <c r="CX1" s="29"/>
-      <c r="CY1" s="29"/>
-      <c r="CZ1" s="29"/>
-      <c r="DA1" s="29"/>
-      <c r="DB1" s="29"/>
-      <c r="DC1" s="29"/>
-      <c r="DD1" s="29"/>
-      <c r="DE1" s="29"/>
-      <c r="DF1" s="29"/>
-      <c r="DG1" s="29"/>
-      <c r="DH1" s="29"/>
-      <c r="DI1" s="29"/>
-      <c r="DJ1" s="29"/>
-      <c r="DK1" s="29"/>
-      <c r="DL1" s="29"/>
-      <c r="DM1" s="29"/>
-      <c r="DN1" s="29"/>
-      <c r="DO1" s="29"/>
-      <c r="DP1" s="29"/>
-      <c r="DQ1" s="29"/>
-      <c r="DR1" s="29"/>
-      <c r="DS1" s="29"/>
-      <c r="DT1" s="29"/>
-      <c r="DU1" s="29"/>
-      <c r="DV1" s="29"/>
-      <c r="DW1" s="29"/>
-      <c r="DX1" s="30"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="48"/>
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="48"/>
+      <c r="AI1" s="48"/>
+      <c r="AJ1" s="48"/>
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="48"/>
+      <c r="AM1" s="48"/>
+      <c r="AN1" s="48"/>
+      <c r="AO1" s="48"/>
+      <c r="AP1" s="48"/>
+      <c r="AQ1" s="48"/>
+      <c r="AR1" s="48"/>
+      <c r="AS1" s="48"/>
+      <c r="AT1" s="48"/>
+      <c r="AU1" s="48"/>
+      <c r="AV1" s="48"/>
+      <c r="AW1" s="48"/>
+      <c r="AX1" s="48"/>
+      <c r="AY1" s="48"/>
+      <c r="AZ1" s="48"/>
+      <c r="BA1" s="48"/>
+      <c r="BB1" s="48"/>
+      <c r="BC1" s="48"/>
+      <c r="BD1" s="48"/>
+      <c r="BE1" s="48"/>
+      <c r="BF1" s="48"/>
+      <c r="BG1" s="48"/>
+      <c r="BH1" s="48"/>
+      <c r="BI1" s="48"/>
+      <c r="BJ1" s="48"/>
+      <c r="BK1" s="48"/>
+      <c r="BL1" s="48"/>
+      <c r="BM1" s="48"/>
+      <c r="BN1" s="48"/>
+      <c r="BO1" s="48"/>
+      <c r="BP1" s="48"/>
+      <c r="BQ1" s="48"/>
+      <c r="BR1" s="48"/>
+      <c r="BS1" s="48"/>
+      <c r="BT1" s="48"/>
+      <c r="BU1" s="48"/>
+      <c r="BV1" s="48"/>
+      <c r="BW1" s="48"/>
+      <c r="BX1" s="48"/>
+      <c r="BY1" s="48"/>
+      <c r="BZ1" s="48"/>
+      <c r="CA1" s="48"/>
+      <c r="CB1" s="48"/>
+      <c r="CC1" s="48"/>
+      <c r="CD1" s="48"/>
+      <c r="CE1" s="48"/>
+      <c r="CF1" s="48"/>
+      <c r="CG1" s="48"/>
+      <c r="CH1" s="48"/>
+      <c r="CI1" s="48"/>
+      <c r="CJ1" s="48"/>
+      <c r="CK1" s="48"/>
+      <c r="CL1" s="48"/>
+      <c r="CM1" s="48"/>
+      <c r="CN1" s="48"/>
+      <c r="CO1" s="48"/>
+      <c r="CP1" s="48"/>
+      <c r="CQ1" s="48"/>
+      <c r="CR1" s="48"/>
+      <c r="CS1" s="48"/>
+      <c r="CT1" s="48"/>
+      <c r="CU1" s="48"/>
+      <c r="CV1" s="48"/>
+      <c r="CW1" s="48"/>
+      <c r="CX1" s="48"/>
+      <c r="CY1" s="48"/>
+      <c r="CZ1" s="48"/>
+      <c r="DA1" s="48"/>
+      <c r="DB1" s="48"/>
+      <c r="DC1" s="48"/>
+      <c r="DD1" s="48"/>
+      <c r="DE1" s="48"/>
+      <c r="DF1" s="48"/>
+      <c r="DG1" s="48"/>
+      <c r="DH1" s="48"/>
+      <c r="DI1" s="48"/>
+      <c r="DJ1" s="48"/>
+      <c r="DK1" s="48"/>
+      <c r="DL1" s="48"/>
+      <c r="DM1" s="48"/>
+      <c r="DN1" s="48"/>
+      <c r="DO1" s="48"/>
+      <c r="DP1" s="48"/>
+      <c r="DQ1" s="48"/>
+      <c r="DR1" s="48"/>
+      <c r="DS1" s="48"/>
+      <c r="DT1" s="48"/>
+      <c r="DU1" s="48"/>
+      <c r="DV1" s="48"/>
+      <c r="DW1" s="48"/>
+      <c r="DX1" s="49"/>
     </row>
     <row r="2" spans="1:157" s="4" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
-      <c r="AW2" s="32"/>
-      <c r="AX2" s="32"/>
-      <c r="AY2" s="32"/>
-      <c r="AZ2" s="32"/>
-      <c r="BA2" s="32"/>
-      <c r="BB2" s="32"/>
-      <c r="BC2" s="32"/>
-      <c r="BD2" s="32"/>
-      <c r="BE2" s="32"/>
-      <c r="BF2" s="32"/>
-      <c r="BG2" s="32"/>
-      <c r="BH2" s="32"/>
-      <c r="BI2" s="32"/>
-      <c r="BJ2" s="32"/>
-      <c r="BK2" s="32"/>
-      <c r="BL2" s="32"/>
-      <c r="BM2" s="32"/>
-      <c r="BN2" s="32"/>
-      <c r="BO2" s="32"/>
-      <c r="BP2" s="32"/>
-      <c r="BQ2" s="32"/>
-      <c r="BR2" s="32"/>
-      <c r="BS2" s="32"/>
-      <c r="BT2" s="32"/>
-      <c r="BU2" s="32"/>
-      <c r="BV2" s="32"/>
-      <c r="BW2" s="32"/>
-      <c r="BX2" s="32"/>
-      <c r="BY2" s="32"/>
-      <c r="BZ2" s="32"/>
-      <c r="CA2" s="32"/>
-      <c r="CB2" s="32"/>
-      <c r="CC2" s="32"/>
-      <c r="CD2" s="32"/>
-      <c r="CE2" s="32"/>
-      <c r="CF2" s="32"/>
-      <c r="CG2" s="32"/>
-      <c r="CH2" s="32"/>
-      <c r="CI2" s="32"/>
-      <c r="CJ2" s="32"/>
-      <c r="CK2" s="32"/>
-      <c r="CL2" s="32"/>
-      <c r="CM2" s="32"/>
-      <c r="CN2" s="32"/>
-      <c r="CO2" s="32"/>
-      <c r="CP2" s="32"/>
-      <c r="CQ2" s="32"/>
-      <c r="CR2" s="32"/>
-      <c r="CS2" s="32"/>
-      <c r="CT2" s="32"/>
-      <c r="CU2" s="32"/>
-      <c r="CV2" s="32"/>
-      <c r="CW2" s="32"/>
-      <c r="CX2" s="32"/>
-      <c r="CY2" s="32"/>
-      <c r="CZ2" s="32"/>
-      <c r="DA2" s="32"/>
-      <c r="DB2" s="32"/>
-      <c r="DC2" s="32"/>
-      <c r="DD2" s="32"/>
-      <c r="DE2" s="32"/>
-      <c r="DF2" s="32"/>
-      <c r="DG2" s="32"/>
-      <c r="DH2" s="32"/>
-      <c r="DI2" s="32"/>
-      <c r="DJ2" s="32"/>
-      <c r="DK2" s="32"/>
-      <c r="DL2" s="32"/>
-      <c r="DM2" s="32"/>
-      <c r="DN2" s="32"/>
-      <c r="DO2" s="32"/>
-      <c r="DP2" s="32"/>
-      <c r="DQ2" s="32"/>
-      <c r="DR2" s="32"/>
-      <c r="DS2" s="32"/>
-      <c r="DT2" s="32"/>
-      <c r="DU2" s="32"/>
-      <c r="DV2" s="32"/>
-      <c r="DW2" s="32"/>
-      <c r="DX2" s="33"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="51"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51"/>
+      <c r="AF2" s="51"/>
+      <c r="AG2" s="51"/>
+      <c r="AH2" s="51"/>
+      <c r="AI2" s="51"/>
+      <c r="AJ2" s="51"/>
+      <c r="AK2" s="51"/>
+      <c r="AL2" s="51"/>
+      <c r="AM2" s="51"/>
+      <c r="AN2" s="51"/>
+      <c r="AO2" s="51"/>
+      <c r="AP2" s="51"/>
+      <c r="AQ2" s="51"/>
+      <c r="AR2" s="51"/>
+      <c r="AS2" s="51"/>
+      <c r="AT2" s="51"/>
+      <c r="AU2" s="51"/>
+      <c r="AV2" s="51"/>
+      <c r="AW2" s="51"/>
+      <c r="AX2" s="51"/>
+      <c r="AY2" s="51"/>
+      <c r="AZ2" s="51"/>
+      <c r="BA2" s="51"/>
+      <c r="BB2" s="51"/>
+      <c r="BC2" s="51"/>
+      <c r="BD2" s="51"/>
+      <c r="BE2" s="51"/>
+      <c r="BF2" s="51"/>
+      <c r="BG2" s="51"/>
+      <c r="BH2" s="51"/>
+      <c r="BI2" s="51"/>
+      <c r="BJ2" s="51"/>
+      <c r="BK2" s="51"/>
+      <c r="BL2" s="51"/>
+      <c r="BM2" s="51"/>
+      <c r="BN2" s="51"/>
+      <c r="BO2" s="51"/>
+      <c r="BP2" s="51"/>
+      <c r="BQ2" s="51"/>
+      <c r="BR2" s="51"/>
+      <c r="BS2" s="51"/>
+      <c r="BT2" s="51"/>
+      <c r="BU2" s="51"/>
+      <c r="BV2" s="51"/>
+      <c r="BW2" s="51"/>
+      <c r="BX2" s="51"/>
+      <c r="BY2" s="51"/>
+      <c r="BZ2" s="51"/>
+      <c r="CA2" s="51"/>
+      <c r="CB2" s="51"/>
+      <c r="CC2" s="51"/>
+      <c r="CD2" s="51"/>
+      <c r="CE2" s="51"/>
+      <c r="CF2" s="51"/>
+      <c r="CG2" s="51"/>
+      <c r="CH2" s="51"/>
+      <c r="CI2" s="51"/>
+      <c r="CJ2" s="51"/>
+      <c r="CK2" s="51"/>
+      <c r="CL2" s="51"/>
+      <c r="CM2" s="51"/>
+      <c r="CN2" s="51"/>
+      <c r="CO2" s="51"/>
+      <c r="CP2" s="51"/>
+      <c r="CQ2" s="51"/>
+      <c r="CR2" s="51"/>
+      <c r="CS2" s="51"/>
+      <c r="CT2" s="51"/>
+      <c r="CU2" s="51"/>
+      <c r="CV2" s="51"/>
+      <c r="CW2" s="51"/>
+      <c r="CX2" s="51"/>
+      <c r="CY2" s="51"/>
+      <c r="CZ2" s="51"/>
+      <c r="DA2" s="51"/>
+      <c r="DB2" s="51"/>
+      <c r="DC2" s="51"/>
+      <c r="DD2" s="51"/>
+      <c r="DE2" s="51"/>
+      <c r="DF2" s="51"/>
+      <c r="DG2" s="51"/>
+      <c r="DH2" s="51"/>
+      <c r="DI2" s="51"/>
+      <c r="DJ2" s="51"/>
+      <c r="DK2" s="51"/>
+      <c r="DL2" s="51"/>
+      <c r="DM2" s="51"/>
+      <c r="DN2" s="51"/>
+      <c r="DO2" s="51"/>
+      <c r="DP2" s="51"/>
+      <c r="DQ2" s="51"/>
+      <c r="DR2" s="51"/>
+      <c r="DS2" s="51"/>
+      <c r="DT2" s="51"/>
+      <c r="DU2" s="51"/>
+      <c r="DV2" s="51"/>
+      <c r="DW2" s="51"/>
+      <c r="DX2" s="52"/>
     </row>
     <row r="3" spans="1:157" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2811,169 +2924,169 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="36" t="s">
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36" t="s">
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="25" t="s">
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="58"/>
+      <c r="W4" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="25"/>
-      <c r="AE4" s="25"/>
-      <c r="AF4" s="25"/>
-      <c r="AG4" s="25"/>
-      <c r="AH4" s="25"/>
-      <c r="AI4" s="25"/>
-      <c r="AJ4" s="25"/>
-      <c r="AK4" s="25"/>
-      <c r="AL4" s="25"/>
-      <c r="AM4" s="25"/>
-      <c r="AN4" s="25"/>
-      <c r="AO4" s="25"/>
-      <c r="AP4" s="25"/>
-      <c r="AQ4" s="25"/>
-      <c r="AR4" s="25"/>
-      <c r="AS4" s="25"/>
-      <c r="AT4" s="25"/>
-      <c r="AU4" s="25"/>
-      <c r="AV4" s="25"/>
-      <c r="AW4" s="25"/>
-      <c r="AX4" s="27" t="s">
+      <c r="X4" s="66"/>
+      <c r="Y4" s="66"/>
+      <c r="Z4" s="66"/>
+      <c r="AA4" s="66"/>
+      <c r="AB4" s="66"/>
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="66"/>
+      <c r="AE4" s="66"/>
+      <c r="AF4" s="66"/>
+      <c r="AG4" s="66"/>
+      <c r="AH4" s="66"/>
+      <c r="AI4" s="66"/>
+      <c r="AJ4" s="66"/>
+      <c r="AK4" s="66"/>
+      <c r="AL4" s="66"/>
+      <c r="AM4" s="66"/>
+      <c r="AN4" s="66"/>
+      <c r="AO4" s="66"/>
+      <c r="AP4" s="66"/>
+      <c r="AQ4" s="66"/>
+      <c r="AR4" s="66"/>
+      <c r="AS4" s="66"/>
+      <c r="AT4" s="66"/>
+      <c r="AU4" s="66"/>
+      <c r="AV4" s="66"/>
+      <c r="AW4" s="66"/>
+      <c r="AX4" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="AY4" s="27"/>
-      <c r="AZ4" s="27"/>
-      <c r="BA4" s="27"/>
-      <c r="BB4" s="27"/>
-      <c r="BC4" s="26" t="s">
+      <c r="AY4" s="68"/>
+      <c r="AZ4" s="68"/>
+      <c r="BA4" s="68"/>
+      <c r="BB4" s="68"/>
+      <c r="BC4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="BD4" s="26"/>
-      <c r="BE4" s="38" t="s">
+      <c r="BD4" s="67"/>
+      <c r="BE4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="BF4" s="37" t="s">
+      <c r="BF4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="BG4" s="53" t="s">
+      <c r="BG4" s="29" t="s">
         <v>40</v>
       </c>
-      <c r="BH4" s="54"/>
-      <c r="BI4" s="54"/>
-      <c r="BJ4" s="54"/>
-      <c r="BK4" s="54"/>
-      <c r="BL4" s="55"/>
-      <c r="BM4" s="56" t="s">
+      <c r="BH4" s="30"/>
+      <c r="BI4" s="30"/>
+      <c r="BJ4" s="30"/>
+      <c r="BK4" s="30"/>
+      <c r="BL4" s="31"/>
+      <c r="BM4" s="32" t="s">
         <v>41</v>
       </c>
-      <c r="BN4" s="57"/>
-      <c r="BO4" s="57"/>
-      <c r="BP4" s="57"/>
-      <c r="BQ4" s="57"/>
-      <c r="BR4" s="57"/>
-      <c r="BS4" s="58"/>
-      <c r="BT4" s="59" t="s">
+      <c r="BN4" s="33"/>
+      <c r="BO4" s="33"/>
+      <c r="BP4" s="33"/>
+      <c r="BQ4" s="33"/>
+      <c r="BR4" s="33"/>
+      <c r="BS4" s="34"/>
+      <c r="BT4" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="BU4" s="60"/>
-      <c r="BV4" s="60"/>
-      <c r="BW4" s="60"/>
-      <c r="BX4" s="60"/>
-      <c r="BY4" s="60"/>
-      <c r="BZ4" s="61"/>
-      <c r="CA4" s="62" t="s">
+      <c r="BU4" s="36"/>
+      <c r="BV4" s="36"/>
+      <c r="BW4" s="36"/>
+      <c r="BX4" s="36"/>
+      <c r="BY4" s="36"/>
+      <c r="BZ4" s="37"/>
+      <c r="CA4" s="38" t="s">
         <v>43</v>
       </c>
-      <c r="CB4" s="63"/>
-      <c r="CC4" s="63"/>
-      <c r="CD4" s="63"/>
-      <c r="CE4" s="63"/>
-      <c r="CF4" s="63"/>
-      <c r="CG4" s="64"/>
-      <c r="CH4" s="65" t="s">
+      <c r="CB4" s="39"/>
+      <c r="CC4" s="39"/>
+      <c r="CD4" s="39"/>
+      <c r="CE4" s="39"/>
+      <c r="CF4" s="39"/>
+      <c r="CG4" s="40"/>
+      <c r="CH4" s="41" t="s">
         <v>44</v>
       </c>
-      <c r="CI4" s="66"/>
-      <c r="CJ4" s="66"/>
-      <c r="CK4" s="66"/>
-      <c r="CL4" s="66"/>
-      <c r="CM4" s="66"/>
-      <c r="CN4" s="67"/>
-      <c r="CO4" s="47" t="s">
+      <c r="CI4" s="42"/>
+      <c r="CJ4" s="42"/>
+      <c r="CK4" s="42"/>
+      <c r="CL4" s="42"/>
+      <c r="CM4" s="42"/>
+      <c r="CN4" s="43"/>
+      <c r="CO4" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="CP4" s="48"/>
-      <c r="CQ4" s="48"/>
-      <c r="CR4" s="48"/>
-      <c r="CS4" s="48"/>
-      <c r="CT4" s="49"/>
-      <c r="CU4" s="50" t="s">
+      <c r="CP4" s="24"/>
+      <c r="CQ4" s="24"/>
+      <c r="CR4" s="24"/>
+      <c r="CS4" s="24"/>
+      <c r="CT4" s="25"/>
+      <c r="CU4" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="CV4" s="51"/>
-      <c r="CW4" s="51"/>
-      <c r="CX4" s="51"/>
-      <c r="CY4" s="51"/>
-      <c r="CZ4" s="51"/>
-      <c r="DA4" s="52"/>
-      <c r="DB4" s="68" t="s">
+      <c r="CV4" s="27"/>
+      <c r="CW4" s="27"/>
+      <c r="CX4" s="27"/>
+      <c r="CY4" s="27"/>
+      <c r="CZ4" s="27"/>
+      <c r="DA4" s="28"/>
+      <c r="DB4" s="44" t="s">
         <v>39</v>
       </c>
-      <c r="DC4" s="69"/>
-      <c r="DD4" s="69"/>
-      <c r="DE4" s="69"/>
-      <c r="DF4" s="69"/>
-      <c r="DG4" s="69"/>
-      <c r="DH4" s="69"/>
-      <c r="DI4" s="69"/>
-      <c r="DJ4" s="69"/>
-      <c r="DK4" s="69"/>
-      <c r="DL4" s="69"/>
-      <c r="DM4" s="69"/>
-      <c r="DN4" s="69"/>
-      <c r="DO4" s="69"/>
-      <c r="DP4" s="70"/>
-      <c r="DQ4" s="44" t="s">
+      <c r="DC4" s="45"/>
+      <c r="DD4" s="45"/>
+      <c r="DE4" s="45"/>
+      <c r="DF4" s="45"/>
+      <c r="DG4" s="45"/>
+      <c r="DH4" s="45"/>
+      <c r="DI4" s="45"/>
+      <c r="DJ4" s="45"/>
+      <c r="DK4" s="45"/>
+      <c r="DL4" s="45"/>
+      <c r="DM4" s="45"/>
+      <c r="DN4" s="45"/>
+      <c r="DO4" s="45"/>
+      <c r="DP4" s="46"/>
+      <c r="DQ4" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="DR4" s="45"/>
-      <c r="DS4" s="45"/>
-      <c r="DT4" s="45"/>
-      <c r="DU4" s="45"/>
-      <c r="DV4" s="46"/>
-      <c r="DW4" s="38" t="s">
+      <c r="DR4" s="21"/>
+      <c r="DS4" s="21"/>
+      <c r="DT4" s="21"/>
+      <c r="DU4" s="21"/>
+      <c r="DV4" s="22"/>
+      <c r="DW4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="DX4" s="37" t="s">
+      <c r="DX4" s="59" t="s">
         <v>12</v>
       </c>
       <c r="DY4" s="5"/>
@@ -3013,193 +3126,193 @@
       <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="21"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
       <c r="N5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="22" t="s">
+      <c r="O5" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="21"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="55"/>
       <c r="V5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="22" t="s">
+      <c r="W5" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="X5" s="20"/>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="21"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="54"/>
+      <c r="AB5" s="55"/>
       <c r="AC5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="22" t="s">
+      <c r="AD5" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="20"/>
-      <c r="AH5" s="20"/>
-      <c r="AI5" s="21"/>
+      <c r="AE5" s="54"/>
+      <c r="AF5" s="54"/>
+      <c r="AG5" s="54"/>
+      <c r="AH5" s="54"/>
+      <c r="AI5" s="55"/>
       <c r="AJ5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AK5" s="22" t="s">
+      <c r="AK5" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="AL5" s="20"/>
-      <c r="AM5" s="20"/>
-      <c r="AN5" s="20"/>
-      <c r="AO5" s="20"/>
-      <c r="AP5" s="21"/>
+      <c r="AL5" s="54"/>
+      <c r="AM5" s="54"/>
+      <c r="AN5" s="54"/>
+      <c r="AO5" s="54"/>
+      <c r="AP5" s="55"/>
       <c r="AQ5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AR5" s="22" t="s">
+      <c r="AR5" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="AS5" s="20"/>
-      <c r="AT5" s="20"/>
-      <c r="AU5" s="20"/>
-      <c r="AV5" s="20"/>
-      <c r="AW5" s="21"/>
+      <c r="AS5" s="54"/>
+      <c r="AT5" s="54"/>
+      <c r="AU5" s="54"/>
+      <c r="AV5" s="54"/>
+      <c r="AW5" s="55"/>
       <c r="AX5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AY5" s="22" t="s">
+      <c r="AY5" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="AZ5" s="20"/>
-      <c r="BA5" s="20"/>
-      <c r="BB5" s="21"/>
-      <c r="BC5" s="22" t="s">
+      <c r="AZ5" s="54"/>
+      <c r="BA5" s="54"/>
+      <c r="BB5" s="55"/>
+      <c r="BC5" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="BD5" s="21"/>
-      <c r="BE5" s="38"/>
-      <c r="BF5" s="37"/>
-      <c r="BG5" s="22" t="s">
+      <c r="BD5" s="55"/>
+      <c r="BE5" s="60"/>
+      <c r="BF5" s="59"/>
+      <c r="BG5" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="BH5" s="20"/>
-      <c r="BI5" s="20"/>
-      <c r="BJ5" s="20"/>
-      <c r="BK5" s="21"/>
+      <c r="BH5" s="54"/>
+      <c r="BI5" s="54"/>
+      <c r="BJ5" s="54"/>
+      <c r="BK5" s="55"/>
       <c r="BL5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="BM5" s="22" t="s">
+      <c r="BM5" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="BN5" s="20"/>
-      <c r="BO5" s="20"/>
-      <c r="BP5" s="20"/>
-      <c r="BQ5" s="20"/>
-      <c r="BR5" s="21"/>
+      <c r="BN5" s="54"/>
+      <c r="BO5" s="54"/>
+      <c r="BP5" s="54"/>
+      <c r="BQ5" s="54"/>
+      <c r="BR5" s="55"/>
       <c r="BS5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="BT5" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="BU5" s="20"/>
-      <c r="BV5" s="20"/>
-      <c r="BW5" s="20"/>
-      <c r="BX5" s="20"/>
-      <c r="BY5" s="21"/>
+      <c r="BT5" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="BU5" s="54"/>
+      <c r="BV5" s="54"/>
+      <c r="BW5" s="54"/>
+      <c r="BX5" s="54"/>
+      <c r="BY5" s="55"/>
       <c r="BZ5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="CA5" s="22" t="s">
-        <v>60</v>
-      </c>
-      <c r="CB5" s="20"/>
-      <c r="CC5" s="20"/>
-      <c r="CD5" s="20"/>
-      <c r="CE5" s="20"/>
-      <c r="CF5" s="21"/>
+      <c r="CA5" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="CB5" s="54"/>
+      <c r="CC5" s="54"/>
+      <c r="CD5" s="54"/>
+      <c r="CE5" s="54"/>
+      <c r="CF5" s="55"/>
       <c r="CG5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="CH5" s="22" t="s">
+      <c r="CH5" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="CI5" s="20"/>
-      <c r="CJ5" s="20"/>
-      <c r="CK5" s="20"/>
-      <c r="CL5" s="20"/>
-      <c r="CM5" s="21"/>
+      <c r="CI5" s="54"/>
+      <c r="CJ5" s="54"/>
+      <c r="CK5" s="54"/>
+      <c r="CL5" s="54"/>
+      <c r="CM5" s="55"/>
       <c r="CN5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="CO5" s="22" t="s">
+      <c r="CO5" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="CP5" s="20"/>
-      <c r="CQ5" s="20"/>
-      <c r="CR5" s="20"/>
-      <c r="CS5" s="20"/>
-      <c r="CT5" s="21"/>
+      <c r="CP5" s="54"/>
+      <c r="CQ5" s="54"/>
+      <c r="CR5" s="54"/>
+      <c r="CS5" s="54"/>
+      <c r="CT5" s="55"/>
       <c r="CU5" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="CV5" s="22" t="s">
+      <c r="CV5" s="53" t="s">
         <v>60</v>
       </c>
-      <c r="CW5" s="20"/>
-      <c r="CX5" s="20"/>
-      <c r="CY5" s="20"/>
-      <c r="CZ5" s="20"/>
-      <c r="DA5" s="21"/>
+      <c r="CW5" s="54"/>
+      <c r="CX5" s="54"/>
+      <c r="CY5" s="54"/>
+      <c r="CZ5" s="54"/>
+      <c r="DA5" s="55"/>
       <c r="DB5" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="DC5" s="19" t="s">
+      <c r="DC5" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="DD5" s="23"/>
-      <c r="DE5" s="23"/>
-      <c r="DF5" s="23"/>
-      <c r="DG5" s="23"/>
-      <c r="DH5" s="24"/>
+      <c r="DD5" s="70"/>
+      <c r="DE5" s="70"/>
+      <c r="DF5" s="70"/>
+      <c r="DG5" s="70"/>
+      <c r="DH5" s="71"/>
       <c r="DI5" s="17" t="s">
         <v>64</v>
       </c>
       <c r="DP5" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="DQ5" s="22" t="s">
+      <c r="DQ5" s="53" t="s">
         <v>66</v>
       </c>
-      <c r="DR5" s="20"/>
-      <c r="DS5" s="20"/>
-      <c r="DT5" s="20"/>
-      <c r="DU5" s="20"/>
-      <c r="DV5" s="21"/>
-      <c r="DW5" s="38"/>
-      <c r="DX5" s="37"/>
+      <c r="DR5" s="54"/>
+      <c r="DS5" s="54"/>
+      <c r="DT5" s="54"/>
+      <c r="DU5" s="54"/>
+      <c r="DV5" s="55"/>
+      <c r="DW5" s="60"/>
+      <c r="DX5" s="59"/>
     </row>
     <row r="6" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -3211,65 +3324,61 @@
       <c r="N6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="39" t="s">
+      <c r="V6" s="61" t="s">
         <v>24</v>
       </c>
       <c r="AC6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AK6" s="19" t="s">
+      <c r="AK6" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="AL6" s="23"/>
-      <c r="AM6" s="23"/>
-      <c r="AN6" s="23"/>
-      <c r="AO6" s="23"/>
-      <c r="AP6" s="24"/>
-      <c r="AV6" s="42" t="s">
+      <c r="AL6" s="70"/>
+      <c r="AM6" s="70"/>
+      <c r="AN6" s="70"/>
+      <c r="AO6" s="70"/>
+      <c r="AP6" s="71"/>
+      <c r="AV6" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="AW6" s="43"/>
+      <c r="AW6" s="65"/>
       <c r="AX6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AY6" s="22"/>
-      <c r="AZ6" s="20"/>
-      <c r="BA6" s="20"/>
-      <c r="BB6" s="21"/>
-      <c r="BC6" s="22" t="s">
+      <c r="AY6" s="53"/>
+      <c r="AZ6" s="54"/>
+      <c r="BA6" s="54"/>
+      <c r="BB6" s="55"/>
+      <c r="BC6" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="BD6" s="21"/>
-      <c r="BE6" s="38"/>
-      <c r="BF6" s="37"/>
-      <c r="BG6" s="22" t="s">
+      <c r="BD6" s="55"/>
+      <c r="BE6" s="60"/>
+      <c r="BF6" s="59"/>
+      <c r="BG6" s="53" t="s">
         <v>67</v>
       </c>
-      <c r="BH6" s="20"/>
-      <c r="BI6" s="20"/>
-      <c r="BJ6" s="20"/>
-      <c r="BK6" s="21"/>
-      <c r="BM6" s="22" t="s">
+      <c r="BH6" s="54"/>
+      <c r="BI6" s="54"/>
+      <c r="BJ6" s="54"/>
+      <c r="BK6" s="55"/>
+      <c r="BM6" s="53" t="s">
         <v>68</v>
       </c>
-      <c r="BN6" s="20"/>
-      <c r="BO6" s="20"/>
-      <c r="BP6" s="20"/>
-      <c r="BQ6" s="20"/>
-      <c r="BR6" s="21"/>
-      <c r="BZ6" s="71" t="s">
+      <c r="BN6" s="54"/>
+      <c r="BO6" s="54"/>
+      <c r="BP6" s="54"/>
+      <c r="BQ6" s="54"/>
+      <c r="BR6" s="55"/>
+      <c r="BZ6" s="18" t="s">
+        <v>73</v>
+      </c>
+      <c r="CG6" s="19" t="s">
+        <v>72</v>
+      </c>
+      <c r="CH6" s="72" t="s">
         <v>69</v>
       </c>
-      <c r="CA6" s="72" t="s">
-        <v>70</v>
-      </c>
-      <c r="CB6" s="73"/>
-      <c r="CC6" s="73"/>
-      <c r="CD6" s="73"/>
-      <c r="CE6" s="73"/>
-      <c r="CF6" s="73"/>
-      <c r="CG6" s="73"/>
-      <c r="CH6" s="73"/>
       <c r="CI6" s="73"/>
       <c r="CJ6" s="73"/>
       <c r="CK6" s="73"/>
@@ -3278,40 +3387,40 @@
       <c r="CN6" s="18" t="s">
         <v>57</v>
       </c>
-      <c r="CO6" s="22" t="s">
+      <c r="CO6" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="CP6" s="20"/>
-      <c r="CQ6" s="20"/>
-      <c r="CR6" s="20"/>
-      <c r="CS6" s="20"/>
-      <c r="CT6" s="21"/>
-      <c r="CV6" s="22" t="s">
+      <c r="CP6" s="54"/>
+      <c r="CQ6" s="54"/>
+      <c r="CR6" s="54"/>
+      <c r="CS6" s="54"/>
+      <c r="CT6" s="55"/>
+      <c r="CV6" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="CW6" s="20"/>
-      <c r="CX6" s="20"/>
-      <c r="CY6" s="20"/>
-      <c r="CZ6" s="20"/>
-      <c r="DA6" s="21"/>
-      <c r="DC6" s="19" t="s">
+      <c r="CW6" s="54"/>
+      <c r="CX6" s="54"/>
+      <c r="CY6" s="54"/>
+      <c r="CZ6" s="54"/>
+      <c r="DA6" s="55"/>
+      <c r="DC6" s="69" t="s">
         <v>62</v>
       </c>
-      <c r="DD6" s="20"/>
-      <c r="DE6" s="20"/>
-      <c r="DF6" s="20"/>
-      <c r="DG6" s="20"/>
-      <c r="DH6" s="21"/>
+      <c r="DD6" s="54"/>
+      <c r="DE6" s="54"/>
+      <c r="DF6" s="54"/>
+      <c r="DG6" s="54"/>
+      <c r="DH6" s="55"/>
       <c r="DI6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="DW6" s="38"/>
-      <c r="DX6" s="37"/>
+      <c r="DW6" s="60"/>
+      <c r="DX6" s="59"/>
     </row>
     <row r="7" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V7" s="40"/>
-      <c r="BF7" s="37"/>
-      <c r="DX7" s="37"/>
+      <c r="V7" s="62"/>
+      <c r="BF7" s="59"/>
+      <c r="DX7" s="59"/>
     </row>
     <row r="8" spans="1:157" s="4" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -3319,21 +3428,35 @@
       </c>
       <c r="B8" s="7">
         <f ca="1">TODAY()</f>
-        <v>44752</v>
-      </c>
-      <c r="V8" s="41"/>
+        <v>44766</v>
+      </c>
+      <c r="V8" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="DQ4:DV4"/>
-    <mergeCell ref="CO4:CT4"/>
-    <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="BG4:BL4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="DB4:DP4"/>
+  <mergeCells count="48">
+    <mergeCell ref="DC6:DH6"/>
+    <mergeCell ref="DQ5:DV5"/>
+    <mergeCell ref="DC5:DH5"/>
+    <mergeCell ref="BT5:BY5"/>
+    <mergeCell ref="CA5:CF5"/>
+    <mergeCell ref="CH5:CM5"/>
+    <mergeCell ref="CO5:CT5"/>
+    <mergeCell ref="CV5:DA5"/>
+    <mergeCell ref="BG5:BK5"/>
+    <mergeCell ref="BM5:BR5"/>
+    <mergeCell ref="CO6:CT6"/>
+    <mergeCell ref="CV6:DA6"/>
+    <mergeCell ref="W4:AW4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="AX4:BB4"/>
+    <mergeCell ref="AK6:AP6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="AD5:AI5"/>
+    <mergeCell ref="AK5:AP5"/>
+    <mergeCell ref="AR5:AW5"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BG6:BK6"/>
+    <mergeCell ref="BM6:BR6"/>
     <mergeCell ref="A1:DX2"/>
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="O5:U5"/>
@@ -3350,30 +3473,15 @@
     <mergeCell ref="AY6:BB6"/>
     <mergeCell ref="AV6:AW6"/>
     <mergeCell ref="AY5:BB5"/>
-    <mergeCell ref="BG5:BK5"/>
-    <mergeCell ref="BM5:BR5"/>
-    <mergeCell ref="CO6:CT6"/>
-    <mergeCell ref="CV6:DA6"/>
-    <mergeCell ref="W4:AW4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="AX4:BB4"/>
-    <mergeCell ref="AK6:AP6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="AD5:AI5"/>
-    <mergeCell ref="AK5:AP5"/>
-    <mergeCell ref="AR5:AW5"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BG6:BK6"/>
-    <mergeCell ref="BM6:BR6"/>
-    <mergeCell ref="CA6:CM6"/>
-    <mergeCell ref="DC6:DH6"/>
-    <mergeCell ref="DQ5:DV5"/>
-    <mergeCell ref="DC5:DH5"/>
-    <mergeCell ref="BT5:BY5"/>
-    <mergeCell ref="CA5:CF5"/>
-    <mergeCell ref="CH5:CM5"/>
-    <mergeCell ref="CO5:CT5"/>
-    <mergeCell ref="CV5:DA5"/>
+    <mergeCell ref="DQ4:DV4"/>
+    <mergeCell ref="CO4:CT4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="BG4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="DB4:DP4"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:XFD3">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Meeting log from 31 Jul 22 // timeline update
</commit_message>
<xml_diff>
--- a/Timeline/Project_Timeline.xlsx
+++ b/Timeline/Project_Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Desktop/agile/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2B3BD9E-B404-6E4C-A8E5-534FA9FCA1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF87ADA-6766-1244-AAB1-661B4A60A455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="15920" yWindow="4020" windowWidth="28800" windowHeight="22140" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
   <si>
     <t>ASP - Group Project</t>
   </si>
@@ -1274,6 +1274,90 @@
       <t>Unable to achieve this timeline, review next week</t>
     </r>
   </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>continue devleopment as per the team meeting</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Update no team meeting - continue development as per the Slack channel</t>
+    </r>
+  </si>
+  <si>
+    <t>Duties as per the team meeting 
+Aim for the MVP to be complete at the end of this period.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">DEVELOPMENT CONTINGENCY PERIOD
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">IF TIME PERMITS … </t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">
+Add in more features to the software
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>If MVP NOT CREATED
+Continue with MVP development as a contingency period</t>
+    </r>
+  </si>
 </sst>
 </file>
 
@@ -1282,7 +1366,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="15" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1361,6 +1445,35 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri (Body)"/>
     </font>
   </fonts>
   <fills count="27">
@@ -1684,7 +1797,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="75">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1740,172 +1853,175 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2263,8 +2379,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3400B0-A312-474B-BDD8-7EBBB1942BA5}">
   <dimension ref="A1:FA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CE2" workbookViewId="0">
-      <selection activeCell="CB6" sqref="CB6"/>
+    <sheetView tabSelected="1" topLeftCell="CZ1" workbookViewId="0">
+      <selection activeCell="CO5" sqref="CO5:CT5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2273,266 +2389,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AI1" s="48"/>
-      <c r="AJ1" s="48"/>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="48"/>
-      <c r="AN1" s="48"/>
-      <c r="AO1" s="48"/>
-      <c r="AP1" s="48"/>
-      <c r="AQ1" s="48"/>
-      <c r="AR1" s="48"/>
-      <c r="AS1" s="48"/>
-      <c r="AT1" s="48"/>
-      <c r="AU1" s="48"/>
-      <c r="AV1" s="48"/>
-      <c r="AW1" s="48"/>
-      <c r="AX1" s="48"/>
-      <c r="AY1" s="48"/>
-      <c r="AZ1" s="48"/>
-      <c r="BA1" s="48"/>
-      <c r="BB1" s="48"/>
-      <c r="BC1" s="48"/>
-      <c r="BD1" s="48"/>
-      <c r="BE1" s="48"/>
-      <c r="BF1" s="48"/>
-      <c r="BG1" s="48"/>
-      <c r="BH1" s="48"/>
-      <c r="BI1" s="48"/>
-      <c r="BJ1" s="48"/>
-      <c r="BK1" s="48"/>
-      <c r="BL1" s="48"/>
-      <c r="BM1" s="48"/>
-      <c r="BN1" s="48"/>
-      <c r="BO1" s="48"/>
-      <c r="BP1" s="48"/>
-      <c r="BQ1" s="48"/>
-      <c r="BR1" s="48"/>
-      <c r="BS1" s="48"/>
-      <c r="BT1" s="48"/>
-      <c r="BU1" s="48"/>
-      <c r="BV1" s="48"/>
-      <c r="BW1" s="48"/>
-      <c r="BX1" s="48"/>
-      <c r="BY1" s="48"/>
-      <c r="BZ1" s="48"/>
-      <c r="CA1" s="48"/>
-      <c r="CB1" s="48"/>
-      <c r="CC1" s="48"/>
-      <c r="CD1" s="48"/>
-      <c r="CE1" s="48"/>
-      <c r="CF1" s="48"/>
-      <c r="CG1" s="48"/>
-      <c r="CH1" s="48"/>
-      <c r="CI1" s="48"/>
-      <c r="CJ1" s="48"/>
-      <c r="CK1" s="48"/>
-      <c r="CL1" s="48"/>
-      <c r="CM1" s="48"/>
-      <c r="CN1" s="48"/>
-      <c r="CO1" s="48"/>
-      <c r="CP1" s="48"/>
-      <c r="CQ1" s="48"/>
-      <c r="CR1" s="48"/>
-      <c r="CS1" s="48"/>
-      <c r="CT1" s="48"/>
-      <c r="CU1" s="48"/>
-      <c r="CV1" s="48"/>
-      <c r="CW1" s="48"/>
-      <c r="CX1" s="48"/>
-      <c r="CY1" s="48"/>
-      <c r="CZ1" s="48"/>
-      <c r="DA1" s="48"/>
-      <c r="DB1" s="48"/>
-      <c r="DC1" s="48"/>
-      <c r="DD1" s="48"/>
-      <c r="DE1" s="48"/>
-      <c r="DF1" s="48"/>
-      <c r="DG1" s="48"/>
-      <c r="DH1" s="48"/>
-      <c r="DI1" s="48"/>
-      <c r="DJ1" s="48"/>
-      <c r="DK1" s="48"/>
-      <c r="DL1" s="48"/>
-      <c r="DM1" s="48"/>
-      <c r="DN1" s="48"/>
-      <c r="DO1" s="48"/>
-      <c r="DP1" s="48"/>
-      <c r="DQ1" s="48"/>
-      <c r="DR1" s="48"/>
-      <c r="DS1" s="48"/>
-      <c r="DT1" s="48"/>
-      <c r="DU1" s="48"/>
-      <c r="DV1" s="48"/>
-      <c r="DW1" s="48"/>
-      <c r="DX1" s="49"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
+      <c r="Y1" s="29"/>
+      <c r="Z1" s="29"/>
+      <c r="AA1" s="29"/>
+      <c r="AB1" s="29"/>
+      <c r="AC1" s="29"/>
+      <c r="AD1" s="29"/>
+      <c r="AE1" s="29"/>
+      <c r="AF1" s="29"/>
+      <c r="AG1" s="29"/>
+      <c r="AH1" s="29"/>
+      <c r="AI1" s="29"/>
+      <c r="AJ1" s="29"/>
+      <c r="AK1" s="29"/>
+      <c r="AL1" s="29"/>
+      <c r="AM1" s="29"/>
+      <c r="AN1" s="29"/>
+      <c r="AO1" s="29"/>
+      <c r="AP1" s="29"/>
+      <c r="AQ1" s="29"/>
+      <c r="AR1" s="29"/>
+      <c r="AS1" s="29"/>
+      <c r="AT1" s="29"/>
+      <c r="AU1" s="29"/>
+      <c r="AV1" s="29"/>
+      <c r="AW1" s="29"/>
+      <c r="AX1" s="29"/>
+      <c r="AY1" s="29"/>
+      <c r="AZ1" s="29"/>
+      <c r="BA1" s="29"/>
+      <c r="BB1" s="29"/>
+      <c r="BC1" s="29"/>
+      <c r="BD1" s="29"/>
+      <c r="BE1" s="29"/>
+      <c r="BF1" s="29"/>
+      <c r="BG1" s="29"/>
+      <c r="BH1" s="29"/>
+      <c r="BI1" s="29"/>
+      <c r="BJ1" s="29"/>
+      <c r="BK1" s="29"/>
+      <c r="BL1" s="29"/>
+      <c r="BM1" s="29"/>
+      <c r="BN1" s="29"/>
+      <c r="BO1" s="29"/>
+      <c r="BP1" s="29"/>
+      <c r="BQ1" s="29"/>
+      <c r="BR1" s="29"/>
+      <c r="BS1" s="29"/>
+      <c r="BT1" s="29"/>
+      <c r="BU1" s="29"/>
+      <c r="BV1" s="29"/>
+      <c r="BW1" s="29"/>
+      <c r="BX1" s="29"/>
+      <c r="BY1" s="29"/>
+      <c r="BZ1" s="29"/>
+      <c r="CA1" s="29"/>
+      <c r="CB1" s="29"/>
+      <c r="CC1" s="29"/>
+      <c r="CD1" s="29"/>
+      <c r="CE1" s="29"/>
+      <c r="CF1" s="29"/>
+      <c r="CG1" s="29"/>
+      <c r="CH1" s="29"/>
+      <c r="CI1" s="29"/>
+      <c r="CJ1" s="29"/>
+      <c r="CK1" s="29"/>
+      <c r="CL1" s="29"/>
+      <c r="CM1" s="29"/>
+      <c r="CN1" s="29"/>
+      <c r="CO1" s="29"/>
+      <c r="CP1" s="29"/>
+      <c r="CQ1" s="29"/>
+      <c r="CR1" s="29"/>
+      <c r="CS1" s="29"/>
+      <c r="CT1" s="29"/>
+      <c r="CU1" s="29"/>
+      <c r="CV1" s="29"/>
+      <c r="CW1" s="29"/>
+      <c r="CX1" s="29"/>
+      <c r="CY1" s="29"/>
+      <c r="CZ1" s="29"/>
+      <c r="DA1" s="29"/>
+      <c r="DB1" s="29"/>
+      <c r="DC1" s="29"/>
+      <c r="DD1" s="29"/>
+      <c r="DE1" s="29"/>
+      <c r="DF1" s="29"/>
+      <c r="DG1" s="29"/>
+      <c r="DH1" s="29"/>
+      <c r="DI1" s="29"/>
+      <c r="DJ1" s="29"/>
+      <c r="DK1" s="29"/>
+      <c r="DL1" s="29"/>
+      <c r="DM1" s="29"/>
+      <c r="DN1" s="29"/>
+      <c r="DO1" s="29"/>
+      <c r="DP1" s="29"/>
+      <c r="DQ1" s="29"/>
+      <c r="DR1" s="29"/>
+      <c r="DS1" s="29"/>
+      <c r="DT1" s="29"/>
+      <c r="DU1" s="29"/>
+      <c r="DV1" s="29"/>
+      <c r="DW1" s="29"/>
+      <c r="DX1" s="30"/>
     </row>
     <row r="2" spans="1:157" s="4" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
-      <c r="AF2" s="51"/>
-      <c r="AG2" s="51"/>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
-      <c r="AW2" s="51"/>
-      <c r="AX2" s="51"/>
-      <c r="AY2" s="51"/>
-      <c r="AZ2" s="51"/>
-      <c r="BA2" s="51"/>
-      <c r="BB2" s="51"/>
-      <c r="BC2" s="51"/>
-      <c r="BD2" s="51"/>
-      <c r="BE2" s="51"/>
-      <c r="BF2" s="51"/>
-      <c r="BG2" s="51"/>
-      <c r="BH2" s="51"/>
-      <c r="BI2" s="51"/>
-      <c r="BJ2" s="51"/>
-      <c r="BK2" s="51"/>
-      <c r="BL2" s="51"/>
-      <c r="BM2" s="51"/>
-      <c r="BN2" s="51"/>
-      <c r="BO2" s="51"/>
-      <c r="BP2" s="51"/>
-      <c r="BQ2" s="51"/>
-      <c r="BR2" s="51"/>
-      <c r="BS2" s="51"/>
-      <c r="BT2" s="51"/>
-      <c r="BU2" s="51"/>
-      <c r="BV2" s="51"/>
-      <c r="BW2" s="51"/>
-      <c r="BX2" s="51"/>
-      <c r="BY2" s="51"/>
-      <c r="BZ2" s="51"/>
-      <c r="CA2" s="51"/>
-      <c r="CB2" s="51"/>
-      <c r="CC2" s="51"/>
-      <c r="CD2" s="51"/>
-      <c r="CE2" s="51"/>
-      <c r="CF2" s="51"/>
-      <c r="CG2" s="51"/>
-      <c r="CH2" s="51"/>
-      <c r="CI2" s="51"/>
-      <c r="CJ2" s="51"/>
-      <c r="CK2" s="51"/>
-      <c r="CL2" s="51"/>
-      <c r="CM2" s="51"/>
-      <c r="CN2" s="51"/>
-      <c r="CO2" s="51"/>
-      <c r="CP2" s="51"/>
-      <c r="CQ2" s="51"/>
-      <c r="CR2" s="51"/>
-      <c r="CS2" s="51"/>
-      <c r="CT2" s="51"/>
-      <c r="CU2" s="51"/>
-      <c r="CV2" s="51"/>
-      <c r="CW2" s="51"/>
-      <c r="CX2" s="51"/>
-      <c r="CY2" s="51"/>
-      <c r="CZ2" s="51"/>
-      <c r="DA2" s="51"/>
-      <c r="DB2" s="51"/>
-      <c r="DC2" s="51"/>
-      <c r="DD2" s="51"/>
-      <c r="DE2" s="51"/>
-      <c r="DF2" s="51"/>
-      <c r="DG2" s="51"/>
-      <c r="DH2" s="51"/>
-      <c r="DI2" s="51"/>
-      <c r="DJ2" s="51"/>
-      <c r="DK2" s="51"/>
-      <c r="DL2" s="51"/>
-      <c r="DM2" s="51"/>
-      <c r="DN2" s="51"/>
-      <c r="DO2" s="51"/>
-      <c r="DP2" s="51"/>
-      <c r="DQ2" s="51"/>
-      <c r="DR2" s="51"/>
-      <c r="DS2" s="51"/>
-      <c r="DT2" s="51"/>
-      <c r="DU2" s="51"/>
-      <c r="DV2" s="51"/>
-      <c r="DW2" s="51"/>
-      <c r="DX2" s="52"/>
+      <c r="A2" s="31"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
+      <c r="G2" s="32"/>
+      <c r="H2" s="32"/>
+      <c r="I2" s="32"/>
+      <c r="J2" s="32"/>
+      <c r="K2" s="32"/>
+      <c r="L2" s="32"/>
+      <c r="M2" s="32"/>
+      <c r="N2" s="32"/>
+      <c r="O2" s="32"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="32"/>
+      <c r="R2" s="32"/>
+      <c r="S2" s="32"/>
+      <c r="T2" s="32"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="32"/>
+      <c r="W2" s="32"/>
+      <c r="X2" s="32"/>
+      <c r="Y2" s="32"/>
+      <c r="Z2" s="32"/>
+      <c r="AA2" s="32"/>
+      <c r="AB2" s="32"/>
+      <c r="AC2" s="32"/>
+      <c r="AD2" s="32"/>
+      <c r="AE2" s="32"/>
+      <c r="AF2" s="32"/>
+      <c r="AG2" s="32"/>
+      <c r="AH2" s="32"/>
+      <c r="AI2" s="32"/>
+      <c r="AJ2" s="32"/>
+      <c r="AK2" s="32"/>
+      <c r="AL2" s="32"/>
+      <c r="AM2" s="32"/>
+      <c r="AN2" s="32"/>
+      <c r="AO2" s="32"/>
+      <c r="AP2" s="32"/>
+      <c r="AQ2" s="32"/>
+      <c r="AR2" s="32"/>
+      <c r="AS2" s="32"/>
+      <c r="AT2" s="32"/>
+      <c r="AU2" s="32"/>
+      <c r="AV2" s="32"/>
+      <c r="AW2" s="32"/>
+      <c r="AX2" s="32"/>
+      <c r="AY2" s="32"/>
+      <c r="AZ2" s="32"/>
+      <c r="BA2" s="32"/>
+      <c r="BB2" s="32"/>
+      <c r="BC2" s="32"/>
+      <c r="BD2" s="32"/>
+      <c r="BE2" s="32"/>
+      <c r="BF2" s="32"/>
+      <c r="BG2" s="32"/>
+      <c r="BH2" s="32"/>
+      <c r="BI2" s="32"/>
+      <c r="BJ2" s="32"/>
+      <c r="BK2" s="32"/>
+      <c r="BL2" s="32"/>
+      <c r="BM2" s="32"/>
+      <c r="BN2" s="32"/>
+      <c r="BO2" s="32"/>
+      <c r="BP2" s="32"/>
+      <c r="BQ2" s="32"/>
+      <c r="BR2" s="32"/>
+      <c r="BS2" s="32"/>
+      <c r="BT2" s="32"/>
+      <c r="BU2" s="32"/>
+      <c r="BV2" s="32"/>
+      <c r="BW2" s="32"/>
+      <c r="BX2" s="32"/>
+      <c r="BY2" s="32"/>
+      <c r="BZ2" s="32"/>
+      <c r="CA2" s="32"/>
+      <c r="CB2" s="32"/>
+      <c r="CC2" s="32"/>
+      <c r="CD2" s="32"/>
+      <c r="CE2" s="32"/>
+      <c r="CF2" s="32"/>
+      <c r="CG2" s="32"/>
+      <c r="CH2" s="32"/>
+      <c r="CI2" s="32"/>
+      <c r="CJ2" s="32"/>
+      <c r="CK2" s="32"/>
+      <c r="CL2" s="32"/>
+      <c r="CM2" s="32"/>
+      <c r="CN2" s="32"/>
+      <c r="CO2" s="32"/>
+      <c r="CP2" s="32"/>
+      <c r="CQ2" s="32"/>
+      <c r="CR2" s="32"/>
+      <c r="CS2" s="32"/>
+      <c r="CT2" s="32"/>
+      <c r="CU2" s="32"/>
+      <c r="CV2" s="32"/>
+      <c r="CW2" s="32"/>
+      <c r="CX2" s="32"/>
+      <c r="CY2" s="32"/>
+      <c r="CZ2" s="32"/>
+      <c r="DA2" s="32"/>
+      <c r="DB2" s="32"/>
+      <c r="DC2" s="32"/>
+      <c r="DD2" s="32"/>
+      <c r="DE2" s="32"/>
+      <c r="DF2" s="32"/>
+      <c r="DG2" s="32"/>
+      <c r="DH2" s="32"/>
+      <c r="DI2" s="32"/>
+      <c r="DJ2" s="32"/>
+      <c r="DK2" s="32"/>
+      <c r="DL2" s="32"/>
+      <c r="DM2" s="32"/>
+      <c r="DN2" s="32"/>
+      <c r="DO2" s="32"/>
+      <c r="DP2" s="32"/>
+      <c r="DQ2" s="32"/>
+      <c r="DR2" s="32"/>
+      <c r="DS2" s="32"/>
+      <c r="DT2" s="32"/>
+      <c r="DU2" s="32"/>
+      <c r="DV2" s="32"/>
+      <c r="DW2" s="32"/>
+      <c r="DX2" s="33"/>
     </row>
     <row r="3" spans="1:157" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2924,169 +3040,169 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="34" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="58" t="s">
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58" t="s">
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="66" t="s">
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="66"/>
-      <c r="Z4" s="66"/>
-      <c r="AA4" s="66"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="66"/>
-      <c r="AD4" s="66"/>
-      <c r="AE4" s="66"/>
-      <c r="AF4" s="66"/>
-      <c r="AG4" s="66"/>
-      <c r="AH4" s="66"/>
-      <c r="AI4" s="66"/>
-      <c r="AJ4" s="66"/>
-      <c r="AK4" s="66"/>
-      <c r="AL4" s="66"/>
-      <c r="AM4" s="66"/>
-      <c r="AN4" s="66"/>
-      <c r="AO4" s="66"/>
-      <c r="AP4" s="66"/>
-      <c r="AQ4" s="66"/>
-      <c r="AR4" s="66"/>
-      <c r="AS4" s="66"/>
-      <c r="AT4" s="66"/>
-      <c r="AU4" s="66"/>
-      <c r="AV4" s="66"/>
-      <c r="AW4" s="66"/>
-      <c r="AX4" s="68" t="s">
+      <c r="X4" s="25"/>
+      <c r="Y4" s="25"/>
+      <c r="Z4" s="25"/>
+      <c r="AA4" s="25"/>
+      <c r="AB4" s="25"/>
+      <c r="AC4" s="25"/>
+      <c r="AD4" s="25"/>
+      <c r="AE4" s="25"/>
+      <c r="AF4" s="25"/>
+      <c r="AG4" s="25"/>
+      <c r="AH4" s="25"/>
+      <c r="AI4" s="25"/>
+      <c r="AJ4" s="25"/>
+      <c r="AK4" s="25"/>
+      <c r="AL4" s="25"/>
+      <c r="AM4" s="25"/>
+      <c r="AN4" s="25"/>
+      <c r="AO4" s="25"/>
+      <c r="AP4" s="25"/>
+      <c r="AQ4" s="25"/>
+      <c r="AR4" s="25"/>
+      <c r="AS4" s="25"/>
+      <c r="AT4" s="25"/>
+      <c r="AU4" s="25"/>
+      <c r="AV4" s="25"/>
+      <c r="AW4" s="25"/>
+      <c r="AX4" s="27" t="s">
         <v>16</v>
       </c>
-      <c r="AY4" s="68"/>
-      <c r="AZ4" s="68"/>
-      <c r="BA4" s="68"/>
-      <c r="BB4" s="68"/>
-      <c r="BC4" s="67" t="s">
+      <c r="AY4" s="27"/>
+      <c r="AZ4" s="27"/>
+      <c r="BA4" s="27"/>
+      <c r="BB4" s="27"/>
+      <c r="BC4" s="26" t="s">
         <v>17</v>
       </c>
-      <c r="BD4" s="67"/>
-      <c r="BE4" s="60" t="s">
+      <c r="BD4" s="26"/>
+      <c r="BE4" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="BF4" s="59" t="s">
+      <c r="BF4" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="BG4" s="29" t="s">
+      <c r="BG4" s="53" t="s">
         <v>40</v>
       </c>
-      <c r="BH4" s="30"/>
-      <c r="BI4" s="30"/>
-      <c r="BJ4" s="30"/>
-      <c r="BK4" s="30"/>
-      <c r="BL4" s="31"/>
-      <c r="BM4" s="32" t="s">
+      <c r="BH4" s="54"/>
+      <c r="BI4" s="54"/>
+      <c r="BJ4" s="54"/>
+      <c r="BK4" s="54"/>
+      <c r="BL4" s="55"/>
+      <c r="BM4" s="56" t="s">
         <v>41</v>
       </c>
-      <c r="BN4" s="33"/>
-      <c r="BO4" s="33"/>
-      <c r="BP4" s="33"/>
-      <c r="BQ4" s="33"/>
-      <c r="BR4" s="33"/>
-      <c r="BS4" s="34"/>
-      <c r="BT4" s="35" t="s">
+      <c r="BN4" s="57"/>
+      <c r="BO4" s="57"/>
+      <c r="BP4" s="57"/>
+      <c r="BQ4" s="57"/>
+      <c r="BR4" s="57"/>
+      <c r="BS4" s="58"/>
+      <c r="BT4" s="59" t="s">
         <v>42</v>
       </c>
-      <c r="BU4" s="36"/>
-      <c r="BV4" s="36"/>
-      <c r="BW4" s="36"/>
-      <c r="BX4" s="36"/>
-      <c r="BY4" s="36"/>
-      <c r="BZ4" s="37"/>
-      <c r="CA4" s="38" t="s">
+      <c r="BU4" s="60"/>
+      <c r="BV4" s="60"/>
+      <c r="BW4" s="60"/>
+      <c r="BX4" s="60"/>
+      <c r="BY4" s="60"/>
+      <c r="BZ4" s="61"/>
+      <c r="CA4" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="CB4" s="39"/>
-      <c r="CC4" s="39"/>
-      <c r="CD4" s="39"/>
-      <c r="CE4" s="39"/>
-      <c r="CF4" s="39"/>
-      <c r="CG4" s="40"/>
-      <c r="CH4" s="41" t="s">
+      <c r="CB4" s="63"/>
+      <c r="CC4" s="63"/>
+      <c r="CD4" s="63"/>
+      <c r="CE4" s="63"/>
+      <c r="CF4" s="63"/>
+      <c r="CG4" s="64"/>
+      <c r="CH4" s="65" t="s">
         <v>44</v>
       </c>
-      <c r="CI4" s="42"/>
-      <c r="CJ4" s="42"/>
-      <c r="CK4" s="42"/>
-      <c r="CL4" s="42"/>
-      <c r="CM4" s="42"/>
-      <c r="CN4" s="43"/>
-      <c r="CO4" s="23" t="s">
+      <c r="CI4" s="66"/>
+      <c r="CJ4" s="66"/>
+      <c r="CK4" s="66"/>
+      <c r="CL4" s="66"/>
+      <c r="CM4" s="66"/>
+      <c r="CN4" s="67"/>
+      <c r="CO4" s="47" t="s">
         <v>46</v>
       </c>
-      <c r="CP4" s="24"/>
-      <c r="CQ4" s="24"/>
-      <c r="CR4" s="24"/>
-      <c r="CS4" s="24"/>
-      <c r="CT4" s="25"/>
-      <c r="CU4" s="26" t="s">
+      <c r="CP4" s="48"/>
+      <c r="CQ4" s="48"/>
+      <c r="CR4" s="48"/>
+      <c r="CS4" s="48"/>
+      <c r="CT4" s="49"/>
+      <c r="CU4" s="50" t="s">
         <v>47</v>
       </c>
-      <c r="CV4" s="27"/>
-      <c r="CW4" s="27"/>
-      <c r="CX4" s="27"/>
-      <c r="CY4" s="27"/>
-      <c r="CZ4" s="27"/>
-      <c r="DA4" s="28"/>
-      <c r="DB4" s="44" t="s">
+      <c r="CV4" s="51"/>
+      <c r="CW4" s="51"/>
+      <c r="CX4" s="51"/>
+      <c r="CY4" s="51"/>
+      <c r="CZ4" s="51"/>
+      <c r="DA4" s="52"/>
+      <c r="DB4" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="DC4" s="45"/>
-      <c r="DD4" s="45"/>
-      <c r="DE4" s="45"/>
-      <c r="DF4" s="45"/>
-      <c r="DG4" s="45"/>
-      <c r="DH4" s="45"/>
-      <c r="DI4" s="45"/>
-      <c r="DJ4" s="45"/>
-      <c r="DK4" s="45"/>
-      <c r="DL4" s="45"/>
-      <c r="DM4" s="45"/>
-      <c r="DN4" s="45"/>
-      <c r="DO4" s="45"/>
-      <c r="DP4" s="46"/>
-      <c r="DQ4" s="20" t="s">
+      <c r="DC4" s="69"/>
+      <c r="DD4" s="69"/>
+      <c r="DE4" s="69"/>
+      <c r="DF4" s="69"/>
+      <c r="DG4" s="69"/>
+      <c r="DH4" s="69"/>
+      <c r="DI4" s="69"/>
+      <c r="DJ4" s="69"/>
+      <c r="DK4" s="69"/>
+      <c r="DL4" s="69"/>
+      <c r="DM4" s="69"/>
+      <c r="DN4" s="69"/>
+      <c r="DO4" s="69"/>
+      <c r="DP4" s="70"/>
+      <c r="DQ4" s="44" t="s">
         <v>45</v>
       </c>
-      <c r="DR4" s="21"/>
-      <c r="DS4" s="21"/>
-      <c r="DT4" s="21"/>
-      <c r="DU4" s="21"/>
-      <c r="DV4" s="22"/>
-      <c r="DW4" s="60" t="s">
+      <c r="DR4" s="45"/>
+      <c r="DS4" s="45"/>
+      <c r="DT4" s="45"/>
+      <c r="DU4" s="45"/>
+      <c r="DV4" s="46"/>
+      <c r="DW4" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="DX4" s="59" t="s">
+      <c r="DX4" s="37" t="s">
         <v>12</v>
       </c>
       <c r="DY4" s="5"/>
@@ -3126,193 +3242,193 @@
       <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="55"/>
+      <c r="J5" s="20"/>
+      <c r="K5" s="20"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="21"/>
       <c r="N5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="53" t="s">
+      <c r="O5" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="55"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="20"/>
+      <c r="T5" s="20"/>
+      <c r="U5" s="21"/>
       <c r="V5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="53" t="s">
+      <c r="W5" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="55"/>
+      <c r="X5" s="20"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="21"/>
       <c r="AC5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="53" t="s">
+      <c r="AD5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="AE5" s="54"/>
-      <c r="AF5" s="54"/>
-      <c r="AG5" s="54"/>
-      <c r="AH5" s="54"/>
-      <c r="AI5" s="55"/>
+      <c r="AE5" s="20"/>
+      <c r="AF5" s="20"/>
+      <c r="AG5" s="20"/>
+      <c r="AH5" s="20"/>
+      <c r="AI5" s="21"/>
       <c r="AJ5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AK5" s="53" t="s">
+      <c r="AK5" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="AL5" s="54"/>
-      <c r="AM5" s="54"/>
-      <c r="AN5" s="54"/>
-      <c r="AO5" s="54"/>
-      <c r="AP5" s="55"/>
+      <c r="AL5" s="20"/>
+      <c r="AM5" s="20"/>
+      <c r="AN5" s="20"/>
+      <c r="AO5" s="20"/>
+      <c r="AP5" s="21"/>
       <c r="AQ5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AR5" s="53" t="s">
+      <c r="AR5" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="AS5" s="54"/>
-      <c r="AT5" s="54"/>
-      <c r="AU5" s="54"/>
-      <c r="AV5" s="54"/>
-      <c r="AW5" s="55"/>
+      <c r="AS5" s="20"/>
+      <c r="AT5" s="20"/>
+      <c r="AU5" s="20"/>
+      <c r="AV5" s="20"/>
+      <c r="AW5" s="21"/>
       <c r="AX5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AY5" s="53" t="s">
+      <c r="AY5" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="AZ5" s="54"/>
-      <c r="BA5" s="54"/>
-      <c r="BB5" s="55"/>
-      <c r="BC5" s="53" t="s">
+      <c r="AZ5" s="20"/>
+      <c r="BA5" s="20"/>
+      <c r="BB5" s="21"/>
+      <c r="BC5" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="BD5" s="55"/>
-      <c r="BE5" s="60"/>
-      <c r="BF5" s="59"/>
-      <c r="BG5" s="53" t="s">
+      <c r="BD5" s="21"/>
+      <c r="BE5" s="38"/>
+      <c r="BF5" s="37"/>
+      <c r="BG5" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="BH5" s="54"/>
-      <c r="BI5" s="54"/>
-      <c r="BJ5" s="54"/>
-      <c r="BK5" s="55"/>
+      <c r="BH5" s="20"/>
+      <c r="BI5" s="20"/>
+      <c r="BJ5" s="20"/>
+      <c r="BK5" s="21"/>
       <c r="BL5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="BM5" s="53" t="s">
+      <c r="BM5" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="BN5" s="54"/>
-      <c r="BO5" s="54"/>
-      <c r="BP5" s="54"/>
-      <c r="BQ5" s="54"/>
-      <c r="BR5" s="55"/>
+      <c r="BN5" s="20"/>
+      <c r="BO5" s="20"/>
+      <c r="BP5" s="20"/>
+      <c r="BQ5" s="20"/>
+      <c r="BR5" s="21"/>
       <c r="BS5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="BT5" s="53" t="s">
+      <c r="BT5" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="BU5" s="54"/>
-      <c r="BV5" s="54"/>
-      <c r="BW5" s="54"/>
-      <c r="BX5" s="54"/>
-      <c r="BY5" s="55"/>
+      <c r="BU5" s="20"/>
+      <c r="BV5" s="20"/>
+      <c r="BW5" s="20"/>
+      <c r="BX5" s="20"/>
+      <c r="BY5" s="21"/>
       <c r="BZ5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="CA5" s="53" t="s">
+      <c r="CA5" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="CB5" s="54"/>
-      <c r="CC5" s="54"/>
-      <c r="CD5" s="54"/>
-      <c r="CE5" s="54"/>
-      <c r="CF5" s="55"/>
+      <c r="CB5" s="20"/>
+      <c r="CC5" s="20"/>
+      <c r="CD5" s="20"/>
+      <c r="CE5" s="20"/>
+      <c r="CF5" s="21"/>
       <c r="CG5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="CH5" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="CI5" s="54"/>
-      <c r="CJ5" s="54"/>
-      <c r="CK5" s="54"/>
-      <c r="CL5" s="54"/>
-      <c r="CM5" s="55"/>
+      <c r="CH5" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="CI5" s="20"/>
+      <c r="CJ5" s="20"/>
+      <c r="CK5" s="20"/>
+      <c r="CL5" s="20"/>
+      <c r="CM5" s="21"/>
       <c r="CN5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="CO5" s="53" t="s">
-        <v>60</v>
-      </c>
-      <c r="CP5" s="54"/>
-      <c r="CQ5" s="54"/>
-      <c r="CR5" s="54"/>
-      <c r="CS5" s="54"/>
-      <c r="CT5" s="55"/>
+      <c r="CO5" s="22" t="s">
+        <v>75</v>
+      </c>
+      <c r="CP5" s="20"/>
+      <c r="CQ5" s="20"/>
+      <c r="CR5" s="20"/>
+      <c r="CS5" s="20"/>
+      <c r="CT5" s="21"/>
       <c r="CU5" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="CV5" s="53" t="s">
+      <c r="CV5" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="CW5" s="54"/>
-      <c r="CX5" s="54"/>
-      <c r="CY5" s="54"/>
-      <c r="CZ5" s="54"/>
-      <c r="DA5" s="55"/>
+      <c r="CW5" s="20"/>
+      <c r="CX5" s="20"/>
+      <c r="CY5" s="20"/>
+      <c r="CZ5" s="20"/>
+      <c r="DA5" s="21"/>
       <c r="DB5" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="DC5" s="69" t="s">
+      <c r="DC5" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="DD5" s="70"/>
-      <c r="DE5" s="70"/>
-      <c r="DF5" s="70"/>
-      <c r="DG5" s="70"/>
-      <c r="DH5" s="71"/>
+      <c r="DD5" s="23"/>
+      <c r="DE5" s="23"/>
+      <c r="DF5" s="23"/>
+      <c r="DG5" s="23"/>
+      <c r="DH5" s="24"/>
       <c r="DI5" s="17" t="s">
         <v>64</v>
       </c>
       <c r="DP5" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="DQ5" s="53" t="s">
+      <c r="DQ5" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="DR5" s="54"/>
-      <c r="DS5" s="54"/>
-      <c r="DT5" s="54"/>
-      <c r="DU5" s="54"/>
-      <c r="DV5" s="55"/>
-      <c r="DW5" s="60"/>
-      <c r="DX5" s="59"/>
+      <c r="DR5" s="20"/>
+      <c r="DS5" s="20"/>
+      <c r="DT5" s="20"/>
+      <c r="DU5" s="20"/>
+      <c r="DV5" s="21"/>
+      <c r="DW5" s="38"/>
+      <c r="DX5" s="37"/>
     </row>
     <row r="6" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -3324,56 +3440,56 @@
       <c r="N6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="61" t="s">
+      <c r="V6" s="39" t="s">
         <v>24</v>
       </c>
       <c r="AC6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AK6" s="69" t="s">
+      <c r="AK6" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="AL6" s="70"/>
-      <c r="AM6" s="70"/>
-      <c r="AN6" s="70"/>
-      <c r="AO6" s="70"/>
-      <c r="AP6" s="71"/>
-      <c r="AV6" s="64" t="s">
+      <c r="AL6" s="23"/>
+      <c r="AM6" s="23"/>
+      <c r="AN6" s="23"/>
+      <c r="AO6" s="23"/>
+      <c r="AP6" s="24"/>
+      <c r="AV6" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="AW6" s="65"/>
+      <c r="AW6" s="43"/>
       <c r="AX6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AY6" s="53"/>
-      <c r="AZ6" s="54"/>
-      <c r="BA6" s="54"/>
-      <c r="BB6" s="55"/>
-      <c r="BC6" s="53" t="s">
+      <c r="AY6" s="22"/>
+      <c r="AZ6" s="20"/>
+      <c r="BA6" s="20"/>
+      <c r="BB6" s="21"/>
+      <c r="BC6" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="BD6" s="55"/>
-      <c r="BE6" s="60"/>
-      <c r="BF6" s="59"/>
-      <c r="BG6" s="53" t="s">
+      <c r="BD6" s="21"/>
+      <c r="BE6" s="38"/>
+      <c r="BF6" s="37"/>
+      <c r="BG6" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="BH6" s="54"/>
-      <c r="BI6" s="54"/>
-      <c r="BJ6" s="54"/>
-      <c r="BK6" s="55"/>
-      <c r="BM6" s="53" t="s">
+      <c r="BH6" s="20"/>
+      <c r="BI6" s="20"/>
+      <c r="BJ6" s="20"/>
+      <c r="BK6" s="21"/>
+      <c r="BM6" s="22" t="s">
         <v>68</v>
       </c>
-      <c r="BN6" s="54"/>
-      <c r="BO6" s="54"/>
-      <c r="BP6" s="54"/>
-      <c r="BQ6" s="54"/>
-      <c r="BR6" s="55"/>
+      <c r="BN6" s="20"/>
+      <c r="BO6" s="20"/>
+      <c r="BP6" s="20"/>
+      <c r="BQ6" s="20"/>
+      <c r="BR6" s="21"/>
       <c r="BZ6" s="18" t="s">
         <v>73</v>
       </c>
-      <c r="CG6" s="19" t="s">
+      <c r="CG6" s="71" t="s">
         <v>72</v>
       </c>
       <c r="CH6" s="72" t="s">
@@ -3384,43 +3500,43 @@
       <c r="CK6" s="73"/>
       <c r="CL6" s="73"/>
       <c r="CM6" s="74"/>
-      <c r="CN6" s="18" t="s">
+      <c r="CN6" s="75" t="s">
         <v>57</v>
       </c>
-      <c r="CO6" s="53" t="s">
+      <c r="CO6" s="22" t="s">
+        <v>76</v>
+      </c>
+      <c r="CP6" s="20"/>
+      <c r="CQ6" s="20"/>
+      <c r="CR6" s="20"/>
+      <c r="CS6" s="20"/>
+      <c r="CT6" s="21"/>
+      <c r="CV6" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="CP6" s="54"/>
-      <c r="CQ6" s="54"/>
-      <c r="CR6" s="54"/>
-      <c r="CS6" s="54"/>
-      <c r="CT6" s="55"/>
-      <c r="CV6" s="53" t="s">
-        <v>61</v>
-      </c>
-      <c r="CW6" s="54"/>
-      <c r="CX6" s="54"/>
-      <c r="CY6" s="54"/>
-      <c r="CZ6" s="54"/>
-      <c r="DA6" s="55"/>
-      <c r="DC6" s="69" t="s">
+      <c r="CW6" s="20"/>
+      <c r="CX6" s="20"/>
+      <c r="CY6" s="20"/>
+      <c r="CZ6" s="20"/>
+      <c r="DA6" s="21"/>
+      <c r="DC6" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="DD6" s="54"/>
-      <c r="DE6" s="54"/>
-      <c r="DF6" s="54"/>
-      <c r="DG6" s="54"/>
-      <c r="DH6" s="55"/>
+      <c r="DD6" s="20"/>
+      <c r="DE6" s="20"/>
+      <c r="DF6" s="20"/>
+      <c r="DG6" s="20"/>
+      <c r="DH6" s="21"/>
       <c r="DI6" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="DW6" s="60"/>
-      <c r="DX6" s="59"/>
+      <c r="DW6" s="38"/>
+      <c r="DX6" s="37"/>
     </row>
     <row r="7" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V7" s="62"/>
-      <c r="BF7" s="59"/>
-      <c r="DX7" s="59"/>
+      <c r="V7" s="40"/>
+      <c r="BF7" s="37"/>
+      <c r="DX7" s="37"/>
     </row>
     <row r="8" spans="1:157" s="4" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -3428,35 +3544,21 @@
       </c>
       <c r="B8" s="7">
         <f ca="1">TODAY()</f>
-        <v>44766</v>
-      </c>
-      <c r="V8" s="63"/>
+        <v>44773</v>
+      </c>
+      <c r="V8" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="DC6:DH6"/>
-    <mergeCell ref="DQ5:DV5"/>
-    <mergeCell ref="DC5:DH5"/>
-    <mergeCell ref="BT5:BY5"/>
-    <mergeCell ref="CA5:CF5"/>
-    <mergeCell ref="CH5:CM5"/>
-    <mergeCell ref="CO5:CT5"/>
-    <mergeCell ref="CV5:DA5"/>
-    <mergeCell ref="BG5:BK5"/>
-    <mergeCell ref="BM5:BR5"/>
-    <mergeCell ref="CO6:CT6"/>
-    <mergeCell ref="CV6:DA6"/>
-    <mergeCell ref="W4:AW4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="AX4:BB4"/>
-    <mergeCell ref="AK6:AP6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="AD5:AI5"/>
-    <mergeCell ref="AK5:AP5"/>
-    <mergeCell ref="AR5:AW5"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BG6:BK6"/>
-    <mergeCell ref="BM6:BR6"/>
+  <mergeCells count="49">
+    <mergeCell ref="DQ4:DV4"/>
+    <mergeCell ref="CO4:CT4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="BG4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="DB4:DP4"/>
     <mergeCell ref="A1:DX2"/>
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="O5:U5"/>
@@ -3473,15 +3575,30 @@
     <mergeCell ref="AY6:BB6"/>
     <mergeCell ref="AV6:AW6"/>
     <mergeCell ref="AY5:BB5"/>
-    <mergeCell ref="DQ4:DV4"/>
-    <mergeCell ref="CO4:CT4"/>
-    <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="BG4:BL4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="DB4:DP4"/>
+    <mergeCell ref="BG5:BK5"/>
+    <mergeCell ref="BM5:BR5"/>
+    <mergeCell ref="CO6:CT6"/>
+    <mergeCell ref="CV6:DA6"/>
+    <mergeCell ref="W4:AW4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="AX4:BB4"/>
+    <mergeCell ref="AK6:AP6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="AD5:AI5"/>
+    <mergeCell ref="AK5:AP5"/>
+    <mergeCell ref="AR5:AW5"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BG6:BK6"/>
+    <mergeCell ref="BM6:BR6"/>
+    <mergeCell ref="CH6:CM6"/>
+    <mergeCell ref="DC6:DH6"/>
+    <mergeCell ref="DQ5:DV5"/>
+    <mergeCell ref="DC5:DH5"/>
+    <mergeCell ref="BT5:BY5"/>
+    <mergeCell ref="CA5:CF5"/>
+    <mergeCell ref="CH5:CM5"/>
+    <mergeCell ref="CO5:CT5"/>
+    <mergeCell ref="CV5:DA5"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:XFD3">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
meeting logs and timeline updates // T&E period reduced to 1 week to facilitate MVP completion
</commit_message>
<xml_diff>
--- a/Timeline/Project_Timeline.xlsx
+++ b/Timeline/Project_Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Desktop/agile/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF87ADA-6766-1244-AAB1-661B4A60A455}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AB20AF-0CE0-4944-B8C7-71F489ADE315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15920" yWindow="4020" windowWidth="28800" windowHeight="22140" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
+    <workbookView xWindow="16420" yWindow="1180" windowWidth="28800" windowHeight="22140" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="78">
   <si>
     <t>ASP - Group Project</t>
   </si>
@@ -986,80 +986,7 @@
     <t>Intended MVP deadline</t>
   </si>
   <si>
-    <t>THIS WEEK MAY BE CONTINGENCY DEVELOPMENT TIME AS SPRINT 8 IF REQUIRED</t>
-  </si>
-  <si>
     <t>DEVELOPMENT DEADLINE</t>
-  </si>
-  <si>
-    <t>TBC</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">DEVELOPMENT CONTINGENCY PERIOD
-IF TIME PERMITS … </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Add in more features to the software
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>If MVP NOT CREATED</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Continue with MVP development as a contingency period</t>
-    </r>
-  </si>
-  <si>
-    <t>OPTIONAL DEVELOPMENT CONTINGENCY PERIOD IF FURTHER DEVELOPEMT IS NEEDED</t>
-  </si>
-  <si>
-    <r>
-      <t>Team Meeting 15 - T&amp;E meeting</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Update on the project build</t>
-    </r>
   </si>
   <si>
     <r>
@@ -1259,23 +1186,6 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">Accelerated MVP intended timeline
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Unable to achieve this timeline, review next week</t>
-    </r>
-  </si>
-  <si>
-    <r>
       <rPr>
         <strike/>
         <sz val="12"/>
@@ -1318,7 +1228,7 @@
         <b/>
         <strike/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
       <t xml:space="preserve">IF TIME PERMITS … </t>
@@ -1327,7 +1237,7 @@
       <rPr>
         <strike/>
         <sz val="12"/>
-        <color theme="1"/>
+        <color rgb="FFFF0000"/>
         <rFont val="Calibri (Body)"/>
       </rPr>
       <t xml:space="preserve">
@@ -1356,6 +1266,137 @@
       </rPr>
       <t>If MVP NOT CREATED
 Continue with MVP development as a contingency period</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Duties as per the team meeting 
+Aim for the MVP to be complete at the end of this period."					</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">THIS WEEK MAY BE CONTINGENCY DEVELOPMENT TIME AS SPRINT 8 IF REQUIRED
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>CHANGED TO SPRINT 8 TO COMPLETE MVP</t>
+    </r>
+  </si>
+  <si>
+    <t>Sprint 8 - Software Development</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Team Meeting 15 - T&amp;E meeting</t>
+    </r>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">
+Update on the project build</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <strike/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Team Meeting 15 -  Final Development Update 
+Update on the project build</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">OPTIONAL DEVELOPMENT CONTINGENCY PERIOD IF FURTHER DEVELOPEMT IS NEEDED
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Additional development time required to achieve MVP</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Blackbox testing
+Whitebox testing 
+Accessibility testing </t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <strike/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri (Body)"/>
+      </rPr>
+      <t>Accelerated MVP intended timeline</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Unable to achieve this timeline, review next week</t>
     </r>
   </si>
 </sst>
@@ -1366,7 +1407,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-809]dd\ mmmm\ yyyy;@"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1475,8 +1516,47 @@
       <color theme="1"/>
       <name val="Calibri (Body)"/>
     </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <strike/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri (Body)"/>
+    </font>
   </fonts>
-  <fills count="27">
+  <fills count="28">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1630,6 +1710,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1797,7 +1883,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="76">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1853,176 +1939,188 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="25" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="27" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="27" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="27" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2379,8 +2477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3400B0-A312-474B-BDD8-7EBBB1942BA5}">
   <dimension ref="A1:FA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CZ1" workbookViewId="0">
-      <selection activeCell="CO5" sqref="CO5:CT5"/>
+    <sheetView tabSelected="1" topLeftCell="DB5" workbookViewId="0">
+      <selection activeCell="DJ6" sqref="DJ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2389,266 +2487,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="47" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="29"/>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-      <c r="F1" s="29"/>
-      <c r="G1" s="29"/>
-      <c r="H1" s="29"/>
-      <c r="I1" s="29"/>
-      <c r="J1" s="29"/>
-      <c r="K1" s="29"/>
-      <c r="L1" s="29"/>
-      <c r="M1" s="29"/>
-      <c r="N1" s="29"/>
-      <c r="O1" s="29"/>
-      <c r="P1" s="29"/>
-      <c r="Q1" s="29"/>
-      <c r="R1" s="29"/>
-      <c r="S1" s="29"/>
-      <c r="T1" s="29"/>
-      <c r="U1" s="29"/>
-      <c r="V1" s="29"/>
-      <c r="W1" s="29"/>
-      <c r="X1" s="29"/>
-      <c r="Y1" s="29"/>
-      <c r="Z1" s="29"/>
-      <c r="AA1" s="29"/>
-      <c r="AB1" s="29"/>
-      <c r="AC1" s="29"/>
-      <c r="AD1" s="29"/>
-      <c r="AE1" s="29"/>
-      <c r="AF1" s="29"/>
-      <c r="AG1" s="29"/>
-      <c r="AH1" s="29"/>
-      <c r="AI1" s="29"/>
-      <c r="AJ1" s="29"/>
-      <c r="AK1" s="29"/>
-      <c r="AL1" s="29"/>
-      <c r="AM1" s="29"/>
-      <c r="AN1" s="29"/>
-      <c r="AO1" s="29"/>
-      <c r="AP1" s="29"/>
-      <c r="AQ1" s="29"/>
-      <c r="AR1" s="29"/>
-      <c r="AS1" s="29"/>
-      <c r="AT1" s="29"/>
-      <c r="AU1" s="29"/>
-      <c r="AV1" s="29"/>
-      <c r="AW1" s="29"/>
-      <c r="AX1" s="29"/>
-      <c r="AY1" s="29"/>
-      <c r="AZ1" s="29"/>
-      <c r="BA1" s="29"/>
-      <c r="BB1" s="29"/>
-      <c r="BC1" s="29"/>
-      <c r="BD1" s="29"/>
-      <c r="BE1" s="29"/>
-      <c r="BF1" s="29"/>
-      <c r="BG1" s="29"/>
-      <c r="BH1" s="29"/>
-      <c r="BI1" s="29"/>
-      <c r="BJ1" s="29"/>
-      <c r="BK1" s="29"/>
-      <c r="BL1" s="29"/>
-      <c r="BM1" s="29"/>
-      <c r="BN1" s="29"/>
-      <c r="BO1" s="29"/>
-      <c r="BP1" s="29"/>
-      <c r="BQ1" s="29"/>
-      <c r="BR1" s="29"/>
-      <c r="BS1" s="29"/>
-      <c r="BT1" s="29"/>
-      <c r="BU1" s="29"/>
-      <c r="BV1" s="29"/>
-      <c r="BW1" s="29"/>
-      <c r="BX1" s="29"/>
-      <c r="BY1" s="29"/>
-      <c r="BZ1" s="29"/>
-      <c r="CA1" s="29"/>
-      <c r="CB1" s="29"/>
-      <c r="CC1" s="29"/>
-      <c r="CD1" s="29"/>
-      <c r="CE1" s="29"/>
-      <c r="CF1" s="29"/>
-      <c r="CG1" s="29"/>
-      <c r="CH1" s="29"/>
-      <c r="CI1" s="29"/>
-      <c r="CJ1" s="29"/>
-      <c r="CK1" s="29"/>
-      <c r="CL1" s="29"/>
-      <c r="CM1" s="29"/>
-      <c r="CN1" s="29"/>
-      <c r="CO1" s="29"/>
-      <c r="CP1" s="29"/>
-      <c r="CQ1" s="29"/>
-      <c r="CR1" s="29"/>
-      <c r="CS1" s="29"/>
-      <c r="CT1" s="29"/>
-      <c r="CU1" s="29"/>
-      <c r="CV1" s="29"/>
-      <c r="CW1" s="29"/>
-      <c r="CX1" s="29"/>
-      <c r="CY1" s="29"/>
-      <c r="CZ1" s="29"/>
-      <c r="DA1" s="29"/>
-      <c r="DB1" s="29"/>
-      <c r="DC1" s="29"/>
-      <c r="DD1" s="29"/>
-      <c r="DE1" s="29"/>
-      <c r="DF1" s="29"/>
-      <c r="DG1" s="29"/>
-      <c r="DH1" s="29"/>
-      <c r="DI1" s="29"/>
-      <c r="DJ1" s="29"/>
-      <c r="DK1" s="29"/>
-      <c r="DL1" s="29"/>
-      <c r="DM1" s="29"/>
-      <c r="DN1" s="29"/>
-      <c r="DO1" s="29"/>
-      <c r="DP1" s="29"/>
-      <c r="DQ1" s="29"/>
-      <c r="DR1" s="29"/>
-      <c r="DS1" s="29"/>
-      <c r="DT1" s="29"/>
-      <c r="DU1" s="29"/>
-      <c r="DV1" s="29"/>
-      <c r="DW1" s="29"/>
-      <c r="DX1" s="30"/>
+      <c r="B1" s="48"/>
+      <c r="C1" s="48"/>
+      <c r="D1" s="48"/>
+      <c r="E1" s="48"/>
+      <c r="F1" s="48"/>
+      <c r="G1" s="48"/>
+      <c r="H1" s="48"/>
+      <c r="I1" s="48"/>
+      <c r="J1" s="48"/>
+      <c r="K1" s="48"/>
+      <c r="L1" s="48"/>
+      <c r="M1" s="48"/>
+      <c r="N1" s="48"/>
+      <c r="O1" s="48"/>
+      <c r="P1" s="48"/>
+      <c r="Q1" s="48"/>
+      <c r="R1" s="48"/>
+      <c r="S1" s="48"/>
+      <c r="T1" s="48"/>
+      <c r="U1" s="48"/>
+      <c r="V1" s="48"/>
+      <c r="W1" s="48"/>
+      <c r="X1" s="48"/>
+      <c r="Y1" s="48"/>
+      <c r="Z1" s="48"/>
+      <c r="AA1" s="48"/>
+      <c r="AB1" s="48"/>
+      <c r="AC1" s="48"/>
+      <c r="AD1" s="48"/>
+      <c r="AE1" s="48"/>
+      <c r="AF1" s="48"/>
+      <c r="AG1" s="48"/>
+      <c r="AH1" s="48"/>
+      <c r="AI1" s="48"/>
+      <c r="AJ1" s="48"/>
+      <c r="AK1" s="48"/>
+      <c r="AL1" s="48"/>
+      <c r="AM1" s="48"/>
+      <c r="AN1" s="48"/>
+      <c r="AO1" s="48"/>
+      <c r="AP1" s="48"/>
+      <c r="AQ1" s="48"/>
+      <c r="AR1" s="48"/>
+      <c r="AS1" s="48"/>
+      <c r="AT1" s="48"/>
+      <c r="AU1" s="48"/>
+      <c r="AV1" s="48"/>
+      <c r="AW1" s="48"/>
+      <c r="AX1" s="48"/>
+      <c r="AY1" s="48"/>
+      <c r="AZ1" s="48"/>
+      <c r="BA1" s="48"/>
+      <c r="BB1" s="48"/>
+      <c r="BC1" s="48"/>
+      <c r="BD1" s="48"/>
+      <c r="BE1" s="48"/>
+      <c r="BF1" s="48"/>
+      <c r="BG1" s="48"/>
+      <c r="BH1" s="48"/>
+      <c r="BI1" s="48"/>
+      <c r="BJ1" s="48"/>
+      <c r="BK1" s="48"/>
+      <c r="BL1" s="48"/>
+      <c r="BM1" s="48"/>
+      <c r="BN1" s="48"/>
+      <c r="BO1" s="48"/>
+      <c r="BP1" s="48"/>
+      <c r="BQ1" s="48"/>
+      <c r="BR1" s="48"/>
+      <c r="BS1" s="48"/>
+      <c r="BT1" s="48"/>
+      <c r="BU1" s="48"/>
+      <c r="BV1" s="48"/>
+      <c r="BW1" s="48"/>
+      <c r="BX1" s="48"/>
+      <c r="BY1" s="48"/>
+      <c r="BZ1" s="48"/>
+      <c r="CA1" s="48"/>
+      <c r="CB1" s="48"/>
+      <c r="CC1" s="48"/>
+      <c r="CD1" s="48"/>
+      <c r="CE1" s="48"/>
+      <c r="CF1" s="48"/>
+      <c r="CG1" s="48"/>
+      <c r="CH1" s="48"/>
+      <c r="CI1" s="48"/>
+      <c r="CJ1" s="48"/>
+      <c r="CK1" s="48"/>
+      <c r="CL1" s="48"/>
+      <c r="CM1" s="48"/>
+      <c r="CN1" s="48"/>
+      <c r="CO1" s="48"/>
+      <c r="CP1" s="48"/>
+      <c r="CQ1" s="48"/>
+      <c r="CR1" s="48"/>
+      <c r="CS1" s="48"/>
+      <c r="CT1" s="48"/>
+      <c r="CU1" s="48"/>
+      <c r="CV1" s="48"/>
+      <c r="CW1" s="48"/>
+      <c r="CX1" s="48"/>
+      <c r="CY1" s="48"/>
+      <c r="CZ1" s="48"/>
+      <c r="DA1" s="48"/>
+      <c r="DB1" s="48"/>
+      <c r="DC1" s="48"/>
+      <c r="DD1" s="48"/>
+      <c r="DE1" s="48"/>
+      <c r="DF1" s="48"/>
+      <c r="DG1" s="48"/>
+      <c r="DH1" s="48"/>
+      <c r="DI1" s="48"/>
+      <c r="DJ1" s="48"/>
+      <c r="DK1" s="48"/>
+      <c r="DL1" s="48"/>
+      <c r="DM1" s="48"/>
+      <c r="DN1" s="48"/>
+      <c r="DO1" s="48"/>
+      <c r="DP1" s="48"/>
+      <c r="DQ1" s="48"/>
+      <c r="DR1" s="48"/>
+      <c r="DS1" s="48"/>
+      <c r="DT1" s="48"/>
+      <c r="DU1" s="48"/>
+      <c r="DV1" s="48"/>
+      <c r="DW1" s="48"/>
+      <c r="DX1" s="49"/>
     </row>
     <row r="2" spans="1:157" s="4" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="31"/>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
-      <c r="L2" s="32"/>
-      <c r="M2" s="32"/>
-      <c r="N2" s="32"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="32"/>
-      <c r="Q2" s="32"/>
-      <c r="R2" s="32"/>
-      <c r="S2" s="32"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="32"/>
-      <c r="V2" s="32"/>
-      <c r="W2" s="32"/>
-      <c r="X2" s="32"/>
-      <c r="Y2" s="32"/>
-      <c r="Z2" s="32"/>
-      <c r="AA2" s="32"/>
-      <c r="AB2" s="32"/>
-      <c r="AC2" s="32"/>
-      <c r="AD2" s="32"/>
-      <c r="AE2" s="32"/>
-      <c r="AF2" s="32"/>
-      <c r="AG2" s="32"/>
-      <c r="AH2" s="32"/>
-      <c r="AI2" s="32"/>
-      <c r="AJ2" s="32"/>
-      <c r="AK2" s="32"/>
-      <c r="AL2" s="32"/>
-      <c r="AM2" s="32"/>
-      <c r="AN2" s="32"/>
-      <c r="AO2" s="32"/>
-      <c r="AP2" s="32"/>
-      <c r="AQ2" s="32"/>
-      <c r="AR2" s="32"/>
-      <c r="AS2" s="32"/>
-      <c r="AT2" s="32"/>
-      <c r="AU2" s="32"/>
-      <c r="AV2" s="32"/>
-      <c r="AW2" s="32"/>
-      <c r="AX2" s="32"/>
-      <c r="AY2" s="32"/>
-      <c r="AZ2" s="32"/>
-      <c r="BA2" s="32"/>
-      <c r="BB2" s="32"/>
-      <c r="BC2" s="32"/>
-      <c r="BD2" s="32"/>
-      <c r="BE2" s="32"/>
-      <c r="BF2" s="32"/>
-      <c r="BG2" s="32"/>
-      <c r="BH2" s="32"/>
-      <c r="BI2" s="32"/>
-      <c r="BJ2" s="32"/>
-      <c r="BK2" s="32"/>
-      <c r="BL2" s="32"/>
-      <c r="BM2" s="32"/>
-      <c r="BN2" s="32"/>
-      <c r="BO2" s="32"/>
-      <c r="BP2" s="32"/>
-      <c r="BQ2" s="32"/>
-      <c r="BR2" s="32"/>
-      <c r="BS2" s="32"/>
-      <c r="BT2" s="32"/>
-      <c r="BU2" s="32"/>
-      <c r="BV2" s="32"/>
-      <c r="BW2" s="32"/>
-      <c r="BX2" s="32"/>
-      <c r="BY2" s="32"/>
-      <c r="BZ2" s="32"/>
-      <c r="CA2" s="32"/>
-      <c r="CB2" s="32"/>
-      <c r="CC2" s="32"/>
-      <c r="CD2" s="32"/>
-      <c r="CE2" s="32"/>
-      <c r="CF2" s="32"/>
-      <c r="CG2" s="32"/>
-      <c r="CH2" s="32"/>
-      <c r="CI2" s="32"/>
-      <c r="CJ2" s="32"/>
-      <c r="CK2" s="32"/>
-      <c r="CL2" s="32"/>
-      <c r="CM2" s="32"/>
-      <c r="CN2" s="32"/>
-      <c r="CO2" s="32"/>
-      <c r="CP2" s="32"/>
-      <c r="CQ2" s="32"/>
-      <c r="CR2" s="32"/>
-      <c r="CS2" s="32"/>
-      <c r="CT2" s="32"/>
-      <c r="CU2" s="32"/>
-      <c r="CV2" s="32"/>
-      <c r="CW2" s="32"/>
-      <c r="CX2" s="32"/>
-      <c r="CY2" s="32"/>
-      <c r="CZ2" s="32"/>
-      <c r="DA2" s="32"/>
-      <c r="DB2" s="32"/>
-      <c r="DC2" s="32"/>
-      <c r="DD2" s="32"/>
-      <c r="DE2" s="32"/>
-      <c r="DF2" s="32"/>
-      <c r="DG2" s="32"/>
-      <c r="DH2" s="32"/>
-      <c r="DI2" s="32"/>
-      <c r="DJ2" s="32"/>
-      <c r="DK2" s="32"/>
-      <c r="DL2" s="32"/>
-      <c r="DM2" s="32"/>
-      <c r="DN2" s="32"/>
-      <c r="DO2" s="32"/>
-      <c r="DP2" s="32"/>
-      <c r="DQ2" s="32"/>
-      <c r="DR2" s="32"/>
-      <c r="DS2" s="32"/>
-      <c r="DT2" s="32"/>
-      <c r="DU2" s="32"/>
-      <c r="DV2" s="32"/>
-      <c r="DW2" s="32"/>
-      <c r="DX2" s="33"/>
+      <c r="A2" s="50"/>
+      <c r="B2" s="51"/>
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="M2" s="51"/>
+      <c r="N2" s="51"/>
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Y2" s="51"/>
+      <c r="Z2" s="51"/>
+      <c r="AA2" s="51"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51"/>
+      <c r="AF2" s="51"/>
+      <c r="AG2" s="51"/>
+      <c r="AH2" s="51"/>
+      <c r="AI2" s="51"/>
+      <c r="AJ2" s="51"/>
+      <c r="AK2" s="51"/>
+      <c r="AL2" s="51"/>
+      <c r="AM2" s="51"/>
+      <c r="AN2" s="51"/>
+      <c r="AO2" s="51"/>
+      <c r="AP2" s="51"/>
+      <c r="AQ2" s="51"/>
+      <c r="AR2" s="51"/>
+      <c r="AS2" s="51"/>
+      <c r="AT2" s="51"/>
+      <c r="AU2" s="51"/>
+      <c r="AV2" s="51"/>
+      <c r="AW2" s="51"/>
+      <c r="AX2" s="51"/>
+      <c r="AY2" s="51"/>
+      <c r="AZ2" s="51"/>
+      <c r="BA2" s="51"/>
+      <c r="BB2" s="51"/>
+      <c r="BC2" s="51"/>
+      <c r="BD2" s="51"/>
+      <c r="BE2" s="51"/>
+      <c r="BF2" s="51"/>
+      <c r="BG2" s="51"/>
+      <c r="BH2" s="51"/>
+      <c r="BI2" s="51"/>
+      <c r="BJ2" s="51"/>
+      <c r="BK2" s="51"/>
+      <c r="BL2" s="51"/>
+      <c r="BM2" s="51"/>
+      <c r="BN2" s="51"/>
+      <c r="BO2" s="51"/>
+      <c r="BP2" s="51"/>
+      <c r="BQ2" s="51"/>
+      <c r="BR2" s="51"/>
+      <c r="BS2" s="51"/>
+      <c r="BT2" s="51"/>
+      <c r="BU2" s="51"/>
+      <c r="BV2" s="51"/>
+      <c r="BW2" s="51"/>
+      <c r="BX2" s="51"/>
+      <c r="BY2" s="51"/>
+      <c r="BZ2" s="51"/>
+      <c r="CA2" s="51"/>
+      <c r="CB2" s="51"/>
+      <c r="CC2" s="51"/>
+      <c r="CD2" s="51"/>
+      <c r="CE2" s="51"/>
+      <c r="CF2" s="51"/>
+      <c r="CG2" s="51"/>
+      <c r="CH2" s="51"/>
+      <c r="CI2" s="51"/>
+      <c r="CJ2" s="51"/>
+      <c r="CK2" s="51"/>
+      <c r="CL2" s="51"/>
+      <c r="CM2" s="51"/>
+      <c r="CN2" s="51"/>
+      <c r="CO2" s="51"/>
+      <c r="CP2" s="51"/>
+      <c r="CQ2" s="51"/>
+      <c r="CR2" s="51"/>
+      <c r="CS2" s="51"/>
+      <c r="CT2" s="51"/>
+      <c r="CU2" s="51"/>
+      <c r="CV2" s="51"/>
+      <c r="CW2" s="51"/>
+      <c r="CX2" s="51"/>
+      <c r="CY2" s="51"/>
+      <c r="CZ2" s="51"/>
+      <c r="DA2" s="51"/>
+      <c r="DB2" s="51"/>
+      <c r="DC2" s="51"/>
+      <c r="DD2" s="51"/>
+      <c r="DE2" s="51"/>
+      <c r="DF2" s="51"/>
+      <c r="DG2" s="51"/>
+      <c r="DH2" s="51"/>
+      <c r="DI2" s="51"/>
+      <c r="DJ2" s="51"/>
+      <c r="DK2" s="51"/>
+      <c r="DL2" s="51"/>
+      <c r="DM2" s="51"/>
+      <c r="DN2" s="51"/>
+      <c r="DO2" s="51"/>
+      <c r="DP2" s="51"/>
+      <c r="DQ2" s="51"/>
+      <c r="DR2" s="51"/>
+      <c r="DS2" s="51"/>
+      <c r="DT2" s="51"/>
+      <c r="DU2" s="51"/>
+      <c r="DV2" s="51"/>
+      <c r="DW2" s="51"/>
+      <c r="DX2" s="52"/>
     </row>
     <row r="3" spans="1:157" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -3040,169 +3138,171 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="36" t="s">
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36" t="s">
+      <c r="J4" s="58"/>
+      <c r="K4" s="58"/>
+      <c r="L4" s="58"/>
+      <c r="M4" s="58"/>
+      <c r="N4" s="58"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="25" t="s">
+      <c r="Q4" s="58"/>
+      <c r="R4" s="58"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="58"/>
+      <c r="U4" s="58"/>
+      <c r="V4" s="58"/>
+      <c r="W4" s="66" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="25"/>
-      <c r="Y4" s="25"/>
-      <c r="Z4" s="25"/>
-      <c r="AA4" s="25"/>
-      <c r="AB4" s="25"/>
-      <c r="AC4" s="25"/>
-      <c r="AD4" s="25"/>
-      <c r="AE4" s="25"/>
-      <c r="AF4" s="25"/>
-      <c r="AG4" s="25"/>
-      <c r="AH4" s="25"/>
-      <c r="AI4" s="25"/>
-      <c r="AJ4" s="25"/>
-      <c r="AK4" s="25"/>
-      <c r="AL4" s="25"/>
-      <c r="AM4" s="25"/>
-      <c r="AN4" s="25"/>
-      <c r="AO4" s="25"/>
-      <c r="AP4" s="25"/>
-      <c r="AQ4" s="25"/>
-      <c r="AR4" s="25"/>
-      <c r="AS4" s="25"/>
-      <c r="AT4" s="25"/>
-      <c r="AU4" s="25"/>
-      <c r="AV4" s="25"/>
-      <c r="AW4" s="25"/>
-      <c r="AX4" s="27" t="s">
+      <c r="X4" s="66"/>
+      <c r="Y4" s="66"/>
+      <c r="Z4" s="66"/>
+      <c r="AA4" s="66"/>
+      <c r="AB4" s="66"/>
+      <c r="AC4" s="66"/>
+      <c r="AD4" s="66"/>
+      <c r="AE4" s="66"/>
+      <c r="AF4" s="66"/>
+      <c r="AG4" s="66"/>
+      <c r="AH4" s="66"/>
+      <c r="AI4" s="66"/>
+      <c r="AJ4" s="66"/>
+      <c r="AK4" s="66"/>
+      <c r="AL4" s="66"/>
+      <c r="AM4" s="66"/>
+      <c r="AN4" s="66"/>
+      <c r="AO4" s="66"/>
+      <c r="AP4" s="66"/>
+      <c r="AQ4" s="66"/>
+      <c r="AR4" s="66"/>
+      <c r="AS4" s="66"/>
+      <c r="AT4" s="66"/>
+      <c r="AU4" s="66"/>
+      <c r="AV4" s="66"/>
+      <c r="AW4" s="66"/>
+      <c r="AX4" s="68" t="s">
         <v>16</v>
       </c>
-      <c r="AY4" s="27"/>
-      <c r="AZ4" s="27"/>
-      <c r="BA4" s="27"/>
-      <c r="BB4" s="27"/>
-      <c r="BC4" s="26" t="s">
+      <c r="AY4" s="68"/>
+      <c r="AZ4" s="68"/>
+      <c r="BA4" s="68"/>
+      <c r="BB4" s="68"/>
+      <c r="BC4" s="67" t="s">
         <v>17</v>
       </c>
-      <c r="BD4" s="26"/>
-      <c r="BE4" s="38" t="s">
+      <c r="BD4" s="67"/>
+      <c r="BE4" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="BF4" s="37" t="s">
+      <c r="BF4" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="BG4" s="53" t="s">
+      <c r="BG4" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="BH4" s="54"/>
-      <c r="BI4" s="54"/>
-      <c r="BJ4" s="54"/>
-      <c r="BK4" s="54"/>
-      <c r="BL4" s="55"/>
-      <c r="BM4" s="56" t="s">
+      <c r="BH4" s="31"/>
+      <c r="BI4" s="31"/>
+      <c r="BJ4" s="31"/>
+      <c r="BK4" s="31"/>
+      <c r="BL4" s="32"/>
+      <c r="BM4" s="33" t="s">
         <v>41</v>
       </c>
-      <c r="BN4" s="57"/>
-      <c r="BO4" s="57"/>
-      <c r="BP4" s="57"/>
-      <c r="BQ4" s="57"/>
-      <c r="BR4" s="57"/>
-      <c r="BS4" s="58"/>
-      <c r="BT4" s="59" t="s">
+      <c r="BN4" s="34"/>
+      <c r="BO4" s="34"/>
+      <c r="BP4" s="34"/>
+      <c r="BQ4" s="34"/>
+      <c r="BR4" s="34"/>
+      <c r="BS4" s="35"/>
+      <c r="BT4" s="36" t="s">
         <v>42</v>
       </c>
-      <c r="BU4" s="60"/>
-      <c r="BV4" s="60"/>
-      <c r="BW4" s="60"/>
-      <c r="BX4" s="60"/>
-      <c r="BY4" s="60"/>
-      <c r="BZ4" s="61"/>
-      <c r="CA4" s="62" t="s">
+      <c r="BU4" s="37"/>
+      <c r="BV4" s="37"/>
+      <c r="BW4" s="37"/>
+      <c r="BX4" s="37"/>
+      <c r="BY4" s="37"/>
+      <c r="BZ4" s="38"/>
+      <c r="CA4" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="CB4" s="63"/>
-      <c r="CC4" s="63"/>
-      <c r="CD4" s="63"/>
-      <c r="CE4" s="63"/>
-      <c r="CF4" s="63"/>
-      <c r="CG4" s="64"/>
-      <c r="CH4" s="65" t="s">
+      <c r="CB4" s="40"/>
+      <c r="CC4" s="40"/>
+      <c r="CD4" s="40"/>
+      <c r="CE4" s="40"/>
+      <c r="CF4" s="40"/>
+      <c r="CG4" s="41"/>
+      <c r="CH4" s="42" t="s">
         <v>44</v>
       </c>
-      <c r="CI4" s="66"/>
-      <c r="CJ4" s="66"/>
-      <c r="CK4" s="66"/>
-      <c r="CL4" s="66"/>
-      <c r="CM4" s="66"/>
-      <c r="CN4" s="67"/>
-      <c r="CO4" s="47" t="s">
+      <c r="CI4" s="43"/>
+      <c r="CJ4" s="43"/>
+      <c r="CK4" s="43"/>
+      <c r="CL4" s="43"/>
+      <c r="CM4" s="43"/>
+      <c r="CN4" s="44"/>
+      <c r="CO4" s="24" t="s">
         <v>46</v>
       </c>
-      <c r="CP4" s="48"/>
-      <c r="CQ4" s="48"/>
-      <c r="CR4" s="48"/>
-      <c r="CS4" s="48"/>
-      <c r="CT4" s="49"/>
-      <c r="CU4" s="50" t="s">
+      <c r="CP4" s="25"/>
+      <c r="CQ4" s="25"/>
+      <c r="CR4" s="25"/>
+      <c r="CS4" s="25"/>
+      <c r="CT4" s="26"/>
+      <c r="CU4" s="27" t="s">
         <v>47</v>
       </c>
-      <c r="CV4" s="51"/>
-      <c r="CW4" s="51"/>
-      <c r="CX4" s="51"/>
-      <c r="CY4" s="51"/>
-      <c r="CZ4" s="51"/>
-      <c r="DA4" s="52"/>
-      <c r="DB4" s="68" t="s">
+      <c r="CV4" s="28"/>
+      <c r="CW4" s="28"/>
+      <c r="CX4" s="28"/>
+      <c r="CY4" s="28"/>
+      <c r="CZ4" s="28"/>
+      <c r="DA4" s="29"/>
+      <c r="DB4" s="77" t="s">
+        <v>73</v>
+      </c>
+      <c r="DC4" s="78"/>
+      <c r="DD4" s="78"/>
+      <c r="DE4" s="78"/>
+      <c r="DF4" s="78"/>
+      <c r="DG4" s="78"/>
+      <c r="DH4" s="79"/>
+      <c r="DI4" s="45" t="s">
         <v>39</v>
       </c>
-      <c r="DC4" s="69"/>
-      <c r="DD4" s="69"/>
-      <c r="DE4" s="69"/>
-      <c r="DF4" s="69"/>
-      <c r="DG4" s="69"/>
-      <c r="DH4" s="69"/>
-      <c r="DI4" s="69"/>
-      <c r="DJ4" s="69"/>
-      <c r="DK4" s="69"/>
-      <c r="DL4" s="69"/>
-      <c r="DM4" s="69"/>
-      <c r="DN4" s="69"/>
-      <c r="DO4" s="69"/>
-      <c r="DP4" s="70"/>
-      <c r="DQ4" s="44" t="s">
+      <c r="DJ4" s="46"/>
+      <c r="DK4" s="46"/>
+      <c r="DL4" s="46"/>
+      <c r="DM4" s="46"/>
+      <c r="DN4" s="46"/>
+      <c r="DO4" s="46"/>
+      <c r="DP4" s="76"/>
+      <c r="DQ4" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="DR4" s="45"/>
-      <c r="DS4" s="45"/>
-      <c r="DT4" s="45"/>
-      <c r="DU4" s="45"/>
-      <c r="DV4" s="46"/>
-      <c r="DW4" s="38" t="s">
+      <c r="DR4" s="22"/>
+      <c r="DS4" s="22"/>
+      <c r="DT4" s="22"/>
+      <c r="DU4" s="22"/>
+      <c r="DV4" s="23"/>
+      <c r="DW4" s="60" t="s">
         <v>13</v>
       </c>
-      <c r="DX4" s="37" t="s">
+      <c r="DX4" s="59" t="s">
         <v>12</v>
       </c>
       <c r="DY4" s="5"/>
@@ -3242,193 +3342,201 @@
       <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="35"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="D5" s="57"/>
+      <c r="E5" s="57"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="53" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="21"/>
+      <c r="J5" s="54"/>
+      <c r="K5" s="54"/>
+      <c r="L5" s="54"/>
+      <c r="M5" s="55"/>
       <c r="N5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="22" t="s">
+      <c r="O5" s="53" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="20"/>
-      <c r="T5" s="20"/>
-      <c r="U5" s="21"/>
+      <c r="P5" s="54"/>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="54"/>
+      <c r="S5" s="54"/>
+      <c r="T5" s="54"/>
+      <c r="U5" s="55"/>
       <c r="V5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="22" t="s">
+      <c r="W5" s="53" t="s">
         <v>25</v>
       </c>
-      <c r="X5" s="20"/>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="21"/>
+      <c r="X5" s="54"/>
+      <c r="Y5" s="54"/>
+      <c r="Z5" s="54"/>
+      <c r="AA5" s="54"/>
+      <c r="AB5" s="55"/>
       <c r="AC5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="22" t="s">
+      <c r="AD5" s="53" t="s">
         <v>30</v>
       </c>
-      <c r="AE5" s="20"/>
-      <c r="AF5" s="20"/>
-      <c r="AG5" s="20"/>
-      <c r="AH5" s="20"/>
-      <c r="AI5" s="21"/>
+      <c r="AE5" s="54"/>
+      <c r="AF5" s="54"/>
+      <c r="AG5" s="54"/>
+      <c r="AH5" s="54"/>
+      <c r="AI5" s="55"/>
       <c r="AJ5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AK5" s="22" t="s">
+      <c r="AK5" s="53" t="s">
         <v>35</v>
       </c>
-      <c r="AL5" s="20"/>
-      <c r="AM5" s="20"/>
-      <c r="AN5" s="20"/>
-      <c r="AO5" s="20"/>
-      <c r="AP5" s="21"/>
+      <c r="AL5" s="54"/>
+      <c r="AM5" s="54"/>
+      <c r="AN5" s="54"/>
+      <c r="AO5" s="54"/>
+      <c r="AP5" s="55"/>
       <c r="AQ5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AR5" s="22" t="s">
+      <c r="AR5" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="AS5" s="20"/>
-      <c r="AT5" s="20"/>
-      <c r="AU5" s="20"/>
-      <c r="AV5" s="20"/>
-      <c r="AW5" s="21"/>
+      <c r="AS5" s="54"/>
+      <c r="AT5" s="54"/>
+      <c r="AU5" s="54"/>
+      <c r="AV5" s="54"/>
+      <c r="AW5" s="55"/>
       <c r="AX5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AY5" s="22" t="s">
+      <c r="AY5" s="53" t="s">
         <v>37</v>
       </c>
-      <c r="AZ5" s="20"/>
-      <c r="BA5" s="20"/>
-      <c r="BB5" s="21"/>
-      <c r="BC5" s="22" t="s">
+      <c r="AZ5" s="54"/>
+      <c r="BA5" s="54"/>
+      <c r="BB5" s="55"/>
+      <c r="BC5" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="BD5" s="21"/>
-      <c r="BE5" s="38"/>
-      <c r="BF5" s="37"/>
-      <c r="BG5" s="22" t="s">
+      <c r="BD5" s="55"/>
+      <c r="BE5" s="60"/>
+      <c r="BF5" s="59"/>
+      <c r="BG5" s="53" t="s">
         <v>50</v>
       </c>
-      <c r="BH5" s="20"/>
-      <c r="BI5" s="20"/>
-      <c r="BJ5" s="20"/>
-      <c r="BK5" s="21"/>
+      <c r="BH5" s="54"/>
+      <c r="BI5" s="54"/>
+      <c r="BJ5" s="54"/>
+      <c r="BK5" s="55"/>
       <c r="BL5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="BM5" s="22" t="s">
+      <c r="BM5" s="53" t="s">
         <v>51</v>
       </c>
-      <c r="BN5" s="20"/>
-      <c r="BO5" s="20"/>
-      <c r="BP5" s="20"/>
-      <c r="BQ5" s="20"/>
-      <c r="BR5" s="21"/>
+      <c r="BN5" s="54"/>
+      <c r="BO5" s="54"/>
+      <c r="BP5" s="54"/>
+      <c r="BQ5" s="54"/>
+      <c r="BR5" s="55"/>
       <c r="BS5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="BT5" s="22" t="s">
-        <v>70</v>
-      </c>
-      <c r="BU5" s="20"/>
-      <c r="BV5" s="20"/>
-      <c r="BW5" s="20"/>
-      <c r="BX5" s="20"/>
-      <c r="BY5" s="21"/>
+      <c r="BT5" s="53" t="s">
+        <v>65</v>
+      </c>
+      <c r="BU5" s="54"/>
+      <c r="BV5" s="54"/>
+      <c r="BW5" s="54"/>
+      <c r="BX5" s="54"/>
+      <c r="BY5" s="55"/>
       <c r="BZ5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="CA5" s="22" t="s">
-        <v>71</v>
-      </c>
-      <c r="CB5" s="20"/>
-      <c r="CC5" s="20"/>
-      <c r="CD5" s="20"/>
-      <c r="CE5" s="20"/>
-      <c r="CF5" s="21"/>
+      <c r="CA5" s="53" t="s">
+        <v>66</v>
+      </c>
+      <c r="CB5" s="54"/>
+      <c r="CC5" s="54"/>
+      <c r="CD5" s="54"/>
+      <c r="CE5" s="54"/>
+      <c r="CF5" s="55"/>
       <c r="CG5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="CH5" s="22" t="s">
-        <v>74</v>
-      </c>
-      <c r="CI5" s="20"/>
-      <c r="CJ5" s="20"/>
-      <c r="CK5" s="20"/>
-      <c r="CL5" s="20"/>
-      <c r="CM5" s="21"/>
+      <c r="CH5" s="53" t="s">
+        <v>68</v>
+      </c>
+      <c r="CI5" s="54"/>
+      <c r="CJ5" s="54"/>
+      <c r="CK5" s="54"/>
+      <c r="CL5" s="54"/>
+      <c r="CM5" s="55"/>
       <c r="CN5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="CO5" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="CP5" s="20"/>
-      <c r="CQ5" s="20"/>
-      <c r="CR5" s="20"/>
-      <c r="CS5" s="20"/>
-      <c r="CT5" s="21"/>
+      <c r="CO5" s="53" t="s">
+        <v>69</v>
+      </c>
+      <c r="CP5" s="54"/>
+      <c r="CQ5" s="54"/>
+      <c r="CR5" s="54"/>
+      <c r="CS5" s="54"/>
+      <c r="CT5" s="55"/>
       <c r="CU5" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="CV5" s="22" t="s">
+      <c r="CV5" s="53" t="s">
+        <v>71</v>
+      </c>
+      <c r="CW5" s="54"/>
+      <c r="CX5" s="54"/>
+      <c r="CY5" s="54"/>
+      <c r="CZ5" s="54"/>
+      <c r="DA5" s="55"/>
+      <c r="DB5" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="DC5" s="75" t="s">
+        <v>72</v>
+      </c>
+      <c r="DD5" s="70"/>
+      <c r="DE5" s="70"/>
+      <c r="DF5" s="70"/>
+      <c r="DG5" s="70"/>
+      <c r="DH5" s="71"/>
+      <c r="DI5" s="17" t="s">
+        <v>59</v>
+      </c>
+      <c r="DJ5" s="53" t="s">
+        <v>76</v>
+      </c>
+      <c r="DK5" s="54"/>
+      <c r="DL5" s="54"/>
+      <c r="DM5" s="54"/>
+      <c r="DN5" s="54"/>
+      <c r="DO5" s="55"/>
+      <c r="DP5" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="CW5" s="20"/>
-      <c r="CX5" s="20"/>
-      <c r="CY5" s="20"/>
-      <c r="CZ5" s="20"/>
-      <c r="DA5" s="21"/>
-      <c r="DB5" s="16" t="s">
-        <v>63</v>
-      </c>
-      <c r="DC5" s="19" t="s">
-        <v>58</v>
-      </c>
-      <c r="DD5" s="23"/>
-      <c r="DE5" s="23"/>
-      <c r="DF5" s="23"/>
-      <c r="DG5" s="23"/>
-      <c r="DH5" s="24"/>
-      <c r="DI5" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="DP5" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="DQ5" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="DR5" s="20"/>
-      <c r="DS5" s="20"/>
-      <c r="DT5" s="20"/>
-      <c r="DU5" s="20"/>
-      <c r="DV5" s="21"/>
-      <c r="DW5" s="38"/>
-      <c r="DX5" s="37"/>
+      <c r="DQ5" s="53" t="s">
+        <v>61</v>
+      </c>
+      <c r="DR5" s="54"/>
+      <c r="DS5" s="54"/>
+      <c r="DT5" s="54"/>
+      <c r="DU5" s="54"/>
+      <c r="DV5" s="55"/>
+      <c r="DW5" s="60"/>
+      <c r="DX5" s="59"/>
     </row>
     <row r="6" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -3440,103 +3548,103 @@
       <c r="N6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="39" t="s">
+      <c r="V6" s="61" t="s">
         <v>24</v>
       </c>
       <c r="AC6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AK6" s="19" t="s">
+      <c r="AK6" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="AL6" s="23"/>
-      <c r="AM6" s="23"/>
-      <c r="AN6" s="23"/>
-      <c r="AO6" s="23"/>
-      <c r="AP6" s="24"/>
-      <c r="AV6" s="42" t="s">
+      <c r="AL6" s="70"/>
+      <c r="AM6" s="70"/>
+      <c r="AN6" s="70"/>
+      <c r="AO6" s="70"/>
+      <c r="AP6" s="71"/>
+      <c r="AV6" s="64" t="s">
         <v>33</v>
       </c>
-      <c r="AW6" s="43"/>
+      <c r="AW6" s="65"/>
       <c r="AX6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AY6" s="22"/>
-      <c r="AZ6" s="20"/>
-      <c r="BA6" s="20"/>
-      <c r="BB6" s="21"/>
-      <c r="BC6" s="22" t="s">
+      <c r="AY6" s="53"/>
+      <c r="AZ6" s="54"/>
+      <c r="BA6" s="54"/>
+      <c r="BB6" s="55"/>
+      <c r="BC6" s="53" t="s">
         <v>31</v>
       </c>
-      <c r="BD6" s="21"/>
-      <c r="BE6" s="38"/>
-      <c r="BF6" s="37"/>
-      <c r="BG6" s="22" t="s">
+      <c r="BD6" s="55"/>
+      <c r="BE6" s="60"/>
+      <c r="BF6" s="59"/>
+      <c r="BG6" s="53" t="s">
+        <v>62</v>
+      </c>
+      <c r="BH6" s="54"/>
+      <c r="BI6" s="54"/>
+      <c r="BJ6" s="54"/>
+      <c r="BK6" s="55"/>
+      <c r="BM6" s="53" t="s">
+        <v>63</v>
+      </c>
+      <c r="BN6" s="54"/>
+      <c r="BO6" s="54"/>
+      <c r="BP6" s="54"/>
+      <c r="BQ6" s="54"/>
+      <c r="BR6" s="55"/>
+      <c r="BZ6" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="CG6" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="BH6" s="20"/>
-      <c r="BI6" s="20"/>
-      <c r="BJ6" s="20"/>
-      <c r="BK6" s="21"/>
-      <c r="BM6" s="22" t="s">
-        <v>68</v>
-      </c>
-      <c r="BN6" s="20"/>
-      <c r="BO6" s="20"/>
-      <c r="BP6" s="20"/>
-      <c r="BQ6" s="20"/>
-      <c r="BR6" s="21"/>
-      <c r="BZ6" s="18" t="s">
-        <v>73</v>
-      </c>
-      <c r="CG6" s="71" t="s">
-        <v>72</v>
-      </c>
       <c r="CH6" s="72" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="CI6" s="73"/>
       <c r="CJ6" s="73"/>
       <c r="CK6" s="73"/>
       <c r="CL6" s="73"/>
       <c r="CM6" s="74"/>
-      <c r="CN6" s="75" t="s">
+      <c r="CN6" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="CO6" s="22" t="s">
-        <v>76</v>
-      </c>
-      <c r="CP6" s="20"/>
-      <c r="CQ6" s="20"/>
-      <c r="CR6" s="20"/>
-      <c r="CS6" s="20"/>
-      <c r="CT6" s="21"/>
-      <c r="CV6" s="22" t="s">
-        <v>61</v>
-      </c>
-      <c r="CW6" s="20"/>
-      <c r="CX6" s="20"/>
-      <c r="CY6" s="20"/>
-      <c r="CZ6" s="20"/>
-      <c r="DA6" s="21"/>
-      <c r="DC6" s="19" t="s">
-        <v>62</v>
-      </c>
-      <c r="DD6" s="20"/>
-      <c r="DE6" s="20"/>
-      <c r="DF6" s="20"/>
-      <c r="DG6" s="20"/>
-      <c r="DH6" s="21"/>
+      <c r="CO6" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="CP6" s="54"/>
+      <c r="CQ6" s="54"/>
+      <c r="CR6" s="54"/>
+      <c r="CS6" s="54"/>
+      <c r="CT6" s="55"/>
+      <c r="CV6" s="53" t="s">
+        <v>70</v>
+      </c>
+      <c r="CW6" s="54"/>
+      <c r="CX6" s="54"/>
+      <c r="CY6" s="54"/>
+      <c r="CZ6" s="54"/>
+      <c r="DA6" s="55"/>
+      <c r="DC6" s="69" t="s">
+        <v>75</v>
+      </c>
+      <c r="DD6" s="54"/>
+      <c r="DE6" s="54"/>
+      <c r="DF6" s="54"/>
+      <c r="DG6" s="54"/>
+      <c r="DH6" s="55"/>
       <c r="DI6" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="DW6" s="38"/>
-      <c r="DX6" s="37"/>
+        <v>58</v>
+      </c>
+      <c r="DW6" s="60"/>
+      <c r="DX6" s="59"/>
     </row>
     <row r="7" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V7" s="40"/>
-      <c r="BF7" s="37"/>
-      <c r="DX7" s="37"/>
+      <c r="V7" s="62"/>
+      <c r="BF7" s="59"/>
+      <c r="DX7" s="59"/>
     </row>
     <row r="8" spans="1:157" s="4" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -3544,21 +3652,37 @@
       </c>
       <c r="B8" s="7">
         <f ca="1">TODAY()</f>
-        <v>44773</v>
-      </c>
-      <c r="V8" s="41"/>
+        <v>44787</v>
+      </c>
+      <c r="V8" s="63"/>
     </row>
   </sheetData>
-  <mergeCells count="49">
-    <mergeCell ref="DQ4:DV4"/>
-    <mergeCell ref="CO4:CT4"/>
-    <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="BG4:BL4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="DB4:DP4"/>
+  <mergeCells count="51">
+    <mergeCell ref="DC6:DH6"/>
+    <mergeCell ref="DQ5:DV5"/>
+    <mergeCell ref="DC5:DH5"/>
+    <mergeCell ref="BT5:BY5"/>
+    <mergeCell ref="CA5:CF5"/>
+    <mergeCell ref="CH5:CM5"/>
+    <mergeCell ref="CO5:CT5"/>
+    <mergeCell ref="CV5:DA5"/>
+    <mergeCell ref="DJ5:DO5"/>
+    <mergeCell ref="BG5:BK5"/>
+    <mergeCell ref="BM5:BR5"/>
+    <mergeCell ref="CO6:CT6"/>
+    <mergeCell ref="CV6:DA6"/>
+    <mergeCell ref="W4:AW4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="AX4:BB4"/>
+    <mergeCell ref="AK6:AP6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="AD5:AI5"/>
+    <mergeCell ref="AK5:AP5"/>
+    <mergeCell ref="AR5:AW5"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BG6:BK6"/>
+    <mergeCell ref="BM6:BR6"/>
+    <mergeCell ref="CH6:CM6"/>
     <mergeCell ref="A1:DX2"/>
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="O5:U5"/>
@@ -3575,30 +3699,16 @@
     <mergeCell ref="AY6:BB6"/>
     <mergeCell ref="AV6:AW6"/>
     <mergeCell ref="AY5:BB5"/>
-    <mergeCell ref="BG5:BK5"/>
-    <mergeCell ref="BM5:BR5"/>
-    <mergeCell ref="CO6:CT6"/>
-    <mergeCell ref="CV6:DA6"/>
-    <mergeCell ref="W4:AW4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="AX4:BB4"/>
-    <mergeCell ref="AK6:AP6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="AD5:AI5"/>
-    <mergeCell ref="AK5:AP5"/>
-    <mergeCell ref="AR5:AW5"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BG6:BK6"/>
-    <mergeCell ref="BM6:BR6"/>
-    <mergeCell ref="CH6:CM6"/>
-    <mergeCell ref="DC6:DH6"/>
-    <mergeCell ref="DQ5:DV5"/>
-    <mergeCell ref="DC5:DH5"/>
-    <mergeCell ref="BT5:BY5"/>
-    <mergeCell ref="CA5:CF5"/>
-    <mergeCell ref="CH5:CM5"/>
-    <mergeCell ref="CO5:CT5"/>
-    <mergeCell ref="CV5:DA5"/>
+    <mergeCell ref="DQ4:DV4"/>
+    <mergeCell ref="CO4:CT4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="BG4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="DI4:DO4"/>
+    <mergeCell ref="DB4:DH4"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:XFD3">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
meeting notes from 21 Aug 22 // timeline update
</commit_message>
<xml_diff>
--- a/Timeline/Project_Timeline.xlsx
+++ b/Timeline/Project_Timeline.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Desktop/agile/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07AB20AF-0CE0-4944-B8C7-71F489ADE315}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA01DED7-9256-9B40-930F-97D4B5D58D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16420" yWindow="1180" windowWidth="28800" windowHeight="22140" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16660" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1945,173 +1945,173 @@
     <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="15" fontId="2" fillId="27" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -2477,8 +2477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3400B0-A312-474B-BDD8-7EBBB1942BA5}">
   <dimension ref="A1:FA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DB5" workbookViewId="0">
-      <selection activeCell="DJ6" sqref="DJ6"/>
+    <sheetView tabSelected="1" topLeftCell="DE2" zoomScale="75" workbookViewId="0">
+      <selection activeCell="DJ5" sqref="DJ5:DO5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2487,266 +2487,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="47" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="48"/>
-      <c r="J1" s="48"/>
-      <c r="K1" s="48"/>
-      <c r="L1" s="48"/>
-      <c r="M1" s="48"/>
-      <c r="N1" s="48"/>
-      <c r="O1" s="48"/>
-      <c r="P1" s="48"/>
-      <c r="Q1" s="48"/>
-      <c r="R1" s="48"/>
-      <c r="S1" s="48"/>
-      <c r="T1" s="48"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="48"/>
-      <c r="W1" s="48"/>
-      <c r="X1" s="48"/>
-      <c r="Y1" s="48"/>
-      <c r="Z1" s="48"/>
-      <c r="AA1" s="48"/>
-      <c r="AB1" s="48"/>
-      <c r="AC1" s="48"/>
-      <c r="AD1" s="48"/>
-      <c r="AE1" s="48"/>
-      <c r="AF1" s="48"/>
-      <c r="AG1" s="48"/>
-      <c r="AH1" s="48"/>
-      <c r="AI1" s="48"/>
-      <c r="AJ1" s="48"/>
-      <c r="AK1" s="48"/>
-      <c r="AL1" s="48"/>
-      <c r="AM1" s="48"/>
-      <c r="AN1" s="48"/>
-      <c r="AO1" s="48"/>
-      <c r="AP1" s="48"/>
-      <c r="AQ1" s="48"/>
-      <c r="AR1" s="48"/>
-      <c r="AS1" s="48"/>
-      <c r="AT1" s="48"/>
-      <c r="AU1" s="48"/>
-      <c r="AV1" s="48"/>
-      <c r="AW1" s="48"/>
-      <c r="AX1" s="48"/>
-      <c r="AY1" s="48"/>
-      <c r="AZ1" s="48"/>
-      <c r="BA1" s="48"/>
-      <c r="BB1" s="48"/>
-      <c r="BC1" s="48"/>
-      <c r="BD1" s="48"/>
-      <c r="BE1" s="48"/>
-      <c r="BF1" s="48"/>
-      <c r="BG1" s="48"/>
-      <c r="BH1" s="48"/>
-      <c r="BI1" s="48"/>
-      <c r="BJ1" s="48"/>
-      <c r="BK1" s="48"/>
-      <c r="BL1" s="48"/>
-      <c r="BM1" s="48"/>
-      <c r="BN1" s="48"/>
-      <c r="BO1" s="48"/>
-      <c r="BP1" s="48"/>
-      <c r="BQ1" s="48"/>
-      <c r="BR1" s="48"/>
-      <c r="BS1" s="48"/>
-      <c r="BT1" s="48"/>
-      <c r="BU1" s="48"/>
-      <c r="BV1" s="48"/>
-      <c r="BW1" s="48"/>
-      <c r="BX1" s="48"/>
-      <c r="BY1" s="48"/>
-      <c r="BZ1" s="48"/>
-      <c r="CA1" s="48"/>
-      <c r="CB1" s="48"/>
-      <c r="CC1" s="48"/>
-      <c r="CD1" s="48"/>
-      <c r="CE1" s="48"/>
-      <c r="CF1" s="48"/>
-      <c r="CG1" s="48"/>
-      <c r="CH1" s="48"/>
-      <c r="CI1" s="48"/>
-      <c r="CJ1" s="48"/>
-      <c r="CK1" s="48"/>
-      <c r="CL1" s="48"/>
-      <c r="CM1" s="48"/>
-      <c r="CN1" s="48"/>
-      <c r="CO1" s="48"/>
-      <c r="CP1" s="48"/>
-      <c r="CQ1" s="48"/>
-      <c r="CR1" s="48"/>
-      <c r="CS1" s="48"/>
-      <c r="CT1" s="48"/>
-      <c r="CU1" s="48"/>
-      <c r="CV1" s="48"/>
-      <c r="CW1" s="48"/>
-      <c r="CX1" s="48"/>
-      <c r="CY1" s="48"/>
-      <c r="CZ1" s="48"/>
-      <c r="DA1" s="48"/>
-      <c r="DB1" s="48"/>
-      <c r="DC1" s="48"/>
-      <c r="DD1" s="48"/>
-      <c r="DE1" s="48"/>
-      <c r="DF1" s="48"/>
-      <c r="DG1" s="48"/>
-      <c r="DH1" s="48"/>
-      <c r="DI1" s="48"/>
-      <c r="DJ1" s="48"/>
-      <c r="DK1" s="48"/>
-      <c r="DL1" s="48"/>
-      <c r="DM1" s="48"/>
-      <c r="DN1" s="48"/>
-      <c r="DO1" s="48"/>
-      <c r="DP1" s="48"/>
-      <c r="DQ1" s="48"/>
-      <c r="DR1" s="48"/>
-      <c r="DS1" s="48"/>
-      <c r="DT1" s="48"/>
-      <c r="DU1" s="48"/>
-      <c r="DV1" s="48"/>
-      <c r="DW1" s="48"/>
-      <c r="DX1" s="49"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="36"/>
+      <c r="V1" s="36"/>
+      <c r="W1" s="36"/>
+      <c r="X1" s="36"/>
+      <c r="Y1" s="36"/>
+      <c r="Z1" s="36"/>
+      <c r="AA1" s="36"/>
+      <c r="AB1" s="36"/>
+      <c r="AC1" s="36"/>
+      <c r="AD1" s="36"/>
+      <c r="AE1" s="36"/>
+      <c r="AF1" s="36"/>
+      <c r="AG1" s="36"/>
+      <c r="AH1" s="36"/>
+      <c r="AI1" s="36"/>
+      <c r="AJ1" s="36"/>
+      <c r="AK1" s="36"/>
+      <c r="AL1" s="36"/>
+      <c r="AM1" s="36"/>
+      <c r="AN1" s="36"/>
+      <c r="AO1" s="36"/>
+      <c r="AP1" s="36"/>
+      <c r="AQ1" s="36"/>
+      <c r="AR1" s="36"/>
+      <c r="AS1" s="36"/>
+      <c r="AT1" s="36"/>
+      <c r="AU1" s="36"/>
+      <c r="AV1" s="36"/>
+      <c r="AW1" s="36"/>
+      <c r="AX1" s="36"/>
+      <c r="AY1" s="36"/>
+      <c r="AZ1" s="36"/>
+      <c r="BA1" s="36"/>
+      <c r="BB1" s="36"/>
+      <c r="BC1" s="36"/>
+      <c r="BD1" s="36"/>
+      <c r="BE1" s="36"/>
+      <c r="BF1" s="36"/>
+      <c r="BG1" s="36"/>
+      <c r="BH1" s="36"/>
+      <c r="BI1" s="36"/>
+      <c r="BJ1" s="36"/>
+      <c r="BK1" s="36"/>
+      <c r="BL1" s="36"/>
+      <c r="BM1" s="36"/>
+      <c r="BN1" s="36"/>
+      <c r="BO1" s="36"/>
+      <c r="BP1" s="36"/>
+      <c r="BQ1" s="36"/>
+      <c r="BR1" s="36"/>
+      <c r="BS1" s="36"/>
+      <c r="BT1" s="36"/>
+      <c r="BU1" s="36"/>
+      <c r="BV1" s="36"/>
+      <c r="BW1" s="36"/>
+      <c r="BX1" s="36"/>
+      <c r="BY1" s="36"/>
+      <c r="BZ1" s="36"/>
+      <c r="CA1" s="36"/>
+      <c r="CB1" s="36"/>
+      <c r="CC1" s="36"/>
+      <c r="CD1" s="36"/>
+      <c r="CE1" s="36"/>
+      <c r="CF1" s="36"/>
+      <c r="CG1" s="36"/>
+      <c r="CH1" s="36"/>
+      <c r="CI1" s="36"/>
+      <c r="CJ1" s="36"/>
+      <c r="CK1" s="36"/>
+      <c r="CL1" s="36"/>
+      <c r="CM1" s="36"/>
+      <c r="CN1" s="36"/>
+      <c r="CO1" s="36"/>
+      <c r="CP1" s="36"/>
+      <c r="CQ1" s="36"/>
+      <c r="CR1" s="36"/>
+      <c r="CS1" s="36"/>
+      <c r="CT1" s="36"/>
+      <c r="CU1" s="36"/>
+      <c r="CV1" s="36"/>
+      <c r="CW1" s="36"/>
+      <c r="CX1" s="36"/>
+      <c r="CY1" s="36"/>
+      <c r="CZ1" s="36"/>
+      <c r="DA1" s="36"/>
+      <c r="DB1" s="36"/>
+      <c r="DC1" s="36"/>
+      <c r="DD1" s="36"/>
+      <c r="DE1" s="36"/>
+      <c r="DF1" s="36"/>
+      <c r="DG1" s="36"/>
+      <c r="DH1" s="36"/>
+      <c r="DI1" s="36"/>
+      <c r="DJ1" s="36"/>
+      <c r="DK1" s="36"/>
+      <c r="DL1" s="36"/>
+      <c r="DM1" s="36"/>
+      <c r="DN1" s="36"/>
+      <c r="DO1" s="36"/>
+      <c r="DP1" s="36"/>
+      <c r="DQ1" s="36"/>
+      <c r="DR1" s="36"/>
+      <c r="DS1" s="36"/>
+      <c r="DT1" s="36"/>
+      <c r="DU1" s="36"/>
+      <c r="DV1" s="36"/>
+      <c r="DW1" s="36"/>
+      <c r="DX1" s="37"/>
     </row>
     <row r="2" spans="1:157" s="4" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="50"/>
-      <c r="B2" s="51"/>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="M2" s="51"/>
-      <c r="N2" s="51"/>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Y2" s="51"/>
-      <c r="Z2" s="51"/>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
-      <c r="AF2" s="51"/>
-      <c r="AG2" s="51"/>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
-      <c r="AK2" s="51"/>
-      <c r="AL2" s="51"/>
-      <c r="AM2" s="51"/>
-      <c r="AN2" s="51"/>
-      <c r="AO2" s="51"/>
-      <c r="AP2" s="51"/>
-      <c r="AQ2" s="51"/>
-      <c r="AR2" s="51"/>
-      <c r="AS2" s="51"/>
-      <c r="AT2" s="51"/>
-      <c r="AU2" s="51"/>
-      <c r="AV2" s="51"/>
-      <c r="AW2" s="51"/>
-      <c r="AX2" s="51"/>
-      <c r="AY2" s="51"/>
-      <c r="AZ2" s="51"/>
-      <c r="BA2" s="51"/>
-      <c r="BB2" s="51"/>
-      <c r="BC2" s="51"/>
-      <c r="BD2" s="51"/>
-      <c r="BE2" s="51"/>
-      <c r="BF2" s="51"/>
-      <c r="BG2" s="51"/>
-      <c r="BH2" s="51"/>
-      <c r="BI2" s="51"/>
-      <c r="BJ2" s="51"/>
-      <c r="BK2" s="51"/>
-      <c r="BL2" s="51"/>
-      <c r="BM2" s="51"/>
-      <c r="BN2" s="51"/>
-      <c r="BO2" s="51"/>
-      <c r="BP2" s="51"/>
-      <c r="BQ2" s="51"/>
-      <c r="BR2" s="51"/>
-      <c r="BS2" s="51"/>
-      <c r="BT2" s="51"/>
-      <c r="BU2" s="51"/>
-      <c r="BV2" s="51"/>
-      <c r="BW2" s="51"/>
-      <c r="BX2" s="51"/>
-      <c r="BY2" s="51"/>
-      <c r="BZ2" s="51"/>
-      <c r="CA2" s="51"/>
-      <c r="CB2" s="51"/>
-      <c r="CC2" s="51"/>
-      <c r="CD2" s="51"/>
-      <c r="CE2" s="51"/>
-      <c r="CF2" s="51"/>
-      <c r="CG2" s="51"/>
-      <c r="CH2" s="51"/>
-      <c r="CI2" s="51"/>
-      <c r="CJ2" s="51"/>
-      <c r="CK2" s="51"/>
-      <c r="CL2" s="51"/>
-      <c r="CM2" s="51"/>
-      <c r="CN2" s="51"/>
-      <c r="CO2" s="51"/>
-      <c r="CP2" s="51"/>
-      <c r="CQ2" s="51"/>
-      <c r="CR2" s="51"/>
-      <c r="CS2" s="51"/>
-      <c r="CT2" s="51"/>
-      <c r="CU2" s="51"/>
-      <c r="CV2" s="51"/>
-      <c r="CW2" s="51"/>
-      <c r="CX2" s="51"/>
-      <c r="CY2" s="51"/>
-      <c r="CZ2" s="51"/>
-      <c r="DA2" s="51"/>
-      <c r="DB2" s="51"/>
-      <c r="DC2" s="51"/>
-      <c r="DD2" s="51"/>
-      <c r="DE2" s="51"/>
-      <c r="DF2" s="51"/>
-      <c r="DG2" s="51"/>
-      <c r="DH2" s="51"/>
-      <c r="DI2" s="51"/>
-      <c r="DJ2" s="51"/>
-      <c r="DK2" s="51"/>
-      <c r="DL2" s="51"/>
-      <c r="DM2" s="51"/>
-      <c r="DN2" s="51"/>
-      <c r="DO2" s="51"/>
-      <c r="DP2" s="51"/>
-      <c r="DQ2" s="51"/>
-      <c r="DR2" s="51"/>
-      <c r="DS2" s="51"/>
-      <c r="DT2" s="51"/>
-      <c r="DU2" s="51"/>
-      <c r="DV2" s="51"/>
-      <c r="DW2" s="51"/>
-      <c r="DX2" s="52"/>
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="39"/>
+      <c r="V2" s="39"/>
+      <c r="W2" s="39"/>
+      <c r="X2" s="39"/>
+      <c r="Y2" s="39"/>
+      <c r="Z2" s="39"/>
+      <c r="AA2" s="39"/>
+      <c r="AB2" s="39"/>
+      <c r="AC2" s="39"/>
+      <c r="AD2" s="39"/>
+      <c r="AE2" s="39"/>
+      <c r="AF2" s="39"/>
+      <c r="AG2" s="39"/>
+      <c r="AH2" s="39"/>
+      <c r="AI2" s="39"/>
+      <c r="AJ2" s="39"/>
+      <c r="AK2" s="39"/>
+      <c r="AL2" s="39"/>
+      <c r="AM2" s="39"/>
+      <c r="AN2" s="39"/>
+      <c r="AO2" s="39"/>
+      <c r="AP2" s="39"/>
+      <c r="AQ2" s="39"/>
+      <c r="AR2" s="39"/>
+      <c r="AS2" s="39"/>
+      <c r="AT2" s="39"/>
+      <c r="AU2" s="39"/>
+      <c r="AV2" s="39"/>
+      <c r="AW2" s="39"/>
+      <c r="AX2" s="39"/>
+      <c r="AY2" s="39"/>
+      <c r="AZ2" s="39"/>
+      <c r="BA2" s="39"/>
+      <c r="BB2" s="39"/>
+      <c r="BC2" s="39"/>
+      <c r="BD2" s="39"/>
+      <c r="BE2" s="39"/>
+      <c r="BF2" s="39"/>
+      <c r="BG2" s="39"/>
+      <c r="BH2" s="39"/>
+      <c r="BI2" s="39"/>
+      <c r="BJ2" s="39"/>
+      <c r="BK2" s="39"/>
+      <c r="BL2" s="39"/>
+      <c r="BM2" s="39"/>
+      <c r="BN2" s="39"/>
+      <c r="BO2" s="39"/>
+      <c r="BP2" s="39"/>
+      <c r="BQ2" s="39"/>
+      <c r="BR2" s="39"/>
+      <c r="BS2" s="39"/>
+      <c r="BT2" s="39"/>
+      <c r="BU2" s="39"/>
+      <c r="BV2" s="39"/>
+      <c r="BW2" s="39"/>
+      <c r="BX2" s="39"/>
+      <c r="BY2" s="39"/>
+      <c r="BZ2" s="39"/>
+      <c r="CA2" s="39"/>
+      <c r="CB2" s="39"/>
+      <c r="CC2" s="39"/>
+      <c r="CD2" s="39"/>
+      <c r="CE2" s="39"/>
+      <c r="CF2" s="39"/>
+      <c r="CG2" s="39"/>
+      <c r="CH2" s="39"/>
+      <c r="CI2" s="39"/>
+      <c r="CJ2" s="39"/>
+      <c r="CK2" s="39"/>
+      <c r="CL2" s="39"/>
+      <c r="CM2" s="39"/>
+      <c r="CN2" s="39"/>
+      <c r="CO2" s="39"/>
+      <c r="CP2" s="39"/>
+      <c r="CQ2" s="39"/>
+      <c r="CR2" s="39"/>
+      <c r="CS2" s="39"/>
+      <c r="CT2" s="39"/>
+      <c r="CU2" s="39"/>
+      <c r="CV2" s="39"/>
+      <c r="CW2" s="39"/>
+      <c r="CX2" s="39"/>
+      <c r="CY2" s="39"/>
+      <c r="CZ2" s="39"/>
+      <c r="DA2" s="39"/>
+      <c r="DB2" s="39"/>
+      <c r="DC2" s="39"/>
+      <c r="DD2" s="39"/>
+      <c r="DE2" s="39"/>
+      <c r="DF2" s="39"/>
+      <c r="DG2" s="39"/>
+      <c r="DH2" s="39"/>
+      <c r="DI2" s="39"/>
+      <c r="DJ2" s="39"/>
+      <c r="DK2" s="39"/>
+      <c r="DL2" s="39"/>
+      <c r="DM2" s="39"/>
+      <c r="DN2" s="39"/>
+      <c r="DO2" s="39"/>
+      <c r="DP2" s="39"/>
+      <c r="DQ2" s="39"/>
+      <c r="DR2" s="39"/>
+      <c r="DS2" s="39"/>
+      <c r="DT2" s="39"/>
+      <c r="DU2" s="39"/>
+      <c r="DV2" s="39"/>
+      <c r="DW2" s="39"/>
+      <c r="DX2" s="40"/>
     </row>
     <row r="3" spans="1:157" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -3138,140 +3138,140 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="56" t="s">
+      <c r="B4" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="58" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
+      <c r="G4" s="41"/>
+      <c r="H4" s="41"/>
+      <c r="I4" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="58"/>
-      <c r="K4" s="58"/>
-      <c r="L4" s="58"/>
-      <c r="M4" s="58"/>
-      <c r="N4" s="58"/>
-      <c r="O4" s="58"/>
-      <c r="P4" s="58" t="s">
+      <c r="J4" s="43"/>
+      <c r="K4" s="43"/>
+      <c r="L4" s="43"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="43"/>
+      <c r="O4" s="43"/>
+      <c r="P4" s="43" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="58"/>
-      <c r="R4" s="58"/>
-      <c r="S4" s="58"/>
-      <c r="T4" s="58"/>
-      <c r="U4" s="58"/>
-      <c r="V4" s="58"/>
-      <c r="W4" s="66" t="s">
+      <c r="Q4" s="43"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="43"/>
+      <c r="T4" s="43"/>
+      <c r="U4" s="43"/>
+      <c r="V4" s="43"/>
+      <c r="W4" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="66"/>
-      <c r="Y4" s="66"/>
-      <c r="Z4" s="66"/>
-      <c r="AA4" s="66"/>
-      <c r="AB4" s="66"/>
-      <c r="AC4" s="66"/>
-      <c r="AD4" s="66"/>
-      <c r="AE4" s="66"/>
-      <c r="AF4" s="66"/>
-      <c r="AG4" s="66"/>
-      <c r="AH4" s="66"/>
-      <c r="AI4" s="66"/>
-      <c r="AJ4" s="66"/>
-      <c r="AK4" s="66"/>
-      <c r="AL4" s="66"/>
-      <c r="AM4" s="66"/>
-      <c r="AN4" s="66"/>
-      <c r="AO4" s="66"/>
-      <c r="AP4" s="66"/>
-      <c r="AQ4" s="66"/>
-      <c r="AR4" s="66"/>
-      <c r="AS4" s="66"/>
-      <c r="AT4" s="66"/>
-      <c r="AU4" s="66"/>
-      <c r="AV4" s="66"/>
-      <c r="AW4" s="66"/>
-      <c r="AX4" s="68" t="s">
+      <c r="X4" s="29"/>
+      <c r="Y4" s="29"/>
+      <c r="Z4" s="29"/>
+      <c r="AA4" s="29"/>
+      <c r="AB4" s="29"/>
+      <c r="AC4" s="29"/>
+      <c r="AD4" s="29"/>
+      <c r="AE4" s="29"/>
+      <c r="AF4" s="29"/>
+      <c r="AG4" s="29"/>
+      <c r="AH4" s="29"/>
+      <c r="AI4" s="29"/>
+      <c r="AJ4" s="29"/>
+      <c r="AK4" s="29"/>
+      <c r="AL4" s="29"/>
+      <c r="AM4" s="29"/>
+      <c r="AN4" s="29"/>
+      <c r="AO4" s="29"/>
+      <c r="AP4" s="29"/>
+      <c r="AQ4" s="29"/>
+      <c r="AR4" s="29"/>
+      <c r="AS4" s="29"/>
+      <c r="AT4" s="29"/>
+      <c r="AU4" s="29"/>
+      <c r="AV4" s="29"/>
+      <c r="AW4" s="29"/>
+      <c r="AX4" s="31" t="s">
         <v>16</v>
       </c>
-      <c r="AY4" s="68"/>
-      <c r="AZ4" s="68"/>
-      <c r="BA4" s="68"/>
-      <c r="BB4" s="68"/>
-      <c r="BC4" s="67" t="s">
+      <c r="AY4" s="31"/>
+      <c r="AZ4" s="31"/>
+      <c r="BA4" s="31"/>
+      <c r="BB4" s="31"/>
+      <c r="BC4" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="BD4" s="67"/>
-      <c r="BE4" s="60" t="s">
+      <c r="BD4" s="30"/>
+      <c r="BE4" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="BF4" s="59" t="s">
+      <c r="BF4" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="BG4" s="30" t="s">
+      <c r="BG4" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="BH4" s="31"/>
-      <c r="BI4" s="31"/>
-      <c r="BJ4" s="31"/>
-      <c r="BK4" s="31"/>
-      <c r="BL4" s="32"/>
-      <c r="BM4" s="33" t="s">
+      <c r="BH4" s="61"/>
+      <c r="BI4" s="61"/>
+      <c r="BJ4" s="61"/>
+      <c r="BK4" s="61"/>
+      <c r="BL4" s="62"/>
+      <c r="BM4" s="63" t="s">
         <v>41</v>
       </c>
-      <c r="BN4" s="34"/>
-      <c r="BO4" s="34"/>
-      <c r="BP4" s="34"/>
-      <c r="BQ4" s="34"/>
-      <c r="BR4" s="34"/>
-      <c r="BS4" s="35"/>
-      <c r="BT4" s="36" t="s">
+      <c r="BN4" s="64"/>
+      <c r="BO4" s="64"/>
+      <c r="BP4" s="64"/>
+      <c r="BQ4" s="64"/>
+      <c r="BR4" s="64"/>
+      <c r="BS4" s="65"/>
+      <c r="BT4" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="BU4" s="37"/>
-      <c r="BV4" s="37"/>
-      <c r="BW4" s="37"/>
-      <c r="BX4" s="37"/>
-      <c r="BY4" s="37"/>
-      <c r="BZ4" s="38"/>
-      <c r="CA4" s="39" t="s">
+      <c r="BU4" s="67"/>
+      <c r="BV4" s="67"/>
+      <c r="BW4" s="67"/>
+      <c r="BX4" s="67"/>
+      <c r="BY4" s="67"/>
+      <c r="BZ4" s="68"/>
+      <c r="CA4" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="CB4" s="40"/>
-      <c r="CC4" s="40"/>
-      <c r="CD4" s="40"/>
-      <c r="CE4" s="40"/>
-      <c r="CF4" s="40"/>
-      <c r="CG4" s="41"/>
-      <c r="CH4" s="42" t="s">
+      <c r="CB4" s="70"/>
+      <c r="CC4" s="70"/>
+      <c r="CD4" s="70"/>
+      <c r="CE4" s="70"/>
+      <c r="CF4" s="70"/>
+      <c r="CG4" s="71"/>
+      <c r="CH4" s="72" t="s">
         <v>44</v>
       </c>
-      <c r="CI4" s="43"/>
-      <c r="CJ4" s="43"/>
-      <c r="CK4" s="43"/>
-      <c r="CL4" s="43"/>
-      <c r="CM4" s="43"/>
-      <c r="CN4" s="44"/>
-      <c r="CO4" s="24" t="s">
+      <c r="CI4" s="73"/>
+      <c r="CJ4" s="73"/>
+      <c r="CK4" s="73"/>
+      <c r="CL4" s="73"/>
+      <c r="CM4" s="73"/>
+      <c r="CN4" s="74"/>
+      <c r="CO4" s="54" t="s">
         <v>46</v>
       </c>
-      <c r="CP4" s="25"/>
-      <c r="CQ4" s="25"/>
-      <c r="CR4" s="25"/>
-      <c r="CS4" s="25"/>
-      <c r="CT4" s="26"/>
-      <c r="CU4" s="27" t="s">
+      <c r="CP4" s="55"/>
+      <c r="CQ4" s="55"/>
+      <c r="CR4" s="55"/>
+      <c r="CS4" s="55"/>
+      <c r="CT4" s="56"/>
+      <c r="CU4" s="57" t="s">
         <v>47</v>
       </c>
-      <c r="CV4" s="28"/>
-      <c r="CW4" s="28"/>
-      <c r="CX4" s="28"/>
-      <c r="CY4" s="28"/>
-      <c r="CZ4" s="28"/>
-      <c r="DA4" s="29"/>
+      <c r="CV4" s="58"/>
+      <c r="CW4" s="58"/>
+      <c r="CX4" s="58"/>
+      <c r="CY4" s="58"/>
+      <c r="CZ4" s="58"/>
+      <c r="DA4" s="59"/>
       <c r="DB4" s="77" t="s">
         <v>73</v>
       </c>
@@ -3281,28 +3281,28 @@
       <c r="DF4" s="78"/>
       <c r="DG4" s="78"/>
       <c r="DH4" s="79"/>
-      <c r="DI4" s="45" t="s">
+      <c r="DI4" s="75" t="s">
         <v>39</v>
       </c>
-      <c r="DJ4" s="46"/>
-      <c r="DK4" s="46"/>
-      <c r="DL4" s="46"/>
-      <c r="DM4" s="46"/>
-      <c r="DN4" s="46"/>
-      <c r="DO4" s="46"/>
-      <c r="DP4" s="76"/>
-      <c r="DQ4" s="21" t="s">
+      <c r="DJ4" s="76"/>
+      <c r="DK4" s="76"/>
+      <c r="DL4" s="76"/>
+      <c r="DM4" s="76"/>
+      <c r="DN4" s="76"/>
+      <c r="DO4" s="76"/>
+      <c r="DP4" s="21"/>
+      <c r="DQ4" s="51" t="s">
         <v>45</v>
       </c>
-      <c r="DR4" s="22"/>
-      <c r="DS4" s="22"/>
-      <c r="DT4" s="22"/>
-      <c r="DU4" s="22"/>
-      <c r="DV4" s="23"/>
-      <c r="DW4" s="60" t="s">
+      <c r="DR4" s="52"/>
+      <c r="DS4" s="52"/>
+      <c r="DT4" s="52"/>
+      <c r="DU4" s="52"/>
+      <c r="DV4" s="53"/>
+      <c r="DW4" s="45" t="s">
         <v>13</v>
       </c>
-      <c r="DX4" s="59" t="s">
+      <c r="DX4" s="44" t="s">
         <v>12</v>
       </c>
       <c r="DY4" s="5"/>
@@ -3342,201 +3342,201 @@
       <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="42" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="57"/>
-      <c r="E5" s="57"/>
-      <c r="F5" s="57"/>
+      <c r="D5" s="42"/>
+      <c r="E5" s="42"/>
+      <c r="F5" s="42"/>
       <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="53" t="s">
+      <c r="I5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="54"/>
-      <c r="K5" s="54"/>
-      <c r="L5" s="54"/>
-      <c r="M5" s="55"/>
+      <c r="J5" s="23"/>
+      <c r="K5" s="23"/>
+      <c r="L5" s="23"/>
+      <c r="M5" s="24"/>
       <c r="N5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="53" t="s">
+      <c r="O5" s="25" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="54"/>
-      <c r="Q5" s="54"/>
-      <c r="R5" s="54"/>
-      <c r="S5" s="54"/>
-      <c r="T5" s="54"/>
-      <c r="U5" s="55"/>
+      <c r="P5" s="23"/>
+      <c r="Q5" s="23"/>
+      <c r="R5" s="23"/>
+      <c r="S5" s="23"/>
+      <c r="T5" s="23"/>
+      <c r="U5" s="24"/>
       <c r="V5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="53" t="s">
+      <c r="W5" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="X5" s="54"/>
-      <c r="Y5" s="54"/>
-      <c r="Z5" s="54"/>
-      <c r="AA5" s="54"/>
-      <c r="AB5" s="55"/>
+      <c r="X5" s="23"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23"/>
+      <c r="AB5" s="24"/>
       <c r="AC5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="53" t="s">
+      <c r="AD5" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="AE5" s="54"/>
-      <c r="AF5" s="54"/>
-      <c r="AG5" s="54"/>
-      <c r="AH5" s="54"/>
-      <c r="AI5" s="55"/>
+      <c r="AE5" s="23"/>
+      <c r="AF5" s="23"/>
+      <c r="AG5" s="23"/>
+      <c r="AH5" s="23"/>
+      <c r="AI5" s="24"/>
       <c r="AJ5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AK5" s="53" t="s">
+      <c r="AK5" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="AL5" s="54"/>
-      <c r="AM5" s="54"/>
-      <c r="AN5" s="54"/>
-      <c r="AO5" s="54"/>
-      <c r="AP5" s="55"/>
+      <c r="AL5" s="23"/>
+      <c r="AM5" s="23"/>
+      <c r="AN5" s="23"/>
+      <c r="AO5" s="23"/>
+      <c r="AP5" s="24"/>
       <c r="AQ5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AR5" s="53" t="s">
+      <c r="AR5" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="AS5" s="54"/>
-      <c r="AT5" s="54"/>
-      <c r="AU5" s="54"/>
-      <c r="AV5" s="54"/>
-      <c r="AW5" s="55"/>
+      <c r="AS5" s="23"/>
+      <c r="AT5" s="23"/>
+      <c r="AU5" s="23"/>
+      <c r="AV5" s="23"/>
+      <c r="AW5" s="24"/>
       <c r="AX5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AY5" s="53" t="s">
+      <c r="AY5" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="AZ5" s="54"/>
-      <c r="BA5" s="54"/>
-      <c r="BB5" s="55"/>
-      <c r="BC5" s="53" t="s">
+      <c r="AZ5" s="23"/>
+      <c r="BA5" s="23"/>
+      <c r="BB5" s="24"/>
+      <c r="BC5" s="25" t="s">
         <v>38</v>
       </c>
-      <c r="BD5" s="55"/>
-      <c r="BE5" s="60"/>
-      <c r="BF5" s="59"/>
-      <c r="BG5" s="53" t="s">
+      <c r="BD5" s="24"/>
+      <c r="BE5" s="45"/>
+      <c r="BF5" s="44"/>
+      <c r="BG5" s="25" t="s">
         <v>50</v>
       </c>
-      <c r="BH5" s="54"/>
-      <c r="BI5" s="54"/>
-      <c r="BJ5" s="54"/>
-      <c r="BK5" s="55"/>
+      <c r="BH5" s="23"/>
+      <c r="BI5" s="23"/>
+      <c r="BJ5" s="23"/>
+      <c r="BK5" s="24"/>
       <c r="BL5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="BM5" s="53" t="s">
+      <c r="BM5" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="BN5" s="54"/>
-      <c r="BO5" s="54"/>
-      <c r="BP5" s="54"/>
-      <c r="BQ5" s="54"/>
-      <c r="BR5" s="55"/>
+      <c r="BN5" s="23"/>
+      <c r="BO5" s="23"/>
+      <c r="BP5" s="23"/>
+      <c r="BQ5" s="23"/>
+      <c r="BR5" s="24"/>
       <c r="BS5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="BT5" s="53" t="s">
+      <c r="BT5" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="BU5" s="54"/>
-      <c r="BV5" s="54"/>
-      <c r="BW5" s="54"/>
-      <c r="BX5" s="54"/>
-      <c r="BY5" s="55"/>
+      <c r="BU5" s="23"/>
+      <c r="BV5" s="23"/>
+      <c r="BW5" s="23"/>
+      <c r="BX5" s="23"/>
+      <c r="BY5" s="24"/>
       <c r="BZ5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="CA5" s="53" t="s">
+      <c r="CA5" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="CB5" s="54"/>
-      <c r="CC5" s="54"/>
-      <c r="CD5" s="54"/>
-      <c r="CE5" s="54"/>
-      <c r="CF5" s="55"/>
+      <c r="CB5" s="23"/>
+      <c r="CC5" s="23"/>
+      <c r="CD5" s="23"/>
+      <c r="CE5" s="23"/>
+      <c r="CF5" s="24"/>
       <c r="CG5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="CH5" s="53" t="s">
+      <c r="CH5" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="CI5" s="54"/>
-      <c r="CJ5" s="54"/>
-      <c r="CK5" s="54"/>
-      <c r="CL5" s="54"/>
-      <c r="CM5" s="55"/>
+      <c r="CI5" s="23"/>
+      <c r="CJ5" s="23"/>
+      <c r="CK5" s="23"/>
+      <c r="CL5" s="23"/>
+      <c r="CM5" s="24"/>
       <c r="CN5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="CO5" s="53" t="s">
+      <c r="CO5" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="CP5" s="54"/>
-      <c r="CQ5" s="54"/>
-      <c r="CR5" s="54"/>
-      <c r="CS5" s="54"/>
-      <c r="CT5" s="55"/>
+      <c r="CP5" s="23"/>
+      <c r="CQ5" s="23"/>
+      <c r="CR5" s="23"/>
+      <c r="CS5" s="23"/>
+      <c r="CT5" s="24"/>
       <c r="CU5" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="CV5" s="53" t="s">
+      <c r="CV5" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="CW5" s="54"/>
-      <c r="CX5" s="54"/>
-      <c r="CY5" s="54"/>
-      <c r="CZ5" s="54"/>
-      <c r="DA5" s="55"/>
+      <c r="CW5" s="23"/>
+      <c r="CX5" s="23"/>
+      <c r="CY5" s="23"/>
+      <c r="CZ5" s="23"/>
+      <c r="DA5" s="24"/>
       <c r="DB5" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="DC5" s="75" t="s">
+      <c r="DC5" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="DD5" s="70"/>
-      <c r="DE5" s="70"/>
-      <c r="DF5" s="70"/>
-      <c r="DG5" s="70"/>
-      <c r="DH5" s="71"/>
+      <c r="DD5" s="27"/>
+      <c r="DE5" s="27"/>
+      <c r="DF5" s="27"/>
+      <c r="DG5" s="27"/>
+      <c r="DH5" s="28"/>
       <c r="DI5" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="DJ5" s="53" t="s">
+      <c r="DJ5" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="DK5" s="54"/>
-      <c r="DL5" s="54"/>
-      <c r="DM5" s="54"/>
-      <c r="DN5" s="54"/>
-      <c r="DO5" s="55"/>
+      <c r="DK5" s="23"/>
+      <c r="DL5" s="23"/>
+      <c r="DM5" s="23"/>
+      <c r="DN5" s="23"/>
+      <c r="DO5" s="24"/>
       <c r="DP5" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="DQ5" s="53" t="s">
+      <c r="DQ5" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="DR5" s="54"/>
-      <c r="DS5" s="54"/>
-      <c r="DT5" s="54"/>
-      <c r="DU5" s="54"/>
-      <c r="DV5" s="55"/>
-      <c r="DW5" s="60"/>
-      <c r="DX5" s="59"/>
+      <c r="DR5" s="23"/>
+      <c r="DS5" s="23"/>
+      <c r="DT5" s="23"/>
+      <c r="DU5" s="23"/>
+      <c r="DV5" s="24"/>
+      <c r="DW5" s="45"/>
+      <c r="DX5" s="44"/>
     </row>
     <row r="6" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -3548,103 +3548,103 @@
       <c r="N6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="61" t="s">
+      <c r="V6" s="46" t="s">
         <v>24</v>
       </c>
       <c r="AC6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AK6" s="69" t="s">
+      <c r="AK6" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="AL6" s="70"/>
-      <c r="AM6" s="70"/>
-      <c r="AN6" s="70"/>
-      <c r="AO6" s="70"/>
-      <c r="AP6" s="71"/>
-      <c r="AV6" s="64" t="s">
+      <c r="AL6" s="27"/>
+      <c r="AM6" s="27"/>
+      <c r="AN6" s="27"/>
+      <c r="AO6" s="27"/>
+      <c r="AP6" s="28"/>
+      <c r="AV6" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="AW6" s="65"/>
+      <c r="AW6" s="50"/>
       <c r="AX6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AY6" s="53"/>
-      <c r="AZ6" s="54"/>
-      <c r="BA6" s="54"/>
-      <c r="BB6" s="55"/>
-      <c r="BC6" s="53" t="s">
+      <c r="AY6" s="25"/>
+      <c r="AZ6" s="23"/>
+      <c r="BA6" s="23"/>
+      <c r="BB6" s="24"/>
+      <c r="BC6" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="BD6" s="55"/>
-      <c r="BE6" s="60"/>
-      <c r="BF6" s="59"/>
-      <c r="BG6" s="53" t="s">
+      <c r="BD6" s="24"/>
+      <c r="BE6" s="45"/>
+      <c r="BF6" s="44"/>
+      <c r="BG6" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="BH6" s="54"/>
-      <c r="BI6" s="54"/>
-      <c r="BJ6" s="54"/>
-      <c r="BK6" s="55"/>
-      <c r="BM6" s="53" t="s">
+      <c r="BH6" s="23"/>
+      <c r="BI6" s="23"/>
+      <c r="BJ6" s="23"/>
+      <c r="BK6" s="24"/>
+      <c r="BM6" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="BN6" s="54"/>
-      <c r="BO6" s="54"/>
-      <c r="BP6" s="54"/>
-      <c r="BQ6" s="54"/>
-      <c r="BR6" s="55"/>
+      <c r="BN6" s="23"/>
+      <c r="BO6" s="23"/>
+      <c r="BP6" s="23"/>
+      <c r="BQ6" s="23"/>
+      <c r="BR6" s="24"/>
       <c r="BZ6" s="18" t="s">
         <v>77</v>
       </c>
       <c r="CG6" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="CH6" s="72" t="s">
+      <c r="CH6" s="32" t="s">
         <v>64</v>
       </c>
-      <c r="CI6" s="73"/>
-      <c r="CJ6" s="73"/>
-      <c r="CK6" s="73"/>
-      <c r="CL6" s="73"/>
-      <c r="CM6" s="74"/>
+      <c r="CI6" s="33"/>
+      <c r="CJ6" s="33"/>
+      <c r="CK6" s="33"/>
+      <c r="CL6" s="33"/>
+      <c r="CM6" s="34"/>
       <c r="CN6" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="CO6" s="53" t="s">
+      <c r="CO6" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="CP6" s="54"/>
-      <c r="CQ6" s="54"/>
-      <c r="CR6" s="54"/>
-      <c r="CS6" s="54"/>
-      <c r="CT6" s="55"/>
-      <c r="CV6" s="53" t="s">
+      <c r="CP6" s="23"/>
+      <c r="CQ6" s="23"/>
+      <c r="CR6" s="23"/>
+      <c r="CS6" s="23"/>
+      <c r="CT6" s="24"/>
+      <c r="CV6" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="CW6" s="54"/>
-      <c r="CX6" s="54"/>
-      <c r="CY6" s="54"/>
-      <c r="CZ6" s="54"/>
-      <c r="DA6" s="55"/>
-      <c r="DC6" s="69" t="s">
+      <c r="CW6" s="23"/>
+      <c r="CX6" s="23"/>
+      <c r="CY6" s="23"/>
+      <c r="CZ6" s="23"/>
+      <c r="DA6" s="24"/>
+      <c r="DC6" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="DD6" s="54"/>
-      <c r="DE6" s="54"/>
-      <c r="DF6" s="54"/>
-      <c r="DG6" s="54"/>
-      <c r="DH6" s="55"/>
+      <c r="DD6" s="23"/>
+      <c r="DE6" s="23"/>
+      <c r="DF6" s="23"/>
+      <c r="DG6" s="23"/>
+      <c r="DH6" s="24"/>
       <c r="DI6" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="DW6" s="60"/>
-      <c r="DX6" s="59"/>
+      <c r="DW6" s="45"/>
+      <c r="DX6" s="44"/>
     </row>
     <row r="7" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V7" s="62"/>
-      <c r="BF7" s="59"/>
-      <c r="DX7" s="59"/>
+      <c r="V7" s="47"/>
+      <c r="BF7" s="44"/>
+      <c r="DX7" s="44"/>
     </row>
     <row r="8" spans="1:157" s="4" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -3652,21 +3652,38 @@
       </c>
       <c r="B8" s="7">
         <f ca="1">TODAY()</f>
-        <v>44787</v>
-      </c>
-      <c r="V8" s="63"/>
+        <v>44794</v>
+      </c>
+      <c r="V8" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="DC6:DH6"/>
-    <mergeCell ref="DQ5:DV5"/>
-    <mergeCell ref="DC5:DH5"/>
-    <mergeCell ref="BT5:BY5"/>
-    <mergeCell ref="CA5:CF5"/>
-    <mergeCell ref="CH5:CM5"/>
-    <mergeCell ref="CO5:CT5"/>
-    <mergeCell ref="CV5:DA5"/>
-    <mergeCell ref="DJ5:DO5"/>
+    <mergeCell ref="DQ4:DV4"/>
+    <mergeCell ref="CO4:CT4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="BG4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="DI4:DO4"/>
+    <mergeCell ref="DB4:DH4"/>
+    <mergeCell ref="A1:DX2"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="O5:U5"/>
+    <mergeCell ref="W5:AB5"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="I4:O4"/>
+    <mergeCell ref="BF4:BF7"/>
+    <mergeCell ref="BE4:BE6"/>
+    <mergeCell ref="V6:V8"/>
+    <mergeCell ref="DX4:DX7"/>
+    <mergeCell ref="DW4:DW6"/>
+    <mergeCell ref="P4:V4"/>
+    <mergeCell ref="AY6:BB6"/>
+    <mergeCell ref="AV6:AW6"/>
+    <mergeCell ref="AY5:BB5"/>
     <mergeCell ref="BG5:BK5"/>
     <mergeCell ref="BM5:BR5"/>
     <mergeCell ref="CO6:CT6"/>
@@ -3683,32 +3700,15 @@
     <mergeCell ref="BG6:BK6"/>
     <mergeCell ref="BM6:BR6"/>
     <mergeCell ref="CH6:CM6"/>
-    <mergeCell ref="A1:DX2"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="O5:U5"/>
-    <mergeCell ref="W5:AB5"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="I4:O4"/>
-    <mergeCell ref="BF4:BF7"/>
-    <mergeCell ref="BE4:BE6"/>
-    <mergeCell ref="V6:V8"/>
-    <mergeCell ref="DX4:DX7"/>
-    <mergeCell ref="DW4:DW6"/>
-    <mergeCell ref="P4:V4"/>
-    <mergeCell ref="AY6:BB6"/>
-    <mergeCell ref="AV6:AW6"/>
-    <mergeCell ref="AY5:BB5"/>
-    <mergeCell ref="DQ4:DV4"/>
-    <mergeCell ref="CO4:CT4"/>
-    <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="BG4:BL4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="DI4:DO4"/>
-    <mergeCell ref="DB4:DH4"/>
+    <mergeCell ref="DC6:DH6"/>
+    <mergeCell ref="DQ5:DV5"/>
+    <mergeCell ref="DC5:DH5"/>
+    <mergeCell ref="BT5:BY5"/>
+    <mergeCell ref="CA5:CF5"/>
+    <mergeCell ref="CH5:CM5"/>
+    <mergeCell ref="CO5:CT5"/>
+    <mergeCell ref="CV5:DA5"/>
+    <mergeCell ref="DJ5:DO5"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:XFD3">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
updated meeting notes for 28 Aug 22 // timeline update
</commit_message>
<xml_diff>
--- a/Timeline/Project_Timeline.xlsx
+++ b/Timeline/Project_Timeline.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/connorking/Desktop/agile/Timeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA01DED7-9256-9B40-930F-97D4B5D58D3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E88873FA-36BC-BB40-A415-BF47C996925F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16660" xr2:uid="{C0250E2D-CCD8-0B44-BBCE-ECB7E25C673B}"/>
   </bookViews>
@@ -1021,9 +1021,6 @@
     </r>
   </si>
   <si>
-    <t>Prepare group submission</t>
-  </si>
-  <si>
     <t xml:space="preserve">Initial HMTL skeleton produced with sample code created for the backend </t>
   </si>
   <si>
@@ -1398,6 +1395,14 @@
       </rPr>
       <t>Unable to achieve this timeline, review next week</t>
     </r>
+  </si>
+  <si>
+    <t>Prepare group submission
+Connor - conclusion and summary
+Ben - references
+Thavelarn - Testing
+David - work summary
+Kashka - not seen in weeks, tasks will be given to him if he reaches out</t>
   </si>
 </sst>
 </file>
@@ -1948,178 +1953,178 @@
     <xf numFmtId="15" fontId="2" fillId="24" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="27" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="27" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="27" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="8" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="26" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="20" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="19" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="15" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="0" fillId="16" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="17" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="18" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="24" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="27" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="27" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="27" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2477,8 +2482,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE3400B0-A312-474B-BDD8-7EBBB1942BA5}">
   <dimension ref="A1:FA8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DE2" zoomScale="75" workbookViewId="0">
-      <selection activeCell="DJ5" sqref="DJ5:DO5"/>
+    <sheetView tabSelected="1" topLeftCell="DM4" zoomScale="75" workbookViewId="0">
+      <selection activeCell="DQ6" sqref="DQ6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="21.33203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2487,266 +2492,266 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:157" s="4" customFormat="1" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="51" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
-      <c r="K1" s="36"/>
-      <c r="L1" s="36"/>
-      <c r="M1" s="36"/>
-      <c r="N1" s="36"/>
-      <c r="O1" s="36"/>
-      <c r="P1" s="36"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
-      <c r="S1" s="36"/>
-      <c r="T1" s="36"/>
-      <c r="U1" s="36"/>
-      <c r="V1" s="36"/>
-      <c r="W1" s="36"/>
-      <c r="X1" s="36"/>
-      <c r="Y1" s="36"/>
-      <c r="Z1" s="36"/>
-      <c r="AA1" s="36"/>
-      <c r="AB1" s="36"/>
-      <c r="AC1" s="36"/>
-      <c r="AD1" s="36"/>
-      <c r="AE1" s="36"/>
-      <c r="AF1" s="36"/>
-      <c r="AG1" s="36"/>
-      <c r="AH1" s="36"/>
-      <c r="AI1" s="36"/>
-      <c r="AJ1" s="36"/>
-      <c r="AK1" s="36"/>
-      <c r="AL1" s="36"/>
-      <c r="AM1" s="36"/>
-      <c r="AN1" s="36"/>
-      <c r="AO1" s="36"/>
-      <c r="AP1" s="36"/>
-      <c r="AQ1" s="36"/>
-      <c r="AR1" s="36"/>
-      <c r="AS1" s="36"/>
-      <c r="AT1" s="36"/>
-      <c r="AU1" s="36"/>
-      <c r="AV1" s="36"/>
-      <c r="AW1" s="36"/>
-      <c r="AX1" s="36"/>
-      <c r="AY1" s="36"/>
-      <c r="AZ1" s="36"/>
-      <c r="BA1" s="36"/>
-      <c r="BB1" s="36"/>
-      <c r="BC1" s="36"/>
-      <c r="BD1" s="36"/>
-      <c r="BE1" s="36"/>
-      <c r="BF1" s="36"/>
-      <c r="BG1" s="36"/>
-      <c r="BH1" s="36"/>
-      <c r="BI1" s="36"/>
-      <c r="BJ1" s="36"/>
-      <c r="BK1" s="36"/>
-      <c r="BL1" s="36"/>
-      <c r="BM1" s="36"/>
-      <c r="BN1" s="36"/>
-      <c r="BO1" s="36"/>
-      <c r="BP1" s="36"/>
-      <c r="BQ1" s="36"/>
-      <c r="BR1" s="36"/>
-      <c r="BS1" s="36"/>
-      <c r="BT1" s="36"/>
-      <c r="BU1" s="36"/>
-      <c r="BV1" s="36"/>
-      <c r="BW1" s="36"/>
-      <c r="BX1" s="36"/>
-      <c r="BY1" s="36"/>
-      <c r="BZ1" s="36"/>
-      <c r="CA1" s="36"/>
-      <c r="CB1" s="36"/>
-      <c r="CC1" s="36"/>
-      <c r="CD1" s="36"/>
-      <c r="CE1" s="36"/>
-      <c r="CF1" s="36"/>
-      <c r="CG1" s="36"/>
-      <c r="CH1" s="36"/>
-      <c r="CI1" s="36"/>
-      <c r="CJ1" s="36"/>
-      <c r="CK1" s="36"/>
-      <c r="CL1" s="36"/>
-      <c r="CM1" s="36"/>
-      <c r="CN1" s="36"/>
-      <c r="CO1" s="36"/>
-      <c r="CP1" s="36"/>
-      <c r="CQ1" s="36"/>
-      <c r="CR1" s="36"/>
-      <c r="CS1" s="36"/>
-      <c r="CT1" s="36"/>
-      <c r="CU1" s="36"/>
-      <c r="CV1" s="36"/>
-      <c r="CW1" s="36"/>
-      <c r="CX1" s="36"/>
-      <c r="CY1" s="36"/>
-      <c r="CZ1" s="36"/>
-      <c r="DA1" s="36"/>
-      <c r="DB1" s="36"/>
-      <c r="DC1" s="36"/>
-      <c r="DD1" s="36"/>
-      <c r="DE1" s="36"/>
-      <c r="DF1" s="36"/>
-      <c r="DG1" s="36"/>
-      <c r="DH1" s="36"/>
-      <c r="DI1" s="36"/>
-      <c r="DJ1" s="36"/>
-      <c r="DK1" s="36"/>
-      <c r="DL1" s="36"/>
-      <c r="DM1" s="36"/>
-      <c r="DN1" s="36"/>
-      <c r="DO1" s="36"/>
-      <c r="DP1" s="36"/>
-      <c r="DQ1" s="36"/>
-      <c r="DR1" s="36"/>
-      <c r="DS1" s="36"/>
-      <c r="DT1" s="36"/>
-      <c r="DU1" s="36"/>
-      <c r="DV1" s="36"/>
-      <c r="DW1" s="36"/>
-      <c r="DX1" s="37"/>
+      <c r="B1" s="52"/>
+      <c r="C1" s="52"/>
+      <c r="D1" s="52"/>
+      <c r="E1" s="52"/>
+      <c r="F1" s="52"/>
+      <c r="G1" s="52"/>
+      <c r="H1" s="52"/>
+      <c r="I1" s="52"/>
+      <c r="J1" s="52"/>
+      <c r="K1" s="52"/>
+      <c r="L1" s="52"/>
+      <c r="M1" s="52"/>
+      <c r="N1" s="52"/>
+      <c r="O1" s="52"/>
+      <c r="P1" s="52"/>
+      <c r="Q1" s="52"/>
+      <c r="R1" s="52"/>
+      <c r="S1" s="52"/>
+      <c r="T1" s="52"/>
+      <c r="U1" s="52"/>
+      <c r="V1" s="52"/>
+      <c r="W1" s="52"/>
+      <c r="X1" s="52"/>
+      <c r="Y1" s="52"/>
+      <c r="Z1" s="52"/>
+      <c r="AA1" s="52"/>
+      <c r="AB1" s="52"/>
+      <c r="AC1" s="52"/>
+      <c r="AD1" s="52"/>
+      <c r="AE1" s="52"/>
+      <c r="AF1" s="52"/>
+      <c r="AG1" s="52"/>
+      <c r="AH1" s="52"/>
+      <c r="AI1" s="52"/>
+      <c r="AJ1" s="52"/>
+      <c r="AK1" s="52"/>
+      <c r="AL1" s="52"/>
+      <c r="AM1" s="52"/>
+      <c r="AN1" s="52"/>
+      <c r="AO1" s="52"/>
+      <c r="AP1" s="52"/>
+      <c r="AQ1" s="52"/>
+      <c r="AR1" s="52"/>
+      <c r="AS1" s="52"/>
+      <c r="AT1" s="52"/>
+      <c r="AU1" s="52"/>
+      <c r="AV1" s="52"/>
+      <c r="AW1" s="52"/>
+      <c r="AX1" s="52"/>
+      <c r="AY1" s="52"/>
+      <c r="AZ1" s="52"/>
+      <c r="BA1" s="52"/>
+      <c r="BB1" s="52"/>
+      <c r="BC1" s="52"/>
+      <c r="BD1" s="52"/>
+      <c r="BE1" s="52"/>
+      <c r="BF1" s="52"/>
+      <c r="BG1" s="52"/>
+      <c r="BH1" s="52"/>
+      <c r="BI1" s="52"/>
+      <c r="BJ1" s="52"/>
+      <c r="BK1" s="52"/>
+      <c r="BL1" s="52"/>
+      <c r="BM1" s="52"/>
+      <c r="BN1" s="52"/>
+      <c r="BO1" s="52"/>
+      <c r="BP1" s="52"/>
+      <c r="BQ1" s="52"/>
+      <c r="BR1" s="52"/>
+      <c r="BS1" s="52"/>
+      <c r="BT1" s="52"/>
+      <c r="BU1" s="52"/>
+      <c r="BV1" s="52"/>
+      <c r="BW1" s="52"/>
+      <c r="BX1" s="52"/>
+      <c r="BY1" s="52"/>
+      <c r="BZ1" s="52"/>
+      <c r="CA1" s="52"/>
+      <c r="CB1" s="52"/>
+      <c r="CC1" s="52"/>
+      <c r="CD1" s="52"/>
+      <c r="CE1" s="52"/>
+      <c r="CF1" s="52"/>
+      <c r="CG1" s="52"/>
+      <c r="CH1" s="52"/>
+      <c r="CI1" s="52"/>
+      <c r="CJ1" s="52"/>
+      <c r="CK1" s="52"/>
+      <c r="CL1" s="52"/>
+      <c r="CM1" s="52"/>
+      <c r="CN1" s="52"/>
+      <c r="CO1" s="52"/>
+      <c r="CP1" s="52"/>
+      <c r="CQ1" s="52"/>
+      <c r="CR1" s="52"/>
+      <c r="CS1" s="52"/>
+      <c r="CT1" s="52"/>
+      <c r="CU1" s="52"/>
+      <c r="CV1" s="52"/>
+      <c r="CW1" s="52"/>
+      <c r="CX1" s="52"/>
+      <c r="CY1" s="52"/>
+      <c r="CZ1" s="52"/>
+      <c r="DA1" s="52"/>
+      <c r="DB1" s="52"/>
+      <c r="DC1" s="52"/>
+      <c r="DD1" s="52"/>
+      <c r="DE1" s="52"/>
+      <c r="DF1" s="52"/>
+      <c r="DG1" s="52"/>
+      <c r="DH1" s="52"/>
+      <c r="DI1" s="52"/>
+      <c r="DJ1" s="52"/>
+      <c r="DK1" s="52"/>
+      <c r="DL1" s="52"/>
+      <c r="DM1" s="52"/>
+      <c r="DN1" s="52"/>
+      <c r="DO1" s="52"/>
+      <c r="DP1" s="52"/>
+      <c r="DQ1" s="52"/>
+      <c r="DR1" s="52"/>
+      <c r="DS1" s="52"/>
+      <c r="DT1" s="52"/>
+      <c r="DU1" s="52"/>
+      <c r="DV1" s="52"/>
+      <c r="DW1" s="52"/>
+      <c r="DX1" s="53"/>
     </row>
     <row r="2" spans="1:157" s="4" customFormat="1" ht="118" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="39"/>
-      <c r="N2" s="39"/>
-      <c r="O2" s="39"/>
-      <c r="P2" s="39"/>
-      <c r="Q2" s="39"/>
-      <c r="R2" s="39"/>
-      <c r="S2" s="39"/>
-      <c r="T2" s="39"/>
-      <c r="U2" s="39"/>
-      <c r="V2" s="39"/>
-      <c r="W2" s="39"/>
-      <c r="X2" s="39"/>
-      <c r="Y2" s="39"/>
-      <c r="Z2" s="39"/>
-      <c r="AA2" s="39"/>
-      <c r="AB2" s="39"/>
-      <c r="AC2" s="39"/>
-      <c r="AD2" s="39"/>
-      <c r="AE2" s="39"/>
-      <c r="AF2" s="39"/>
-      <c r="AG2" s="39"/>
-      <c r="AH2" s="39"/>
-      <c r="AI2" s="39"/>
-      <c r="AJ2" s="39"/>
-      <c r="AK2" s="39"/>
-      <c r="AL2" s="39"/>
-      <c r="AM2" s="39"/>
-      <c r="AN2" s="39"/>
-      <c r="AO2" s="39"/>
-      <c r="AP2" s="39"/>
-      <c r="AQ2" s="39"/>
-      <c r="AR2" s="39"/>
-      <c r="AS2" s="39"/>
-      <c r="AT2" s="39"/>
-      <c r="AU2" s="39"/>
-      <c r="AV2" s="39"/>
-      <c r="AW2" s="39"/>
-      <c r="AX2" s="39"/>
-      <c r="AY2" s="39"/>
-      <c r="AZ2" s="39"/>
-      <c r="BA2" s="39"/>
-      <c r="BB2" s="39"/>
-      <c r="BC2" s="39"/>
-      <c r="BD2" s="39"/>
-      <c r="BE2" s="39"/>
-      <c r="BF2" s="39"/>
-      <c r="BG2" s="39"/>
-      <c r="BH2" s="39"/>
-      <c r="BI2" s="39"/>
-      <c r="BJ2" s="39"/>
-      <c r="BK2" s="39"/>
-      <c r="BL2" s="39"/>
-      <c r="BM2" s="39"/>
-      <c r="BN2" s="39"/>
-      <c r="BO2" s="39"/>
-      <c r="BP2" s="39"/>
-      <c r="BQ2" s="39"/>
-      <c r="BR2" s="39"/>
-      <c r="BS2" s="39"/>
-      <c r="BT2" s="39"/>
-      <c r="BU2" s="39"/>
-      <c r="BV2" s="39"/>
-      <c r="BW2" s="39"/>
-      <c r="BX2" s="39"/>
-      <c r="BY2" s="39"/>
-      <c r="BZ2" s="39"/>
-      <c r="CA2" s="39"/>
-      <c r="CB2" s="39"/>
-      <c r="CC2" s="39"/>
-      <c r="CD2" s="39"/>
-      <c r="CE2" s="39"/>
-      <c r="CF2" s="39"/>
-      <c r="CG2" s="39"/>
-      <c r="CH2" s="39"/>
-      <c r="CI2" s="39"/>
-      <c r="CJ2" s="39"/>
-      <c r="CK2" s="39"/>
-      <c r="CL2" s="39"/>
-      <c r="CM2" s="39"/>
-      <c r="CN2" s="39"/>
-      <c r="CO2" s="39"/>
-      <c r="CP2" s="39"/>
-      <c r="CQ2" s="39"/>
-      <c r="CR2" s="39"/>
-      <c r="CS2" s="39"/>
-      <c r="CT2" s="39"/>
-      <c r="CU2" s="39"/>
-      <c r="CV2" s="39"/>
-      <c r="CW2" s="39"/>
-      <c r="CX2" s="39"/>
-      <c r="CY2" s="39"/>
-      <c r="CZ2" s="39"/>
-      <c r="DA2" s="39"/>
-      <c r="DB2" s="39"/>
-      <c r="DC2" s="39"/>
-      <c r="DD2" s="39"/>
-      <c r="DE2" s="39"/>
-      <c r="DF2" s="39"/>
-      <c r="DG2" s="39"/>
-      <c r="DH2" s="39"/>
-      <c r="DI2" s="39"/>
-      <c r="DJ2" s="39"/>
-      <c r="DK2" s="39"/>
-      <c r="DL2" s="39"/>
-      <c r="DM2" s="39"/>
-      <c r="DN2" s="39"/>
-      <c r="DO2" s="39"/>
-      <c r="DP2" s="39"/>
-      <c r="DQ2" s="39"/>
-      <c r="DR2" s="39"/>
-      <c r="DS2" s="39"/>
-      <c r="DT2" s="39"/>
-      <c r="DU2" s="39"/>
-      <c r="DV2" s="39"/>
-      <c r="DW2" s="39"/>
-      <c r="DX2" s="40"/>
+      <c r="A2" s="54"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
+      <c r="K2" s="55"/>
+      <c r="L2" s="55"/>
+      <c r="M2" s="55"/>
+      <c r="N2" s="55"/>
+      <c r="O2" s="55"/>
+      <c r="P2" s="55"/>
+      <c r="Q2" s="55"/>
+      <c r="R2" s="55"/>
+      <c r="S2" s="55"/>
+      <c r="T2" s="55"/>
+      <c r="U2" s="55"/>
+      <c r="V2" s="55"/>
+      <c r="W2" s="55"/>
+      <c r="X2" s="55"/>
+      <c r="Y2" s="55"/>
+      <c r="Z2" s="55"/>
+      <c r="AA2" s="55"/>
+      <c r="AB2" s="55"/>
+      <c r="AC2" s="55"/>
+      <c r="AD2" s="55"/>
+      <c r="AE2" s="55"/>
+      <c r="AF2" s="55"/>
+      <c r="AG2" s="55"/>
+      <c r="AH2" s="55"/>
+      <c r="AI2" s="55"/>
+      <c r="AJ2" s="55"/>
+      <c r="AK2" s="55"/>
+      <c r="AL2" s="55"/>
+      <c r="AM2" s="55"/>
+      <c r="AN2" s="55"/>
+      <c r="AO2" s="55"/>
+      <c r="AP2" s="55"/>
+      <c r="AQ2" s="55"/>
+      <c r="AR2" s="55"/>
+      <c r="AS2" s="55"/>
+      <c r="AT2" s="55"/>
+      <c r="AU2" s="55"/>
+      <c r="AV2" s="55"/>
+      <c r="AW2" s="55"/>
+      <c r="AX2" s="55"/>
+      <c r="AY2" s="55"/>
+      <c r="AZ2" s="55"/>
+      <c r="BA2" s="55"/>
+      <c r="BB2" s="55"/>
+      <c r="BC2" s="55"/>
+      <c r="BD2" s="55"/>
+      <c r="BE2" s="55"/>
+      <c r="BF2" s="55"/>
+      <c r="BG2" s="55"/>
+      <c r="BH2" s="55"/>
+      <c r="BI2" s="55"/>
+      <c r="BJ2" s="55"/>
+      <c r="BK2" s="55"/>
+      <c r="BL2" s="55"/>
+      <c r="BM2" s="55"/>
+      <c r="BN2" s="55"/>
+      <c r="BO2" s="55"/>
+      <c r="BP2" s="55"/>
+      <c r="BQ2" s="55"/>
+      <c r="BR2" s="55"/>
+      <c r="BS2" s="55"/>
+      <c r="BT2" s="55"/>
+      <c r="BU2" s="55"/>
+      <c r="BV2" s="55"/>
+      <c r="BW2" s="55"/>
+      <c r="BX2" s="55"/>
+      <c r="BY2" s="55"/>
+      <c r="BZ2" s="55"/>
+      <c r="CA2" s="55"/>
+      <c r="CB2" s="55"/>
+      <c r="CC2" s="55"/>
+      <c r="CD2" s="55"/>
+      <c r="CE2" s="55"/>
+      <c r="CF2" s="55"/>
+      <c r="CG2" s="55"/>
+      <c r="CH2" s="55"/>
+      <c r="CI2" s="55"/>
+      <c r="CJ2" s="55"/>
+      <c r="CK2" s="55"/>
+      <c r="CL2" s="55"/>
+      <c r="CM2" s="55"/>
+      <c r="CN2" s="55"/>
+      <c r="CO2" s="55"/>
+      <c r="CP2" s="55"/>
+      <c r="CQ2" s="55"/>
+      <c r="CR2" s="55"/>
+      <c r="CS2" s="55"/>
+      <c r="CT2" s="55"/>
+      <c r="CU2" s="55"/>
+      <c r="CV2" s="55"/>
+      <c r="CW2" s="55"/>
+      <c r="CX2" s="55"/>
+      <c r="CY2" s="55"/>
+      <c r="CZ2" s="55"/>
+      <c r="DA2" s="55"/>
+      <c r="DB2" s="55"/>
+      <c r="DC2" s="55"/>
+      <c r="DD2" s="55"/>
+      <c r="DE2" s="55"/>
+      <c r="DF2" s="55"/>
+      <c r="DG2" s="55"/>
+      <c r="DH2" s="55"/>
+      <c r="DI2" s="55"/>
+      <c r="DJ2" s="55"/>
+      <c r="DK2" s="55"/>
+      <c r="DL2" s="55"/>
+      <c r="DM2" s="55"/>
+      <c r="DN2" s="55"/>
+      <c r="DO2" s="55"/>
+      <c r="DP2" s="55"/>
+      <c r="DQ2" s="55"/>
+      <c r="DR2" s="55"/>
+      <c r="DS2" s="55"/>
+      <c r="DT2" s="55"/>
+      <c r="DU2" s="55"/>
+      <c r="DV2" s="55"/>
+      <c r="DW2" s="55"/>
+      <c r="DX2" s="56"/>
     </row>
     <row r="3" spans="1:157" s="3" customFormat="1" ht="22" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -3138,171 +3143,171 @@
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="60" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="41"/>
-      <c r="G4" s="41"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="43" t="s">
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="60"/>
+      <c r="G4" s="60"/>
+      <c r="H4" s="60"/>
+      <c r="I4" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="J4" s="43"/>
-      <c r="K4" s="43"/>
-      <c r="L4" s="43"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="43"/>
-      <c r="O4" s="43"/>
-      <c r="P4" s="43" t="s">
+      <c r="J4" s="62"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="62"/>
+      <c r="O4" s="62"/>
+      <c r="P4" s="62" t="s">
         <v>8</v>
       </c>
-      <c r="Q4" s="43"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="43"/>
-      <c r="T4" s="43"/>
-      <c r="U4" s="43"/>
-      <c r="V4" s="43"/>
-      <c r="W4" s="29" t="s">
+      <c r="Q4" s="62"/>
+      <c r="R4" s="62"/>
+      <c r="S4" s="62"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="62"/>
+      <c r="V4" s="62"/>
+      <c r="W4" s="70" t="s">
         <v>15</v>
       </c>
-      <c r="X4" s="29"/>
-      <c r="Y4" s="29"/>
-      <c r="Z4" s="29"/>
-      <c r="AA4" s="29"/>
-      <c r="AB4" s="29"/>
-      <c r="AC4" s="29"/>
-      <c r="AD4" s="29"/>
-      <c r="AE4" s="29"/>
-      <c r="AF4" s="29"/>
-      <c r="AG4" s="29"/>
-      <c r="AH4" s="29"/>
-      <c r="AI4" s="29"/>
-      <c r="AJ4" s="29"/>
-      <c r="AK4" s="29"/>
-      <c r="AL4" s="29"/>
-      <c r="AM4" s="29"/>
-      <c r="AN4" s="29"/>
-      <c r="AO4" s="29"/>
-      <c r="AP4" s="29"/>
-      <c r="AQ4" s="29"/>
-      <c r="AR4" s="29"/>
-      <c r="AS4" s="29"/>
-      <c r="AT4" s="29"/>
-      <c r="AU4" s="29"/>
-      <c r="AV4" s="29"/>
-      <c r="AW4" s="29"/>
-      <c r="AX4" s="31" t="s">
+      <c r="X4" s="70"/>
+      <c r="Y4" s="70"/>
+      <c r="Z4" s="70"/>
+      <c r="AA4" s="70"/>
+      <c r="AB4" s="70"/>
+      <c r="AC4" s="70"/>
+      <c r="AD4" s="70"/>
+      <c r="AE4" s="70"/>
+      <c r="AF4" s="70"/>
+      <c r="AG4" s="70"/>
+      <c r="AH4" s="70"/>
+      <c r="AI4" s="70"/>
+      <c r="AJ4" s="70"/>
+      <c r="AK4" s="70"/>
+      <c r="AL4" s="70"/>
+      <c r="AM4" s="70"/>
+      <c r="AN4" s="70"/>
+      <c r="AO4" s="70"/>
+      <c r="AP4" s="70"/>
+      <c r="AQ4" s="70"/>
+      <c r="AR4" s="70"/>
+      <c r="AS4" s="70"/>
+      <c r="AT4" s="70"/>
+      <c r="AU4" s="70"/>
+      <c r="AV4" s="70"/>
+      <c r="AW4" s="70"/>
+      <c r="AX4" s="72" t="s">
         <v>16</v>
       </c>
-      <c r="AY4" s="31"/>
-      <c r="AZ4" s="31"/>
-      <c r="BA4" s="31"/>
-      <c r="BB4" s="31"/>
-      <c r="BC4" s="30" t="s">
+      <c r="AY4" s="72"/>
+      <c r="AZ4" s="72"/>
+      <c r="BA4" s="72"/>
+      <c r="BB4" s="72"/>
+      <c r="BC4" s="71" t="s">
         <v>17</v>
       </c>
-      <c r="BD4" s="30"/>
-      <c r="BE4" s="45" t="s">
+      <c r="BD4" s="71"/>
+      <c r="BE4" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="BF4" s="44" t="s">
+      <c r="BF4" s="63" t="s">
         <v>9</v>
       </c>
-      <c r="BG4" s="60" t="s">
+      <c r="BG4" s="31" t="s">
         <v>40</v>
       </c>
-      <c r="BH4" s="61"/>
-      <c r="BI4" s="61"/>
-      <c r="BJ4" s="61"/>
-      <c r="BK4" s="61"/>
-      <c r="BL4" s="62"/>
-      <c r="BM4" s="63" t="s">
+      <c r="BH4" s="32"/>
+      <c r="BI4" s="32"/>
+      <c r="BJ4" s="32"/>
+      <c r="BK4" s="32"/>
+      <c r="BL4" s="33"/>
+      <c r="BM4" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="BN4" s="64"/>
-      <c r="BO4" s="64"/>
-      <c r="BP4" s="64"/>
-      <c r="BQ4" s="64"/>
-      <c r="BR4" s="64"/>
-      <c r="BS4" s="65"/>
-      <c r="BT4" s="66" t="s">
+      <c r="BN4" s="35"/>
+      <c r="BO4" s="35"/>
+      <c r="BP4" s="35"/>
+      <c r="BQ4" s="35"/>
+      <c r="BR4" s="35"/>
+      <c r="BS4" s="36"/>
+      <c r="BT4" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="BU4" s="67"/>
-      <c r="BV4" s="67"/>
-      <c r="BW4" s="67"/>
-      <c r="BX4" s="67"/>
-      <c r="BY4" s="67"/>
-      <c r="BZ4" s="68"/>
-      <c r="CA4" s="69" t="s">
+      <c r="BU4" s="38"/>
+      <c r="BV4" s="38"/>
+      <c r="BW4" s="38"/>
+      <c r="BX4" s="38"/>
+      <c r="BY4" s="38"/>
+      <c r="BZ4" s="39"/>
+      <c r="CA4" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="CB4" s="70"/>
-      <c r="CC4" s="70"/>
-      <c r="CD4" s="70"/>
-      <c r="CE4" s="70"/>
-      <c r="CF4" s="70"/>
-      <c r="CG4" s="71"/>
-      <c r="CH4" s="72" t="s">
+      <c r="CB4" s="41"/>
+      <c r="CC4" s="41"/>
+      <c r="CD4" s="41"/>
+      <c r="CE4" s="41"/>
+      <c r="CF4" s="41"/>
+      <c r="CG4" s="42"/>
+      <c r="CH4" s="43" t="s">
         <v>44</v>
       </c>
-      <c r="CI4" s="73"/>
-      <c r="CJ4" s="73"/>
-      <c r="CK4" s="73"/>
-      <c r="CL4" s="73"/>
-      <c r="CM4" s="73"/>
-      <c r="CN4" s="74"/>
-      <c r="CO4" s="54" t="s">
+      <c r="CI4" s="44"/>
+      <c r="CJ4" s="44"/>
+      <c r="CK4" s="44"/>
+      <c r="CL4" s="44"/>
+      <c r="CM4" s="44"/>
+      <c r="CN4" s="45"/>
+      <c r="CO4" s="25" t="s">
         <v>46</v>
       </c>
-      <c r="CP4" s="55"/>
-      <c r="CQ4" s="55"/>
-      <c r="CR4" s="55"/>
-      <c r="CS4" s="55"/>
-      <c r="CT4" s="56"/>
-      <c r="CU4" s="57" t="s">
+      <c r="CP4" s="26"/>
+      <c r="CQ4" s="26"/>
+      <c r="CR4" s="26"/>
+      <c r="CS4" s="26"/>
+      <c r="CT4" s="27"/>
+      <c r="CU4" s="28" t="s">
         <v>47</v>
       </c>
-      <c r="CV4" s="58"/>
-      <c r="CW4" s="58"/>
-      <c r="CX4" s="58"/>
-      <c r="CY4" s="58"/>
-      <c r="CZ4" s="58"/>
-      <c r="DA4" s="59"/>
-      <c r="DB4" s="77" t="s">
-        <v>73</v>
-      </c>
-      <c r="DC4" s="78"/>
-      <c r="DD4" s="78"/>
-      <c r="DE4" s="78"/>
-      <c r="DF4" s="78"/>
-      <c r="DG4" s="78"/>
-      <c r="DH4" s="79"/>
-      <c r="DI4" s="75" t="s">
+      <c r="CV4" s="29"/>
+      <c r="CW4" s="29"/>
+      <c r="CX4" s="29"/>
+      <c r="CY4" s="29"/>
+      <c r="CZ4" s="29"/>
+      <c r="DA4" s="30"/>
+      <c r="DB4" s="48" t="s">
+        <v>72</v>
+      </c>
+      <c r="DC4" s="49"/>
+      <c r="DD4" s="49"/>
+      <c r="DE4" s="49"/>
+      <c r="DF4" s="49"/>
+      <c r="DG4" s="49"/>
+      <c r="DH4" s="50"/>
+      <c r="DI4" s="46" t="s">
         <v>39</v>
       </c>
-      <c r="DJ4" s="76"/>
-      <c r="DK4" s="76"/>
-      <c r="DL4" s="76"/>
-      <c r="DM4" s="76"/>
-      <c r="DN4" s="76"/>
-      <c r="DO4" s="76"/>
+      <c r="DJ4" s="47"/>
+      <c r="DK4" s="47"/>
+      <c r="DL4" s="47"/>
+      <c r="DM4" s="47"/>
+      <c r="DN4" s="47"/>
+      <c r="DO4" s="47"/>
       <c r="DP4" s="21"/>
-      <c r="DQ4" s="51" t="s">
+      <c r="DQ4" s="22" t="s">
         <v>45</v>
       </c>
-      <c r="DR4" s="52"/>
-      <c r="DS4" s="52"/>
-      <c r="DT4" s="52"/>
-      <c r="DU4" s="52"/>
-      <c r="DV4" s="53"/>
-      <c r="DW4" s="45" t="s">
+      <c r="DR4" s="23"/>
+      <c r="DS4" s="23"/>
+      <c r="DT4" s="23"/>
+      <c r="DU4" s="23"/>
+      <c r="DV4" s="24"/>
+      <c r="DW4" s="64" t="s">
         <v>13</v>
       </c>
-      <c r="DX4" s="44" t="s">
+      <c r="DX4" s="63" t="s">
         <v>12</v>
       </c>
       <c r="DY4" s="5"/>
@@ -3342,201 +3347,201 @@
       <c r="B5" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="42" t="s">
+      <c r="C5" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
+      <c r="D5" s="61"/>
+      <c r="E5" s="61"/>
+      <c r="F5" s="61"/>
       <c r="G5" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I5" s="25" t="s">
+      <c r="I5" s="57" t="s">
         <v>19</v>
       </c>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="24"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="58"/>
+      <c r="L5" s="58"/>
+      <c r="M5" s="59"/>
       <c r="N5" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="25" t="s">
+      <c r="O5" s="57" t="s">
         <v>23</v>
       </c>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="24"/>
+      <c r="P5" s="58"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="58"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="58"/>
+      <c r="U5" s="59"/>
       <c r="V5" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="W5" s="25" t="s">
+      <c r="W5" s="57" t="s">
         <v>25</v>
       </c>
-      <c r="X5" s="23"/>
-      <c r="Y5" s="23"/>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23"/>
-      <c r="AB5" s="24"/>
+      <c r="X5" s="58"/>
+      <c r="Y5" s="58"/>
+      <c r="Z5" s="58"/>
+      <c r="AA5" s="58"/>
+      <c r="AB5" s="59"/>
       <c r="AC5" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="25" t="s">
+      <c r="AD5" s="57" t="s">
         <v>30</v>
       </c>
-      <c r="AE5" s="23"/>
-      <c r="AF5" s="23"/>
-      <c r="AG5" s="23"/>
-      <c r="AH5" s="23"/>
-      <c r="AI5" s="24"/>
+      <c r="AE5" s="58"/>
+      <c r="AF5" s="58"/>
+      <c r="AG5" s="58"/>
+      <c r="AH5" s="58"/>
+      <c r="AI5" s="59"/>
       <c r="AJ5" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AK5" s="25" t="s">
+      <c r="AK5" s="57" t="s">
         <v>35</v>
       </c>
-      <c r="AL5" s="23"/>
-      <c r="AM5" s="23"/>
-      <c r="AN5" s="23"/>
-      <c r="AO5" s="23"/>
-      <c r="AP5" s="24"/>
+      <c r="AL5" s="58"/>
+      <c r="AM5" s="58"/>
+      <c r="AN5" s="58"/>
+      <c r="AO5" s="58"/>
+      <c r="AP5" s="59"/>
       <c r="AQ5" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AR5" s="25" t="s">
+      <c r="AR5" s="57" t="s">
         <v>36</v>
       </c>
-      <c r="AS5" s="23"/>
-      <c r="AT5" s="23"/>
-      <c r="AU5" s="23"/>
-      <c r="AV5" s="23"/>
-      <c r="AW5" s="24"/>
+      <c r="AS5" s="58"/>
+      <c r="AT5" s="58"/>
+      <c r="AU5" s="58"/>
+      <c r="AV5" s="58"/>
+      <c r="AW5" s="59"/>
       <c r="AX5" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="AY5" s="25" t="s">
+      <c r="AY5" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="AZ5" s="23"/>
-      <c r="BA5" s="23"/>
-      <c r="BB5" s="24"/>
-      <c r="BC5" s="25" t="s">
+      <c r="AZ5" s="58"/>
+      <c r="BA5" s="58"/>
+      <c r="BB5" s="59"/>
+      <c r="BC5" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="BD5" s="24"/>
-      <c r="BE5" s="45"/>
-      <c r="BF5" s="44"/>
-      <c r="BG5" s="25" t="s">
+      <c r="BD5" s="59"/>
+      <c r="BE5" s="64"/>
+      <c r="BF5" s="63"/>
+      <c r="BG5" s="57" t="s">
         <v>50</v>
       </c>
-      <c r="BH5" s="23"/>
-      <c r="BI5" s="23"/>
-      <c r="BJ5" s="23"/>
-      <c r="BK5" s="24"/>
+      <c r="BH5" s="58"/>
+      <c r="BI5" s="58"/>
+      <c r="BJ5" s="58"/>
+      <c r="BK5" s="59"/>
       <c r="BL5" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="BM5" s="25" t="s">
+      <c r="BM5" s="57" t="s">
         <v>51</v>
       </c>
-      <c r="BN5" s="23"/>
-      <c r="BO5" s="23"/>
-      <c r="BP5" s="23"/>
-      <c r="BQ5" s="23"/>
-      <c r="BR5" s="24"/>
+      <c r="BN5" s="58"/>
+      <c r="BO5" s="58"/>
+      <c r="BP5" s="58"/>
+      <c r="BQ5" s="58"/>
+      <c r="BR5" s="59"/>
       <c r="BS5" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="BT5" s="25" t="s">
-        <v>65</v>
-      </c>
-      <c r="BU5" s="23"/>
-      <c r="BV5" s="23"/>
-      <c r="BW5" s="23"/>
-      <c r="BX5" s="23"/>
-      <c r="BY5" s="24"/>
+      <c r="BT5" s="57" t="s">
+        <v>64</v>
+      </c>
+      <c r="BU5" s="58"/>
+      <c r="BV5" s="58"/>
+      <c r="BW5" s="58"/>
+      <c r="BX5" s="58"/>
+      <c r="BY5" s="59"/>
       <c r="BZ5" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="CA5" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="CB5" s="23"/>
-      <c r="CC5" s="23"/>
-      <c r="CD5" s="23"/>
-      <c r="CE5" s="23"/>
-      <c r="CF5" s="24"/>
+      <c r="CA5" s="57" t="s">
+        <v>65</v>
+      </c>
+      <c r="CB5" s="58"/>
+      <c r="CC5" s="58"/>
+      <c r="CD5" s="58"/>
+      <c r="CE5" s="58"/>
+      <c r="CF5" s="59"/>
       <c r="CG5" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="CH5" s="25" t="s">
-        <v>68</v>
-      </c>
-      <c r="CI5" s="23"/>
-      <c r="CJ5" s="23"/>
-      <c r="CK5" s="23"/>
-      <c r="CL5" s="23"/>
-      <c r="CM5" s="24"/>
+      <c r="CH5" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="CI5" s="58"/>
+      <c r="CJ5" s="58"/>
+      <c r="CK5" s="58"/>
+      <c r="CL5" s="58"/>
+      <c r="CM5" s="59"/>
       <c r="CN5" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="CO5" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="CP5" s="23"/>
-      <c r="CQ5" s="23"/>
-      <c r="CR5" s="23"/>
-      <c r="CS5" s="23"/>
-      <c r="CT5" s="24"/>
+      <c r="CO5" s="57" t="s">
+        <v>68</v>
+      </c>
+      <c r="CP5" s="58"/>
+      <c r="CQ5" s="58"/>
+      <c r="CR5" s="58"/>
+      <c r="CS5" s="58"/>
+      <c r="CT5" s="59"/>
       <c r="CU5" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="CV5" s="25" t="s">
+      <c r="CV5" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="CW5" s="58"/>
+      <c r="CX5" s="58"/>
+      <c r="CY5" s="58"/>
+      <c r="CZ5" s="58"/>
+      <c r="DA5" s="59"/>
+      <c r="DB5" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="DC5" s="79" t="s">
         <v>71</v>
       </c>
-      <c r="CW5" s="23"/>
-      <c r="CX5" s="23"/>
-      <c r="CY5" s="23"/>
-      <c r="CZ5" s="23"/>
-      <c r="DA5" s="24"/>
-      <c r="DB5" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="DC5" s="26" t="s">
-        <v>72</v>
-      </c>
-      <c r="DD5" s="27"/>
-      <c r="DE5" s="27"/>
-      <c r="DF5" s="27"/>
-      <c r="DG5" s="27"/>
-      <c r="DH5" s="28"/>
+      <c r="DD5" s="74"/>
+      <c r="DE5" s="74"/>
+      <c r="DF5" s="74"/>
+      <c r="DG5" s="74"/>
+      <c r="DH5" s="75"/>
       <c r="DI5" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="DJ5" s="25" t="s">
-        <v>76</v>
-      </c>
-      <c r="DK5" s="23"/>
-      <c r="DL5" s="23"/>
-      <c r="DM5" s="23"/>
-      <c r="DN5" s="23"/>
-      <c r="DO5" s="24"/>
+      <c r="DJ5" s="57" t="s">
+        <v>75</v>
+      </c>
+      <c r="DK5" s="58"/>
+      <c r="DL5" s="58"/>
+      <c r="DM5" s="58"/>
+      <c r="DN5" s="58"/>
+      <c r="DO5" s="59"/>
       <c r="DP5" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="DQ5" s="25" t="s">
-        <v>61</v>
-      </c>
-      <c r="DR5" s="23"/>
-      <c r="DS5" s="23"/>
-      <c r="DT5" s="23"/>
-      <c r="DU5" s="23"/>
-      <c r="DV5" s="24"/>
-      <c r="DW5" s="45"/>
-      <c r="DX5" s="44"/>
+      <c r="DQ5" s="57" t="s">
+        <v>77</v>
+      </c>
+      <c r="DR5" s="58"/>
+      <c r="DS5" s="58"/>
+      <c r="DT5" s="58"/>
+      <c r="DU5" s="58"/>
+      <c r="DV5" s="59"/>
+      <c r="DW5" s="64"/>
+      <c r="DX5" s="63"/>
     </row>
     <row r="6" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
@@ -3548,103 +3553,103 @@
       <c r="N6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="V6" s="46" t="s">
+      <c r="V6" s="65" t="s">
         <v>24</v>
       </c>
       <c r="AC6" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="AK6" s="22" t="s">
+      <c r="AK6" s="73" t="s">
         <v>32</v>
       </c>
-      <c r="AL6" s="27"/>
-      <c r="AM6" s="27"/>
-      <c r="AN6" s="27"/>
-      <c r="AO6" s="27"/>
-      <c r="AP6" s="28"/>
-      <c r="AV6" s="49" t="s">
+      <c r="AL6" s="74"/>
+      <c r="AM6" s="74"/>
+      <c r="AN6" s="74"/>
+      <c r="AO6" s="74"/>
+      <c r="AP6" s="75"/>
+      <c r="AV6" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="AW6" s="50"/>
+      <c r="AW6" s="69"/>
       <c r="AX6" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="AY6" s="25"/>
-      <c r="AZ6" s="23"/>
-      <c r="BA6" s="23"/>
-      <c r="BB6" s="24"/>
-      <c r="BC6" s="25" t="s">
+      <c r="AY6" s="57"/>
+      <c r="AZ6" s="58"/>
+      <c r="BA6" s="58"/>
+      <c r="BB6" s="59"/>
+      <c r="BC6" s="57" t="s">
         <v>31</v>
       </c>
-      <c r="BD6" s="24"/>
-      <c r="BE6" s="45"/>
-      <c r="BF6" s="44"/>
-      <c r="BG6" s="25" t="s">
+      <c r="BD6" s="59"/>
+      <c r="BE6" s="64"/>
+      <c r="BF6" s="63"/>
+      <c r="BG6" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="BH6" s="58"/>
+      <c r="BI6" s="58"/>
+      <c r="BJ6" s="58"/>
+      <c r="BK6" s="59"/>
+      <c r="BM6" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="BH6" s="23"/>
-      <c r="BI6" s="23"/>
-      <c r="BJ6" s="23"/>
-      <c r="BK6" s="24"/>
-      <c r="BM6" s="25" t="s">
+      <c r="BN6" s="58"/>
+      <c r="BO6" s="58"/>
+      <c r="BP6" s="58"/>
+      <c r="BQ6" s="58"/>
+      <c r="BR6" s="59"/>
+      <c r="BZ6" s="18" t="s">
+        <v>76</v>
+      </c>
+      <c r="CG6" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="CH6" s="76" t="s">
         <v>63</v>
       </c>
-      <c r="BN6" s="23"/>
-      <c r="BO6" s="23"/>
-      <c r="BP6" s="23"/>
-      <c r="BQ6" s="23"/>
-      <c r="BR6" s="24"/>
-      <c r="BZ6" s="18" t="s">
-        <v>77</v>
-      </c>
-      <c r="CG6" s="19" t="s">
-        <v>67</v>
-      </c>
-      <c r="CH6" s="32" t="s">
-        <v>64</v>
-      </c>
-      <c r="CI6" s="33"/>
-      <c r="CJ6" s="33"/>
-      <c r="CK6" s="33"/>
-      <c r="CL6" s="33"/>
-      <c r="CM6" s="34"/>
+      <c r="CI6" s="77"/>
+      <c r="CJ6" s="77"/>
+      <c r="CK6" s="77"/>
+      <c r="CL6" s="77"/>
+      <c r="CM6" s="78"/>
       <c r="CN6" s="20" t="s">
         <v>57</v>
       </c>
-      <c r="CO6" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="CP6" s="23"/>
-      <c r="CQ6" s="23"/>
-      <c r="CR6" s="23"/>
-      <c r="CS6" s="23"/>
-      <c r="CT6" s="24"/>
-      <c r="CV6" s="25" t="s">
-        <v>70</v>
-      </c>
-      <c r="CW6" s="23"/>
-      <c r="CX6" s="23"/>
-      <c r="CY6" s="23"/>
-      <c r="CZ6" s="23"/>
-      <c r="DA6" s="24"/>
-      <c r="DC6" s="22" t="s">
-        <v>75</v>
-      </c>
-      <c r="DD6" s="23"/>
-      <c r="DE6" s="23"/>
-      <c r="DF6" s="23"/>
-      <c r="DG6" s="23"/>
-      <c r="DH6" s="24"/>
+      <c r="CO6" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="CP6" s="58"/>
+      <c r="CQ6" s="58"/>
+      <c r="CR6" s="58"/>
+      <c r="CS6" s="58"/>
+      <c r="CT6" s="59"/>
+      <c r="CV6" s="57" t="s">
+        <v>69</v>
+      </c>
+      <c r="CW6" s="58"/>
+      <c r="CX6" s="58"/>
+      <c r="CY6" s="58"/>
+      <c r="CZ6" s="58"/>
+      <c r="DA6" s="59"/>
+      <c r="DC6" s="73" t="s">
+        <v>74</v>
+      </c>
+      <c r="DD6" s="58"/>
+      <c r="DE6" s="58"/>
+      <c r="DF6" s="58"/>
+      <c r="DG6" s="58"/>
+      <c r="DH6" s="59"/>
       <c r="DI6" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="DW6" s="45"/>
-      <c r="DX6" s="44"/>
+      <c r="DW6" s="64"/>
+      <c r="DX6" s="63"/>
     </row>
     <row r="7" spans="1:157" s="4" customFormat="1" ht="409" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="V7" s="47"/>
-      <c r="BF7" s="44"/>
-      <c r="DX7" s="44"/>
+      <c r="V7" s="66"/>
+      <c r="BF7" s="63"/>
+      <c r="DX7" s="63"/>
     </row>
     <row r="8" spans="1:157" s="4" customFormat="1" ht="234" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
@@ -3652,22 +3657,37 @@
       </c>
       <c r="B8" s="7">
         <f ca="1">TODAY()</f>
-        <v>44794</v>
-      </c>
-      <c r="V8" s="48"/>
+        <v>44801</v>
+      </c>
+      <c r="V8" s="67"/>
     </row>
   </sheetData>
   <mergeCells count="51">
-    <mergeCell ref="DQ4:DV4"/>
-    <mergeCell ref="CO4:CT4"/>
-    <mergeCell ref="CU4:DA4"/>
-    <mergeCell ref="BG4:BL4"/>
-    <mergeCell ref="BM4:BS4"/>
-    <mergeCell ref="BT4:BZ4"/>
-    <mergeCell ref="CA4:CG4"/>
-    <mergeCell ref="CH4:CN4"/>
-    <mergeCell ref="DI4:DO4"/>
-    <mergeCell ref="DB4:DH4"/>
+    <mergeCell ref="DC6:DH6"/>
+    <mergeCell ref="DQ5:DV5"/>
+    <mergeCell ref="DC5:DH5"/>
+    <mergeCell ref="BT5:BY5"/>
+    <mergeCell ref="CA5:CF5"/>
+    <mergeCell ref="CH5:CM5"/>
+    <mergeCell ref="CO5:CT5"/>
+    <mergeCell ref="CV5:DA5"/>
+    <mergeCell ref="DJ5:DO5"/>
+    <mergeCell ref="BG5:BK5"/>
+    <mergeCell ref="BM5:BR5"/>
+    <mergeCell ref="CO6:CT6"/>
+    <mergeCell ref="CV6:DA6"/>
+    <mergeCell ref="W4:AW4"/>
+    <mergeCell ref="BC4:BD4"/>
+    <mergeCell ref="AX4:BB4"/>
+    <mergeCell ref="AK6:AP6"/>
+    <mergeCell ref="BC6:BD6"/>
+    <mergeCell ref="AD5:AI5"/>
+    <mergeCell ref="AK5:AP5"/>
+    <mergeCell ref="AR5:AW5"/>
+    <mergeCell ref="BC5:BD5"/>
+    <mergeCell ref="BG6:BK6"/>
+    <mergeCell ref="BM6:BR6"/>
+    <mergeCell ref="CH6:CM6"/>
     <mergeCell ref="A1:DX2"/>
     <mergeCell ref="I5:M5"/>
     <mergeCell ref="O5:U5"/>
@@ -3684,31 +3704,16 @@
     <mergeCell ref="AY6:BB6"/>
     <mergeCell ref="AV6:AW6"/>
     <mergeCell ref="AY5:BB5"/>
-    <mergeCell ref="BG5:BK5"/>
-    <mergeCell ref="BM5:BR5"/>
-    <mergeCell ref="CO6:CT6"/>
-    <mergeCell ref="CV6:DA6"/>
-    <mergeCell ref="W4:AW4"/>
-    <mergeCell ref="BC4:BD4"/>
-    <mergeCell ref="AX4:BB4"/>
-    <mergeCell ref="AK6:AP6"/>
-    <mergeCell ref="BC6:BD6"/>
-    <mergeCell ref="AD5:AI5"/>
-    <mergeCell ref="AK5:AP5"/>
-    <mergeCell ref="AR5:AW5"/>
-    <mergeCell ref="BC5:BD5"/>
-    <mergeCell ref="BG6:BK6"/>
-    <mergeCell ref="BM6:BR6"/>
-    <mergeCell ref="CH6:CM6"/>
-    <mergeCell ref="DC6:DH6"/>
-    <mergeCell ref="DQ5:DV5"/>
-    <mergeCell ref="DC5:DH5"/>
-    <mergeCell ref="BT5:BY5"/>
-    <mergeCell ref="CA5:CF5"/>
-    <mergeCell ref="CH5:CM5"/>
-    <mergeCell ref="CO5:CT5"/>
-    <mergeCell ref="CV5:DA5"/>
-    <mergeCell ref="DJ5:DO5"/>
+    <mergeCell ref="DQ4:DV4"/>
+    <mergeCell ref="CO4:CT4"/>
+    <mergeCell ref="CU4:DA4"/>
+    <mergeCell ref="BG4:BL4"/>
+    <mergeCell ref="BM4:BS4"/>
+    <mergeCell ref="BT4:BZ4"/>
+    <mergeCell ref="CA4:CG4"/>
+    <mergeCell ref="CH4:CN4"/>
+    <mergeCell ref="DI4:DO4"/>
+    <mergeCell ref="DB4:DH4"/>
   </mergeCells>
   <conditionalFormatting sqref="B3:XFD3">
     <cfRule type="cellIs" dxfId="2" priority="1" operator="lessThan">

</xml_diff>